<commit_message>
Teacher sets Switch #$38
</commit_message>
<xml_diff>
--- a/data/Switches.xlsx
+++ b/data/Switches.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="793" uniqueCount="424">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="794" uniqueCount="425">
   <si>
     <t>ID</t>
   </si>
@@ -1289,6 +1289,9 @@
   </si>
   <si>
     <t>Great Wall Hidden DS</t>
+  </si>
+  <si>
+    <t>Talk to teacher</t>
   </si>
 </sst>
 </file>
@@ -1308,28 +1311,28 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1337,7 +1340,7 @@
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1345,7 +1348,7 @@
       <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1353,7 +1356,7 @@
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2395,7 +2398,43 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="47" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="32" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="33" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="27" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="25" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="3" applyBorder="1" applyAlignment="1">
@@ -2404,13 +2443,13 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="28" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="42" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="41" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
@@ -2428,40 +2467,16 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="27" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="25" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="41" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="32" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="42" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2480,18 +2495,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="33" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2804,8 +2807,8 @@
   <dimension ref="A1:O513"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H44" sqref="H44"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -2878,16 +2881,16 @@
         <f>8*A2&amp;"-"&amp;(8*A2+7)</f>
         <v>0-7</v>
       </c>
-      <c r="D2" s="123" t="s">
+      <c r="D2" s="140" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="124"/>
-      <c r="F2" s="124"/>
-      <c r="G2" s="124"/>
-      <c r="H2" s="124"/>
-      <c r="I2" s="124"/>
-      <c r="J2" s="124"/>
-      <c r="K2" s="125"/>
+      <c r="E2" s="136"/>
+      <c r="F2" s="136"/>
+      <c r="G2" s="136"/>
+      <c r="H2" s="136"/>
+      <c r="I2" s="136"/>
+      <c r="J2" s="136"/>
+      <c r="K2" s="137"/>
       <c r="L2" s="119" t="s">
         <v>7</v>
       </c>
@@ -2905,14 +2908,14 @@
         <f t="shared" ref="C3:C33" si="1">8*A3&amp;"-"&amp;(8*A3+7)</f>
         <v>8-15</v>
       </c>
-      <c r="D3" s="129"/>
-      <c r="E3" s="130"/>
-      <c r="F3" s="130"/>
-      <c r="G3" s="130"/>
-      <c r="H3" s="130"/>
-      <c r="I3" s="130"/>
-      <c r="J3" s="130"/>
-      <c r="K3" s="131"/>
+      <c r="D3" s="141"/>
+      <c r="E3" s="142"/>
+      <c r="F3" s="142"/>
+      <c r="G3" s="142"/>
+      <c r="H3" s="142"/>
+      <c r="I3" s="142"/>
+      <c r="J3" s="142"/>
+      <c r="K3" s="143"/>
       <c r="L3" s="119" t="s">
         <v>8</v>
       </c>
@@ -3081,7 +3084,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" ht="15.75" thickBot="1">
       <c r="A8" s="12">
         <f t="shared" si="2"/>
         <v>6</v>
@@ -3122,7 +3125,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:15" ht="15.75" thickBot="1">
       <c r="A9" s="12">
         <f t="shared" si="2"/>
         <v>7</v>
@@ -3154,12 +3157,14 @@
         <v>50</v>
       </c>
       <c r="J9" s="30"/>
-      <c r="K9" s="28"/>
+      <c r="K9" s="99" t="s">
+        <v>424</v>
+      </c>
       <c r="L9" s="6">
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:15" ht="15.75" thickBot="1">
       <c r="A10" s="12">
         <f t="shared" si="2"/>
         <v>8</v>
@@ -8969,16 +8974,16 @@
         <v>AA6</v>
       </c>
       <c r="C168" s="13"/>
-      <c r="D168" s="155" t="s">
+      <c r="D168" s="123" t="s">
         <v>348</v>
       </c>
-      <c r="E168" s="155"/>
-      <c r="F168" s="155"/>
-      <c r="G168" s="155"/>
-      <c r="H168" s="155"/>
-      <c r="I168" s="155"/>
-      <c r="J168" s="155"/>
-      <c r="K168" s="155"/>
+      <c r="E168" s="123"/>
+      <c r="F168" s="123"/>
+      <c r="G168" s="123"/>
+      <c r="H168" s="123"/>
+      <c r="I168" s="123"/>
+      <c r="J168" s="123"/>
+      <c r="K168" s="123"/>
     </row>
     <row r="169" spans="1:14">
       <c r="A169" s="12">
@@ -9104,16 +9109,16 @@
         <v>AAD</v>
       </c>
       <c r="C175" s="13"/>
-      <c r="D175" s="155" t="s">
+      <c r="D175" s="123" t="s">
         <v>349</v>
       </c>
-      <c r="E175" s="155"/>
-      <c r="F175" s="155"/>
-      <c r="G175" s="155"/>
-      <c r="H175" s="155"/>
-      <c r="I175" s="155"/>
-      <c r="J175" s="155"/>
-      <c r="K175" s="155"/>
+      <c r="E175" s="123"/>
+      <c r="F175" s="123"/>
+      <c r="G175" s="123"/>
+      <c r="H175" s="123"/>
+      <c r="I175" s="123"/>
+      <c r="J175" s="123"/>
+      <c r="K175" s="123"/>
     </row>
     <row r="176" spans="1:14">
       <c r="A176" s="12">
@@ -9166,16 +9171,16 @@
         <v>AB0</v>
       </c>
       <c r="C178" s="39"/>
-      <c r="D178" s="155" t="s">
+      <c r="D178" s="123" t="s">
         <v>350</v>
       </c>
-      <c r="E178" s="155"/>
-      <c r="F178" s="155"/>
-      <c r="G178" s="155"/>
-      <c r="H178" s="155"/>
-      <c r="I178" s="155"/>
-      <c r="J178" s="155"/>
-      <c r="K178" s="155"/>
+      <c r="E178" s="123"/>
+      <c r="F178" s="123"/>
+      <c r="G178" s="123"/>
+      <c r="H178" s="123"/>
+      <c r="I178" s="123"/>
+      <c r="J178" s="123"/>
+      <c r="K178" s="123"/>
     </row>
     <row r="179" spans="1:14">
       <c r="A179" s="12">
@@ -9244,16 +9249,16 @@
         <v>AB4</v>
       </c>
       <c r="C182" s="13"/>
-      <c r="D182" s="141" t="s">
+      <c r="D182" s="124" t="s">
         <v>351</v>
       </c>
-      <c r="E182" s="142"/>
-      <c r="F182" s="142"/>
-      <c r="G182" s="142"/>
-      <c r="H182" s="142"/>
-      <c r="I182" s="142"/>
-      <c r="J182" s="142"/>
-      <c r="K182" s="143"/>
+      <c r="E182" s="125"/>
+      <c r="F182" s="125"/>
+      <c r="G182" s="125"/>
+      <c r="H182" s="125"/>
+      <c r="I182" s="125"/>
+      <c r="J182" s="125"/>
+      <c r="K182" s="126"/>
     </row>
     <row r="183" spans="1:14">
       <c r="A183" s="12">
@@ -9265,16 +9270,16 @@
         <v>AB5</v>
       </c>
       <c r="C183" s="13"/>
-      <c r="D183" s="141" t="s">
+      <c r="D183" s="124" t="s">
         <v>352</v>
       </c>
-      <c r="E183" s="142"/>
-      <c r="F183" s="142"/>
-      <c r="G183" s="142"/>
-      <c r="H183" s="142"/>
-      <c r="I183" s="142"/>
-      <c r="J183" s="142"/>
-      <c r="K183" s="143"/>
+      <c r="E183" s="125"/>
+      <c r="F183" s="125"/>
+      <c r="G183" s="125"/>
+      <c r="H183" s="125"/>
+      <c r="I183" s="125"/>
+      <c r="J183" s="125"/>
+      <c r="K183" s="126"/>
     </row>
     <row r="184" spans="1:14">
       <c r="A184" s="12">
@@ -9286,16 +9291,16 @@
         <v>AB6</v>
       </c>
       <c r="C184" s="13"/>
-      <c r="D184" s="141" t="s">
+      <c r="D184" s="124" t="s">
         <v>353</v>
       </c>
-      <c r="E184" s="142"/>
-      <c r="F184" s="142"/>
-      <c r="G184" s="142"/>
-      <c r="H184" s="142"/>
-      <c r="I184" s="142"/>
-      <c r="J184" s="142"/>
-      <c r="K184" s="143"/>
+      <c r="E184" s="125"/>
+      <c r="F184" s="125"/>
+      <c r="G184" s="125"/>
+      <c r="H184" s="125"/>
+      <c r="I184" s="125"/>
+      <c r="J184" s="125"/>
+      <c r="K184" s="126"/>
     </row>
     <row r="185" spans="1:14">
       <c r="A185" s="12">
@@ -9307,16 +9312,16 @@
         <v>AB7</v>
       </c>
       <c r="C185" s="13"/>
-      <c r="D185" s="141" t="s">
+      <c r="D185" s="124" t="s">
         <v>354</v>
       </c>
-      <c r="E185" s="142"/>
-      <c r="F185" s="142"/>
-      <c r="G185" s="142"/>
-      <c r="H185" s="142"/>
-      <c r="I185" s="142"/>
-      <c r="J185" s="142"/>
-      <c r="K185" s="143"/>
+      <c r="E185" s="125"/>
+      <c r="F185" s="125"/>
+      <c r="G185" s="125"/>
+      <c r="H185" s="125"/>
+      <c r="I185" s="125"/>
+      <c r="J185" s="125"/>
+      <c r="K185" s="126"/>
     </row>
     <row r="186" spans="1:14">
       <c r="A186" s="12">
@@ -9328,16 +9333,16 @@
         <v>AB8</v>
       </c>
       <c r="C186" s="13"/>
-      <c r="D186" s="141" t="s">
+      <c r="D186" s="124" t="s">
         <v>355</v>
       </c>
-      <c r="E186" s="142"/>
-      <c r="F186" s="142"/>
-      <c r="G186" s="142"/>
-      <c r="H186" s="142"/>
-      <c r="I186" s="142"/>
-      <c r="J186" s="142"/>
-      <c r="K186" s="143"/>
+      <c r="E186" s="125"/>
+      <c r="F186" s="125"/>
+      <c r="G186" s="125"/>
+      <c r="H186" s="125"/>
+      <c r="I186" s="125"/>
+      <c r="J186" s="125"/>
+      <c r="K186" s="126"/>
     </row>
     <row r="187" spans="1:14">
       <c r="A187" s="12">
@@ -9349,16 +9354,16 @@
         <v>AB9</v>
       </c>
       <c r="C187" s="13"/>
-      <c r="D187" s="141" t="s">
+      <c r="D187" s="124" t="s">
         <v>356</v>
       </c>
-      <c r="E187" s="142"/>
-      <c r="F187" s="142"/>
-      <c r="G187" s="142"/>
-      <c r="H187" s="142"/>
-      <c r="I187" s="142"/>
-      <c r="J187" s="142"/>
-      <c r="K187" s="143"/>
+      <c r="E187" s="125"/>
+      <c r="F187" s="125"/>
+      <c r="G187" s="125"/>
+      <c r="H187" s="125"/>
+      <c r="I187" s="125"/>
+      <c r="J187" s="125"/>
+      <c r="K187" s="126"/>
     </row>
     <row r="188" spans="1:14">
       <c r="A188" s="12">
@@ -9370,16 +9375,16 @@
         <v>ABA</v>
       </c>
       <c r="C188" s="13"/>
-      <c r="D188" s="141" t="s">
+      <c r="D188" s="124" t="s">
         <v>357</v>
       </c>
-      <c r="E188" s="142"/>
-      <c r="F188" s="142"/>
-      <c r="G188" s="142"/>
-      <c r="H188" s="142"/>
-      <c r="I188" s="142"/>
-      <c r="J188" s="142"/>
-      <c r="K188" s="143"/>
+      <c r="E188" s="125"/>
+      <c r="F188" s="125"/>
+      <c r="G188" s="125"/>
+      <c r="H188" s="125"/>
+      <c r="I188" s="125"/>
+      <c r="J188" s="125"/>
+      <c r="K188" s="126"/>
     </row>
     <row r="189" spans="1:14">
       <c r="A189" s="12">
@@ -9391,16 +9396,16 @@
         <v>ABB</v>
       </c>
       <c r="C189" s="13"/>
-      <c r="D189" s="141" t="s">
+      <c r="D189" s="124" t="s">
         <v>358</v>
       </c>
-      <c r="E189" s="142"/>
-      <c r="F189" s="142"/>
-      <c r="G189" s="142"/>
-      <c r="H189" s="142"/>
-      <c r="I189" s="142"/>
-      <c r="J189" s="142"/>
-      <c r="K189" s="143"/>
+      <c r="E189" s="125"/>
+      <c r="F189" s="125"/>
+      <c r="G189" s="125"/>
+      <c r="H189" s="125"/>
+      <c r="I189" s="125"/>
+      <c r="J189" s="125"/>
+      <c r="K189" s="126"/>
     </row>
     <row r="190" spans="1:14">
       <c r="A190" s="12">
@@ -9412,16 +9417,16 @@
         <v>ABC</v>
       </c>
       <c r="C190" s="13"/>
-      <c r="D190" s="141" t="s">
+      <c r="D190" s="124" t="s">
         <v>359</v>
       </c>
-      <c r="E190" s="142"/>
-      <c r="F190" s="142"/>
-      <c r="G190" s="142"/>
-      <c r="H190" s="142"/>
-      <c r="I190" s="142"/>
-      <c r="J190" s="142"/>
-      <c r="K190" s="143"/>
+      <c r="E190" s="125"/>
+      <c r="F190" s="125"/>
+      <c r="G190" s="125"/>
+      <c r="H190" s="125"/>
+      <c r="I190" s="125"/>
+      <c r="J190" s="125"/>
+      <c r="K190" s="126"/>
     </row>
     <row r="191" spans="1:14">
       <c r="A191" s="12">
@@ -9433,16 +9438,16 @@
         <v>ABD</v>
       </c>
       <c r="C191" s="13"/>
-      <c r="D191" s="141" t="s">
+      <c r="D191" s="124" t="s">
         <v>360</v>
       </c>
-      <c r="E191" s="142"/>
-      <c r="F191" s="142"/>
-      <c r="G191" s="142"/>
-      <c r="H191" s="142"/>
-      <c r="I191" s="142"/>
-      <c r="J191" s="142"/>
-      <c r="K191" s="143"/>
+      <c r="E191" s="125"/>
+      <c r="F191" s="125"/>
+      <c r="G191" s="125"/>
+      <c r="H191" s="125"/>
+      <c r="I191" s="125"/>
+      <c r="J191" s="125"/>
+      <c r="K191" s="126"/>
     </row>
     <row r="192" spans="1:14">
       <c r="A192" s="12">
@@ -9454,16 +9459,16 @@
         <v>ABE</v>
       </c>
       <c r="C192" s="13"/>
-      <c r="D192" s="141" t="s">
+      <c r="D192" s="124" t="s">
         <v>361</v>
       </c>
-      <c r="E192" s="142"/>
-      <c r="F192" s="142"/>
-      <c r="G192" s="142"/>
-      <c r="H192" s="142"/>
-      <c r="I192" s="142"/>
-      <c r="J192" s="142"/>
-      <c r="K192" s="143"/>
+      <c r="E192" s="125"/>
+      <c r="F192" s="125"/>
+      <c r="G192" s="125"/>
+      <c r="H192" s="125"/>
+      <c r="I192" s="125"/>
+      <c r="J192" s="125"/>
+      <c r="K192" s="126"/>
     </row>
     <row r="193" spans="1:14" s="1" customFormat="1">
       <c r="A193" s="32">
@@ -9475,16 +9480,16 @@
         <v>ABF</v>
       </c>
       <c r="C193" s="33"/>
-      <c r="D193" s="152" t="s">
+      <c r="D193" s="127" t="s">
         <v>362</v>
       </c>
-      <c r="E193" s="153"/>
-      <c r="F193" s="153"/>
-      <c r="G193" s="153"/>
-      <c r="H193" s="153"/>
-      <c r="I193" s="153"/>
-      <c r="J193" s="153"/>
-      <c r="K193" s="154"/>
+      <c r="E193" s="128"/>
+      <c r="F193" s="128"/>
+      <c r="G193" s="128"/>
+      <c r="H193" s="128"/>
+      <c r="I193" s="128"/>
+      <c r="J193" s="128"/>
+      <c r="K193" s="129"/>
       <c r="L193" s="57"/>
       <c r="M193" s="58"/>
       <c r="N193" s="58"/>
@@ -9499,16 +9504,16 @@
         <v>AC0</v>
       </c>
       <c r="C194" s="39"/>
-      <c r="D194" s="134" t="s">
+      <c r="D194" s="130" t="s">
         <v>363</v>
       </c>
-      <c r="E194" s="127"/>
-      <c r="F194" s="127"/>
-      <c r="G194" s="127"/>
-      <c r="H194" s="127"/>
-      <c r="I194" s="127"/>
-      <c r="J194" s="127"/>
-      <c r="K194" s="135"/>
+      <c r="E194" s="131"/>
+      <c r="F194" s="131"/>
+      <c r="G194" s="131"/>
+      <c r="H194" s="131"/>
+      <c r="I194" s="131"/>
+      <c r="J194" s="131"/>
+      <c r="K194" s="132"/>
     </row>
     <row r="195" spans="1:14">
       <c r="A195" s="12">
@@ -9520,16 +9525,16 @@
         <v>AC1</v>
       </c>
       <c r="C195" s="13"/>
-      <c r="D195" s="141" t="s">
+      <c r="D195" s="124" t="s">
         <v>364</v>
       </c>
-      <c r="E195" s="142"/>
-      <c r="F195" s="142"/>
-      <c r="G195" s="142"/>
-      <c r="H195" s="142"/>
-      <c r="I195" s="142"/>
-      <c r="J195" s="142"/>
-      <c r="K195" s="143"/>
+      <c r="E195" s="125"/>
+      <c r="F195" s="125"/>
+      <c r="G195" s="125"/>
+      <c r="H195" s="125"/>
+      <c r="I195" s="125"/>
+      <c r="J195" s="125"/>
+      <c r="K195" s="126"/>
     </row>
     <row r="196" spans="1:14">
       <c r="A196" s="12">
@@ -9541,16 +9546,16 @@
         <v>AC2</v>
       </c>
       <c r="C196" s="13"/>
-      <c r="D196" s="141" t="s">
+      <c r="D196" s="124" t="s">
         <v>365</v>
       </c>
-      <c r="E196" s="142"/>
-      <c r="F196" s="142"/>
-      <c r="G196" s="142"/>
-      <c r="H196" s="142"/>
-      <c r="I196" s="142"/>
-      <c r="J196" s="142"/>
-      <c r="K196" s="143"/>
+      <c r="E196" s="125"/>
+      <c r="F196" s="125"/>
+      <c r="G196" s="125"/>
+      <c r="H196" s="125"/>
+      <c r="I196" s="125"/>
+      <c r="J196" s="125"/>
+      <c r="K196" s="126"/>
     </row>
     <row r="197" spans="1:14">
       <c r="A197" s="12">
@@ -9562,16 +9567,16 @@
         <v>AC3</v>
       </c>
       <c r="C197" s="13"/>
-      <c r="D197" s="141" t="s">
+      <c r="D197" s="124" t="s">
         <v>366</v>
       </c>
-      <c r="E197" s="142"/>
-      <c r="F197" s="142"/>
-      <c r="G197" s="142"/>
-      <c r="H197" s="142"/>
-      <c r="I197" s="142"/>
-      <c r="J197" s="142"/>
-      <c r="K197" s="143"/>
+      <c r="E197" s="125"/>
+      <c r="F197" s="125"/>
+      <c r="G197" s="125"/>
+      <c r="H197" s="125"/>
+      <c r="I197" s="125"/>
+      <c r="J197" s="125"/>
+      <c r="K197" s="126"/>
     </row>
     <row r="198" spans="1:14">
       <c r="A198" s="12">
@@ -9583,16 +9588,16 @@
         <v>AC4</v>
       </c>
       <c r="C198" s="13"/>
-      <c r="D198" s="141" t="s">
+      <c r="D198" s="124" t="s">
         <v>367</v>
       </c>
-      <c r="E198" s="142"/>
-      <c r="F198" s="142"/>
-      <c r="G198" s="142"/>
-      <c r="H198" s="142"/>
-      <c r="I198" s="142"/>
-      <c r="J198" s="142"/>
-      <c r="K198" s="143"/>
+      <c r="E198" s="125"/>
+      <c r="F198" s="125"/>
+      <c r="G198" s="125"/>
+      <c r="H198" s="125"/>
+      <c r="I198" s="125"/>
+      <c r="J198" s="125"/>
+      <c r="K198" s="126"/>
     </row>
     <row r="199" spans="1:14">
       <c r="A199" s="12">
@@ -9623,16 +9628,16 @@
         <v>AC6</v>
       </c>
       <c r="C200" s="13"/>
-      <c r="D200" s="141" t="s">
+      <c r="D200" s="124" t="s">
         <v>368</v>
       </c>
-      <c r="E200" s="142"/>
-      <c r="F200" s="142"/>
-      <c r="G200" s="142"/>
-      <c r="H200" s="142"/>
-      <c r="I200" s="142"/>
-      <c r="J200" s="142"/>
-      <c r="K200" s="143"/>
+      <c r="E200" s="125"/>
+      <c r="F200" s="125"/>
+      <c r="G200" s="125"/>
+      <c r="H200" s="125"/>
+      <c r="I200" s="125"/>
+      <c r="J200" s="125"/>
+      <c r="K200" s="126"/>
     </row>
     <row r="201" spans="1:14">
       <c r="A201" s="12">
@@ -9663,16 +9668,16 @@
         <v>AC8</v>
       </c>
       <c r="C202" s="13"/>
-      <c r="D202" s="149" t="s">
+      <c r="D202" s="153" t="s">
         <v>369</v>
       </c>
-      <c r="E202" s="150"/>
-      <c r="F202" s="150"/>
-      <c r="G202" s="150"/>
-      <c r="H202" s="150"/>
-      <c r="I202" s="150"/>
-      <c r="J202" s="150"/>
-      <c r="K202" s="151"/>
+      <c r="E202" s="154"/>
+      <c r="F202" s="154"/>
+      <c r="G202" s="154"/>
+      <c r="H202" s="154"/>
+      <c r="I202" s="154"/>
+      <c r="J202" s="154"/>
+      <c r="K202" s="155"/>
     </row>
     <row r="203" spans="1:14">
       <c r="A203" s="12">
@@ -9703,16 +9708,16 @@
         <v>ACA</v>
       </c>
       <c r="C204" s="13"/>
-      <c r="D204" s="141" t="s">
+      <c r="D204" s="124" t="s">
         <v>370</v>
       </c>
-      <c r="E204" s="142"/>
-      <c r="F204" s="142"/>
-      <c r="G204" s="142"/>
-      <c r="H204" s="142"/>
-      <c r="I204" s="142"/>
-      <c r="J204" s="142"/>
-      <c r="K204" s="143"/>
+      <c r="E204" s="125"/>
+      <c r="F204" s="125"/>
+      <c r="G204" s="125"/>
+      <c r="H204" s="125"/>
+      <c r="I204" s="125"/>
+      <c r="J204" s="125"/>
+      <c r="K204" s="126"/>
     </row>
     <row r="205" spans="1:14">
       <c r="A205" s="12">
@@ -9743,16 +9748,16 @@
         <v>ACC</v>
       </c>
       <c r="C206" s="13"/>
-      <c r="D206" s="141" t="s">
+      <c r="D206" s="124" t="s">
         <v>370</v>
       </c>
-      <c r="E206" s="142"/>
-      <c r="F206" s="142"/>
-      <c r="G206" s="142"/>
-      <c r="H206" s="142"/>
-      <c r="I206" s="142"/>
-      <c r="J206" s="142"/>
-      <c r="K206" s="143"/>
+      <c r="E206" s="125"/>
+      <c r="F206" s="125"/>
+      <c r="G206" s="125"/>
+      <c r="H206" s="125"/>
+      <c r="I206" s="125"/>
+      <c r="J206" s="125"/>
+      <c r="K206" s="126"/>
     </row>
     <row r="207" spans="1:14">
       <c r="A207" s="12">
@@ -9783,16 +9788,16 @@
         <v>ACE</v>
       </c>
       <c r="C208" s="13"/>
-      <c r="D208" s="141" t="s">
+      <c r="D208" s="124" t="s">
         <v>371</v>
       </c>
-      <c r="E208" s="142"/>
-      <c r="F208" s="142"/>
-      <c r="G208" s="142"/>
-      <c r="H208" s="142"/>
-      <c r="I208" s="142"/>
-      <c r="J208" s="142"/>
-      <c r="K208" s="143"/>
+      <c r="E208" s="125"/>
+      <c r="F208" s="125"/>
+      <c r="G208" s="125"/>
+      <c r="H208" s="125"/>
+      <c r="I208" s="125"/>
+      <c r="J208" s="125"/>
+      <c r="K208" s="126"/>
     </row>
     <row r="209" spans="1:14" s="1" customFormat="1">
       <c r="A209" s="32">
@@ -9826,16 +9831,16 @@
         <v>AD0</v>
       </c>
       <c r="C210" s="39"/>
-      <c r="D210" s="134" t="s">
+      <c r="D210" s="130" t="s">
         <v>371</v>
       </c>
-      <c r="E210" s="127"/>
-      <c r="F210" s="127"/>
-      <c r="G210" s="127"/>
-      <c r="H210" s="127"/>
-      <c r="I210" s="127"/>
-      <c r="J210" s="127"/>
-      <c r="K210" s="135"/>
+      <c r="E210" s="131"/>
+      <c r="F210" s="131"/>
+      <c r="G210" s="131"/>
+      <c r="H210" s="131"/>
+      <c r="I210" s="131"/>
+      <c r="J210" s="131"/>
+      <c r="K210" s="132"/>
     </row>
     <row r="211" spans="1:14">
       <c r="A211" s="12">
@@ -9904,16 +9909,16 @@
         <v>AD4</v>
       </c>
       <c r="C214" s="13"/>
-      <c r="D214" s="141" t="s">
+      <c r="D214" s="124" t="s">
         <v>372</v>
       </c>
-      <c r="E214" s="142"/>
-      <c r="F214" s="142"/>
-      <c r="G214" s="142"/>
-      <c r="H214" s="142"/>
-      <c r="I214" s="142"/>
-      <c r="J214" s="142"/>
-      <c r="K214" s="143"/>
+      <c r="E214" s="125"/>
+      <c r="F214" s="125"/>
+      <c r="G214" s="125"/>
+      <c r="H214" s="125"/>
+      <c r="I214" s="125"/>
+      <c r="J214" s="125"/>
+      <c r="K214" s="126"/>
     </row>
     <row r="215" spans="1:14">
       <c r="A215" s="12">
@@ -9944,16 +9949,16 @@
         <v>AD6</v>
       </c>
       <c r="C216" s="13"/>
-      <c r="D216" s="132" t="s">
+      <c r="D216" s="144" t="s">
         <v>373</v>
       </c>
-      <c r="E216" s="124"/>
-      <c r="F216" s="124"/>
-      <c r="G216" s="124"/>
-      <c r="H216" s="124"/>
-      <c r="I216" s="124"/>
-      <c r="J216" s="124"/>
-      <c r="K216" s="133"/>
+      <c r="E216" s="136"/>
+      <c r="F216" s="136"/>
+      <c r="G216" s="136"/>
+      <c r="H216" s="136"/>
+      <c r="I216" s="136"/>
+      <c r="J216" s="136"/>
+      <c r="K216" s="145"/>
     </row>
     <row r="217" spans="1:14">
       <c r="A217" s="12">
@@ -9965,14 +9970,14 @@
         <v>AD7</v>
       </c>
       <c r="C217" s="13"/>
-      <c r="D217" s="134"/>
-      <c r="E217" s="127"/>
-      <c r="F217" s="127"/>
-      <c r="G217" s="127"/>
-      <c r="H217" s="127"/>
-      <c r="I217" s="127"/>
-      <c r="J217" s="127"/>
-      <c r="K217" s="135"/>
+      <c r="D217" s="130"/>
+      <c r="E217" s="131"/>
+      <c r="F217" s="131"/>
+      <c r="G217" s="131"/>
+      <c r="H217" s="131"/>
+      <c r="I217" s="131"/>
+      <c r="J217" s="131"/>
+      <c r="K217" s="132"/>
     </row>
     <row r="218" spans="1:14">
       <c r="A218" s="12">
@@ -9984,16 +9989,16 @@
         <v>AD8</v>
       </c>
       <c r="C218" s="13"/>
-      <c r="D218" s="132" t="s">
+      <c r="D218" s="144" t="s">
         <v>374</v>
       </c>
-      <c r="E218" s="124"/>
-      <c r="F218" s="124"/>
-      <c r="G218" s="124"/>
-      <c r="H218" s="124"/>
-      <c r="I218" s="124"/>
-      <c r="J218" s="124"/>
-      <c r="K218" s="133"/>
+      <c r="E218" s="136"/>
+      <c r="F218" s="136"/>
+      <c r="G218" s="136"/>
+      <c r="H218" s="136"/>
+      <c r="I218" s="136"/>
+      <c r="J218" s="136"/>
+      <c r="K218" s="145"/>
     </row>
     <row r="219" spans="1:14">
       <c r="A219" s="12">
@@ -10005,14 +10010,14 @@
         <v>AD9</v>
       </c>
       <c r="C219" s="13"/>
-      <c r="D219" s="134"/>
-      <c r="E219" s="127"/>
-      <c r="F219" s="127"/>
-      <c r="G219" s="127"/>
-      <c r="H219" s="127"/>
-      <c r="I219" s="127"/>
-      <c r="J219" s="127"/>
-      <c r="K219" s="135"/>
+      <c r="D219" s="130"/>
+      <c r="E219" s="131"/>
+      <c r="F219" s="131"/>
+      <c r="G219" s="131"/>
+      <c r="H219" s="131"/>
+      <c r="I219" s="131"/>
+      <c r="J219" s="131"/>
+      <c r="K219" s="132"/>
     </row>
     <row r="220" spans="1:14">
       <c r="A220" s="12">
@@ -10024,16 +10029,16 @@
         <v>ADA</v>
       </c>
       <c r="C220" s="13"/>
-      <c r="D220" s="132" t="s">
+      <c r="D220" s="144" t="s">
         <v>375</v>
       </c>
-      <c r="E220" s="124"/>
-      <c r="F220" s="124"/>
-      <c r="G220" s="124"/>
-      <c r="H220" s="124"/>
-      <c r="I220" s="124"/>
-      <c r="J220" s="124"/>
-      <c r="K220" s="133"/>
+      <c r="E220" s="136"/>
+      <c r="F220" s="136"/>
+      <c r="G220" s="136"/>
+      <c r="H220" s="136"/>
+      <c r="I220" s="136"/>
+      <c r="J220" s="136"/>
+      <c r="K220" s="145"/>
     </row>
     <row r="221" spans="1:14">
       <c r="A221" s="12">
@@ -10045,14 +10050,14 @@
         <v>ADB</v>
       </c>
       <c r="C221" s="13"/>
-      <c r="D221" s="134"/>
-      <c r="E221" s="127"/>
-      <c r="F221" s="127"/>
-      <c r="G221" s="127"/>
-      <c r="H221" s="127"/>
-      <c r="I221" s="127"/>
-      <c r="J221" s="127"/>
-      <c r="K221" s="135"/>
+      <c r="D221" s="130"/>
+      <c r="E221" s="131"/>
+      <c r="F221" s="131"/>
+      <c r="G221" s="131"/>
+      <c r="H221" s="131"/>
+      <c r="I221" s="131"/>
+      <c r="J221" s="131"/>
+      <c r="K221" s="132"/>
     </row>
     <row r="222" spans="1:14">
       <c r="A222" s="12">
@@ -10064,16 +10069,16 @@
         <v>ADC</v>
       </c>
       <c r="C222" s="13"/>
-      <c r="D222" s="141" t="s">
+      <c r="D222" s="124" t="s">
         <v>376</v>
       </c>
-      <c r="E222" s="142"/>
-      <c r="F222" s="142"/>
-      <c r="G222" s="142"/>
-      <c r="H222" s="142"/>
-      <c r="I222" s="142"/>
-      <c r="J222" s="142"/>
-      <c r="K222" s="143"/>
+      <c r="E222" s="125"/>
+      <c r="F222" s="125"/>
+      <c r="G222" s="125"/>
+      <c r="H222" s="125"/>
+      <c r="I222" s="125"/>
+      <c r="J222" s="125"/>
+      <c r="K222" s="126"/>
     </row>
     <row r="223" spans="1:14">
       <c r="A223" s="12">
@@ -10104,16 +10109,16 @@
         <v>ADE</v>
       </c>
       <c r="C224" s="13"/>
-      <c r="D224" s="141" t="s">
+      <c r="D224" s="124" t="s">
         <v>377</v>
       </c>
-      <c r="E224" s="142"/>
-      <c r="F224" s="142"/>
-      <c r="G224" s="142"/>
-      <c r="H224" s="142"/>
-      <c r="I224" s="142"/>
-      <c r="J224" s="142"/>
-      <c r="K224" s="143"/>
+      <c r="E224" s="125"/>
+      <c r="F224" s="125"/>
+      <c r="G224" s="125"/>
+      <c r="H224" s="125"/>
+      <c r="I224" s="125"/>
+      <c r="J224" s="125"/>
+      <c r="K224" s="126"/>
     </row>
     <row r="225" spans="1:14" s="1" customFormat="1">
       <c r="A225" s="32">
@@ -10147,16 +10152,16 @@
         <v>AE0</v>
       </c>
       <c r="C226" s="39"/>
-      <c r="D226" s="146" t="s">
+      <c r="D226" s="150" t="s">
         <v>378</v>
       </c>
-      <c r="E226" s="147"/>
-      <c r="F226" s="147"/>
-      <c r="G226" s="147"/>
-      <c r="H226" s="147"/>
-      <c r="I226" s="147"/>
-      <c r="J226" s="147"/>
-      <c r="K226" s="148"/>
+      <c r="E226" s="151"/>
+      <c r="F226" s="151"/>
+      <c r="G226" s="151"/>
+      <c r="H226" s="151"/>
+      <c r="I226" s="151"/>
+      <c r="J226" s="151"/>
+      <c r="K226" s="152"/>
     </row>
     <row r="227" spans="1:14">
       <c r="A227" s="12">
@@ -10301,16 +10306,16 @@
         <v>AE8</v>
       </c>
       <c r="C234" s="13"/>
-      <c r="D234" s="136" t="s">
+      <c r="D234" s="148" t="s">
         <v>379</v>
       </c>
-      <c r="E234" s="137"/>
-      <c r="F234" s="137"/>
-      <c r="G234" s="137"/>
-      <c r="H234" s="137"/>
-      <c r="I234" s="137"/>
-      <c r="J234" s="137"/>
-      <c r="K234" s="138"/>
+      <c r="E234" s="134"/>
+      <c r="F234" s="134"/>
+      <c r="G234" s="134"/>
+      <c r="H234" s="134"/>
+      <c r="I234" s="134"/>
+      <c r="J234" s="134"/>
+      <c r="K234" s="149"/>
     </row>
     <row r="235" spans="1:14">
       <c r="A235" s="12">
@@ -10379,16 +10384,16 @@
         <v>AEC</v>
       </c>
       <c r="C238" s="13"/>
-      <c r="D238" s="123" t="s">
+      <c r="D238" s="140" t="s">
         <v>380</v>
       </c>
-      <c r="E238" s="124"/>
-      <c r="F238" s="124"/>
-      <c r="G238" s="124"/>
-      <c r="H238" s="124"/>
-      <c r="I238" s="124"/>
-      <c r="J238" s="124"/>
-      <c r="K238" s="125"/>
+      <c r="E238" s="136"/>
+      <c r="F238" s="136"/>
+      <c r="G238" s="136"/>
+      <c r="H238" s="136"/>
+      <c r="I238" s="136"/>
+      <c r="J238" s="136"/>
+      <c r="K238" s="137"/>
     </row>
     <row r="239" spans="1:14">
       <c r="A239" s="12">
@@ -10400,14 +10405,14 @@
         <v>AED</v>
       </c>
       <c r="C239" s="13"/>
-      <c r="D239" s="126"/>
-      <c r="E239" s="127"/>
-      <c r="F239" s="127"/>
-      <c r="G239" s="127"/>
-      <c r="H239" s="127"/>
-      <c r="I239" s="127"/>
-      <c r="J239" s="127"/>
-      <c r="K239" s="128"/>
+      <c r="D239" s="146"/>
+      <c r="E239" s="131"/>
+      <c r="F239" s="131"/>
+      <c r="G239" s="131"/>
+      <c r="H239" s="131"/>
+      <c r="I239" s="131"/>
+      <c r="J239" s="131"/>
+      <c r="K239" s="147"/>
     </row>
     <row r="240" spans="1:14">
       <c r="A240" s="12">
@@ -10419,16 +10424,16 @@
         <v>AEE</v>
       </c>
       <c r="C240" s="70"/>
-      <c r="D240" s="124" t="s">
+      <c r="D240" s="136" t="s">
         <v>381</v>
       </c>
-      <c r="E240" s="124"/>
-      <c r="F240" s="124"/>
-      <c r="G240" s="124"/>
-      <c r="H240" s="124"/>
-      <c r="I240" s="124"/>
-      <c r="J240" s="124"/>
-      <c r="K240" s="125"/>
+      <c r="E240" s="136"/>
+      <c r="F240" s="136"/>
+      <c r="G240" s="136"/>
+      <c r="H240" s="136"/>
+      <c r="I240" s="136"/>
+      <c r="J240" s="136"/>
+      <c r="K240" s="137"/>
     </row>
     <row r="241" spans="1:14" s="1" customFormat="1">
       <c r="A241" s="32">
@@ -10440,14 +10445,14 @@
         <v>AEF</v>
       </c>
       <c r="C241" s="34"/>
-      <c r="D241" s="144"/>
-      <c r="E241" s="144"/>
-      <c r="F241" s="144"/>
-      <c r="G241" s="144"/>
-      <c r="H241" s="144"/>
-      <c r="I241" s="144"/>
-      <c r="J241" s="144"/>
-      <c r="K241" s="145"/>
+      <c r="D241" s="138"/>
+      <c r="E241" s="138"/>
+      <c r="F241" s="138"/>
+      <c r="G241" s="138"/>
+      <c r="H241" s="138"/>
+      <c r="I241" s="138"/>
+      <c r="J241" s="138"/>
+      <c r="K241" s="139"/>
       <c r="L241" s="57"/>
       <c r="M241" s="58"/>
       <c r="N241" s="58"/>
@@ -10638,16 +10643,16 @@
         <v>AF8</v>
       </c>
       <c r="C250" s="13"/>
-      <c r="D250" s="139" t="s">
+      <c r="D250" s="133" t="s">
         <v>382</v>
       </c>
-      <c r="E250" s="137"/>
-      <c r="F250" s="137"/>
-      <c r="G250" s="137"/>
-      <c r="H250" s="137"/>
-      <c r="I250" s="137"/>
-      <c r="J250" s="137"/>
-      <c r="K250" s="140"/>
+      <c r="E250" s="134"/>
+      <c r="F250" s="134"/>
+      <c r="G250" s="134"/>
+      <c r="H250" s="134"/>
+      <c r="I250" s="134"/>
+      <c r="J250" s="134"/>
+      <c r="K250" s="135"/>
     </row>
     <row r="251" spans="1:14">
       <c r="A251" s="12">
@@ -11216,16 +11221,16 @@
         <v>B16</v>
       </c>
       <c r="C280" s="13"/>
-      <c r="D280" s="141" t="s">
+      <c r="D280" s="124" t="s">
         <v>383</v>
       </c>
-      <c r="E280" s="142"/>
-      <c r="F280" s="142"/>
-      <c r="G280" s="142"/>
-      <c r="H280" s="142"/>
-      <c r="I280" s="142"/>
-      <c r="J280" s="142"/>
-      <c r="K280" s="143"/>
+      <c r="E280" s="125"/>
+      <c r="F280" s="125"/>
+      <c r="G280" s="125"/>
+      <c r="H280" s="125"/>
+      <c r="I280" s="125"/>
+      <c r="J280" s="125"/>
+      <c r="K280" s="126"/>
     </row>
     <row r="281" spans="1:14">
       <c r="A281" s="12">
@@ -11332,16 +11337,16 @@
         <v>B1C</v>
       </c>
       <c r="C286" s="13"/>
-      <c r="D286" s="141" t="s">
+      <c r="D286" s="124" t="s">
         <v>384</v>
       </c>
-      <c r="E286" s="142"/>
-      <c r="F286" s="142"/>
-      <c r="G286" s="142"/>
-      <c r="H286" s="142"/>
-      <c r="I286" s="142"/>
-      <c r="J286" s="142"/>
-      <c r="K286" s="143"/>
+      <c r="E286" s="125"/>
+      <c r="F286" s="125"/>
+      <c r="G286" s="125"/>
+      <c r="H286" s="125"/>
+      <c r="I286" s="125"/>
+      <c r="J286" s="125"/>
+      <c r="K286" s="126"/>
     </row>
     <row r="287" spans="1:14">
       <c r="A287" s="12">
@@ -11529,16 +11534,16 @@
         <v>B26</v>
       </c>
       <c r="C296" s="13"/>
-      <c r="D296" s="141" t="s">
+      <c r="D296" s="124" t="s">
         <v>386</v>
       </c>
-      <c r="E296" s="142"/>
-      <c r="F296" s="142"/>
-      <c r="G296" s="142"/>
-      <c r="H296" s="142"/>
-      <c r="I296" s="142"/>
-      <c r="J296" s="142"/>
-      <c r="K296" s="143"/>
+      <c r="E296" s="125"/>
+      <c r="F296" s="125"/>
+      <c r="G296" s="125"/>
+      <c r="H296" s="125"/>
+      <c r="I296" s="125"/>
+      <c r="J296" s="125"/>
+      <c r="K296" s="126"/>
     </row>
     <row r="297" spans="1:14">
       <c r="A297" s="12">
@@ -11569,16 +11574,16 @@
         <v>B28</v>
       </c>
       <c r="C298" s="13"/>
-      <c r="D298" s="123" t="s">
+      <c r="D298" s="140" t="s">
         <v>387</v>
       </c>
-      <c r="E298" s="124"/>
-      <c r="F298" s="124"/>
-      <c r="G298" s="124"/>
-      <c r="H298" s="124"/>
-      <c r="I298" s="124"/>
-      <c r="J298" s="124"/>
-      <c r="K298" s="125"/>
+      <c r="E298" s="136"/>
+      <c r="F298" s="136"/>
+      <c r="G298" s="136"/>
+      <c r="H298" s="136"/>
+      <c r="I298" s="136"/>
+      <c r="J298" s="136"/>
+      <c r="K298" s="137"/>
     </row>
     <row r="299" spans="1:14">
       <c r="A299" s="12">
@@ -11590,14 +11595,14 @@
         <v>B29</v>
       </c>
       <c r="C299" s="13"/>
-      <c r="D299" s="126"/>
-      <c r="E299" s="127"/>
-      <c r="F299" s="127"/>
-      <c r="G299" s="127"/>
-      <c r="H299" s="127"/>
-      <c r="I299" s="127"/>
-      <c r="J299" s="127"/>
-      <c r="K299" s="128"/>
+      <c r="D299" s="146"/>
+      <c r="E299" s="131"/>
+      <c r="F299" s="131"/>
+      <c r="G299" s="131"/>
+      <c r="H299" s="131"/>
+      <c r="I299" s="131"/>
+      <c r="J299" s="131"/>
+      <c r="K299" s="147"/>
     </row>
     <row r="300" spans="1:14">
       <c r="A300" s="12">
@@ -11609,16 +11614,16 @@
         <v>B2A</v>
       </c>
       <c r="C300" s="13"/>
-      <c r="D300" s="123" t="s">
+      <c r="D300" s="140" t="s">
         <v>388</v>
       </c>
-      <c r="E300" s="124"/>
-      <c r="F300" s="124"/>
-      <c r="G300" s="124"/>
-      <c r="H300" s="124"/>
-      <c r="I300" s="124"/>
-      <c r="J300" s="124"/>
-      <c r="K300" s="125"/>
+      <c r="E300" s="136"/>
+      <c r="F300" s="136"/>
+      <c r="G300" s="136"/>
+      <c r="H300" s="136"/>
+      <c r="I300" s="136"/>
+      <c r="J300" s="136"/>
+      <c r="K300" s="137"/>
     </row>
     <row r="301" spans="1:14">
       <c r="A301" s="12">
@@ -11630,14 +11635,14 @@
         <v>B2B</v>
       </c>
       <c r="C301" s="13"/>
-      <c r="D301" s="126"/>
-      <c r="E301" s="127"/>
-      <c r="F301" s="127"/>
-      <c r="G301" s="127"/>
-      <c r="H301" s="127"/>
-      <c r="I301" s="127"/>
-      <c r="J301" s="127"/>
-      <c r="K301" s="128"/>
+      <c r="D301" s="146"/>
+      <c r="E301" s="131"/>
+      <c r="F301" s="131"/>
+      <c r="G301" s="131"/>
+      <c r="H301" s="131"/>
+      <c r="I301" s="131"/>
+      <c r="J301" s="131"/>
+      <c r="K301" s="147"/>
     </row>
     <row r="302" spans="1:14">
       <c r="A302" s="12">
@@ -11649,16 +11654,16 @@
         <v>B2C</v>
       </c>
       <c r="C302" s="13"/>
-      <c r="D302" s="123" t="s">
+      <c r="D302" s="140" t="s">
         <v>389</v>
       </c>
-      <c r="E302" s="124"/>
-      <c r="F302" s="124"/>
-      <c r="G302" s="124"/>
-      <c r="H302" s="124"/>
-      <c r="I302" s="124"/>
-      <c r="J302" s="124"/>
-      <c r="K302" s="125"/>
+      <c r="E302" s="136"/>
+      <c r="F302" s="136"/>
+      <c r="G302" s="136"/>
+      <c r="H302" s="136"/>
+      <c r="I302" s="136"/>
+      <c r="J302" s="136"/>
+      <c r="K302" s="137"/>
     </row>
     <row r="303" spans="1:14">
       <c r="A303" s="12">
@@ -11670,14 +11675,14 @@
         <v>B2D</v>
       </c>
       <c r="C303" s="13"/>
-      <c r="D303" s="126"/>
-      <c r="E303" s="127"/>
-      <c r="F303" s="127"/>
-      <c r="G303" s="127"/>
-      <c r="H303" s="127"/>
-      <c r="I303" s="127"/>
-      <c r="J303" s="127"/>
-      <c r="K303" s="128"/>
+      <c r="D303" s="146"/>
+      <c r="E303" s="131"/>
+      <c r="F303" s="131"/>
+      <c r="G303" s="131"/>
+      <c r="H303" s="131"/>
+      <c r="I303" s="131"/>
+      <c r="J303" s="131"/>
+      <c r="K303" s="147"/>
     </row>
     <row r="304" spans="1:14">
       <c r="A304" s="12">
@@ -11689,16 +11694,16 @@
         <v>B2E</v>
       </c>
       <c r="C304" s="13"/>
-      <c r="D304" s="123" t="s">
+      <c r="D304" s="140" t="s">
         <v>390</v>
       </c>
-      <c r="E304" s="124"/>
-      <c r="F304" s="124"/>
-      <c r="G304" s="124"/>
-      <c r="H304" s="124"/>
-      <c r="I304" s="124"/>
-      <c r="J304" s="124"/>
-      <c r="K304" s="125"/>
+      <c r="E304" s="136"/>
+      <c r="F304" s="136"/>
+      <c r="G304" s="136"/>
+      <c r="H304" s="136"/>
+      <c r="I304" s="136"/>
+      <c r="J304" s="136"/>
+      <c r="K304" s="137"/>
     </row>
     <row r="305" spans="1:14" s="1" customFormat="1">
       <c r="A305" s="32">
@@ -11710,14 +11715,14 @@
         <v>B2F</v>
       </c>
       <c r="C305" s="33"/>
-      <c r="D305" s="126"/>
-      <c r="E305" s="127"/>
-      <c r="F305" s="127"/>
-      <c r="G305" s="127"/>
-      <c r="H305" s="127"/>
-      <c r="I305" s="127"/>
-      <c r="J305" s="127"/>
-      <c r="K305" s="128"/>
+      <c r="D305" s="146"/>
+      <c r="E305" s="131"/>
+      <c r="F305" s="131"/>
+      <c r="G305" s="131"/>
+      <c r="H305" s="131"/>
+      <c r="I305" s="131"/>
+      <c r="J305" s="131"/>
+      <c r="K305" s="147"/>
       <c r="L305" s="57"/>
       <c r="M305" s="58"/>
       <c r="N305" s="58"/>
@@ -11732,16 +11737,16 @@
         <v>B30</v>
       </c>
       <c r="C306" s="39"/>
-      <c r="D306" s="123" t="s">
+      <c r="D306" s="140" t="s">
         <v>391</v>
       </c>
-      <c r="E306" s="124"/>
-      <c r="F306" s="124"/>
-      <c r="G306" s="124"/>
-      <c r="H306" s="124"/>
-      <c r="I306" s="124"/>
-      <c r="J306" s="124"/>
-      <c r="K306" s="125"/>
+      <c r="E306" s="136"/>
+      <c r="F306" s="136"/>
+      <c r="G306" s="136"/>
+      <c r="H306" s="136"/>
+      <c r="I306" s="136"/>
+      <c r="J306" s="136"/>
+      <c r="K306" s="137"/>
     </row>
     <row r="307" spans="1:14">
       <c r="A307" s="12">
@@ -11753,14 +11758,14 @@
         <v>B31</v>
       </c>
       <c r="C307" s="13"/>
-      <c r="D307" s="126"/>
-      <c r="E307" s="127"/>
-      <c r="F307" s="127"/>
-      <c r="G307" s="127"/>
-      <c r="H307" s="127"/>
-      <c r="I307" s="127"/>
-      <c r="J307" s="127"/>
-      <c r="K307" s="128"/>
+      <c r="D307" s="146"/>
+      <c r="E307" s="131"/>
+      <c r="F307" s="131"/>
+      <c r="G307" s="131"/>
+      <c r="H307" s="131"/>
+      <c r="I307" s="131"/>
+      <c r="J307" s="131"/>
+      <c r="K307" s="147"/>
     </row>
     <row r="308" spans="1:14">
       <c r="A308" s="12">
@@ -11772,16 +11777,16 @@
         <v>B32</v>
       </c>
       <c r="C308" s="13"/>
-      <c r="D308" s="123" t="s">
+      <c r="D308" s="140" t="s">
         <v>392</v>
       </c>
-      <c r="E308" s="124"/>
-      <c r="F308" s="124"/>
-      <c r="G308" s="124"/>
-      <c r="H308" s="124"/>
-      <c r="I308" s="124"/>
-      <c r="J308" s="124"/>
-      <c r="K308" s="125"/>
+      <c r="E308" s="136"/>
+      <c r="F308" s="136"/>
+      <c r="G308" s="136"/>
+      <c r="H308" s="136"/>
+      <c r="I308" s="136"/>
+      <c r="J308" s="136"/>
+      <c r="K308" s="137"/>
     </row>
     <row r="309" spans="1:14">
       <c r="A309" s="12">
@@ -11793,14 +11798,14 @@
         <v>B33</v>
       </c>
       <c r="C309" s="13"/>
-      <c r="D309" s="126"/>
-      <c r="E309" s="127"/>
-      <c r="F309" s="127"/>
-      <c r="G309" s="127"/>
-      <c r="H309" s="127"/>
-      <c r="I309" s="127"/>
-      <c r="J309" s="127"/>
-      <c r="K309" s="128"/>
+      <c r="D309" s="146"/>
+      <c r="E309" s="131"/>
+      <c r="F309" s="131"/>
+      <c r="G309" s="131"/>
+      <c r="H309" s="131"/>
+      <c r="I309" s="131"/>
+      <c r="J309" s="131"/>
+      <c r="K309" s="147"/>
     </row>
     <row r="310" spans="1:14">
       <c r="A310" s="12">
@@ -15680,31 +15685,12 @@
     </row>
   </sheetData>
   <mergeCells count="47">
-    <mergeCell ref="D168:K168"/>
-    <mergeCell ref="D175:K175"/>
-    <mergeCell ref="D178:K178"/>
-    <mergeCell ref="D182:K182"/>
-    <mergeCell ref="D183:K183"/>
-    <mergeCell ref="D184:K184"/>
-    <mergeCell ref="D185:K185"/>
-    <mergeCell ref="D186:K186"/>
-    <mergeCell ref="D187:K187"/>
-    <mergeCell ref="D188:K188"/>
-    <mergeCell ref="D189:K189"/>
-    <mergeCell ref="D190:K190"/>
-    <mergeCell ref="D191:K191"/>
-    <mergeCell ref="D192:K192"/>
-    <mergeCell ref="D193:K193"/>
-    <mergeCell ref="D194:K194"/>
-    <mergeCell ref="D195:K195"/>
-    <mergeCell ref="D196:K196"/>
-    <mergeCell ref="D197:K197"/>
-    <mergeCell ref="D198:K198"/>
-    <mergeCell ref="D250:K250"/>
-    <mergeCell ref="D280:K280"/>
-    <mergeCell ref="D286:K286"/>
-    <mergeCell ref="D296:K296"/>
-    <mergeCell ref="D240:K241"/>
+    <mergeCell ref="D304:K305"/>
+    <mergeCell ref="D306:K307"/>
+    <mergeCell ref="D308:K309"/>
+    <mergeCell ref="D298:K299"/>
+    <mergeCell ref="D300:K301"/>
+    <mergeCell ref="D302:K303"/>
     <mergeCell ref="D2:K3"/>
     <mergeCell ref="D216:K217"/>
     <mergeCell ref="D218:K219"/>
@@ -15721,12 +15707,31 @@
     <mergeCell ref="D204:K204"/>
     <mergeCell ref="D206:K206"/>
     <mergeCell ref="D208:K208"/>
-    <mergeCell ref="D304:K305"/>
-    <mergeCell ref="D306:K307"/>
-    <mergeCell ref="D308:K309"/>
-    <mergeCell ref="D298:K299"/>
-    <mergeCell ref="D300:K301"/>
-    <mergeCell ref="D302:K303"/>
+    <mergeCell ref="D250:K250"/>
+    <mergeCell ref="D280:K280"/>
+    <mergeCell ref="D286:K286"/>
+    <mergeCell ref="D296:K296"/>
+    <mergeCell ref="D240:K241"/>
+    <mergeCell ref="D194:K194"/>
+    <mergeCell ref="D195:K195"/>
+    <mergeCell ref="D196:K196"/>
+    <mergeCell ref="D197:K197"/>
+    <mergeCell ref="D198:K198"/>
+    <mergeCell ref="D189:K189"/>
+    <mergeCell ref="D190:K190"/>
+    <mergeCell ref="D191:K191"/>
+    <mergeCell ref="D192:K192"/>
+    <mergeCell ref="D193:K193"/>
+    <mergeCell ref="D184:K184"/>
+    <mergeCell ref="D185:K185"/>
+    <mergeCell ref="D186:K186"/>
+    <mergeCell ref="D187:K187"/>
+    <mergeCell ref="D188:K188"/>
+    <mergeCell ref="D168:K168"/>
+    <mergeCell ref="D175:K175"/>
+    <mergeCell ref="D178:K178"/>
+    <mergeCell ref="D182:K182"/>
+    <mergeCell ref="D183:K183"/>
   </mergeCells>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="53" fitToHeight="0" orientation="landscape" r:id="rId1"/>
@@ -15812,16 +15817,16 @@
         <f>8*A2&amp;"-"&amp;(8*A2+7)</f>
         <v>0-7</v>
       </c>
-      <c r="D2" s="123" t="s">
+      <c r="D2" s="140" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="124"/>
-      <c r="F2" s="124"/>
-      <c r="G2" s="124"/>
-      <c r="H2" s="124"/>
-      <c r="I2" s="124"/>
-      <c r="J2" s="124"/>
-      <c r="K2" s="125"/>
+      <c r="E2" s="136"/>
+      <c r="F2" s="136"/>
+      <c r="G2" s="136"/>
+      <c r="H2" s="136"/>
+      <c r="I2" s="136"/>
+      <c r="J2" s="136"/>
+      <c r="K2" s="137"/>
       <c r="M2" s="3">
         <v>16</v>
       </c>
@@ -15843,14 +15848,14 @@
         <f t="shared" ref="C3:C33" si="2">8*A3&amp;"-"&amp;(8*A3+7)</f>
         <v>8-15</v>
       </c>
-      <c r="D3" s="126"/>
-      <c r="E3" s="127"/>
-      <c r="F3" s="127"/>
-      <c r="G3" s="127"/>
-      <c r="H3" s="127"/>
-      <c r="I3" s="127"/>
-      <c r="J3" s="127"/>
-      <c r="K3" s="131"/>
+      <c r="D3" s="146"/>
+      <c r="E3" s="131"/>
+      <c r="F3" s="131"/>
+      <c r="G3" s="131"/>
+      <c r="H3" s="131"/>
+      <c r="I3" s="131"/>
+      <c r="J3" s="131"/>
+      <c r="K3" s="143"/>
       <c r="M3" s="3">
         <v>17</v>
       </c>
@@ -22099,16 +22104,16 @@
         <v>AB0</v>
       </c>
       <c r="C178" s="39"/>
-      <c r="D178" s="155" t="s">
+      <c r="D178" s="123" t="s">
         <v>350</v>
       </c>
-      <c r="E178" s="155"/>
-      <c r="F178" s="155"/>
-      <c r="G178" s="155"/>
-      <c r="H178" s="155"/>
-      <c r="I178" s="155"/>
-      <c r="J178" s="155"/>
-      <c r="K178" s="155"/>
+      <c r="E178" s="123"/>
+      <c r="F178" s="123"/>
+      <c r="G178" s="123"/>
+      <c r="H178" s="123"/>
+      <c r="I178" s="123"/>
+      <c r="J178" s="123"/>
+      <c r="K178" s="123"/>
     </row>
     <row r="179" spans="1:14">
       <c r="A179" s="12">
@@ -22177,16 +22182,16 @@
         <v>AB4</v>
       </c>
       <c r="C182" s="13"/>
-      <c r="D182" s="141" t="s">
+      <c r="D182" s="124" t="s">
         <v>351</v>
       </c>
-      <c r="E182" s="142"/>
-      <c r="F182" s="142"/>
-      <c r="G182" s="142"/>
-      <c r="H182" s="142"/>
-      <c r="I182" s="142"/>
-      <c r="J182" s="142"/>
-      <c r="K182" s="143"/>
+      <c r="E182" s="125"/>
+      <c r="F182" s="125"/>
+      <c r="G182" s="125"/>
+      <c r="H182" s="125"/>
+      <c r="I182" s="125"/>
+      <c r="J182" s="125"/>
+      <c r="K182" s="126"/>
     </row>
     <row r="183" spans="1:14">
       <c r="A183" s="12">
@@ -22198,16 +22203,16 @@
         <v>AB5</v>
       </c>
       <c r="C183" s="13"/>
-      <c r="D183" s="141" t="s">
+      <c r="D183" s="124" t="s">
         <v>352</v>
       </c>
-      <c r="E183" s="142"/>
-      <c r="F183" s="142"/>
-      <c r="G183" s="142"/>
-      <c r="H183" s="142"/>
-      <c r="I183" s="142"/>
-      <c r="J183" s="142"/>
-      <c r="K183" s="143"/>
+      <c r="E183" s="125"/>
+      <c r="F183" s="125"/>
+      <c r="G183" s="125"/>
+      <c r="H183" s="125"/>
+      <c r="I183" s="125"/>
+      <c r="J183" s="125"/>
+      <c r="K183" s="126"/>
     </row>
     <row r="184" spans="1:14">
       <c r="A184" s="12">
@@ -22219,16 +22224,16 @@
         <v>AB6</v>
       </c>
       <c r="C184" s="13"/>
-      <c r="D184" s="141" t="s">
+      <c r="D184" s="124" t="s">
         <v>353</v>
       </c>
-      <c r="E184" s="142"/>
-      <c r="F184" s="142"/>
-      <c r="G184" s="142"/>
-      <c r="H184" s="142"/>
-      <c r="I184" s="142"/>
-      <c r="J184" s="142"/>
-      <c r="K184" s="143"/>
+      <c r="E184" s="125"/>
+      <c r="F184" s="125"/>
+      <c r="G184" s="125"/>
+      <c r="H184" s="125"/>
+      <c r="I184" s="125"/>
+      <c r="J184" s="125"/>
+      <c r="K184" s="126"/>
     </row>
     <row r="185" spans="1:14">
       <c r="A185" s="12">
@@ -22240,16 +22245,16 @@
         <v>AB7</v>
       </c>
       <c r="C185" s="13"/>
-      <c r="D185" s="141" t="s">
+      <c r="D185" s="124" t="s">
         <v>354</v>
       </c>
-      <c r="E185" s="142"/>
-      <c r="F185" s="142"/>
-      <c r="G185" s="142"/>
-      <c r="H185" s="142"/>
-      <c r="I185" s="142"/>
-      <c r="J185" s="142"/>
-      <c r="K185" s="143"/>
+      <c r="E185" s="125"/>
+      <c r="F185" s="125"/>
+      <c r="G185" s="125"/>
+      <c r="H185" s="125"/>
+      <c r="I185" s="125"/>
+      <c r="J185" s="125"/>
+      <c r="K185" s="126"/>
     </row>
     <row r="186" spans="1:14">
       <c r="A186" s="12">
@@ -22261,16 +22266,16 @@
         <v>AB8</v>
       </c>
       <c r="C186" s="13"/>
-      <c r="D186" s="141" t="s">
+      <c r="D186" s="124" t="s">
         <v>355</v>
       </c>
-      <c r="E186" s="142"/>
-      <c r="F186" s="142"/>
-      <c r="G186" s="142"/>
-      <c r="H186" s="142"/>
-      <c r="I186" s="142"/>
-      <c r="J186" s="142"/>
-      <c r="K186" s="143"/>
+      <c r="E186" s="125"/>
+      <c r="F186" s="125"/>
+      <c r="G186" s="125"/>
+      <c r="H186" s="125"/>
+      <c r="I186" s="125"/>
+      <c r="J186" s="125"/>
+      <c r="K186" s="126"/>
     </row>
     <row r="187" spans="1:14">
       <c r="A187" s="12">
@@ -22282,16 +22287,16 @@
         <v>AB9</v>
       </c>
       <c r="C187" s="13"/>
-      <c r="D187" s="141" t="s">
+      <c r="D187" s="124" t="s">
         <v>356</v>
       </c>
-      <c r="E187" s="142"/>
-      <c r="F187" s="142"/>
-      <c r="G187" s="142"/>
-      <c r="H187" s="142"/>
-      <c r="I187" s="142"/>
-      <c r="J187" s="142"/>
-      <c r="K187" s="143"/>
+      <c r="E187" s="125"/>
+      <c r="F187" s="125"/>
+      <c r="G187" s="125"/>
+      <c r="H187" s="125"/>
+      <c r="I187" s="125"/>
+      <c r="J187" s="125"/>
+      <c r="K187" s="126"/>
     </row>
     <row r="188" spans="1:14">
       <c r="A188" s="12">
@@ -22303,16 +22308,16 @@
         <v>ABA</v>
       </c>
       <c r="C188" s="13"/>
-      <c r="D188" s="141" t="s">
+      <c r="D188" s="124" t="s">
         <v>357</v>
       </c>
-      <c r="E188" s="142"/>
-      <c r="F188" s="142"/>
-      <c r="G188" s="142"/>
-      <c r="H188" s="142"/>
-      <c r="I188" s="142"/>
-      <c r="J188" s="142"/>
-      <c r="K188" s="143"/>
+      <c r="E188" s="125"/>
+      <c r="F188" s="125"/>
+      <c r="G188" s="125"/>
+      <c r="H188" s="125"/>
+      <c r="I188" s="125"/>
+      <c r="J188" s="125"/>
+      <c r="K188" s="126"/>
     </row>
     <row r="189" spans="1:14">
       <c r="A189" s="12">
@@ -22324,16 +22329,16 @@
         <v>ABB</v>
       </c>
       <c r="C189" s="13"/>
-      <c r="D189" s="141" t="s">
+      <c r="D189" s="124" t="s">
         <v>358</v>
       </c>
-      <c r="E189" s="142"/>
-      <c r="F189" s="142"/>
-      <c r="G189" s="142"/>
-      <c r="H189" s="142"/>
-      <c r="I189" s="142"/>
-      <c r="J189" s="142"/>
-      <c r="K189" s="143"/>
+      <c r="E189" s="125"/>
+      <c r="F189" s="125"/>
+      <c r="G189" s="125"/>
+      <c r="H189" s="125"/>
+      <c r="I189" s="125"/>
+      <c r="J189" s="125"/>
+      <c r="K189" s="126"/>
     </row>
     <row r="190" spans="1:14">
       <c r="A190" s="12">
@@ -22345,16 +22350,16 @@
         <v>ABC</v>
       </c>
       <c r="C190" s="13"/>
-      <c r="D190" s="141" t="s">
+      <c r="D190" s="124" t="s">
         <v>359</v>
       </c>
-      <c r="E190" s="142"/>
-      <c r="F190" s="142"/>
-      <c r="G190" s="142"/>
-      <c r="H190" s="142"/>
-      <c r="I190" s="142"/>
-      <c r="J190" s="142"/>
-      <c r="K190" s="143"/>
+      <c r="E190" s="125"/>
+      <c r="F190" s="125"/>
+      <c r="G190" s="125"/>
+      <c r="H190" s="125"/>
+      <c r="I190" s="125"/>
+      <c r="J190" s="125"/>
+      <c r="K190" s="126"/>
     </row>
     <row r="191" spans="1:14">
       <c r="A191" s="12">
@@ -22366,16 +22371,16 @@
         <v>ABD</v>
       </c>
       <c r="C191" s="13"/>
-      <c r="D191" s="141" t="s">
+      <c r="D191" s="124" t="s">
         <v>360</v>
       </c>
-      <c r="E191" s="142"/>
-      <c r="F191" s="142"/>
-      <c r="G191" s="142"/>
-      <c r="H191" s="142"/>
-      <c r="I191" s="142"/>
-      <c r="J191" s="142"/>
-      <c r="K191" s="143"/>
+      <c r="E191" s="125"/>
+      <c r="F191" s="125"/>
+      <c r="G191" s="125"/>
+      <c r="H191" s="125"/>
+      <c r="I191" s="125"/>
+      <c r="J191" s="125"/>
+      <c r="K191" s="126"/>
     </row>
     <row r="192" spans="1:14">
       <c r="A192" s="12">
@@ -22387,16 +22392,16 @@
         <v>ABE</v>
       </c>
       <c r="C192" s="13"/>
-      <c r="D192" s="141" t="s">
+      <c r="D192" s="124" t="s">
         <v>361</v>
       </c>
-      <c r="E192" s="142"/>
-      <c r="F192" s="142"/>
-      <c r="G192" s="142"/>
-      <c r="H192" s="142"/>
-      <c r="I192" s="142"/>
-      <c r="J192" s="142"/>
-      <c r="K192" s="143"/>
+      <c r="E192" s="125"/>
+      <c r="F192" s="125"/>
+      <c r="G192" s="125"/>
+      <c r="H192" s="125"/>
+      <c r="I192" s="125"/>
+      <c r="J192" s="125"/>
+      <c r="K192" s="126"/>
     </row>
     <row r="193" spans="1:14" s="1" customFormat="1">
       <c r="A193" s="32">
@@ -22408,16 +22413,16 @@
         <v>ABF</v>
       </c>
       <c r="C193" s="33"/>
-      <c r="D193" s="152" t="s">
+      <c r="D193" s="127" t="s">
         <v>362</v>
       </c>
-      <c r="E193" s="153"/>
-      <c r="F193" s="153"/>
-      <c r="G193" s="153"/>
-      <c r="H193" s="153"/>
-      <c r="I193" s="153"/>
-      <c r="J193" s="153"/>
-      <c r="K193" s="154"/>
+      <c r="E193" s="128"/>
+      <c r="F193" s="128"/>
+      <c r="G193" s="128"/>
+      <c r="H193" s="128"/>
+      <c r="I193" s="128"/>
+      <c r="J193" s="128"/>
+      <c r="K193" s="129"/>
       <c r="L193" s="57"/>
       <c r="M193" s="58"/>
       <c r="N193" s="58"/>
@@ -22432,16 +22437,16 @@
         <v>AC0</v>
       </c>
       <c r="C194" s="39"/>
-      <c r="D194" s="134" t="s">
+      <c r="D194" s="130" t="s">
         <v>363</v>
       </c>
-      <c r="E194" s="127"/>
-      <c r="F194" s="127"/>
-      <c r="G194" s="127"/>
-      <c r="H194" s="127"/>
-      <c r="I194" s="127"/>
-      <c r="J194" s="127"/>
-      <c r="K194" s="135"/>
+      <c r="E194" s="131"/>
+      <c r="F194" s="131"/>
+      <c r="G194" s="131"/>
+      <c r="H194" s="131"/>
+      <c r="I194" s="131"/>
+      <c r="J194" s="131"/>
+      <c r="K194" s="132"/>
     </row>
     <row r="195" spans="1:14">
       <c r="A195" s="12">
@@ -22453,16 +22458,16 @@
         <v>AC1</v>
       </c>
       <c r="C195" s="13"/>
-      <c r="D195" s="141" t="s">
+      <c r="D195" s="124" t="s">
         <v>364</v>
       </c>
-      <c r="E195" s="142"/>
-      <c r="F195" s="142"/>
-      <c r="G195" s="142"/>
-      <c r="H195" s="142"/>
-      <c r="I195" s="142"/>
-      <c r="J195" s="142"/>
-      <c r="K195" s="143"/>
+      <c r="E195" s="125"/>
+      <c r="F195" s="125"/>
+      <c r="G195" s="125"/>
+      <c r="H195" s="125"/>
+      <c r="I195" s="125"/>
+      <c r="J195" s="125"/>
+      <c r="K195" s="126"/>
     </row>
     <row r="196" spans="1:14">
       <c r="A196" s="12">
@@ -22474,16 +22479,16 @@
         <v>AC2</v>
       </c>
       <c r="C196" s="13"/>
-      <c r="D196" s="141" t="s">
+      <c r="D196" s="124" t="s">
         <v>365</v>
       </c>
-      <c r="E196" s="142"/>
-      <c r="F196" s="142"/>
-      <c r="G196" s="142"/>
-      <c r="H196" s="142"/>
-      <c r="I196" s="142"/>
-      <c r="J196" s="142"/>
-      <c r="K196" s="143"/>
+      <c r="E196" s="125"/>
+      <c r="F196" s="125"/>
+      <c r="G196" s="125"/>
+      <c r="H196" s="125"/>
+      <c r="I196" s="125"/>
+      <c r="J196" s="125"/>
+      <c r="K196" s="126"/>
     </row>
     <row r="197" spans="1:14">
       <c r="A197" s="12">
@@ -22495,16 +22500,16 @@
         <v>AC3</v>
       </c>
       <c r="C197" s="13"/>
-      <c r="D197" s="141" t="s">
+      <c r="D197" s="124" t="s">
         <v>366</v>
       </c>
-      <c r="E197" s="142"/>
-      <c r="F197" s="142"/>
-      <c r="G197" s="142"/>
-      <c r="H197" s="142"/>
-      <c r="I197" s="142"/>
-      <c r="J197" s="142"/>
-      <c r="K197" s="143"/>
+      <c r="E197" s="125"/>
+      <c r="F197" s="125"/>
+      <c r="G197" s="125"/>
+      <c r="H197" s="125"/>
+      <c r="I197" s="125"/>
+      <c r="J197" s="125"/>
+      <c r="K197" s="126"/>
     </row>
     <row r="198" spans="1:14">
       <c r="A198" s="12">
@@ -22516,16 +22521,16 @@
         <v>AC4</v>
       </c>
       <c r="C198" s="13"/>
-      <c r="D198" s="141" t="s">
+      <c r="D198" s="124" t="s">
         <v>367</v>
       </c>
-      <c r="E198" s="142"/>
-      <c r="F198" s="142"/>
-      <c r="G198" s="142"/>
-      <c r="H198" s="142"/>
-      <c r="I198" s="142"/>
-      <c r="J198" s="142"/>
-      <c r="K198" s="143"/>
+      <c r="E198" s="125"/>
+      <c r="F198" s="125"/>
+      <c r="G198" s="125"/>
+      <c r="H198" s="125"/>
+      <c r="I198" s="125"/>
+      <c r="J198" s="125"/>
+      <c r="K198" s="126"/>
     </row>
     <row r="199" spans="1:14">
       <c r="A199" s="12">
@@ -22556,16 +22561,16 @@
         <v>AC6</v>
       </c>
       <c r="C200" s="13"/>
-      <c r="D200" s="141" t="s">
+      <c r="D200" s="124" t="s">
         <v>368</v>
       </c>
-      <c r="E200" s="142"/>
-      <c r="F200" s="142"/>
-      <c r="G200" s="142"/>
-      <c r="H200" s="142"/>
-      <c r="I200" s="142"/>
-      <c r="J200" s="142"/>
-      <c r="K200" s="143"/>
+      <c r="E200" s="125"/>
+      <c r="F200" s="125"/>
+      <c r="G200" s="125"/>
+      <c r="H200" s="125"/>
+      <c r="I200" s="125"/>
+      <c r="J200" s="125"/>
+      <c r="K200" s="126"/>
     </row>
     <row r="201" spans="1:14">
       <c r="A201" s="12">
@@ -22596,16 +22601,16 @@
         <v>AC8</v>
       </c>
       <c r="C202" s="13"/>
-      <c r="D202" s="149" t="s">
+      <c r="D202" s="153" t="s">
         <v>369</v>
       </c>
-      <c r="E202" s="150"/>
-      <c r="F202" s="150"/>
-      <c r="G202" s="150"/>
-      <c r="H202" s="150"/>
-      <c r="I202" s="150"/>
-      <c r="J202" s="150"/>
-      <c r="K202" s="151"/>
+      <c r="E202" s="154"/>
+      <c r="F202" s="154"/>
+      <c r="G202" s="154"/>
+      <c r="H202" s="154"/>
+      <c r="I202" s="154"/>
+      <c r="J202" s="154"/>
+      <c r="K202" s="155"/>
     </row>
     <row r="203" spans="1:14">
       <c r="A203" s="12">
@@ -22636,16 +22641,16 @@
         <v>ACA</v>
       </c>
       <c r="C204" s="13"/>
-      <c r="D204" s="141" t="s">
+      <c r="D204" s="124" t="s">
         <v>370</v>
       </c>
-      <c r="E204" s="142"/>
-      <c r="F204" s="142"/>
-      <c r="G204" s="142"/>
-      <c r="H204" s="142"/>
-      <c r="I204" s="142"/>
-      <c r="J204" s="142"/>
-      <c r="K204" s="143"/>
+      <c r="E204" s="125"/>
+      <c r="F204" s="125"/>
+      <c r="G204" s="125"/>
+      <c r="H204" s="125"/>
+      <c r="I204" s="125"/>
+      <c r="J204" s="125"/>
+      <c r="K204" s="126"/>
     </row>
     <row r="205" spans="1:14">
       <c r="A205" s="12">
@@ -22676,16 +22681,16 @@
         <v>ACC</v>
       </c>
       <c r="C206" s="13"/>
-      <c r="D206" s="141" t="s">
+      <c r="D206" s="124" t="s">
         <v>370</v>
       </c>
-      <c r="E206" s="142"/>
-      <c r="F206" s="142"/>
-      <c r="G206" s="142"/>
-      <c r="H206" s="142"/>
-      <c r="I206" s="142"/>
-      <c r="J206" s="142"/>
-      <c r="K206" s="143"/>
+      <c r="E206" s="125"/>
+      <c r="F206" s="125"/>
+      <c r="G206" s="125"/>
+      <c r="H206" s="125"/>
+      <c r="I206" s="125"/>
+      <c r="J206" s="125"/>
+      <c r="K206" s="126"/>
     </row>
     <row r="207" spans="1:14">
       <c r="A207" s="12">
@@ -22716,16 +22721,16 @@
         <v>ACE</v>
       </c>
       <c r="C208" s="13"/>
-      <c r="D208" s="141" t="s">
+      <c r="D208" s="124" t="s">
         <v>371</v>
       </c>
-      <c r="E208" s="142"/>
-      <c r="F208" s="142"/>
-      <c r="G208" s="142"/>
-      <c r="H208" s="142"/>
-      <c r="I208" s="142"/>
-      <c r="J208" s="142"/>
-      <c r="K208" s="143"/>
+      <c r="E208" s="125"/>
+      <c r="F208" s="125"/>
+      <c r="G208" s="125"/>
+      <c r="H208" s="125"/>
+      <c r="I208" s="125"/>
+      <c r="J208" s="125"/>
+      <c r="K208" s="126"/>
     </row>
     <row r="209" spans="1:14" s="1" customFormat="1">
       <c r="A209" s="32">
@@ -22759,16 +22764,16 @@
         <v>AD0</v>
       </c>
       <c r="C210" s="39"/>
-      <c r="D210" s="134" t="s">
+      <c r="D210" s="130" t="s">
         <v>371</v>
       </c>
-      <c r="E210" s="127"/>
-      <c r="F210" s="127"/>
-      <c r="G210" s="127"/>
-      <c r="H210" s="127"/>
-      <c r="I210" s="127"/>
-      <c r="J210" s="127"/>
-      <c r="K210" s="135"/>
+      <c r="E210" s="131"/>
+      <c r="F210" s="131"/>
+      <c r="G210" s="131"/>
+      <c r="H210" s="131"/>
+      <c r="I210" s="131"/>
+      <c r="J210" s="131"/>
+      <c r="K210" s="132"/>
     </row>
     <row r="211" spans="1:14">
       <c r="A211" s="12">
@@ -22837,16 +22842,16 @@
         <v>AD4</v>
       </c>
       <c r="C214" s="13"/>
-      <c r="D214" s="141" t="s">
+      <c r="D214" s="124" t="s">
         <v>372</v>
       </c>
-      <c r="E214" s="142"/>
-      <c r="F214" s="142"/>
-      <c r="G214" s="142"/>
-      <c r="H214" s="142"/>
-      <c r="I214" s="142"/>
-      <c r="J214" s="142"/>
-      <c r="K214" s="143"/>
+      <c r="E214" s="125"/>
+      <c r="F214" s="125"/>
+      <c r="G214" s="125"/>
+      <c r="H214" s="125"/>
+      <c r="I214" s="125"/>
+      <c r="J214" s="125"/>
+      <c r="K214" s="126"/>
     </row>
     <row r="215" spans="1:14">
       <c r="A215" s="12">
@@ -22877,16 +22882,16 @@
         <v>AD6</v>
       </c>
       <c r="C216" s="13"/>
-      <c r="D216" s="132" t="s">
+      <c r="D216" s="144" t="s">
         <v>373</v>
       </c>
-      <c r="E216" s="124"/>
-      <c r="F216" s="124"/>
-      <c r="G216" s="124"/>
-      <c r="H216" s="124"/>
-      <c r="I216" s="124"/>
-      <c r="J216" s="124"/>
-      <c r="K216" s="133"/>
+      <c r="E216" s="136"/>
+      <c r="F216" s="136"/>
+      <c r="G216" s="136"/>
+      <c r="H216" s="136"/>
+      <c r="I216" s="136"/>
+      <c r="J216" s="136"/>
+      <c r="K216" s="145"/>
     </row>
     <row r="217" spans="1:14">
       <c r="A217" s="12">
@@ -22898,14 +22903,14 @@
         <v>AD7</v>
       </c>
       <c r="C217" s="13"/>
-      <c r="D217" s="134"/>
-      <c r="E217" s="127"/>
-      <c r="F217" s="127"/>
-      <c r="G217" s="127"/>
-      <c r="H217" s="127"/>
-      <c r="I217" s="127"/>
-      <c r="J217" s="127"/>
-      <c r="K217" s="135"/>
+      <c r="D217" s="130"/>
+      <c r="E217" s="131"/>
+      <c r="F217" s="131"/>
+      <c r="G217" s="131"/>
+      <c r="H217" s="131"/>
+      <c r="I217" s="131"/>
+      <c r="J217" s="131"/>
+      <c r="K217" s="132"/>
     </row>
     <row r="218" spans="1:14">
       <c r="A218" s="12">
@@ -22917,16 +22922,16 @@
         <v>AD8</v>
       </c>
       <c r="C218" s="13"/>
-      <c r="D218" s="132" t="s">
+      <c r="D218" s="144" t="s">
         <v>374</v>
       </c>
-      <c r="E218" s="124"/>
-      <c r="F218" s="124"/>
-      <c r="G218" s="124"/>
-      <c r="H218" s="124"/>
-      <c r="I218" s="124"/>
-      <c r="J218" s="124"/>
-      <c r="K218" s="133"/>
+      <c r="E218" s="136"/>
+      <c r="F218" s="136"/>
+      <c r="G218" s="136"/>
+      <c r="H218" s="136"/>
+      <c r="I218" s="136"/>
+      <c r="J218" s="136"/>
+      <c r="K218" s="145"/>
     </row>
     <row r="219" spans="1:14">
       <c r="A219" s="12">
@@ -22938,14 +22943,14 @@
         <v>AD9</v>
       </c>
       <c r="C219" s="13"/>
-      <c r="D219" s="134"/>
-      <c r="E219" s="127"/>
-      <c r="F219" s="127"/>
-      <c r="G219" s="127"/>
-      <c r="H219" s="127"/>
-      <c r="I219" s="127"/>
-      <c r="J219" s="127"/>
-      <c r="K219" s="135"/>
+      <c r="D219" s="130"/>
+      <c r="E219" s="131"/>
+      <c r="F219" s="131"/>
+      <c r="G219" s="131"/>
+      <c r="H219" s="131"/>
+      <c r="I219" s="131"/>
+      <c r="J219" s="131"/>
+      <c r="K219" s="132"/>
     </row>
     <row r="220" spans="1:14">
       <c r="A220" s="12">
@@ -22957,16 +22962,16 @@
         <v>ADA</v>
       </c>
       <c r="C220" s="13"/>
-      <c r="D220" s="132" t="s">
+      <c r="D220" s="144" t="s">
         <v>375</v>
       </c>
-      <c r="E220" s="124"/>
-      <c r="F220" s="124"/>
-      <c r="G220" s="124"/>
-      <c r="H220" s="124"/>
-      <c r="I220" s="124"/>
-      <c r="J220" s="124"/>
-      <c r="K220" s="133"/>
+      <c r="E220" s="136"/>
+      <c r="F220" s="136"/>
+      <c r="G220" s="136"/>
+      <c r="H220" s="136"/>
+      <c r="I220" s="136"/>
+      <c r="J220" s="136"/>
+      <c r="K220" s="145"/>
     </row>
     <row r="221" spans="1:14">
       <c r="A221" s="12">
@@ -22978,14 +22983,14 @@
         <v>ADB</v>
       </c>
       <c r="C221" s="13"/>
-      <c r="D221" s="134"/>
-      <c r="E221" s="127"/>
-      <c r="F221" s="127"/>
-      <c r="G221" s="127"/>
-      <c r="H221" s="127"/>
-      <c r="I221" s="127"/>
-      <c r="J221" s="127"/>
-      <c r="K221" s="135"/>
+      <c r="D221" s="130"/>
+      <c r="E221" s="131"/>
+      <c r="F221" s="131"/>
+      <c r="G221" s="131"/>
+      <c r="H221" s="131"/>
+      <c r="I221" s="131"/>
+      <c r="J221" s="131"/>
+      <c r="K221" s="132"/>
     </row>
     <row r="222" spans="1:14">
       <c r="A222" s="12">
@@ -22997,16 +23002,16 @@
         <v>ADC</v>
       </c>
       <c r="C222" s="13"/>
-      <c r="D222" s="141" t="s">
+      <c r="D222" s="124" t="s">
         <v>376</v>
       </c>
-      <c r="E222" s="142"/>
-      <c r="F222" s="142"/>
-      <c r="G222" s="142"/>
-      <c r="H222" s="142"/>
-      <c r="I222" s="142"/>
-      <c r="J222" s="142"/>
-      <c r="K222" s="143"/>
+      <c r="E222" s="125"/>
+      <c r="F222" s="125"/>
+      <c r="G222" s="125"/>
+      <c r="H222" s="125"/>
+      <c r="I222" s="125"/>
+      <c r="J222" s="125"/>
+      <c r="K222" s="126"/>
     </row>
     <row r="223" spans="1:14">
       <c r="A223" s="12">
@@ -23037,16 +23042,16 @@
         <v>ADE</v>
       </c>
       <c r="C224" s="13"/>
-      <c r="D224" s="141" t="s">
+      <c r="D224" s="124" t="s">
         <v>377</v>
       </c>
-      <c r="E224" s="142"/>
-      <c r="F224" s="142"/>
-      <c r="G224" s="142"/>
-      <c r="H224" s="142"/>
-      <c r="I224" s="142"/>
-      <c r="J224" s="142"/>
-      <c r="K224" s="143"/>
+      <c r="E224" s="125"/>
+      <c r="F224" s="125"/>
+      <c r="G224" s="125"/>
+      <c r="H224" s="125"/>
+      <c r="I224" s="125"/>
+      <c r="J224" s="125"/>
+      <c r="K224" s="126"/>
     </row>
     <row r="225" spans="1:14" s="1" customFormat="1">
       <c r="A225" s="32">
@@ -23080,16 +23085,16 @@
         <v>AE0</v>
       </c>
       <c r="C226" s="39"/>
-      <c r="D226" s="146" t="s">
+      <c r="D226" s="150" t="s">
         <v>378</v>
       </c>
-      <c r="E226" s="147"/>
-      <c r="F226" s="147"/>
-      <c r="G226" s="147"/>
-      <c r="H226" s="147"/>
-      <c r="I226" s="147"/>
-      <c r="J226" s="147"/>
-      <c r="K226" s="148"/>
+      <c r="E226" s="151"/>
+      <c r="F226" s="151"/>
+      <c r="G226" s="151"/>
+      <c r="H226" s="151"/>
+      <c r="I226" s="151"/>
+      <c r="J226" s="151"/>
+      <c r="K226" s="152"/>
     </row>
     <row r="227" spans="1:14">
       <c r="A227" s="12">
@@ -23234,16 +23239,16 @@
         <v>AE8</v>
       </c>
       <c r="C234" s="13"/>
-      <c r="D234" s="136" t="s">
+      <c r="D234" s="148" t="s">
         <v>379</v>
       </c>
-      <c r="E234" s="137"/>
-      <c r="F234" s="137"/>
-      <c r="G234" s="137"/>
-      <c r="H234" s="137"/>
-      <c r="I234" s="137"/>
-      <c r="J234" s="137"/>
-      <c r="K234" s="138"/>
+      <c r="E234" s="134"/>
+      <c r="F234" s="134"/>
+      <c r="G234" s="134"/>
+      <c r="H234" s="134"/>
+      <c r="I234" s="134"/>
+      <c r="J234" s="134"/>
+      <c r="K234" s="149"/>
     </row>
     <row r="235" spans="1:14">
       <c r="A235" s="12">
@@ -23312,16 +23317,16 @@
         <v>AEC</v>
       </c>
       <c r="C238" s="13"/>
-      <c r="D238" s="123" t="s">
+      <c r="D238" s="140" t="s">
         <v>380</v>
       </c>
-      <c r="E238" s="124"/>
-      <c r="F238" s="124"/>
-      <c r="G238" s="124"/>
-      <c r="H238" s="124"/>
-      <c r="I238" s="124"/>
-      <c r="J238" s="124"/>
-      <c r="K238" s="125"/>
+      <c r="E238" s="136"/>
+      <c r="F238" s="136"/>
+      <c r="G238" s="136"/>
+      <c r="H238" s="136"/>
+      <c r="I238" s="136"/>
+      <c r="J238" s="136"/>
+      <c r="K238" s="137"/>
     </row>
     <row r="239" spans="1:14">
       <c r="A239" s="12">
@@ -23333,14 +23338,14 @@
         <v>AED</v>
       </c>
       <c r="C239" s="13"/>
-      <c r="D239" s="126"/>
-      <c r="E239" s="127"/>
-      <c r="F239" s="127"/>
-      <c r="G239" s="127"/>
-      <c r="H239" s="127"/>
-      <c r="I239" s="127"/>
-      <c r="J239" s="127"/>
-      <c r="K239" s="128"/>
+      <c r="D239" s="146"/>
+      <c r="E239" s="131"/>
+      <c r="F239" s="131"/>
+      <c r="G239" s="131"/>
+      <c r="H239" s="131"/>
+      <c r="I239" s="131"/>
+      <c r="J239" s="131"/>
+      <c r="K239" s="147"/>
     </row>
     <row r="240" spans="1:14">
       <c r="A240" s="12">
@@ -23352,16 +23357,16 @@
         <v>AEE</v>
       </c>
       <c r="C240" s="70"/>
-      <c r="D240" s="124" t="s">
+      <c r="D240" s="136" t="s">
         <v>381</v>
       </c>
-      <c r="E240" s="124"/>
-      <c r="F240" s="124"/>
-      <c r="G240" s="124"/>
-      <c r="H240" s="124"/>
-      <c r="I240" s="124"/>
-      <c r="J240" s="124"/>
-      <c r="K240" s="125"/>
+      <c r="E240" s="136"/>
+      <c r="F240" s="136"/>
+      <c r="G240" s="136"/>
+      <c r="H240" s="136"/>
+      <c r="I240" s="136"/>
+      <c r="J240" s="136"/>
+      <c r="K240" s="137"/>
     </row>
     <row r="241" spans="1:14" s="1" customFormat="1">
       <c r="A241" s="32">
@@ -23373,14 +23378,14 @@
         <v>AEF</v>
       </c>
       <c r="C241" s="34"/>
-      <c r="D241" s="144"/>
-      <c r="E241" s="144"/>
-      <c r="F241" s="144"/>
-      <c r="G241" s="144"/>
-      <c r="H241" s="144"/>
-      <c r="I241" s="144"/>
-      <c r="J241" s="144"/>
-      <c r="K241" s="145"/>
+      <c r="D241" s="138"/>
+      <c r="E241" s="138"/>
+      <c r="F241" s="138"/>
+      <c r="G241" s="138"/>
+      <c r="H241" s="138"/>
+      <c r="I241" s="138"/>
+      <c r="J241" s="138"/>
+      <c r="K241" s="139"/>
       <c r="L241" s="57"/>
       <c r="M241" s="58"/>
       <c r="N241" s="58"/>
@@ -23571,16 +23576,16 @@
         <v>AF8</v>
       </c>
       <c r="C250" s="13"/>
-      <c r="D250" s="139" t="s">
+      <c r="D250" s="133" t="s">
         <v>382</v>
       </c>
-      <c r="E250" s="137"/>
-      <c r="F250" s="137"/>
-      <c r="G250" s="137"/>
-      <c r="H250" s="137"/>
-      <c r="I250" s="137"/>
-      <c r="J250" s="137"/>
-      <c r="K250" s="140"/>
+      <c r="E250" s="134"/>
+      <c r="F250" s="134"/>
+      <c r="G250" s="134"/>
+      <c r="H250" s="134"/>
+      <c r="I250" s="134"/>
+      <c r="J250" s="134"/>
+      <c r="K250" s="135"/>
     </row>
     <row r="251" spans="1:14">
       <c r="A251" s="12">
@@ -24149,16 +24154,16 @@
         <v>B16</v>
       </c>
       <c r="C280" s="13"/>
-      <c r="D280" s="141" t="s">
+      <c r="D280" s="124" t="s">
         <v>383</v>
       </c>
-      <c r="E280" s="142"/>
-      <c r="F280" s="142"/>
-      <c r="G280" s="142"/>
-      <c r="H280" s="142"/>
-      <c r="I280" s="142"/>
-      <c r="J280" s="142"/>
-      <c r="K280" s="143"/>
+      <c r="E280" s="125"/>
+      <c r="F280" s="125"/>
+      <c r="G280" s="125"/>
+      <c r="H280" s="125"/>
+      <c r="I280" s="125"/>
+      <c r="J280" s="125"/>
+      <c r="K280" s="126"/>
     </row>
     <row r="281" spans="1:14">
       <c r="A281" s="12">
@@ -24265,16 +24270,16 @@
         <v>B1C</v>
       </c>
       <c r="C286" s="13"/>
-      <c r="D286" s="141" t="s">
+      <c r="D286" s="124" t="s">
         <v>384</v>
       </c>
-      <c r="E286" s="142"/>
-      <c r="F286" s="142"/>
-      <c r="G286" s="142"/>
-      <c r="H286" s="142"/>
-      <c r="I286" s="142"/>
-      <c r="J286" s="142"/>
-      <c r="K286" s="143"/>
+      <c r="E286" s="125"/>
+      <c r="F286" s="125"/>
+      <c r="G286" s="125"/>
+      <c r="H286" s="125"/>
+      <c r="I286" s="125"/>
+      <c r="J286" s="125"/>
+      <c r="K286" s="126"/>
     </row>
     <row r="287" spans="1:14">
       <c r="A287" s="12">
@@ -24462,16 +24467,16 @@
         <v>B26</v>
       </c>
       <c r="C296" s="13"/>
-      <c r="D296" s="141" t="s">
+      <c r="D296" s="124" t="s">
         <v>386</v>
       </c>
-      <c r="E296" s="142"/>
-      <c r="F296" s="142"/>
-      <c r="G296" s="142"/>
-      <c r="H296" s="142"/>
-      <c r="I296" s="142"/>
-      <c r="J296" s="142"/>
-      <c r="K296" s="143"/>
+      <c r="E296" s="125"/>
+      <c r="F296" s="125"/>
+      <c r="G296" s="125"/>
+      <c r="H296" s="125"/>
+      <c r="I296" s="125"/>
+      <c r="J296" s="125"/>
+      <c r="K296" s="126"/>
     </row>
     <row r="297" spans="1:14">
       <c r="A297" s="12">
@@ -24502,16 +24507,16 @@
         <v>B28</v>
       </c>
       <c r="C298" s="13"/>
-      <c r="D298" s="123" t="s">
+      <c r="D298" s="140" t="s">
         <v>387</v>
       </c>
-      <c r="E298" s="124"/>
-      <c r="F298" s="124"/>
-      <c r="G298" s="124"/>
-      <c r="H298" s="124"/>
-      <c r="I298" s="124"/>
-      <c r="J298" s="124"/>
-      <c r="K298" s="125"/>
+      <c r="E298" s="136"/>
+      <c r="F298" s="136"/>
+      <c r="G298" s="136"/>
+      <c r="H298" s="136"/>
+      <c r="I298" s="136"/>
+      <c r="J298" s="136"/>
+      <c r="K298" s="137"/>
     </row>
     <row r="299" spans="1:14">
       <c r="A299" s="12">
@@ -24523,14 +24528,14 @@
         <v>B29</v>
       </c>
       <c r="C299" s="13"/>
-      <c r="D299" s="126"/>
-      <c r="E299" s="127"/>
-      <c r="F299" s="127"/>
-      <c r="G299" s="127"/>
-      <c r="H299" s="127"/>
-      <c r="I299" s="127"/>
-      <c r="J299" s="127"/>
-      <c r="K299" s="128"/>
+      <c r="D299" s="146"/>
+      <c r="E299" s="131"/>
+      <c r="F299" s="131"/>
+      <c r="G299" s="131"/>
+      <c r="H299" s="131"/>
+      <c r="I299" s="131"/>
+      <c r="J299" s="131"/>
+      <c r="K299" s="147"/>
     </row>
     <row r="300" spans="1:14">
       <c r="A300" s="12">
@@ -24542,16 +24547,16 @@
         <v>B2A</v>
       </c>
       <c r="C300" s="13"/>
-      <c r="D300" s="123" t="s">
+      <c r="D300" s="140" t="s">
         <v>388</v>
       </c>
-      <c r="E300" s="124"/>
-      <c r="F300" s="124"/>
-      <c r="G300" s="124"/>
-      <c r="H300" s="124"/>
-      <c r="I300" s="124"/>
-      <c r="J300" s="124"/>
-      <c r="K300" s="125"/>
+      <c r="E300" s="136"/>
+      <c r="F300" s="136"/>
+      <c r="G300" s="136"/>
+      <c r="H300" s="136"/>
+      <c r="I300" s="136"/>
+      <c r="J300" s="136"/>
+      <c r="K300" s="137"/>
     </row>
     <row r="301" spans="1:14">
       <c r="A301" s="12">
@@ -24563,14 +24568,14 @@
         <v>B2B</v>
       </c>
       <c r="C301" s="13"/>
-      <c r="D301" s="126"/>
-      <c r="E301" s="127"/>
-      <c r="F301" s="127"/>
-      <c r="G301" s="127"/>
-      <c r="H301" s="127"/>
-      <c r="I301" s="127"/>
-      <c r="J301" s="127"/>
-      <c r="K301" s="128"/>
+      <c r="D301" s="146"/>
+      <c r="E301" s="131"/>
+      <c r="F301" s="131"/>
+      <c r="G301" s="131"/>
+      <c r="H301" s="131"/>
+      <c r="I301" s="131"/>
+      <c r="J301" s="131"/>
+      <c r="K301" s="147"/>
     </row>
     <row r="302" spans="1:14">
       <c r="A302" s="12">
@@ -24582,16 +24587,16 @@
         <v>B2C</v>
       </c>
       <c r="C302" s="13"/>
-      <c r="D302" s="123" t="s">
+      <c r="D302" s="140" t="s">
         <v>389</v>
       </c>
-      <c r="E302" s="124"/>
-      <c r="F302" s="124"/>
-      <c r="G302" s="124"/>
-      <c r="H302" s="124"/>
-      <c r="I302" s="124"/>
-      <c r="J302" s="124"/>
-      <c r="K302" s="125"/>
+      <c r="E302" s="136"/>
+      <c r="F302" s="136"/>
+      <c r="G302" s="136"/>
+      <c r="H302" s="136"/>
+      <c r="I302" s="136"/>
+      <c r="J302" s="136"/>
+      <c r="K302" s="137"/>
     </row>
     <row r="303" spans="1:14">
       <c r="A303" s="12">
@@ -24603,14 +24608,14 @@
         <v>B2D</v>
       </c>
       <c r="C303" s="13"/>
-      <c r="D303" s="126"/>
-      <c r="E303" s="127"/>
-      <c r="F303" s="127"/>
-      <c r="G303" s="127"/>
-      <c r="H303" s="127"/>
-      <c r="I303" s="127"/>
-      <c r="J303" s="127"/>
-      <c r="K303" s="128"/>
+      <c r="D303" s="146"/>
+      <c r="E303" s="131"/>
+      <c r="F303" s="131"/>
+      <c r="G303" s="131"/>
+      <c r="H303" s="131"/>
+      <c r="I303" s="131"/>
+      <c r="J303" s="131"/>
+      <c r="K303" s="147"/>
     </row>
     <row r="304" spans="1:14">
       <c r="A304" s="12">
@@ -24622,16 +24627,16 @@
         <v>B2E</v>
       </c>
       <c r="C304" s="13"/>
-      <c r="D304" s="123" t="s">
+      <c r="D304" s="140" t="s">
         <v>390</v>
       </c>
-      <c r="E304" s="124"/>
-      <c r="F304" s="124"/>
-      <c r="G304" s="124"/>
-      <c r="H304" s="124"/>
-      <c r="I304" s="124"/>
-      <c r="J304" s="124"/>
-      <c r="K304" s="125"/>
+      <c r="E304" s="136"/>
+      <c r="F304" s="136"/>
+      <c r="G304" s="136"/>
+      <c r="H304" s="136"/>
+      <c r="I304" s="136"/>
+      <c r="J304" s="136"/>
+      <c r="K304" s="137"/>
     </row>
     <row r="305" spans="1:14" s="1" customFormat="1">
       <c r="A305" s="32">
@@ -24643,14 +24648,14 @@
         <v>B2F</v>
       </c>
       <c r="C305" s="33"/>
-      <c r="D305" s="126"/>
-      <c r="E305" s="127"/>
-      <c r="F305" s="127"/>
-      <c r="G305" s="127"/>
-      <c r="H305" s="127"/>
-      <c r="I305" s="127"/>
-      <c r="J305" s="127"/>
-      <c r="K305" s="128"/>
+      <c r="D305" s="146"/>
+      <c r="E305" s="131"/>
+      <c r="F305" s="131"/>
+      <c r="G305" s="131"/>
+      <c r="H305" s="131"/>
+      <c r="I305" s="131"/>
+      <c r="J305" s="131"/>
+      <c r="K305" s="147"/>
       <c r="L305" s="57"/>
       <c r="M305" s="58"/>
       <c r="N305" s="58"/>
@@ -24665,16 +24670,16 @@
         <v>B30</v>
       </c>
       <c r="C306" s="39"/>
-      <c r="D306" s="123" t="s">
+      <c r="D306" s="140" t="s">
         <v>391</v>
       </c>
-      <c r="E306" s="124"/>
-      <c r="F306" s="124"/>
-      <c r="G306" s="124"/>
-      <c r="H306" s="124"/>
-      <c r="I306" s="124"/>
-      <c r="J306" s="124"/>
-      <c r="K306" s="125"/>
+      <c r="E306" s="136"/>
+      <c r="F306" s="136"/>
+      <c r="G306" s="136"/>
+      <c r="H306" s="136"/>
+      <c r="I306" s="136"/>
+      <c r="J306" s="136"/>
+      <c r="K306" s="137"/>
     </row>
     <row r="307" spans="1:14">
       <c r="A307" s="12">
@@ -24686,14 +24691,14 @@
         <v>B31</v>
       </c>
       <c r="C307" s="13"/>
-      <c r="D307" s="126"/>
-      <c r="E307" s="127"/>
-      <c r="F307" s="127"/>
-      <c r="G307" s="127"/>
-      <c r="H307" s="127"/>
-      <c r="I307" s="127"/>
-      <c r="J307" s="127"/>
-      <c r="K307" s="128"/>
+      <c r="D307" s="146"/>
+      <c r="E307" s="131"/>
+      <c r="F307" s="131"/>
+      <c r="G307" s="131"/>
+      <c r="H307" s="131"/>
+      <c r="I307" s="131"/>
+      <c r="J307" s="131"/>
+      <c r="K307" s="147"/>
     </row>
     <row r="308" spans="1:14">
       <c r="A308" s="12">
@@ -24705,16 +24710,16 @@
         <v>B32</v>
       </c>
       <c r="C308" s="13"/>
-      <c r="D308" s="123" t="s">
+      <c r="D308" s="140" t="s">
         <v>392</v>
       </c>
-      <c r="E308" s="124"/>
-      <c r="F308" s="124"/>
-      <c r="G308" s="124"/>
-      <c r="H308" s="124"/>
-      <c r="I308" s="124"/>
-      <c r="J308" s="124"/>
-      <c r="K308" s="125"/>
+      <c r="E308" s="136"/>
+      <c r="F308" s="136"/>
+      <c r="G308" s="136"/>
+      <c r="H308" s="136"/>
+      <c r="I308" s="136"/>
+      <c r="J308" s="136"/>
+      <c r="K308" s="137"/>
     </row>
     <row r="309" spans="1:14">
       <c r="A309" s="12">
@@ -24726,14 +24731,14 @@
         <v>B33</v>
       </c>
       <c r="C309" s="13"/>
-      <c r="D309" s="126"/>
-      <c r="E309" s="127"/>
-      <c r="F309" s="127"/>
-      <c r="G309" s="127"/>
-      <c r="H309" s="127"/>
-      <c r="I309" s="127"/>
-      <c r="J309" s="127"/>
-      <c r="K309" s="128"/>
+      <c r="D309" s="146"/>
+      <c r="E309" s="131"/>
+      <c r="F309" s="131"/>
+      <c r="G309" s="131"/>
+      <c r="H309" s="131"/>
+      <c r="I309" s="131"/>
+      <c r="J309" s="131"/>
+      <c r="K309" s="147"/>
     </row>
     <row r="310" spans="1:14">
       <c r="A310" s="12">
@@ -28613,29 +28618,12 @@
     </row>
   </sheetData>
   <mergeCells count="45">
-    <mergeCell ref="D178:K178"/>
-    <mergeCell ref="D182:K182"/>
-    <mergeCell ref="D183:K183"/>
-    <mergeCell ref="D184:K184"/>
-    <mergeCell ref="D185:K185"/>
-    <mergeCell ref="D186:K186"/>
-    <mergeCell ref="D187:K187"/>
-    <mergeCell ref="D188:K188"/>
-    <mergeCell ref="D189:K189"/>
-    <mergeCell ref="D190:K190"/>
-    <mergeCell ref="D191:K191"/>
-    <mergeCell ref="D192:K192"/>
-    <mergeCell ref="D193:K193"/>
-    <mergeCell ref="D194:K194"/>
-    <mergeCell ref="D195:K195"/>
-    <mergeCell ref="D208:K208"/>
-    <mergeCell ref="D210:K210"/>
-    <mergeCell ref="D214:K214"/>
-    <mergeCell ref="D196:K196"/>
-    <mergeCell ref="D197:K197"/>
-    <mergeCell ref="D198:K198"/>
-    <mergeCell ref="D200:K200"/>
-    <mergeCell ref="D202:K202"/>
+    <mergeCell ref="D308:K309"/>
+    <mergeCell ref="D298:K299"/>
+    <mergeCell ref="D300:K301"/>
+    <mergeCell ref="D302:K303"/>
+    <mergeCell ref="D304:K305"/>
+    <mergeCell ref="D306:K307"/>
     <mergeCell ref="D280:K280"/>
     <mergeCell ref="D286:K286"/>
     <mergeCell ref="D296:K296"/>
@@ -28652,12 +28640,29 @@
     <mergeCell ref="D250:K250"/>
     <mergeCell ref="D204:K204"/>
     <mergeCell ref="D206:K206"/>
-    <mergeCell ref="D308:K309"/>
-    <mergeCell ref="D298:K299"/>
-    <mergeCell ref="D300:K301"/>
-    <mergeCell ref="D302:K303"/>
-    <mergeCell ref="D304:K305"/>
-    <mergeCell ref="D306:K307"/>
+    <mergeCell ref="D208:K208"/>
+    <mergeCell ref="D210:K210"/>
+    <mergeCell ref="D214:K214"/>
+    <mergeCell ref="D196:K196"/>
+    <mergeCell ref="D197:K197"/>
+    <mergeCell ref="D198:K198"/>
+    <mergeCell ref="D200:K200"/>
+    <mergeCell ref="D202:K202"/>
+    <mergeCell ref="D191:K191"/>
+    <mergeCell ref="D192:K192"/>
+    <mergeCell ref="D193:K193"/>
+    <mergeCell ref="D194:K194"/>
+    <mergeCell ref="D195:K195"/>
+    <mergeCell ref="D186:K186"/>
+    <mergeCell ref="D187:K187"/>
+    <mergeCell ref="D188:K188"/>
+    <mergeCell ref="D189:K189"/>
+    <mergeCell ref="D190:K190"/>
+    <mergeCell ref="D178:K178"/>
+    <mergeCell ref="D182:K182"/>
+    <mergeCell ref="D183:K183"/>
+    <mergeCell ref="D184:K184"/>
+    <mergeCell ref="D185:K185"/>
   </mergeCells>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="53" fitToHeight="0" orientation="landscape"/>

</xml_diff>

<commit_message>
Revert "Teacher sets Switch #$38"
This reverts commit 2e326fa2f8bd06653e075cfb0876b8bc8e6179e9.
</commit_message>
<xml_diff>
--- a/data/Switches.xlsx
+++ b/data/Switches.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="794" uniqueCount="425">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="793" uniqueCount="424">
   <si>
     <t>ID</t>
   </si>
@@ -1289,9 +1289,6 @@
   </si>
   <si>
     <t>Great Wall Hidden DS</t>
-  </si>
-  <si>
-    <t>Talk to teacher</t>
   </si>
 </sst>
 </file>
@@ -1311,28 +1308,28 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1340,7 +1337,7 @@
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1348,7 +1345,7 @@
       <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1356,7 +1353,7 @@
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2398,43 +2395,7 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="47" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="32" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="33" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="27" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="25" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="3" applyBorder="1" applyAlignment="1">
@@ -2443,13 +2404,13 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="28" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="42" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="41" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
@@ -2467,16 +2428,40 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="27" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="41" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="25" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="32" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="42" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2495,6 +2480,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="33" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2807,8 +2804,8 @@
   <dimension ref="A1:O513"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K9" sqref="K9"/>
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H44" sqref="H44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -2881,16 +2878,16 @@
         <f>8*A2&amp;"-"&amp;(8*A2+7)</f>
         <v>0-7</v>
       </c>
-      <c r="D2" s="140" t="s">
+      <c r="D2" s="123" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="136"/>
-      <c r="F2" s="136"/>
-      <c r="G2" s="136"/>
-      <c r="H2" s="136"/>
-      <c r="I2" s="136"/>
-      <c r="J2" s="136"/>
-      <c r="K2" s="137"/>
+      <c r="E2" s="124"/>
+      <c r="F2" s="124"/>
+      <c r="G2" s="124"/>
+      <c r="H2" s="124"/>
+      <c r="I2" s="124"/>
+      <c r="J2" s="124"/>
+      <c r="K2" s="125"/>
       <c r="L2" s="119" t="s">
         <v>7</v>
       </c>
@@ -2908,14 +2905,14 @@
         <f t="shared" ref="C3:C33" si="1">8*A3&amp;"-"&amp;(8*A3+7)</f>
         <v>8-15</v>
       </c>
-      <c r="D3" s="141"/>
-      <c r="E3" s="142"/>
-      <c r="F3" s="142"/>
-      <c r="G3" s="142"/>
-      <c r="H3" s="142"/>
-      <c r="I3" s="142"/>
-      <c r="J3" s="142"/>
-      <c r="K3" s="143"/>
+      <c r="D3" s="129"/>
+      <c r="E3" s="130"/>
+      <c r="F3" s="130"/>
+      <c r="G3" s="130"/>
+      <c r="H3" s="130"/>
+      <c r="I3" s="130"/>
+      <c r="J3" s="130"/>
+      <c r="K3" s="131"/>
       <c r="L3" s="119" t="s">
         <v>8</v>
       </c>
@@ -3084,7 +3081,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="15.75" thickBot="1">
+    <row r="8" spans="1:15">
       <c r="A8" s="12">
         <f t="shared" si="2"/>
         <v>6</v>
@@ -3125,7 +3122,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="15.75" thickBot="1">
+    <row r="9" spans="1:15">
       <c r="A9" s="12">
         <f t="shared" si="2"/>
         <v>7</v>
@@ -3157,14 +3154,12 @@
         <v>50</v>
       </c>
       <c r="J9" s="30"/>
-      <c r="K9" s="99" t="s">
-        <v>424</v>
-      </c>
+      <c r="K9" s="28"/>
       <c r="L9" s="6">
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="15.75" thickBot="1">
+    <row r="10" spans="1:15">
       <c r="A10" s="12">
         <f t="shared" si="2"/>
         <v>8</v>
@@ -8974,16 +8969,16 @@
         <v>AA6</v>
       </c>
       <c r="C168" s="13"/>
-      <c r="D168" s="123" t="s">
+      <c r="D168" s="155" t="s">
         <v>348</v>
       </c>
-      <c r="E168" s="123"/>
-      <c r="F168" s="123"/>
-      <c r="G168" s="123"/>
-      <c r="H168" s="123"/>
-      <c r="I168" s="123"/>
-      <c r="J168" s="123"/>
-      <c r="K168" s="123"/>
+      <c r="E168" s="155"/>
+      <c r="F168" s="155"/>
+      <c r="G168" s="155"/>
+      <c r="H168" s="155"/>
+      <c r="I168" s="155"/>
+      <c r="J168" s="155"/>
+      <c r="K168" s="155"/>
     </row>
     <row r="169" spans="1:14">
       <c r="A169" s="12">
@@ -9109,16 +9104,16 @@
         <v>AAD</v>
       </c>
       <c r="C175" s="13"/>
-      <c r="D175" s="123" t="s">
+      <c r="D175" s="155" t="s">
         <v>349</v>
       </c>
-      <c r="E175" s="123"/>
-      <c r="F175" s="123"/>
-      <c r="G175" s="123"/>
-      <c r="H175" s="123"/>
-      <c r="I175" s="123"/>
-      <c r="J175" s="123"/>
-      <c r="K175" s="123"/>
+      <c r="E175" s="155"/>
+      <c r="F175" s="155"/>
+      <c r="G175" s="155"/>
+      <c r="H175" s="155"/>
+      <c r="I175" s="155"/>
+      <c r="J175" s="155"/>
+      <c r="K175" s="155"/>
     </row>
     <row r="176" spans="1:14">
       <c r="A176" s="12">
@@ -9171,16 +9166,16 @@
         <v>AB0</v>
       </c>
       <c r="C178" s="39"/>
-      <c r="D178" s="123" t="s">
+      <c r="D178" s="155" t="s">
         <v>350</v>
       </c>
-      <c r="E178" s="123"/>
-      <c r="F178" s="123"/>
-      <c r="G178" s="123"/>
-      <c r="H178" s="123"/>
-      <c r="I178" s="123"/>
-      <c r="J178" s="123"/>
-      <c r="K178" s="123"/>
+      <c r="E178" s="155"/>
+      <c r="F178" s="155"/>
+      <c r="G178" s="155"/>
+      <c r="H178" s="155"/>
+      <c r="I178" s="155"/>
+      <c r="J178" s="155"/>
+      <c r="K178" s="155"/>
     </row>
     <row r="179" spans="1:14">
       <c r="A179" s="12">
@@ -9249,16 +9244,16 @@
         <v>AB4</v>
       </c>
       <c r="C182" s="13"/>
-      <c r="D182" s="124" t="s">
+      <c r="D182" s="141" t="s">
         <v>351</v>
       </c>
-      <c r="E182" s="125"/>
-      <c r="F182" s="125"/>
-      <c r="G182" s="125"/>
-      <c r="H182" s="125"/>
-      <c r="I182" s="125"/>
-      <c r="J182" s="125"/>
-      <c r="K182" s="126"/>
+      <c r="E182" s="142"/>
+      <c r="F182" s="142"/>
+      <c r="G182" s="142"/>
+      <c r="H182" s="142"/>
+      <c r="I182" s="142"/>
+      <c r="J182" s="142"/>
+      <c r="K182" s="143"/>
     </row>
     <row r="183" spans="1:14">
       <c r="A183" s="12">
@@ -9270,16 +9265,16 @@
         <v>AB5</v>
       </c>
       <c r="C183" s="13"/>
-      <c r="D183" s="124" t="s">
+      <c r="D183" s="141" t="s">
         <v>352</v>
       </c>
-      <c r="E183" s="125"/>
-      <c r="F183" s="125"/>
-      <c r="G183" s="125"/>
-      <c r="H183" s="125"/>
-      <c r="I183" s="125"/>
-      <c r="J183" s="125"/>
-      <c r="K183" s="126"/>
+      <c r="E183" s="142"/>
+      <c r="F183" s="142"/>
+      <c r="G183" s="142"/>
+      <c r="H183" s="142"/>
+      <c r="I183" s="142"/>
+      <c r="J183" s="142"/>
+      <c r="K183" s="143"/>
     </row>
     <row r="184" spans="1:14">
       <c r="A184" s="12">
@@ -9291,16 +9286,16 @@
         <v>AB6</v>
       </c>
       <c r="C184" s="13"/>
-      <c r="D184" s="124" t="s">
+      <c r="D184" s="141" t="s">
         <v>353</v>
       </c>
-      <c r="E184" s="125"/>
-      <c r="F184" s="125"/>
-      <c r="G184" s="125"/>
-      <c r="H184" s="125"/>
-      <c r="I184" s="125"/>
-      <c r="J184" s="125"/>
-      <c r="K184" s="126"/>
+      <c r="E184" s="142"/>
+      <c r="F184" s="142"/>
+      <c r="G184" s="142"/>
+      <c r="H184" s="142"/>
+      <c r="I184" s="142"/>
+      <c r="J184" s="142"/>
+      <c r="K184" s="143"/>
     </row>
     <row r="185" spans="1:14">
       <c r="A185" s="12">
@@ -9312,16 +9307,16 @@
         <v>AB7</v>
       </c>
       <c r="C185" s="13"/>
-      <c r="D185" s="124" t="s">
+      <c r="D185" s="141" t="s">
         <v>354</v>
       </c>
-      <c r="E185" s="125"/>
-      <c r="F185" s="125"/>
-      <c r="G185" s="125"/>
-      <c r="H185" s="125"/>
-      <c r="I185" s="125"/>
-      <c r="J185" s="125"/>
-      <c r="K185" s="126"/>
+      <c r="E185" s="142"/>
+      <c r="F185" s="142"/>
+      <c r="G185" s="142"/>
+      <c r="H185" s="142"/>
+      <c r="I185" s="142"/>
+      <c r="J185" s="142"/>
+      <c r="K185" s="143"/>
     </row>
     <row r="186" spans="1:14">
       <c r="A186" s="12">
@@ -9333,16 +9328,16 @@
         <v>AB8</v>
       </c>
       <c r="C186" s="13"/>
-      <c r="D186" s="124" t="s">
+      <c r="D186" s="141" t="s">
         <v>355</v>
       </c>
-      <c r="E186" s="125"/>
-      <c r="F186" s="125"/>
-      <c r="G186" s="125"/>
-      <c r="H186" s="125"/>
-      <c r="I186" s="125"/>
-      <c r="J186" s="125"/>
-      <c r="K186" s="126"/>
+      <c r="E186" s="142"/>
+      <c r="F186" s="142"/>
+      <c r="G186" s="142"/>
+      <c r="H186" s="142"/>
+      <c r="I186" s="142"/>
+      <c r="J186" s="142"/>
+      <c r="K186" s="143"/>
     </row>
     <row r="187" spans="1:14">
       <c r="A187" s="12">
@@ -9354,16 +9349,16 @@
         <v>AB9</v>
       </c>
       <c r="C187" s="13"/>
-      <c r="D187" s="124" t="s">
+      <c r="D187" s="141" t="s">
         <v>356</v>
       </c>
-      <c r="E187" s="125"/>
-      <c r="F187" s="125"/>
-      <c r="G187" s="125"/>
-      <c r="H187" s="125"/>
-      <c r="I187" s="125"/>
-      <c r="J187" s="125"/>
-      <c r="K187" s="126"/>
+      <c r="E187" s="142"/>
+      <c r="F187" s="142"/>
+      <c r="G187" s="142"/>
+      <c r="H187" s="142"/>
+      <c r="I187" s="142"/>
+      <c r="J187" s="142"/>
+      <c r="K187" s="143"/>
     </row>
     <row r="188" spans="1:14">
       <c r="A188" s="12">
@@ -9375,16 +9370,16 @@
         <v>ABA</v>
       </c>
       <c r="C188" s="13"/>
-      <c r="D188" s="124" t="s">
+      <c r="D188" s="141" t="s">
         <v>357</v>
       </c>
-      <c r="E188" s="125"/>
-      <c r="F188" s="125"/>
-      <c r="G188" s="125"/>
-      <c r="H188" s="125"/>
-      <c r="I188" s="125"/>
-      <c r="J188" s="125"/>
-      <c r="K188" s="126"/>
+      <c r="E188" s="142"/>
+      <c r="F188" s="142"/>
+      <c r="G188" s="142"/>
+      <c r="H188" s="142"/>
+      <c r="I188" s="142"/>
+      <c r="J188" s="142"/>
+      <c r="K188" s="143"/>
     </row>
     <row r="189" spans="1:14">
       <c r="A189" s="12">
@@ -9396,16 +9391,16 @@
         <v>ABB</v>
       </c>
       <c r="C189" s="13"/>
-      <c r="D189" s="124" t="s">
+      <c r="D189" s="141" t="s">
         <v>358</v>
       </c>
-      <c r="E189" s="125"/>
-      <c r="F189" s="125"/>
-      <c r="G189" s="125"/>
-      <c r="H189" s="125"/>
-      <c r="I189" s="125"/>
-      <c r="J189" s="125"/>
-      <c r="K189" s="126"/>
+      <c r="E189" s="142"/>
+      <c r="F189" s="142"/>
+      <c r="G189" s="142"/>
+      <c r="H189" s="142"/>
+      <c r="I189" s="142"/>
+      <c r="J189" s="142"/>
+      <c r="K189" s="143"/>
     </row>
     <row r="190" spans="1:14">
       <c r="A190" s="12">
@@ -9417,16 +9412,16 @@
         <v>ABC</v>
       </c>
       <c r="C190" s="13"/>
-      <c r="D190" s="124" t="s">
+      <c r="D190" s="141" t="s">
         <v>359</v>
       </c>
-      <c r="E190" s="125"/>
-      <c r="F190" s="125"/>
-      <c r="G190" s="125"/>
-      <c r="H190" s="125"/>
-      <c r="I190" s="125"/>
-      <c r="J190" s="125"/>
-      <c r="K190" s="126"/>
+      <c r="E190" s="142"/>
+      <c r="F190" s="142"/>
+      <c r="G190" s="142"/>
+      <c r="H190" s="142"/>
+      <c r="I190" s="142"/>
+      <c r="J190" s="142"/>
+      <c r="K190" s="143"/>
     </row>
     <row r="191" spans="1:14">
       <c r="A191" s="12">
@@ -9438,16 +9433,16 @@
         <v>ABD</v>
       </c>
       <c r="C191" s="13"/>
-      <c r="D191" s="124" t="s">
+      <c r="D191" s="141" t="s">
         <v>360</v>
       </c>
-      <c r="E191" s="125"/>
-      <c r="F191" s="125"/>
-      <c r="G191" s="125"/>
-      <c r="H191" s="125"/>
-      <c r="I191" s="125"/>
-      <c r="J191" s="125"/>
-      <c r="K191" s="126"/>
+      <c r="E191" s="142"/>
+      <c r="F191" s="142"/>
+      <c r="G191" s="142"/>
+      <c r="H191" s="142"/>
+      <c r="I191" s="142"/>
+      <c r="J191" s="142"/>
+      <c r="K191" s="143"/>
     </row>
     <row r="192" spans="1:14">
       <c r="A192" s="12">
@@ -9459,16 +9454,16 @@
         <v>ABE</v>
       </c>
       <c r="C192" s="13"/>
-      <c r="D192" s="124" t="s">
+      <c r="D192" s="141" t="s">
         <v>361</v>
       </c>
-      <c r="E192" s="125"/>
-      <c r="F192" s="125"/>
-      <c r="G192" s="125"/>
-      <c r="H192" s="125"/>
-      <c r="I192" s="125"/>
-      <c r="J192" s="125"/>
-      <c r="K192" s="126"/>
+      <c r="E192" s="142"/>
+      <c r="F192" s="142"/>
+      <c r="G192" s="142"/>
+      <c r="H192" s="142"/>
+      <c r="I192" s="142"/>
+      <c r="J192" s="142"/>
+      <c r="K192" s="143"/>
     </row>
     <row r="193" spans="1:14" s="1" customFormat="1">
       <c r="A193" s="32">
@@ -9480,16 +9475,16 @@
         <v>ABF</v>
       </c>
       <c r="C193" s="33"/>
-      <c r="D193" s="127" t="s">
+      <c r="D193" s="152" t="s">
         <v>362</v>
       </c>
-      <c r="E193" s="128"/>
-      <c r="F193" s="128"/>
-      <c r="G193" s="128"/>
-      <c r="H193" s="128"/>
-      <c r="I193" s="128"/>
-      <c r="J193" s="128"/>
-      <c r="K193" s="129"/>
+      <c r="E193" s="153"/>
+      <c r="F193" s="153"/>
+      <c r="G193" s="153"/>
+      <c r="H193" s="153"/>
+      <c r="I193" s="153"/>
+      <c r="J193" s="153"/>
+      <c r="K193" s="154"/>
       <c r="L193" s="57"/>
       <c r="M193" s="58"/>
       <c r="N193" s="58"/>
@@ -9504,16 +9499,16 @@
         <v>AC0</v>
       </c>
       <c r="C194" s="39"/>
-      <c r="D194" s="130" t="s">
+      <c r="D194" s="134" t="s">
         <v>363</v>
       </c>
-      <c r="E194" s="131"/>
-      <c r="F194" s="131"/>
-      <c r="G194" s="131"/>
-      <c r="H194" s="131"/>
-      <c r="I194" s="131"/>
-      <c r="J194" s="131"/>
-      <c r="K194" s="132"/>
+      <c r="E194" s="127"/>
+      <c r="F194" s="127"/>
+      <c r="G194" s="127"/>
+      <c r="H194" s="127"/>
+      <c r="I194" s="127"/>
+      <c r="J194" s="127"/>
+      <c r="K194" s="135"/>
     </row>
     <row r="195" spans="1:14">
       <c r="A195" s="12">
@@ -9525,16 +9520,16 @@
         <v>AC1</v>
       </c>
       <c r="C195" s="13"/>
-      <c r="D195" s="124" t="s">
+      <c r="D195" s="141" t="s">
         <v>364</v>
       </c>
-      <c r="E195" s="125"/>
-      <c r="F195" s="125"/>
-      <c r="G195" s="125"/>
-      <c r="H195" s="125"/>
-      <c r="I195" s="125"/>
-      <c r="J195" s="125"/>
-      <c r="K195" s="126"/>
+      <c r="E195" s="142"/>
+      <c r="F195" s="142"/>
+      <c r="G195" s="142"/>
+      <c r="H195" s="142"/>
+      <c r="I195" s="142"/>
+      <c r="J195" s="142"/>
+      <c r="K195" s="143"/>
     </row>
     <row r="196" spans="1:14">
       <c r="A196" s="12">
@@ -9546,16 +9541,16 @@
         <v>AC2</v>
       </c>
       <c r="C196" s="13"/>
-      <c r="D196" s="124" t="s">
+      <c r="D196" s="141" t="s">
         <v>365</v>
       </c>
-      <c r="E196" s="125"/>
-      <c r="F196" s="125"/>
-      <c r="G196" s="125"/>
-      <c r="H196" s="125"/>
-      <c r="I196" s="125"/>
-      <c r="J196" s="125"/>
-      <c r="K196" s="126"/>
+      <c r="E196" s="142"/>
+      <c r="F196" s="142"/>
+      <c r="G196" s="142"/>
+      <c r="H196" s="142"/>
+      <c r="I196" s="142"/>
+      <c r="J196" s="142"/>
+      <c r="K196" s="143"/>
     </row>
     <row r="197" spans="1:14">
       <c r="A197" s="12">
@@ -9567,16 +9562,16 @@
         <v>AC3</v>
       </c>
       <c r="C197" s="13"/>
-      <c r="D197" s="124" t="s">
+      <c r="D197" s="141" t="s">
         <v>366</v>
       </c>
-      <c r="E197" s="125"/>
-      <c r="F197" s="125"/>
-      <c r="G197" s="125"/>
-      <c r="H197" s="125"/>
-      <c r="I197" s="125"/>
-      <c r="J197" s="125"/>
-      <c r="K197" s="126"/>
+      <c r="E197" s="142"/>
+      <c r="F197" s="142"/>
+      <c r="G197" s="142"/>
+      <c r="H197" s="142"/>
+      <c r="I197" s="142"/>
+      <c r="J197" s="142"/>
+      <c r="K197" s="143"/>
     </row>
     <row r="198" spans="1:14">
       <c r="A198" s="12">
@@ -9588,16 +9583,16 @@
         <v>AC4</v>
       </c>
       <c r="C198" s="13"/>
-      <c r="D198" s="124" t="s">
+      <c r="D198" s="141" t="s">
         <v>367</v>
       </c>
-      <c r="E198" s="125"/>
-      <c r="F198" s="125"/>
-      <c r="G198" s="125"/>
-      <c r="H198" s="125"/>
-      <c r="I198" s="125"/>
-      <c r="J198" s="125"/>
-      <c r="K198" s="126"/>
+      <c r="E198" s="142"/>
+      <c r="F198" s="142"/>
+      <c r="G198" s="142"/>
+      <c r="H198" s="142"/>
+      <c r="I198" s="142"/>
+      <c r="J198" s="142"/>
+      <c r="K198" s="143"/>
     </row>
     <row r="199" spans="1:14">
       <c r="A199" s="12">
@@ -9628,16 +9623,16 @@
         <v>AC6</v>
       </c>
       <c r="C200" s="13"/>
-      <c r="D200" s="124" t="s">
+      <c r="D200" s="141" t="s">
         <v>368</v>
       </c>
-      <c r="E200" s="125"/>
-      <c r="F200" s="125"/>
-      <c r="G200" s="125"/>
-      <c r="H200" s="125"/>
-      <c r="I200" s="125"/>
-      <c r="J200" s="125"/>
-      <c r="K200" s="126"/>
+      <c r="E200" s="142"/>
+      <c r="F200" s="142"/>
+      <c r="G200" s="142"/>
+      <c r="H200" s="142"/>
+      <c r="I200" s="142"/>
+      <c r="J200" s="142"/>
+      <c r="K200" s="143"/>
     </row>
     <row r="201" spans="1:14">
       <c r="A201" s="12">
@@ -9668,16 +9663,16 @@
         <v>AC8</v>
       </c>
       <c r="C202" s="13"/>
-      <c r="D202" s="153" t="s">
+      <c r="D202" s="149" t="s">
         <v>369</v>
       </c>
-      <c r="E202" s="154"/>
-      <c r="F202" s="154"/>
-      <c r="G202" s="154"/>
-      <c r="H202" s="154"/>
-      <c r="I202" s="154"/>
-      <c r="J202" s="154"/>
-      <c r="K202" s="155"/>
+      <c r="E202" s="150"/>
+      <c r="F202" s="150"/>
+      <c r="G202" s="150"/>
+      <c r="H202" s="150"/>
+      <c r="I202" s="150"/>
+      <c r="J202" s="150"/>
+      <c r="K202" s="151"/>
     </row>
     <row r="203" spans="1:14">
       <c r="A203" s="12">
@@ -9708,16 +9703,16 @@
         <v>ACA</v>
       </c>
       <c r="C204" s="13"/>
-      <c r="D204" s="124" t="s">
+      <c r="D204" s="141" t="s">
         <v>370</v>
       </c>
-      <c r="E204" s="125"/>
-      <c r="F204" s="125"/>
-      <c r="G204" s="125"/>
-      <c r="H204" s="125"/>
-      <c r="I204" s="125"/>
-      <c r="J204" s="125"/>
-      <c r="K204" s="126"/>
+      <c r="E204" s="142"/>
+      <c r="F204" s="142"/>
+      <c r="G204" s="142"/>
+      <c r="H204" s="142"/>
+      <c r="I204" s="142"/>
+      <c r="J204" s="142"/>
+      <c r="K204" s="143"/>
     </row>
     <row r="205" spans="1:14">
       <c r="A205" s="12">
@@ -9748,16 +9743,16 @@
         <v>ACC</v>
       </c>
       <c r="C206" s="13"/>
-      <c r="D206" s="124" t="s">
+      <c r="D206" s="141" t="s">
         <v>370</v>
       </c>
-      <c r="E206" s="125"/>
-      <c r="F206" s="125"/>
-      <c r="G206" s="125"/>
-      <c r="H206" s="125"/>
-      <c r="I206" s="125"/>
-      <c r="J206" s="125"/>
-      <c r="K206" s="126"/>
+      <c r="E206" s="142"/>
+      <c r="F206" s="142"/>
+      <c r="G206" s="142"/>
+      <c r="H206" s="142"/>
+      <c r="I206" s="142"/>
+      <c r="J206" s="142"/>
+      <c r="K206" s="143"/>
     </row>
     <row r="207" spans="1:14">
       <c r="A207" s="12">
@@ -9788,16 +9783,16 @@
         <v>ACE</v>
       </c>
       <c r="C208" s="13"/>
-      <c r="D208" s="124" t="s">
+      <c r="D208" s="141" t="s">
         <v>371</v>
       </c>
-      <c r="E208" s="125"/>
-      <c r="F208" s="125"/>
-      <c r="G208" s="125"/>
-      <c r="H208" s="125"/>
-      <c r="I208" s="125"/>
-      <c r="J208" s="125"/>
-      <c r="K208" s="126"/>
+      <c r="E208" s="142"/>
+      <c r="F208" s="142"/>
+      <c r="G208" s="142"/>
+      <c r="H208" s="142"/>
+      <c r="I208" s="142"/>
+      <c r="J208" s="142"/>
+      <c r="K208" s="143"/>
     </row>
     <row r="209" spans="1:14" s="1" customFormat="1">
       <c r="A209" s="32">
@@ -9831,16 +9826,16 @@
         <v>AD0</v>
       </c>
       <c r="C210" s="39"/>
-      <c r="D210" s="130" t="s">
+      <c r="D210" s="134" t="s">
         <v>371</v>
       </c>
-      <c r="E210" s="131"/>
-      <c r="F210" s="131"/>
-      <c r="G210" s="131"/>
-      <c r="H210" s="131"/>
-      <c r="I210" s="131"/>
-      <c r="J210" s="131"/>
-      <c r="K210" s="132"/>
+      <c r="E210" s="127"/>
+      <c r="F210" s="127"/>
+      <c r="G210" s="127"/>
+      <c r="H210" s="127"/>
+      <c r="I210" s="127"/>
+      <c r="J210" s="127"/>
+      <c r="K210" s="135"/>
     </row>
     <row r="211" spans="1:14">
       <c r="A211" s="12">
@@ -9909,16 +9904,16 @@
         <v>AD4</v>
       </c>
       <c r="C214" s="13"/>
-      <c r="D214" s="124" t="s">
+      <c r="D214" s="141" t="s">
         <v>372</v>
       </c>
-      <c r="E214" s="125"/>
-      <c r="F214" s="125"/>
-      <c r="G214" s="125"/>
-      <c r="H214" s="125"/>
-      <c r="I214" s="125"/>
-      <c r="J214" s="125"/>
-      <c r="K214" s="126"/>
+      <c r="E214" s="142"/>
+      <c r="F214" s="142"/>
+      <c r="G214" s="142"/>
+      <c r="H214" s="142"/>
+      <c r="I214" s="142"/>
+      <c r="J214" s="142"/>
+      <c r="K214" s="143"/>
     </row>
     <row r="215" spans="1:14">
       <c r="A215" s="12">
@@ -9949,16 +9944,16 @@
         <v>AD6</v>
       </c>
       <c r="C216" s="13"/>
-      <c r="D216" s="144" t="s">
+      <c r="D216" s="132" t="s">
         <v>373</v>
       </c>
-      <c r="E216" s="136"/>
-      <c r="F216" s="136"/>
-      <c r="G216" s="136"/>
-      <c r="H216" s="136"/>
-      <c r="I216" s="136"/>
-      <c r="J216" s="136"/>
-      <c r="K216" s="145"/>
+      <c r="E216" s="124"/>
+      <c r="F216" s="124"/>
+      <c r="G216" s="124"/>
+      <c r="H216" s="124"/>
+      <c r="I216" s="124"/>
+      <c r="J216" s="124"/>
+      <c r="K216" s="133"/>
     </row>
     <row r="217" spans="1:14">
       <c r="A217" s="12">
@@ -9970,14 +9965,14 @@
         <v>AD7</v>
       </c>
       <c r="C217" s="13"/>
-      <c r="D217" s="130"/>
-      <c r="E217" s="131"/>
-      <c r="F217" s="131"/>
-      <c r="G217" s="131"/>
-      <c r="H217" s="131"/>
-      <c r="I217" s="131"/>
-      <c r="J217" s="131"/>
-      <c r="K217" s="132"/>
+      <c r="D217" s="134"/>
+      <c r="E217" s="127"/>
+      <c r="F217" s="127"/>
+      <c r="G217" s="127"/>
+      <c r="H217" s="127"/>
+      <c r="I217" s="127"/>
+      <c r="J217" s="127"/>
+      <c r="K217" s="135"/>
     </row>
     <row r="218" spans="1:14">
       <c r="A218" s="12">
@@ -9989,16 +9984,16 @@
         <v>AD8</v>
       </c>
       <c r="C218" s="13"/>
-      <c r="D218" s="144" t="s">
+      <c r="D218" s="132" t="s">
         <v>374</v>
       </c>
-      <c r="E218" s="136"/>
-      <c r="F218" s="136"/>
-      <c r="G218" s="136"/>
-      <c r="H218" s="136"/>
-      <c r="I218" s="136"/>
-      <c r="J218" s="136"/>
-      <c r="K218" s="145"/>
+      <c r="E218" s="124"/>
+      <c r="F218" s="124"/>
+      <c r="G218" s="124"/>
+      <c r="H218" s="124"/>
+      <c r="I218" s="124"/>
+      <c r="J218" s="124"/>
+      <c r="K218" s="133"/>
     </row>
     <row r="219" spans="1:14">
       <c r="A219" s="12">
@@ -10010,14 +10005,14 @@
         <v>AD9</v>
       </c>
       <c r="C219" s="13"/>
-      <c r="D219" s="130"/>
-      <c r="E219" s="131"/>
-      <c r="F219" s="131"/>
-      <c r="G219" s="131"/>
-      <c r="H219" s="131"/>
-      <c r="I219" s="131"/>
-      <c r="J219" s="131"/>
-      <c r="K219" s="132"/>
+      <c r="D219" s="134"/>
+      <c r="E219" s="127"/>
+      <c r="F219" s="127"/>
+      <c r="G219" s="127"/>
+      <c r="H219" s="127"/>
+      <c r="I219" s="127"/>
+      <c r="J219" s="127"/>
+      <c r="K219" s="135"/>
     </row>
     <row r="220" spans="1:14">
       <c r="A220" s="12">
@@ -10029,16 +10024,16 @@
         <v>ADA</v>
       </c>
       <c r="C220" s="13"/>
-      <c r="D220" s="144" t="s">
+      <c r="D220" s="132" t="s">
         <v>375</v>
       </c>
-      <c r="E220" s="136"/>
-      <c r="F220" s="136"/>
-      <c r="G220" s="136"/>
-      <c r="H220" s="136"/>
-      <c r="I220" s="136"/>
-      <c r="J220" s="136"/>
-      <c r="K220" s="145"/>
+      <c r="E220" s="124"/>
+      <c r="F220" s="124"/>
+      <c r="G220" s="124"/>
+      <c r="H220" s="124"/>
+      <c r="I220" s="124"/>
+      <c r="J220" s="124"/>
+      <c r="K220" s="133"/>
     </row>
     <row r="221" spans="1:14">
       <c r="A221" s="12">
@@ -10050,14 +10045,14 @@
         <v>ADB</v>
       </c>
       <c r="C221" s="13"/>
-      <c r="D221" s="130"/>
-      <c r="E221" s="131"/>
-      <c r="F221" s="131"/>
-      <c r="G221" s="131"/>
-      <c r="H221" s="131"/>
-      <c r="I221" s="131"/>
-      <c r="J221" s="131"/>
-      <c r="K221" s="132"/>
+      <c r="D221" s="134"/>
+      <c r="E221" s="127"/>
+      <c r="F221" s="127"/>
+      <c r="G221" s="127"/>
+      <c r="H221" s="127"/>
+      <c r="I221" s="127"/>
+      <c r="J221" s="127"/>
+      <c r="K221" s="135"/>
     </row>
     <row r="222" spans="1:14">
       <c r="A222" s="12">
@@ -10069,16 +10064,16 @@
         <v>ADC</v>
       </c>
       <c r="C222" s="13"/>
-      <c r="D222" s="124" t="s">
+      <c r="D222" s="141" t="s">
         <v>376</v>
       </c>
-      <c r="E222" s="125"/>
-      <c r="F222" s="125"/>
-      <c r="G222" s="125"/>
-      <c r="H222" s="125"/>
-      <c r="I222" s="125"/>
-      <c r="J222" s="125"/>
-      <c r="K222" s="126"/>
+      <c r="E222" s="142"/>
+      <c r="F222" s="142"/>
+      <c r="G222" s="142"/>
+      <c r="H222" s="142"/>
+      <c r="I222" s="142"/>
+      <c r="J222" s="142"/>
+      <c r="K222" s="143"/>
     </row>
     <row r="223" spans="1:14">
       <c r="A223" s="12">
@@ -10109,16 +10104,16 @@
         <v>ADE</v>
       </c>
       <c r="C224" s="13"/>
-      <c r="D224" s="124" t="s">
+      <c r="D224" s="141" t="s">
         <v>377</v>
       </c>
-      <c r="E224" s="125"/>
-      <c r="F224" s="125"/>
-      <c r="G224" s="125"/>
-      <c r="H224" s="125"/>
-      <c r="I224" s="125"/>
-      <c r="J224" s="125"/>
-      <c r="K224" s="126"/>
+      <c r="E224" s="142"/>
+      <c r="F224" s="142"/>
+      <c r="G224" s="142"/>
+      <c r="H224" s="142"/>
+      <c r="I224" s="142"/>
+      <c r="J224" s="142"/>
+      <c r="K224" s="143"/>
     </row>
     <row r="225" spans="1:14" s="1" customFormat="1">
       <c r="A225" s="32">
@@ -10152,16 +10147,16 @@
         <v>AE0</v>
       </c>
       <c r="C226" s="39"/>
-      <c r="D226" s="150" t="s">
+      <c r="D226" s="146" t="s">
         <v>378</v>
       </c>
-      <c r="E226" s="151"/>
-      <c r="F226" s="151"/>
-      <c r="G226" s="151"/>
-      <c r="H226" s="151"/>
-      <c r="I226" s="151"/>
-      <c r="J226" s="151"/>
-      <c r="K226" s="152"/>
+      <c r="E226" s="147"/>
+      <c r="F226" s="147"/>
+      <c r="G226" s="147"/>
+      <c r="H226" s="147"/>
+      <c r="I226" s="147"/>
+      <c r="J226" s="147"/>
+      <c r="K226" s="148"/>
     </row>
     <row r="227" spans="1:14">
       <c r="A227" s="12">
@@ -10306,16 +10301,16 @@
         <v>AE8</v>
       </c>
       <c r="C234" s="13"/>
-      <c r="D234" s="148" t="s">
+      <c r="D234" s="136" t="s">
         <v>379</v>
       </c>
-      <c r="E234" s="134"/>
-      <c r="F234" s="134"/>
-      <c r="G234" s="134"/>
-      <c r="H234" s="134"/>
-      <c r="I234" s="134"/>
-      <c r="J234" s="134"/>
-      <c r="K234" s="149"/>
+      <c r="E234" s="137"/>
+      <c r="F234" s="137"/>
+      <c r="G234" s="137"/>
+      <c r="H234" s="137"/>
+      <c r="I234" s="137"/>
+      <c r="J234" s="137"/>
+      <c r="K234" s="138"/>
     </row>
     <row r="235" spans="1:14">
       <c r="A235" s="12">
@@ -10384,16 +10379,16 @@
         <v>AEC</v>
       </c>
       <c r="C238" s="13"/>
-      <c r="D238" s="140" t="s">
+      <c r="D238" s="123" t="s">
         <v>380</v>
       </c>
-      <c r="E238" s="136"/>
-      <c r="F238" s="136"/>
-      <c r="G238" s="136"/>
-      <c r="H238" s="136"/>
-      <c r="I238" s="136"/>
-      <c r="J238" s="136"/>
-      <c r="K238" s="137"/>
+      <c r="E238" s="124"/>
+      <c r="F238" s="124"/>
+      <c r="G238" s="124"/>
+      <c r="H238" s="124"/>
+      <c r="I238" s="124"/>
+      <c r="J238" s="124"/>
+      <c r="K238" s="125"/>
     </row>
     <row r="239" spans="1:14">
       <c r="A239" s="12">
@@ -10405,14 +10400,14 @@
         <v>AED</v>
       </c>
       <c r="C239" s="13"/>
-      <c r="D239" s="146"/>
-      <c r="E239" s="131"/>
-      <c r="F239" s="131"/>
-      <c r="G239" s="131"/>
-      <c r="H239" s="131"/>
-      <c r="I239" s="131"/>
-      <c r="J239" s="131"/>
-      <c r="K239" s="147"/>
+      <c r="D239" s="126"/>
+      <c r="E239" s="127"/>
+      <c r="F239" s="127"/>
+      <c r="G239" s="127"/>
+      <c r="H239" s="127"/>
+      <c r="I239" s="127"/>
+      <c r="J239" s="127"/>
+      <c r="K239" s="128"/>
     </row>
     <row r="240" spans="1:14">
       <c r="A240" s="12">
@@ -10424,16 +10419,16 @@
         <v>AEE</v>
       </c>
       <c r="C240" s="70"/>
-      <c r="D240" s="136" t="s">
+      <c r="D240" s="124" t="s">
         <v>381</v>
       </c>
-      <c r="E240" s="136"/>
-      <c r="F240" s="136"/>
-      <c r="G240" s="136"/>
-      <c r="H240" s="136"/>
-      <c r="I240" s="136"/>
-      <c r="J240" s="136"/>
-      <c r="K240" s="137"/>
+      <c r="E240" s="124"/>
+      <c r="F240" s="124"/>
+      <c r="G240" s="124"/>
+      <c r="H240" s="124"/>
+      <c r="I240" s="124"/>
+      <c r="J240" s="124"/>
+      <c r="K240" s="125"/>
     </row>
     <row r="241" spans="1:14" s="1" customFormat="1">
       <c r="A241" s="32">
@@ -10445,14 +10440,14 @@
         <v>AEF</v>
       </c>
       <c r="C241" s="34"/>
-      <c r="D241" s="138"/>
-      <c r="E241" s="138"/>
-      <c r="F241" s="138"/>
-      <c r="G241" s="138"/>
-      <c r="H241" s="138"/>
-      <c r="I241" s="138"/>
-      <c r="J241" s="138"/>
-      <c r="K241" s="139"/>
+      <c r="D241" s="144"/>
+      <c r="E241" s="144"/>
+      <c r="F241" s="144"/>
+      <c r="G241" s="144"/>
+      <c r="H241" s="144"/>
+      <c r="I241" s="144"/>
+      <c r="J241" s="144"/>
+      <c r="K241" s="145"/>
       <c r="L241" s="57"/>
       <c r="M241" s="58"/>
       <c r="N241" s="58"/>
@@ -10643,16 +10638,16 @@
         <v>AF8</v>
       </c>
       <c r="C250" s="13"/>
-      <c r="D250" s="133" t="s">
+      <c r="D250" s="139" t="s">
         <v>382</v>
       </c>
-      <c r="E250" s="134"/>
-      <c r="F250" s="134"/>
-      <c r="G250" s="134"/>
-      <c r="H250" s="134"/>
-      <c r="I250" s="134"/>
-      <c r="J250" s="134"/>
-      <c r="K250" s="135"/>
+      <c r="E250" s="137"/>
+      <c r="F250" s="137"/>
+      <c r="G250" s="137"/>
+      <c r="H250" s="137"/>
+      <c r="I250" s="137"/>
+      <c r="J250" s="137"/>
+      <c r="K250" s="140"/>
     </row>
     <row r="251" spans="1:14">
       <c r="A251" s="12">
@@ -11221,16 +11216,16 @@
         <v>B16</v>
       </c>
       <c r="C280" s="13"/>
-      <c r="D280" s="124" t="s">
+      <c r="D280" s="141" t="s">
         <v>383</v>
       </c>
-      <c r="E280" s="125"/>
-      <c r="F280" s="125"/>
-      <c r="G280" s="125"/>
-      <c r="H280" s="125"/>
-      <c r="I280" s="125"/>
-      <c r="J280" s="125"/>
-      <c r="K280" s="126"/>
+      <c r="E280" s="142"/>
+      <c r="F280" s="142"/>
+      <c r="G280" s="142"/>
+      <c r="H280" s="142"/>
+      <c r="I280" s="142"/>
+      <c r="J280" s="142"/>
+      <c r="K280" s="143"/>
     </row>
     <row r="281" spans="1:14">
       <c r="A281" s="12">
@@ -11337,16 +11332,16 @@
         <v>B1C</v>
       </c>
       <c r="C286" s="13"/>
-      <c r="D286" s="124" t="s">
+      <c r="D286" s="141" t="s">
         <v>384</v>
       </c>
-      <c r="E286" s="125"/>
-      <c r="F286" s="125"/>
-      <c r="G286" s="125"/>
-      <c r="H286" s="125"/>
-      <c r="I286" s="125"/>
-      <c r="J286" s="125"/>
-      <c r="K286" s="126"/>
+      <c r="E286" s="142"/>
+      <c r="F286" s="142"/>
+      <c r="G286" s="142"/>
+      <c r="H286" s="142"/>
+      <c r="I286" s="142"/>
+      <c r="J286" s="142"/>
+      <c r="K286" s="143"/>
     </row>
     <row r="287" spans="1:14">
       <c r="A287" s="12">
@@ -11534,16 +11529,16 @@
         <v>B26</v>
       </c>
       <c r="C296" s="13"/>
-      <c r="D296" s="124" t="s">
+      <c r="D296" s="141" t="s">
         <v>386</v>
       </c>
-      <c r="E296" s="125"/>
-      <c r="F296" s="125"/>
-      <c r="G296" s="125"/>
-      <c r="H296" s="125"/>
-      <c r="I296" s="125"/>
-      <c r="J296" s="125"/>
-      <c r="K296" s="126"/>
+      <c r="E296" s="142"/>
+      <c r="F296" s="142"/>
+      <c r="G296" s="142"/>
+      <c r="H296" s="142"/>
+      <c r="I296" s="142"/>
+      <c r="J296" s="142"/>
+      <c r="K296" s="143"/>
     </row>
     <row r="297" spans="1:14">
       <c r="A297" s="12">
@@ -11574,16 +11569,16 @@
         <v>B28</v>
       </c>
       <c r="C298" s="13"/>
-      <c r="D298" s="140" t="s">
+      <c r="D298" s="123" t="s">
         <v>387</v>
       </c>
-      <c r="E298" s="136"/>
-      <c r="F298" s="136"/>
-      <c r="G298" s="136"/>
-      <c r="H298" s="136"/>
-      <c r="I298" s="136"/>
-      <c r="J298" s="136"/>
-      <c r="K298" s="137"/>
+      <c r="E298" s="124"/>
+      <c r="F298" s="124"/>
+      <c r="G298" s="124"/>
+      <c r="H298" s="124"/>
+      <c r="I298" s="124"/>
+      <c r="J298" s="124"/>
+      <c r="K298" s="125"/>
     </row>
     <row r="299" spans="1:14">
       <c r="A299" s="12">
@@ -11595,14 +11590,14 @@
         <v>B29</v>
       </c>
       <c r="C299" s="13"/>
-      <c r="D299" s="146"/>
-      <c r="E299" s="131"/>
-      <c r="F299" s="131"/>
-      <c r="G299" s="131"/>
-      <c r="H299" s="131"/>
-      <c r="I299" s="131"/>
-      <c r="J299" s="131"/>
-      <c r="K299" s="147"/>
+      <c r="D299" s="126"/>
+      <c r="E299" s="127"/>
+      <c r="F299" s="127"/>
+      <c r="G299" s="127"/>
+      <c r="H299" s="127"/>
+      <c r="I299" s="127"/>
+      <c r="J299" s="127"/>
+      <c r="K299" s="128"/>
     </row>
     <row r="300" spans="1:14">
       <c r="A300" s="12">
@@ -11614,16 +11609,16 @@
         <v>B2A</v>
       </c>
       <c r="C300" s="13"/>
-      <c r="D300" s="140" t="s">
+      <c r="D300" s="123" t="s">
         <v>388</v>
       </c>
-      <c r="E300" s="136"/>
-      <c r="F300" s="136"/>
-      <c r="G300" s="136"/>
-      <c r="H300" s="136"/>
-      <c r="I300" s="136"/>
-      <c r="J300" s="136"/>
-      <c r="K300" s="137"/>
+      <c r="E300" s="124"/>
+      <c r="F300" s="124"/>
+      <c r="G300" s="124"/>
+      <c r="H300" s="124"/>
+      <c r="I300" s="124"/>
+      <c r="J300" s="124"/>
+      <c r="K300" s="125"/>
     </row>
     <row r="301" spans="1:14">
       <c r="A301" s="12">
@@ -11635,14 +11630,14 @@
         <v>B2B</v>
       </c>
       <c r="C301" s="13"/>
-      <c r="D301" s="146"/>
-      <c r="E301" s="131"/>
-      <c r="F301" s="131"/>
-      <c r="G301" s="131"/>
-      <c r="H301" s="131"/>
-      <c r="I301" s="131"/>
-      <c r="J301" s="131"/>
-      <c r="K301" s="147"/>
+      <c r="D301" s="126"/>
+      <c r="E301" s="127"/>
+      <c r="F301" s="127"/>
+      <c r="G301" s="127"/>
+      <c r="H301" s="127"/>
+      <c r="I301" s="127"/>
+      <c r="J301" s="127"/>
+      <c r="K301" s="128"/>
     </row>
     <row r="302" spans="1:14">
       <c r="A302" s="12">
@@ -11654,16 +11649,16 @@
         <v>B2C</v>
       </c>
       <c r="C302" s="13"/>
-      <c r="D302" s="140" t="s">
+      <c r="D302" s="123" t="s">
         <v>389</v>
       </c>
-      <c r="E302" s="136"/>
-      <c r="F302" s="136"/>
-      <c r="G302" s="136"/>
-      <c r="H302" s="136"/>
-      <c r="I302" s="136"/>
-      <c r="J302" s="136"/>
-      <c r="K302" s="137"/>
+      <c r="E302" s="124"/>
+      <c r="F302" s="124"/>
+      <c r="G302" s="124"/>
+      <c r="H302" s="124"/>
+      <c r="I302" s="124"/>
+      <c r="J302" s="124"/>
+      <c r="K302" s="125"/>
     </row>
     <row r="303" spans="1:14">
       <c r="A303" s="12">
@@ -11675,14 +11670,14 @@
         <v>B2D</v>
       </c>
       <c r="C303" s="13"/>
-      <c r="D303" s="146"/>
-      <c r="E303" s="131"/>
-      <c r="F303" s="131"/>
-      <c r="G303" s="131"/>
-      <c r="H303" s="131"/>
-      <c r="I303" s="131"/>
-      <c r="J303" s="131"/>
-      <c r="K303" s="147"/>
+      <c r="D303" s="126"/>
+      <c r="E303" s="127"/>
+      <c r="F303" s="127"/>
+      <c r="G303" s="127"/>
+      <c r="H303" s="127"/>
+      <c r="I303" s="127"/>
+      <c r="J303" s="127"/>
+      <c r="K303" s="128"/>
     </row>
     <row r="304" spans="1:14">
       <c r="A304" s="12">
@@ -11694,16 +11689,16 @@
         <v>B2E</v>
       </c>
       <c r="C304" s="13"/>
-      <c r="D304" s="140" t="s">
+      <c r="D304" s="123" t="s">
         <v>390</v>
       </c>
-      <c r="E304" s="136"/>
-      <c r="F304" s="136"/>
-      <c r="G304" s="136"/>
-      <c r="H304" s="136"/>
-      <c r="I304" s="136"/>
-      <c r="J304" s="136"/>
-      <c r="K304" s="137"/>
+      <c r="E304" s="124"/>
+      <c r="F304" s="124"/>
+      <c r="G304" s="124"/>
+      <c r="H304" s="124"/>
+      <c r="I304" s="124"/>
+      <c r="J304" s="124"/>
+      <c r="K304" s="125"/>
     </row>
     <row r="305" spans="1:14" s="1" customFormat="1">
       <c r="A305" s="32">
@@ -11715,14 +11710,14 @@
         <v>B2F</v>
       </c>
       <c r="C305" s="33"/>
-      <c r="D305" s="146"/>
-      <c r="E305" s="131"/>
-      <c r="F305" s="131"/>
-      <c r="G305" s="131"/>
-      <c r="H305" s="131"/>
-      <c r="I305" s="131"/>
-      <c r="J305" s="131"/>
-      <c r="K305" s="147"/>
+      <c r="D305" s="126"/>
+      <c r="E305" s="127"/>
+      <c r="F305" s="127"/>
+      <c r="G305" s="127"/>
+      <c r="H305" s="127"/>
+      <c r="I305" s="127"/>
+      <c r="J305" s="127"/>
+      <c r="K305" s="128"/>
       <c r="L305" s="57"/>
       <c r="M305" s="58"/>
       <c r="N305" s="58"/>
@@ -11737,16 +11732,16 @@
         <v>B30</v>
       </c>
       <c r="C306" s="39"/>
-      <c r="D306" s="140" t="s">
+      <c r="D306" s="123" t="s">
         <v>391</v>
       </c>
-      <c r="E306" s="136"/>
-      <c r="F306" s="136"/>
-      <c r="G306" s="136"/>
-      <c r="H306" s="136"/>
-      <c r="I306" s="136"/>
-      <c r="J306" s="136"/>
-      <c r="K306" s="137"/>
+      <c r="E306" s="124"/>
+      <c r="F306" s="124"/>
+      <c r="G306" s="124"/>
+      <c r="H306" s="124"/>
+      <c r="I306" s="124"/>
+      <c r="J306" s="124"/>
+      <c r="K306" s="125"/>
     </row>
     <row r="307" spans="1:14">
       <c r="A307" s="12">
@@ -11758,14 +11753,14 @@
         <v>B31</v>
       </c>
       <c r="C307" s="13"/>
-      <c r="D307" s="146"/>
-      <c r="E307" s="131"/>
-      <c r="F307" s="131"/>
-      <c r="G307" s="131"/>
-      <c r="H307" s="131"/>
-      <c r="I307" s="131"/>
-      <c r="J307" s="131"/>
-      <c r="K307" s="147"/>
+      <c r="D307" s="126"/>
+      <c r="E307" s="127"/>
+      <c r="F307" s="127"/>
+      <c r="G307" s="127"/>
+      <c r="H307" s="127"/>
+      <c r="I307" s="127"/>
+      <c r="J307" s="127"/>
+      <c r="K307" s="128"/>
     </row>
     <row r="308" spans="1:14">
       <c r="A308" s="12">
@@ -11777,16 +11772,16 @@
         <v>B32</v>
       </c>
       <c r="C308" s="13"/>
-      <c r="D308" s="140" t="s">
+      <c r="D308" s="123" t="s">
         <v>392</v>
       </c>
-      <c r="E308" s="136"/>
-      <c r="F308" s="136"/>
-      <c r="G308" s="136"/>
-      <c r="H308" s="136"/>
-      <c r="I308" s="136"/>
-      <c r="J308" s="136"/>
-      <c r="K308" s="137"/>
+      <c r="E308" s="124"/>
+      <c r="F308" s="124"/>
+      <c r="G308" s="124"/>
+      <c r="H308" s="124"/>
+      <c r="I308" s="124"/>
+      <c r="J308" s="124"/>
+      <c r="K308" s="125"/>
     </row>
     <row r="309" spans="1:14">
       <c r="A309" s="12">
@@ -11798,14 +11793,14 @@
         <v>B33</v>
       </c>
       <c r="C309" s="13"/>
-      <c r="D309" s="146"/>
-      <c r="E309" s="131"/>
-      <c r="F309" s="131"/>
-      <c r="G309" s="131"/>
-      <c r="H309" s="131"/>
-      <c r="I309" s="131"/>
-      <c r="J309" s="131"/>
-      <c r="K309" s="147"/>
+      <c r="D309" s="126"/>
+      <c r="E309" s="127"/>
+      <c r="F309" s="127"/>
+      <c r="G309" s="127"/>
+      <c r="H309" s="127"/>
+      <c r="I309" s="127"/>
+      <c r="J309" s="127"/>
+      <c r="K309" s="128"/>
     </row>
     <row r="310" spans="1:14">
       <c r="A310" s="12">
@@ -15685,12 +15680,31 @@
     </row>
   </sheetData>
   <mergeCells count="47">
-    <mergeCell ref="D304:K305"/>
-    <mergeCell ref="D306:K307"/>
-    <mergeCell ref="D308:K309"/>
-    <mergeCell ref="D298:K299"/>
-    <mergeCell ref="D300:K301"/>
-    <mergeCell ref="D302:K303"/>
+    <mergeCell ref="D168:K168"/>
+    <mergeCell ref="D175:K175"/>
+    <mergeCell ref="D178:K178"/>
+    <mergeCell ref="D182:K182"/>
+    <mergeCell ref="D183:K183"/>
+    <mergeCell ref="D184:K184"/>
+    <mergeCell ref="D185:K185"/>
+    <mergeCell ref="D186:K186"/>
+    <mergeCell ref="D187:K187"/>
+    <mergeCell ref="D188:K188"/>
+    <mergeCell ref="D189:K189"/>
+    <mergeCell ref="D190:K190"/>
+    <mergeCell ref="D191:K191"/>
+    <mergeCell ref="D192:K192"/>
+    <mergeCell ref="D193:K193"/>
+    <mergeCell ref="D194:K194"/>
+    <mergeCell ref="D195:K195"/>
+    <mergeCell ref="D196:K196"/>
+    <mergeCell ref="D197:K197"/>
+    <mergeCell ref="D198:K198"/>
+    <mergeCell ref="D250:K250"/>
+    <mergeCell ref="D280:K280"/>
+    <mergeCell ref="D286:K286"/>
+    <mergeCell ref="D296:K296"/>
+    <mergeCell ref="D240:K241"/>
     <mergeCell ref="D2:K3"/>
     <mergeCell ref="D216:K217"/>
     <mergeCell ref="D218:K219"/>
@@ -15707,31 +15721,12 @@
     <mergeCell ref="D204:K204"/>
     <mergeCell ref="D206:K206"/>
     <mergeCell ref="D208:K208"/>
-    <mergeCell ref="D250:K250"/>
-    <mergeCell ref="D280:K280"/>
-    <mergeCell ref="D286:K286"/>
-    <mergeCell ref="D296:K296"/>
-    <mergeCell ref="D240:K241"/>
-    <mergeCell ref="D194:K194"/>
-    <mergeCell ref="D195:K195"/>
-    <mergeCell ref="D196:K196"/>
-    <mergeCell ref="D197:K197"/>
-    <mergeCell ref="D198:K198"/>
-    <mergeCell ref="D189:K189"/>
-    <mergeCell ref="D190:K190"/>
-    <mergeCell ref="D191:K191"/>
-    <mergeCell ref="D192:K192"/>
-    <mergeCell ref="D193:K193"/>
-    <mergeCell ref="D184:K184"/>
-    <mergeCell ref="D185:K185"/>
-    <mergeCell ref="D186:K186"/>
-    <mergeCell ref="D187:K187"/>
-    <mergeCell ref="D188:K188"/>
-    <mergeCell ref="D168:K168"/>
-    <mergeCell ref="D175:K175"/>
-    <mergeCell ref="D178:K178"/>
-    <mergeCell ref="D182:K182"/>
-    <mergeCell ref="D183:K183"/>
+    <mergeCell ref="D304:K305"/>
+    <mergeCell ref="D306:K307"/>
+    <mergeCell ref="D308:K309"/>
+    <mergeCell ref="D298:K299"/>
+    <mergeCell ref="D300:K301"/>
+    <mergeCell ref="D302:K303"/>
   </mergeCells>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="53" fitToHeight="0" orientation="landscape" r:id="rId1"/>
@@ -15817,16 +15812,16 @@
         <f>8*A2&amp;"-"&amp;(8*A2+7)</f>
         <v>0-7</v>
       </c>
-      <c r="D2" s="140" t="s">
+      <c r="D2" s="123" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="136"/>
-      <c r="F2" s="136"/>
-      <c r="G2" s="136"/>
-      <c r="H2" s="136"/>
-      <c r="I2" s="136"/>
-      <c r="J2" s="136"/>
-      <c r="K2" s="137"/>
+      <c r="E2" s="124"/>
+      <c r="F2" s="124"/>
+      <c r="G2" s="124"/>
+      <c r="H2" s="124"/>
+      <c r="I2" s="124"/>
+      <c r="J2" s="124"/>
+      <c r="K2" s="125"/>
       <c r="M2" s="3">
         <v>16</v>
       </c>
@@ -15848,14 +15843,14 @@
         <f t="shared" ref="C3:C33" si="2">8*A3&amp;"-"&amp;(8*A3+7)</f>
         <v>8-15</v>
       </c>
-      <c r="D3" s="146"/>
-      <c r="E3" s="131"/>
-      <c r="F3" s="131"/>
-      <c r="G3" s="131"/>
-      <c r="H3" s="131"/>
-      <c r="I3" s="131"/>
-      <c r="J3" s="131"/>
-      <c r="K3" s="143"/>
+      <c r="D3" s="126"/>
+      <c r="E3" s="127"/>
+      <c r="F3" s="127"/>
+      <c r="G3" s="127"/>
+      <c r="H3" s="127"/>
+      <c r="I3" s="127"/>
+      <c r="J3" s="127"/>
+      <c r="K3" s="131"/>
       <c r="M3" s="3">
         <v>17</v>
       </c>
@@ -22104,16 +22099,16 @@
         <v>AB0</v>
       </c>
       <c r="C178" s="39"/>
-      <c r="D178" s="123" t="s">
+      <c r="D178" s="155" t="s">
         <v>350</v>
       </c>
-      <c r="E178" s="123"/>
-      <c r="F178" s="123"/>
-      <c r="G178" s="123"/>
-      <c r="H178" s="123"/>
-      <c r="I178" s="123"/>
-      <c r="J178" s="123"/>
-      <c r="K178" s="123"/>
+      <c r="E178" s="155"/>
+      <c r="F178" s="155"/>
+      <c r="G178" s="155"/>
+      <c r="H178" s="155"/>
+      <c r="I178" s="155"/>
+      <c r="J178" s="155"/>
+      <c r="K178" s="155"/>
     </row>
     <row r="179" spans="1:14">
       <c r="A179" s="12">
@@ -22182,16 +22177,16 @@
         <v>AB4</v>
       </c>
       <c r="C182" s="13"/>
-      <c r="D182" s="124" t="s">
+      <c r="D182" s="141" t="s">
         <v>351</v>
       </c>
-      <c r="E182" s="125"/>
-      <c r="F182" s="125"/>
-      <c r="G182" s="125"/>
-      <c r="H182" s="125"/>
-      <c r="I182" s="125"/>
-      <c r="J182" s="125"/>
-      <c r="K182" s="126"/>
+      <c r="E182" s="142"/>
+      <c r="F182" s="142"/>
+      <c r="G182" s="142"/>
+      <c r="H182" s="142"/>
+      <c r="I182" s="142"/>
+      <c r="J182" s="142"/>
+      <c r="K182" s="143"/>
     </row>
     <row r="183" spans="1:14">
       <c r="A183" s="12">
@@ -22203,16 +22198,16 @@
         <v>AB5</v>
       </c>
       <c r="C183" s="13"/>
-      <c r="D183" s="124" t="s">
+      <c r="D183" s="141" t="s">
         <v>352</v>
       </c>
-      <c r="E183" s="125"/>
-      <c r="F183" s="125"/>
-      <c r="G183" s="125"/>
-      <c r="H183" s="125"/>
-      <c r="I183" s="125"/>
-      <c r="J183" s="125"/>
-      <c r="K183" s="126"/>
+      <c r="E183" s="142"/>
+      <c r="F183" s="142"/>
+      <c r="G183" s="142"/>
+      <c r="H183" s="142"/>
+      <c r="I183" s="142"/>
+      <c r="J183" s="142"/>
+      <c r="K183" s="143"/>
     </row>
     <row r="184" spans="1:14">
       <c r="A184" s="12">
@@ -22224,16 +22219,16 @@
         <v>AB6</v>
       </c>
       <c r="C184" s="13"/>
-      <c r="D184" s="124" t="s">
+      <c r="D184" s="141" t="s">
         <v>353</v>
       </c>
-      <c r="E184" s="125"/>
-      <c r="F184" s="125"/>
-      <c r="G184" s="125"/>
-      <c r="H184" s="125"/>
-      <c r="I184" s="125"/>
-      <c r="J184" s="125"/>
-      <c r="K184" s="126"/>
+      <c r="E184" s="142"/>
+      <c r="F184" s="142"/>
+      <c r="G184" s="142"/>
+      <c r="H184" s="142"/>
+      <c r="I184" s="142"/>
+      <c r="J184" s="142"/>
+      <c r="K184" s="143"/>
     </row>
     <row r="185" spans="1:14">
       <c r="A185" s="12">
@@ -22245,16 +22240,16 @@
         <v>AB7</v>
       </c>
       <c r="C185" s="13"/>
-      <c r="D185" s="124" t="s">
+      <c r="D185" s="141" t="s">
         <v>354</v>
       </c>
-      <c r="E185" s="125"/>
-      <c r="F185" s="125"/>
-      <c r="G185" s="125"/>
-      <c r="H185" s="125"/>
-      <c r="I185" s="125"/>
-      <c r="J185" s="125"/>
-      <c r="K185" s="126"/>
+      <c r="E185" s="142"/>
+      <c r="F185" s="142"/>
+      <c r="G185" s="142"/>
+      <c r="H185" s="142"/>
+      <c r="I185" s="142"/>
+      <c r="J185" s="142"/>
+      <c r="K185" s="143"/>
     </row>
     <row r="186" spans="1:14">
       <c r="A186" s="12">
@@ -22266,16 +22261,16 @@
         <v>AB8</v>
       </c>
       <c r="C186" s="13"/>
-      <c r="D186" s="124" t="s">
+      <c r="D186" s="141" t="s">
         <v>355</v>
       </c>
-      <c r="E186" s="125"/>
-      <c r="F186" s="125"/>
-      <c r="G186" s="125"/>
-      <c r="H186" s="125"/>
-      <c r="I186" s="125"/>
-      <c r="J186" s="125"/>
-      <c r="K186" s="126"/>
+      <c r="E186" s="142"/>
+      <c r="F186" s="142"/>
+      <c r="G186" s="142"/>
+      <c r="H186" s="142"/>
+      <c r="I186" s="142"/>
+      <c r="J186" s="142"/>
+      <c r="K186" s="143"/>
     </row>
     <row r="187" spans="1:14">
       <c r="A187" s="12">
@@ -22287,16 +22282,16 @@
         <v>AB9</v>
       </c>
       <c r="C187" s="13"/>
-      <c r="D187" s="124" t="s">
+      <c r="D187" s="141" t="s">
         <v>356</v>
       </c>
-      <c r="E187" s="125"/>
-      <c r="F187" s="125"/>
-      <c r="G187" s="125"/>
-      <c r="H187" s="125"/>
-      <c r="I187" s="125"/>
-      <c r="J187" s="125"/>
-      <c r="K187" s="126"/>
+      <c r="E187" s="142"/>
+      <c r="F187" s="142"/>
+      <c r="G187" s="142"/>
+      <c r="H187" s="142"/>
+      <c r="I187" s="142"/>
+      <c r="J187" s="142"/>
+      <c r="K187" s="143"/>
     </row>
     <row r="188" spans="1:14">
       <c r="A188" s="12">
@@ -22308,16 +22303,16 @@
         <v>ABA</v>
       </c>
       <c r="C188" s="13"/>
-      <c r="D188" s="124" t="s">
+      <c r="D188" s="141" t="s">
         <v>357</v>
       </c>
-      <c r="E188" s="125"/>
-      <c r="F188" s="125"/>
-      <c r="G188" s="125"/>
-      <c r="H188" s="125"/>
-      <c r="I188" s="125"/>
-      <c r="J188" s="125"/>
-      <c r="K188" s="126"/>
+      <c r="E188" s="142"/>
+      <c r="F188" s="142"/>
+      <c r="G188" s="142"/>
+      <c r="H188" s="142"/>
+      <c r="I188" s="142"/>
+      <c r="J188" s="142"/>
+      <c r="K188" s="143"/>
     </row>
     <row r="189" spans="1:14">
       <c r="A189" s="12">
@@ -22329,16 +22324,16 @@
         <v>ABB</v>
       </c>
       <c r="C189" s="13"/>
-      <c r="D189" s="124" t="s">
+      <c r="D189" s="141" t="s">
         <v>358</v>
       </c>
-      <c r="E189" s="125"/>
-      <c r="F189" s="125"/>
-      <c r="G189" s="125"/>
-      <c r="H189" s="125"/>
-      <c r="I189" s="125"/>
-      <c r="J189" s="125"/>
-      <c r="K189" s="126"/>
+      <c r="E189" s="142"/>
+      <c r="F189" s="142"/>
+      <c r="G189" s="142"/>
+      <c r="H189" s="142"/>
+      <c r="I189" s="142"/>
+      <c r="J189" s="142"/>
+      <c r="K189" s="143"/>
     </row>
     <row r="190" spans="1:14">
       <c r="A190" s="12">
@@ -22350,16 +22345,16 @@
         <v>ABC</v>
       </c>
       <c r="C190" s="13"/>
-      <c r="D190" s="124" t="s">
+      <c r="D190" s="141" t="s">
         <v>359</v>
       </c>
-      <c r="E190" s="125"/>
-      <c r="F190" s="125"/>
-      <c r="G190" s="125"/>
-      <c r="H190" s="125"/>
-      <c r="I190" s="125"/>
-      <c r="J190" s="125"/>
-      <c r="K190" s="126"/>
+      <c r="E190" s="142"/>
+      <c r="F190" s="142"/>
+      <c r="G190" s="142"/>
+      <c r="H190" s="142"/>
+      <c r="I190" s="142"/>
+      <c r="J190" s="142"/>
+      <c r="K190" s="143"/>
     </row>
     <row r="191" spans="1:14">
       <c r="A191" s="12">
@@ -22371,16 +22366,16 @@
         <v>ABD</v>
       </c>
       <c r="C191" s="13"/>
-      <c r="D191" s="124" t="s">
+      <c r="D191" s="141" t="s">
         <v>360</v>
       </c>
-      <c r="E191" s="125"/>
-      <c r="F191" s="125"/>
-      <c r="G191" s="125"/>
-      <c r="H191" s="125"/>
-      <c r="I191" s="125"/>
-      <c r="J191" s="125"/>
-      <c r="K191" s="126"/>
+      <c r="E191" s="142"/>
+      <c r="F191" s="142"/>
+      <c r="G191" s="142"/>
+      <c r="H191" s="142"/>
+      <c r="I191" s="142"/>
+      <c r="J191" s="142"/>
+      <c r="K191" s="143"/>
     </row>
     <row r="192" spans="1:14">
       <c r="A192" s="12">
@@ -22392,16 +22387,16 @@
         <v>ABE</v>
       </c>
       <c r="C192" s="13"/>
-      <c r="D192" s="124" t="s">
+      <c r="D192" s="141" t="s">
         <v>361</v>
       </c>
-      <c r="E192" s="125"/>
-      <c r="F192" s="125"/>
-      <c r="G192" s="125"/>
-      <c r="H192" s="125"/>
-      <c r="I192" s="125"/>
-      <c r="J192" s="125"/>
-      <c r="K192" s="126"/>
+      <c r="E192" s="142"/>
+      <c r="F192" s="142"/>
+      <c r="G192" s="142"/>
+      <c r="H192" s="142"/>
+      <c r="I192" s="142"/>
+      <c r="J192" s="142"/>
+      <c r="K192" s="143"/>
     </row>
     <row r="193" spans="1:14" s="1" customFormat="1">
       <c r="A193" s="32">
@@ -22413,16 +22408,16 @@
         <v>ABF</v>
       </c>
       <c r="C193" s="33"/>
-      <c r="D193" s="127" t="s">
+      <c r="D193" s="152" t="s">
         <v>362</v>
       </c>
-      <c r="E193" s="128"/>
-      <c r="F193" s="128"/>
-      <c r="G193" s="128"/>
-      <c r="H193" s="128"/>
-      <c r="I193" s="128"/>
-      <c r="J193" s="128"/>
-      <c r="K193" s="129"/>
+      <c r="E193" s="153"/>
+      <c r="F193" s="153"/>
+      <c r="G193" s="153"/>
+      <c r="H193" s="153"/>
+      <c r="I193" s="153"/>
+      <c r="J193" s="153"/>
+      <c r="K193" s="154"/>
       <c r="L193" s="57"/>
       <c r="M193" s="58"/>
       <c r="N193" s="58"/>
@@ -22437,16 +22432,16 @@
         <v>AC0</v>
       </c>
       <c r="C194" s="39"/>
-      <c r="D194" s="130" t="s">
+      <c r="D194" s="134" t="s">
         <v>363</v>
       </c>
-      <c r="E194" s="131"/>
-      <c r="F194" s="131"/>
-      <c r="G194" s="131"/>
-      <c r="H194" s="131"/>
-      <c r="I194" s="131"/>
-      <c r="J194" s="131"/>
-      <c r="K194" s="132"/>
+      <c r="E194" s="127"/>
+      <c r="F194" s="127"/>
+      <c r="G194" s="127"/>
+      <c r="H194" s="127"/>
+      <c r="I194" s="127"/>
+      <c r="J194" s="127"/>
+      <c r="K194" s="135"/>
     </row>
     <row r="195" spans="1:14">
       <c r="A195" s="12">
@@ -22458,16 +22453,16 @@
         <v>AC1</v>
       </c>
       <c r="C195" s="13"/>
-      <c r="D195" s="124" t="s">
+      <c r="D195" s="141" t="s">
         <v>364</v>
       </c>
-      <c r="E195" s="125"/>
-      <c r="F195" s="125"/>
-      <c r="G195" s="125"/>
-      <c r="H195" s="125"/>
-      <c r="I195" s="125"/>
-      <c r="J195" s="125"/>
-      <c r="K195" s="126"/>
+      <c r="E195" s="142"/>
+      <c r="F195" s="142"/>
+      <c r="G195" s="142"/>
+      <c r="H195" s="142"/>
+      <c r="I195" s="142"/>
+      <c r="J195" s="142"/>
+      <c r="K195" s="143"/>
     </row>
     <row r="196" spans="1:14">
       <c r="A196" s="12">
@@ -22479,16 +22474,16 @@
         <v>AC2</v>
       </c>
       <c r="C196" s="13"/>
-      <c r="D196" s="124" t="s">
+      <c r="D196" s="141" t="s">
         <v>365</v>
       </c>
-      <c r="E196" s="125"/>
-      <c r="F196" s="125"/>
-      <c r="G196" s="125"/>
-      <c r="H196" s="125"/>
-      <c r="I196" s="125"/>
-      <c r="J196" s="125"/>
-      <c r="K196" s="126"/>
+      <c r="E196" s="142"/>
+      <c r="F196" s="142"/>
+      <c r="G196" s="142"/>
+      <c r="H196" s="142"/>
+      <c r="I196" s="142"/>
+      <c r="J196" s="142"/>
+      <c r="K196" s="143"/>
     </row>
     <row r="197" spans="1:14">
       <c r="A197" s="12">
@@ -22500,16 +22495,16 @@
         <v>AC3</v>
       </c>
       <c r="C197" s="13"/>
-      <c r="D197" s="124" t="s">
+      <c r="D197" s="141" t="s">
         <v>366</v>
       </c>
-      <c r="E197" s="125"/>
-      <c r="F197" s="125"/>
-      <c r="G197" s="125"/>
-      <c r="H197" s="125"/>
-      <c r="I197" s="125"/>
-      <c r="J197" s="125"/>
-      <c r="K197" s="126"/>
+      <c r="E197" s="142"/>
+      <c r="F197" s="142"/>
+      <c r="G197" s="142"/>
+      <c r="H197" s="142"/>
+      <c r="I197" s="142"/>
+      <c r="J197" s="142"/>
+      <c r="K197" s="143"/>
     </row>
     <row r="198" spans="1:14">
       <c r="A198" s="12">
@@ -22521,16 +22516,16 @@
         <v>AC4</v>
       </c>
       <c r="C198" s="13"/>
-      <c r="D198" s="124" t="s">
+      <c r="D198" s="141" t="s">
         <v>367</v>
       </c>
-      <c r="E198" s="125"/>
-      <c r="F198" s="125"/>
-      <c r="G198" s="125"/>
-      <c r="H198" s="125"/>
-      <c r="I198" s="125"/>
-      <c r="J198" s="125"/>
-      <c r="K198" s="126"/>
+      <c r="E198" s="142"/>
+      <c r="F198" s="142"/>
+      <c r="G198" s="142"/>
+      <c r="H198" s="142"/>
+      <c r="I198" s="142"/>
+      <c r="J198" s="142"/>
+      <c r="K198" s="143"/>
     </row>
     <row r="199" spans="1:14">
       <c r="A199" s="12">
@@ -22561,16 +22556,16 @@
         <v>AC6</v>
       </c>
       <c r="C200" s="13"/>
-      <c r="D200" s="124" t="s">
+      <c r="D200" s="141" t="s">
         <v>368</v>
       </c>
-      <c r="E200" s="125"/>
-      <c r="F200" s="125"/>
-      <c r="G200" s="125"/>
-      <c r="H200" s="125"/>
-      <c r="I200" s="125"/>
-      <c r="J200" s="125"/>
-      <c r="K200" s="126"/>
+      <c r="E200" s="142"/>
+      <c r="F200" s="142"/>
+      <c r="G200" s="142"/>
+      <c r="H200" s="142"/>
+      <c r="I200" s="142"/>
+      <c r="J200" s="142"/>
+      <c r="K200" s="143"/>
     </row>
     <row r="201" spans="1:14">
       <c r="A201" s="12">
@@ -22601,16 +22596,16 @@
         <v>AC8</v>
       </c>
       <c r="C202" s="13"/>
-      <c r="D202" s="153" t="s">
+      <c r="D202" s="149" t="s">
         <v>369</v>
       </c>
-      <c r="E202" s="154"/>
-      <c r="F202" s="154"/>
-      <c r="G202" s="154"/>
-      <c r="H202" s="154"/>
-      <c r="I202" s="154"/>
-      <c r="J202" s="154"/>
-      <c r="K202" s="155"/>
+      <c r="E202" s="150"/>
+      <c r="F202" s="150"/>
+      <c r="G202" s="150"/>
+      <c r="H202" s="150"/>
+      <c r="I202" s="150"/>
+      <c r="J202" s="150"/>
+      <c r="K202" s="151"/>
     </row>
     <row r="203" spans="1:14">
       <c r="A203" s="12">
@@ -22641,16 +22636,16 @@
         <v>ACA</v>
       </c>
       <c r="C204" s="13"/>
-      <c r="D204" s="124" t="s">
+      <c r="D204" s="141" t="s">
         <v>370</v>
       </c>
-      <c r="E204" s="125"/>
-      <c r="F204" s="125"/>
-      <c r="G204" s="125"/>
-      <c r="H204" s="125"/>
-      <c r="I204" s="125"/>
-      <c r="J204" s="125"/>
-      <c r="K204" s="126"/>
+      <c r="E204" s="142"/>
+      <c r="F204" s="142"/>
+      <c r="G204" s="142"/>
+      <c r="H204" s="142"/>
+      <c r="I204" s="142"/>
+      <c r="J204" s="142"/>
+      <c r="K204" s="143"/>
     </row>
     <row r="205" spans="1:14">
       <c r="A205" s="12">
@@ -22681,16 +22676,16 @@
         <v>ACC</v>
       </c>
       <c r="C206" s="13"/>
-      <c r="D206" s="124" t="s">
+      <c r="D206" s="141" t="s">
         <v>370</v>
       </c>
-      <c r="E206" s="125"/>
-      <c r="F206" s="125"/>
-      <c r="G206" s="125"/>
-      <c r="H206" s="125"/>
-      <c r="I206" s="125"/>
-      <c r="J206" s="125"/>
-      <c r="K206" s="126"/>
+      <c r="E206" s="142"/>
+      <c r="F206" s="142"/>
+      <c r="G206" s="142"/>
+      <c r="H206" s="142"/>
+      <c r="I206" s="142"/>
+      <c r="J206" s="142"/>
+      <c r="K206" s="143"/>
     </row>
     <row r="207" spans="1:14">
       <c r="A207" s="12">
@@ -22721,16 +22716,16 @@
         <v>ACE</v>
       </c>
       <c r="C208" s="13"/>
-      <c r="D208" s="124" t="s">
+      <c r="D208" s="141" t="s">
         <v>371</v>
       </c>
-      <c r="E208" s="125"/>
-      <c r="F208" s="125"/>
-      <c r="G208" s="125"/>
-      <c r="H208" s="125"/>
-      <c r="I208" s="125"/>
-      <c r="J208" s="125"/>
-      <c r="K208" s="126"/>
+      <c r="E208" s="142"/>
+      <c r="F208" s="142"/>
+      <c r="G208" s="142"/>
+      <c r="H208" s="142"/>
+      <c r="I208" s="142"/>
+      <c r="J208" s="142"/>
+      <c r="K208" s="143"/>
     </row>
     <row r="209" spans="1:14" s="1" customFormat="1">
       <c r="A209" s="32">
@@ -22764,16 +22759,16 @@
         <v>AD0</v>
       </c>
       <c r="C210" s="39"/>
-      <c r="D210" s="130" t="s">
+      <c r="D210" s="134" t="s">
         <v>371</v>
       </c>
-      <c r="E210" s="131"/>
-      <c r="F210" s="131"/>
-      <c r="G210" s="131"/>
-      <c r="H210" s="131"/>
-      <c r="I210" s="131"/>
-      <c r="J210" s="131"/>
-      <c r="K210" s="132"/>
+      <c r="E210" s="127"/>
+      <c r="F210" s="127"/>
+      <c r="G210" s="127"/>
+      <c r="H210" s="127"/>
+      <c r="I210" s="127"/>
+      <c r="J210" s="127"/>
+      <c r="K210" s="135"/>
     </row>
     <row r="211" spans="1:14">
       <c r="A211" s="12">
@@ -22842,16 +22837,16 @@
         <v>AD4</v>
       </c>
       <c r="C214" s="13"/>
-      <c r="D214" s="124" t="s">
+      <c r="D214" s="141" t="s">
         <v>372</v>
       </c>
-      <c r="E214" s="125"/>
-      <c r="F214" s="125"/>
-      <c r="G214" s="125"/>
-      <c r="H214" s="125"/>
-      <c r="I214" s="125"/>
-      <c r="J214" s="125"/>
-      <c r="K214" s="126"/>
+      <c r="E214" s="142"/>
+      <c r="F214" s="142"/>
+      <c r="G214" s="142"/>
+      <c r="H214" s="142"/>
+      <c r="I214" s="142"/>
+      <c r="J214" s="142"/>
+      <c r="K214" s="143"/>
     </row>
     <row r="215" spans="1:14">
       <c r="A215" s="12">
@@ -22882,16 +22877,16 @@
         <v>AD6</v>
       </c>
       <c r="C216" s="13"/>
-      <c r="D216" s="144" t="s">
+      <c r="D216" s="132" t="s">
         <v>373</v>
       </c>
-      <c r="E216" s="136"/>
-      <c r="F216" s="136"/>
-      <c r="G216" s="136"/>
-      <c r="H216" s="136"/>
-      <c r="I216" s="136"/>
-      <c r="J216" s="136"/>
-      <c r="K216" s="145"/>
+      <c r="E216" s="124"/>
+      <c r="F216" s="124"/>
+      <c r="G216" s="124"/>
+      <c r="H216" s="124"/>
+      <c r="I216" s="124"/>
+      <c r="J216" s="124"/>
+      <c r="K216" s="133"/>
     </row>
     <row r="217" spans="1:14">
       <c r="A217" s="12">
@@ -22903,14 +22898,14 @@
         <v>AD7</v>
       </c>
       <c r="C217" s="13"/>
-      <c r="D217" s="130"/>
-      <c r="E217" s="131"/>
-      <c r="F217" s="131"/>
-      <c r="G217" s="131"/>
-      <c r="H217" s="131"/>
-      <c r="I217" s="131"/>
-      <c r="J217" s="131"/>
-      <c r="K217" s="132"/>
+      <c r="D217" s="134"/>
+      <c r="E217" s="127"/>
+      <c r="F217" s="127"/>
+      <c r="G217" s="127"/>
+      <c r="H217" s="127"/>
+      <c r="I217" s="127"/>
+      <c r="J217" s="127"/>
+      <c r="K217" s="135"/>
     </row>
     <row r="218" spans="1:14">
       <c r="A218" s="12">
@@ -22922,16 +22917,16 @@
         <v>AD8</v>
       </c>
       <c r="C218" s="13"/>
-      <c r="D218" s="144" t="s">
+      <c r="D218" s="132" t="s">
         <v>374</v>
       </c>
-      <c r="E218" s="136"/>
-      <c r="F218" s="136"/>
-      <c r="G218" s="136"/>
-      <c r="H218" s="136"/>
-      <c r="I218" s="136"/>
-      <c r="J218" s="136"/>
-      <c r="K218" s="145"/>
+      <c r="E218" s="124"/>
+      <c r="F218" s="124"/>
+      <c r="G218" s="124"/>
+      <c r="H218" s="124"/>
+      <c r="I218" s="124"/>
+      <c r="J218" s="124"/>
+      <c r="K218" s="133"/>
     </row>
     <row r="219" spans="1:14">
       <c r="A219" s="12">
@@ -22943,14 +22938,14 @@
         <v>AD9</v>
       </c>
       <c r="C219" s="13"/>
-      <c r="D219" s="130"/>
-      <c r="E219" s="131"/>
-      <c r="F219" s="131"/>
-      <c r="G219" s="131"/>
-      <c r="H219" s="131"/>
-      <c r="I219" s="131"/>
-      <c r="J219" s="131"/>
-      <c r="K219" s="132"/>
+      <c r="D219" s="134"/>
+      <c r="E219" s="127"/>
+      <c r="F219" s="127"/>
+      <c r="G219" s="127"/>
+      <c r="H219" s="127"/>
+      <c r="I219" s="127"/>
+      <c r="J219" s="127"/>
+      <c r="K219" s="135"/>
     </row>
     <row r="220" spans="1:14">
       <c r="A220" s="12">
@@ -22962,16 +22957,16 @@
         <v>ADA</v>
       </c>
       <c r="C220" s="13"/>
-      <c r="D220" s="144" t="s">
+      <c r="D220" s="132" t="s">
         <v>375</v>
       </c>
-      <c r="E220" s="136"/>
-      <c r="F220" s="136"/>
-      <c r="G220" s="136"/>
-      <c r="H220" s="136"/>
-      <c r="I220" s="136"/>
-      <c r="J220" s="136"/>
-      <c r="K220" s="145"/>
+      <c r="E220" s="124"/>
+      <c r="F220" s="124"/>
+      <c r="G220" s="124"/>
+      <c r="H220" s="124"/>
+      <c r="I220" s="124"/>
+      <c r="J220" s="124"/>
+      <c r="K220" s="133"/>
     </row>
     <row r="221" spans="1:14">
       <c r="A221" s="12">
@@ -22983,14 +22978,14 @@
         <v>ADB</v>
       </c>
       <c r="C221" s="13"/>
-      <c r="D221" s="130"/>
-      <c r="E221" s="131"/>
-      <c r="F221" s="131"/>
-      <c r="G221" s="131"/>
-      <c r="H221" s="131"/>
-      <c r="I221" s="131"/>
-      <c r="J221" s="131"/>
-      <c r="K221" s="132"/>
+      <c r="D221" s="134"/>
+      <c r="E221" s="127"/>
+      <c r="F221" s="127"/>
+      <c r="G221" s="127"/>
+      <c r="H221" s="127"/>
+      <c r="I221" s="127"/>
+      <c r="J221" s="127"/>
+      <c r="K221" s="135"/>
     </row>
     <row r="222" spans="1:14">
       <c r="A222" s="12">
@@ -23002,16 +22997,16 @@
         <v>ADC</v>
       </c>
       <c r="C222" s="13"/>
-      <c r="D222" s="124" t="s">
+      <c r="D222" s="141" t="s">
         <v>376</v>
       </c>
-      <c r="E222" s="125"/>
-      <c r="F222" s="125"/>
-      <c r="G222" s="125"/>
-      <c r="H222" s="125"/>
-      <c r="I222" s="125"/>
-      <c r="J222" s="125"/>
-      <c r="K222" s="126"/>
+      <c r="E222" s="142"/>
+      <c r="F222" s="142"/>
+      <c r="G222" s="142"/>
+      <c r="H222" s="142"/>
+      <c r="I222" s="142"/>
+      <c r="J222" s="142"/>
+      <c r="K222" s="143"/>
     </row>
     <row r="223" spans="1:14">
       <c r="A223" s="12">
@@ -23042,16 +23037,16 @@
         <v>ADE</v>
       </c>
       <c r="C224" s="13"/>
-      <c r="D224" s="124" t="s">
+      <c r="D224" s="141" t="s">
         <v>377</v>
       </c>
-      <c r="E224" s="125"/>
-      <c r="F224" s="125"/>
-      <c r="G224" s="125"/>
-      <c r="H224" s="125"/>
-      <c r="I224" s="125"/>
-      <c r="J224" s="125"/>
-      <c r="K224" s="126"/>
+      <c r="E224" s="142"/>
+      <c r="F224" s="142"/>
+      <c r="G224" s="142"/>
+      <c r="H224" s="142"/>
+      <c r="I224" s="142"/>
+      <c r="J224" s="142"/>
+      <c r="K224" s="143"/>
     </row>
     <row r="225" spans="1:14" s="1" customFormat="1">
       <c r="A225" s="32">
@@ -23085,16 +23080,16 @@
         <v>AE0</v>
       </c>
       <c r="C226" s="39"/>
-      <c r="D226" s="150" t="s">
+      <c r="D226" s="146" t="s">
         <v>378</v>
       </c>
-      <c r="E226" s="151"/>
-      <c r="F226" s="151"/>
-      <c r="G226" s="151"/>
-      <c r="H226" s="151"/>
-      <c r="I226" s="151"/>
-      <c r="J226" s="151"/>
-      <c r="K226" s="152"/>
+      <c r="E226" s="147"/>
+      <c r="F226" s="147"/>
+      <c r="G226" s="147"/>
+      <c r="H226" s="147"/>
+      <c r="I226" s="147"/>
+      <c r="J226" s="147"/>
+      <c r="K226" s="148"/>
     </row>
     <row r="227" spans="1:14">
       <c r="A227" s="12">
@@ -23239,16 +23234,16 @@
         <v>AE8</v>
       </c>
       <c r="C234" s="13"/>
-      <c r="D234" s="148" t="s">
+      <c r="D234" s="136" t="s">
         <v>379</v>
       </c>
-      <c r="E234" s="134"/>
-      <c r="F234" s="134"/>
-      <c r="G234" s="134"/>
-      <c r="H234" s="134"/>
-      <c r="I234" s="134"/>
-      <c r="J234" s="134"/>
-      <c r="K234" s="149"/>
+      <c r="E234" s="137"/>
+      <c r="F234" s="137"/>
+      <c r="G234" s="137"/>
+      <c r="H234" s="137"/>
+      <c r="I234" s="137"/>
+      <c r="J234" s="137"/>
+      <c r="K234" s="138"/>
     </row>
     <row r="235" spans="1:14">
       <c r="A235" s="12">
@@ -23317,16 +23312,16 @@
         <v>AEC</v>
       </c>
       <c r="C238" s="13"/>
-      <c r="D238" s="140" t="s">
+      <c r="D238" s="123" t="s">
         <v>380</v>
       </c>
-      <c r="E238" s="136"/>
-      <c r="F238" s="136"/>
-      <c r="G238" s="136"/>
-      <c r="H238" s="136"/>
-      <c r="I238" s="136"/>
-      <c r="J238" s="136"/>
-      <c r="K238" s="137"/>
+      <c r="E238" s="124"/>
+      <c r="F238" s="124"/>
+      <c r="G238" s="124"/>
+      <c r="H238" s="124"/>
+      <c r="I238" s="124"/>
+      <c r="J238" s="124"/>
+      <c r="K238" s="125"/>
     </row>
     <row r="239" spans="1:14">
       <c r="A239" s="12">
@@ -23338,14 +23333,14 @@
         <v>AED</v>
       </c>
       <c r="C239" s="13"/>
-      <c r="D239" s="146"/>
-      <c r="E239" s="131"/>
-      <c r="F239" s="131"/>
-      <c r="G239" s="131"/>
-      <c r="H239" s="131"/>
-      <c r="I239" s="131"/>
-      <c r="J239" s="131"/>
-      <c r="K239" s="147"/>
+      <c r="D239" s="126"/>
+      <c r="E239" s="127"/>
+      <c r="F239" s="127"/>
+      <c r="G239" s="127"/>
+      <c r="H239" s="127"/>
+      <c r="I239" s="127"/>
+      <c r="J239" s="127"/>
+      <c r="K239" s="128"/>
     </row>
     <row r="240" spans="1:14">
       <c r="A240" s="12">
@@ -23357,16 +23352,16 @@
         <v>AEE</v>
       </c>
       <c r="C240" s="70"/>
-      <c r="D240" s="136" t="s">
+      <c r="D240" s="124" t="s">
         <v>381</v>
       </c>
-      <c r="E240" s="136"/>
-      <c r="F240" s="136"/>
-      <c r="G240" s="136"/>
-      <c r="H240" s="136"/>
-      <c r="I240" s="136"/>
-      <c r="J240" s="136"/>
-      <c r="K240" s="137"/>
+      <c r="E240" s="124"/>
+      <c r="F240" s="124"/>
+      <c r="G240" s="124"/>
+      <c r="H240" s="124"/>
+      <c r="I240" s="124"/>
+      <c r="J240" s="124"/>
+      <c r="K240" s="125"/>
     </row>
     <row r="241" spans="1:14" s="1" customFormat="1">
       <c r="A241" s="32">
@@ -23378,14 +23373,14 @@
         <v>AEF</v>
       </c>
       <c r="C241" s="34"/>
-      <c r="D241" s="138"/>
-      <c r="E241" s="138"/>
-      <c r="F241" s="138"/>
-      <c r="G241" s="138"/>
-      <c r="H241" s="138"/>
-      <c r="I241" s="138"/>
-      <c r="J241" s="138"/>
-      <c r="K241" s="139"/>
+      <c r="D241" s="144"/>
+      <c r="E241" s="144"/>
+      <c r="F241" s="144"/>
+      <c r="G241" s="144"/>
+      <c r="H241" s="144"/>
+      <c r="I241" s="144"/>
+      <c r="J241" s="144"/>
+      <c r="K241" s="145"/>
       <c r="L241" s="57"/>
       <c r="M241" s="58"/>
       <c r="N241" s="58"/>
@@ -23576,16 +23571,16 @@
         <v>AF8</v>
       </c>
       <c r="C250" s="13"/>
-      <c r="D250" s="133" t="s">
+      <c r="D250" s="139" t="s">
         <v>382</v>
       </c>
-      <c r="E250" s="134"/>
-      <c r="F250" s="134"/>
-      <c r="G250" s="134"/>
-      <c r="H250" s="134"/>
-      <c r="I250" s="134"/>
-      <c r="J250" s="134"/>
-      <c r="K250" s="135"/>
+      <c r="E250" s="137"/>
+      <c r="F250" s="137"/>
+      <c r="G250" s="137"/>
+      <c r="H250" s="137"/>
+      <c r="I250" s="137"/>
+      <c r="J250" s="137"/>
+      <c r="K250" s="140"/>
     </row>
     <row r="251" spans="1:14">
       <c r="A251" s="12">
@@ -24154,16 +24149,16 @@
         <v>B16</v>
       </c>
       <c r="C280" s="13"/>
-      <c r="D280" s="124" t="s">
+      <c r="D280" s="141" t="s">
         <v>383</v>
       </c>
-      <c r="E280" s="125"/>
-      <c r="F280" s="125"/>
-      <c r="G280" s="125"/>
-      <c r="H280" s="125"/>
-      <c r="I280" s="125"/>
-      <c r="J280" s="125"/>
-      <c r="K280" s="126"/>
+      <c r="E280" s="142"/>
+      <c r="F280" s="142"/>
+      <c r="G280" s="142"/>
+      <c r="H280" s="142"/>
+      <c r="I280" s="142"/>
+      <c r="J280" s="142"/>
+      <c r="K280" s="143"/>
     </row>
     <row r="281" spans="1:14">
       <c r="A281" s="12">
@@ -24270,16 +24265,16 @@
         <v>B1C</v>
       </c>
       <c r="C286" s="13"/>
-      <c r="D286" s="124" t="s">
+      <c r="D286" s="141" t="s">
         <v>384</v>
       </c>
-      <c r="E286" s="125"/>
-      <c r="F286" s="125"/>
-      <c r="G286" s="125"/>
-      <c r="H286" s="125"/>
-      <c r="I286" s="125"/>
-      <c r="J286" s="125"/>
-      <c r="K286" s="126"/>
+      <c r="E286" s="142"/>
+      <c r="F286" s="142"/>
+      <c r="G286" s="142"/>
+      <c r="H286" s="142"/>
+      <c r="I286" s="142"/>
+      <c r="J286" s="142"/>
+      <c r="K286" s="143"/>
     </row>
     <row r="287" spans="1:14">
       <c r="A287" s="12">
@@ -24467,16 +24462,16 @@
         <v>B26</v>
       </c>
       <c r="C296" s="13"/>
-      <c r="D296" s="124" t="s">
+      <c r="D296" s="141" t="s">
         <v>386</v>
       </c>
-      <c r="E296" s="125"/>
-      <c r="F296" s="125"/>
-      <c r="G296" s="125"/>
-      <c r="H296" s="125"/>
-      <c r="I296" s="125"/>
-      <c r="J296" s="125"/>
-      <c r="K296" s="126"/>
+      <c r="E296" s="142"/>
+      <c r="F296" s="142"/>
+      <c r="G296" s="142"/>
+      <c r="H296" s="142"/>
+      <c r="I296" s="142"/>
+      <c r="J296" s="142"/>
+      <c r="K296" s="143"/>
     </row>
     <row r="297" spans="1:14">
       <c r="A297" s="12">
@@ -24507,16 +24502,16 @@
         <v>B28</v>
       </c>
       <c r="C298" s="13"/>
-      <c r="D298" s="140" t="s">
+      <c r="D298" s="123" t="s">
         <v>387</v>
       </c>
-      <c r="E298" s="136"/>
-      <c r="F298" s="136"/>
-      <c r="G298" s="136"/>
-      <c r="H298" s="136"/>
-      <c r="I298" s="136"/>
-      <c r="J298" s="136"/>
-      <c r="K298" s="137"/>
+      <c r="E298" s="124"/>
+      <c r="F298" s="124"/>
+      <c r="G298" s="124"/>
+      <c r="H298" s="124"/>
+      <c r="I298" s="124"/>
+      <c r="J298" s="124"/>
+      <c r="K298" s="125"/>
     </row>
     <row r="299" spans="1:14">
       <c r="A299" s="12">
@@ -24528,14 +24523,14 @@
         <v>B29</v>
       </c>
       <c r="C299" s="13"/>
-      <c r="D299" s="146"/>
-      <c r="E299" s="131"/>
-      <c r="F299" s="131"/>
-      <c r="G299" s="131"/>
-      <c r="H299" s="131"/>
-      <c r="I299" s="131"/>
-      <c r="J299" s="131"/>
-      <c r="K299" s="147"/>
+      <c r="D299" s="126"/>
+      <c r="E299" s="127"/>
+      <c r="F299" s="127"/>
+      <c r="G299" s="127"/>
+      <c r="H299" s="127"/>
+      <c r="I299" s="127"/>
+      <c r="J299" s="127"/>
+      <c r="K299" s="128"/>
     </row>
     <row r="300" spans="1:14">
       <c r="A300" s="12">
@@ -24547,16 +24542,16 @@
         <v>B2A</v>
       </c>
       <c r="C300" s="13"/>
-      <c r="D300" s="140" t="s">
+      <c r="D300" s="123" t="s">
         <v>388</v>
       </c>
-      <c r="E300" s="136"/>
-      <c r="F300" s="136"/>
-      <c r="G300" s="136"/>
-      <c r="H300" s="136"/>
-      <c r="I300" s="136"/>
-      <c r="J300" s="136"/>
-      <c r="K300" s="137"/>
+      <c r="E300" s="124"/>
+      <c r="F300" s="124"/>
+      <c r="G300" s="124"/>
+      <c r="H300" s="124"/>
+      <c r="I300" s="124"/>
+      <c r="J300" s="124"/>
+      <c r="K300" s="125"/>
     </row>
     <row r="301" spans="1:14">
       <c r="A301" s="12">
@@ -24568,14 +24563,14 @@
         <v>B2B</v>
       </c>
       <c r="C301" s="13"/>
-      <c r="D301" s="146"/>
-      <c r="E301" s="131"/>
-      <c r="F301" s="131"/>
-      <c r="G301" s="131"/>
-      <c r="H301" s="131"/>
-      <c r="I301" s="131"/>
-      <c r="J301" s="131"/>
-      <c r="K301" s="147"/>
+      <c r="D301" s="126"/>
+      <c r="E301" s="127"/>
+      <c r="F301" s="127"/>
+      <c r="G301" s="127"/>
+      <c r="H301" s="127"/>
+      <c r="I301" s="127"/>
+      <c r="J301" s="127"/>
+      <c r="K301" s="128"/>
     </row>
     <row r="302" spans="1:14">
       <c r="A302" s="12">
@@ -24587,16 +24582,16 @@
         <v>B2C</v>
       </c>
       <c r="C302" s="13"/>
-      <c r="D302" s="140" t="s">
+      <c r="D302" s="123" t="s">
         <v>389</v>
       </c>
-      <c r="E302" s="136"/>
-      <c r="F302" s="136"/>
-      <c r="G302" s="136"/>
-      <c r="H302" s="136"/>
-      <c r="I302" s="136"/>
-      <c r="J302" s="136"/>
-      <c r="K302" s="137"/>
+      <c r="E302" s="124"/>
+      <c r="F302" s="124"/>
+      <c r="G302" s="124"/>
+      <c r="H302" s="124"/>
+      <c r="I302" s="124"/>
+      <c r="J302" s="124"/>
+      <c r="K302" s="125"/>
     </row>
     <row r="303" spans="1:14">
       <c r="A303" s="12">
@@ -24608,14 +24603,14 @@
         <v>B2D</v>
       </c>
       <c r="C303" s="13"/>
-      <c r="D303" s="146"/>
-      <c r="E303" s="131"/>
-      <c r="F303" s="131"/>
-      <c r="G303" s="131"/>
-      <c r="H303" s="131"/>
-      <c r="I303" s="131"/>
-      <c r="J303" s="131"/>
-      <c r="K303" s="147"/>
+      <c r="D303" s="126"/>
+      <c r="E303" s="127"/>
+      <c r="F303" s="127"/>
+      <c r="G303" s="127"/>
+      <c r="H303" s="127"/>
+      <c r="I303" s="127"/>
+      <c r="J303" s="127"/>
+      <c r="K303" s="128"/>
     </row>
     <row r="304" spans="1:14">
       <c r="A304" s="12">
@@ -24627,16 +24622,16 @@
         <v>B2E</v>
       </c>
       <c r="C304" s="13"/>
-      <c r="D304" s="140" t="s">
+      <c r="D304" s="123" t="s">
         <v>390</v>
       </c>
-      <c r="E304" s="136"/>
-      <c r="F304" s="136"/>
-      <c r="G304" s="136"/>
-      <c r="H304" s="136"/>
-      <c r="I304" s="136"/>
-      <c r="J304" s="136"/>
-      <c r="K304" s="137"/>
+      <c r="E304" s="124"/>
+      <c r="F304" s="124"/>
+      <c r="G304" s="124"/>
+      <c r="H304" s="124"/>
+      <c r="I304" s="124"/>
+      <c r="J304" s="124"/>
+      <c r="K304" s="125"/>
     </row>
     <row r="305" spans="1:14" s="1" customFormat="1">
       <c r="A305" s="32">
@@ -24648,14 +24643,14 @@
         <v>B2F</v>
       </c>
       <c r="C305" s="33"/>
-      <c r="D305" s="146"/>
-      <c r="E305" s="131"/>
-      <c r="F305" s="131"/>
-      <c r="G305" s="131"/>
-      <c r="H305" s="131"/>
-      <c r="I305" s="131"/>
-      <c r="J305" s="131"/>
-      <c r="K305" s="147"/>
+      <c r="D305" s="126"/>
+      <c r="E305" s="127"/>
+      <c r="F305" s="127"/>
+      <c r="G305" s="127"/>
+      <c r="H305" s="127"/>
+      <c r="I305" s="127"/>
+      <c r="J305" s="127"/>
+      <c r="K305" s="128"/>
       <c r="L305" s="57"/>
       <c r="M305" s="58"/>
       <c r="N305" s="58"/>
@@ -24670,16 +24665,16 @@
         <v>B30</v>
       </c>
       <c r="C306" s="39"/>
-      <c r="D306" s="140" t="s">
+      <c r="D306" s="123" t="s">
         <v>391</v>
       </c>
-      <c r="E306" s="136"/>
-      <c r="F306" s="136"/>
-      <c r="G306" s="136"/>
-      <c r="H306" s="136"/>
-      <c r="I306" s="136"/>
-      <c r="J306" s="136"/>
-      <c r="K306" s="137"/>
+      <c r="E306" s="124"/>
+      <c r="F306" s="124"/>
+      <c r="G306" s="124"/>
+      <c r="H306" s="124"/>
+      <c r="I306" s="124"/>
+      <c r="J306" s="124"/>
+      <c r="K306" s="125"/>
     </row>
     <row r="307" spans="1:14">
       <c r="A307" s="12">
@@ -24691,14 +24686,14 @@
         <v>B31</v>
       </c>
       <c r="C307" s="13"/>
-      <c r="D307" s="146"/>
-      <c r="E307" s="131"/>
-      <c r="F307" s="131"/>
-      <c r="G307" s="131"/>
-      <c r="H307" s="131"/>
-      <c r="I307" s="131"/>
-      <c r="J307" s="131"/>
-      <c r="K307" s="147"/>
+      <c r="D307" s="126"/>
+      <c r="E307" s="127"/>
+      <c r="F307" s="127"/>
+      <c r="G307" s="127"/>
+      <c r="H307" s="127"/>
+      <c r="I307" s="127"/>
+      <c r="J307" s="127"/>
+      <c r="K307" s="128"/>
     </row>
     <row r="308" spans="1:14">
       <c r="A308" s="12">
@@ -24710,16 +24705,16 @@
         <v>B32</v>
       </c>
       <c r="C308" s="13"/>
-      <c r="D308" s="140" t="s">
+      <c r="D308" s="123" t="s">
         <v>392</v>
       </c>
-      <c r="E308" s="136"/>
-      <c r="F308" s="136"/>
-      <c r="G308" s="136"/>
-      <c r="H308" s="136"/>
-      <c r="I308" s="136"/>
-      <c r="J308" s="136"/>
-      <c r="K308" s="137"/>
+      <c r="E308" s="124"/>
+      <c r="F308" s="124"/>
+      <c r="G308" s="124"/>
+      <c r="H308" s="124"/>
+      <c r="I308" s="124"/>
+      <c r="J308" s="124"/>
+      <c r="K308" s="125"/>
     </row>
     <row r="309" spans="1:14">
       <c r="A309" s="12">
@@ -24731,14 +24726,14 @@
         <v>B33</v>
       </c>
       <c r="C309" s="13"/>
-      <c r="D309" s="146"/>
-      <c r="E309" s="131"/>
-      <c r="F309" s="131"/>
-      <c r="G309" s="131"/>
-      <c r="H309" s="131"/>
-      <c r="I309" s="131"/>
-      <c r="J309" s="131"/>
-      <c r="K309" s="147"/>
+      <c r="D309" s="126"/>
+      <c r="E309" s="127"/>
+      <c r="F309" s="127"/>
+      <c r="G309" s="127"/>
+      <c r="H309" s="127"/>
+      <c r="I309" s="127"/>
+      <c r="J309" s="127"/>
+      <c r="K309" s="128"/>
     </row>
     <row r="310" spans="1:14">
       <c r="A310" s="12">
@@ -28618,12 +28613,29 @@
     </row>
   </sheetData>
   <mergeCells count="45">
-    <mergeCell ref="D308:K309"/>
-    <mergeCell ref="D298:K299"/>
-    <mergeCell ref="D300:K301"/>
-    <mergeCell ref="D302:K303"/>
-    <mergeCell ref="D304:K305"/>
-    <mergeCell ref="D306:K307"/>
+    <mergeCell ref="D178:K178"/>
+    <mergeCell ref="D182:K182"/>
+    <mergeCell ref="D183:K183"/>
+    <mergeCell ref="D184:K184"/>
+    <mergeCell ref="D185:K185"/>
+    <mergeCell ref="D186:K186"/>
+    <mergeCell ref="D187:K187"/>
+    <mergeCell ref="D188:K188"/>
+    <mergeCell ref="D189:K189"/>
+    <mergeCell ref="D190:K190"/>
+    <mergeCell ref="D191:K191"/>
+    <mergeCell ref="D192:K192"/>
+    <mergeCell ref="D193:K193"/>
+    <mergeCell ref="D194:K194"/>
+    <mergeCell ref="D195:K195"/>
+    <mergeCell ref="D208:K208"/>
+    <mergeCell ref="D210:K210"/>
+    <mergeCell ref="D214:K214"/>
+    <mergeCell ref="D196:K196"/>
+    <mergeCell ref="D197:K197"/>
+    <mergeCell ref="D198:K198"/>
+    <mergeCell ref="D200:K200"/>
+    <mergeCell ref="D202:K202"/>
     <mergeCell ref="D280:K280"/>
     <mergeCell ref="D286:K286"/>
     <mergeCell ref="D296:K296"/>
@@ -28640,29 +28652,12 @@
     <mergeCell ref="D250:K250"/>
     <mergeCell ref="D204:K204"/>
     <mergeCell ref="D206:K206"/>
-    <mergeCell ref="D208:K208"/>
-    <mergeCell ref="D210:K210"/>
-    <mergeCell ref="D214:K214"/>
-    <mergeCell ref="D196:K196"/>
-    <mergeCell ref="D197:K197"/>
-    <mergeCell ref="D198:K198"/>
-    <mergeCell ref="D200:K200"/>
-    <mergeCell ref="D202:K202"/>
-    <mergeCell ref="D191:K191"/>
-    <mergeCell ref="D192:K192"/>
-    <mergeCell ref="D193:K193"/>
-    <mergeCell ref="D194:K194"/>
-    <mergeCell ref="D195:K195"/>
-    <mergeCell ref="D186:K186"/>
-    <mergeCell ref="D187:K187"/>
-    <mergeCell ref="D188:K188"/>
-    <mergeCell ref="D189:K189"/>
-    <mergeCell ref="D190:K190"/>
-    <mergeCell ref="D178:K178"/>
-    <mergeCell ref="D182:K182"/>
-    <mergeCell ref="D183:K183"/>
-    <mergeCell ref="D184:K184"/>
-    <mergeCell ref="D185:K185"/>
+    <mergeCell ref="D308:K309"/>
+    <mergeCell ref="D298:K299"/>
+    <mergeCell ref="D300:K301"/>
+    <mergeCell ref="D302:K303"/>
+    <mergeCell ref="D304:K305"/>
+    <mergeCell ref="D306:K307"/>
   </mergeCells>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="53" fitToHeight="0" orientation="landscape"/>

</xml_diff>

<commit_message>
Made room in RAM for Jeweler rewards
</commit_message>
<xml_diff>
--- a/data/Switches.xlsx
+++ b/data/Switches.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="807" uniqueCount="437">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="814" uniqueCount="444">
   <si>
     <t>ID</t>
   </si>
@@ -1328,6 +1328,27 @@
   </si>
   <si>
     <t>Hieroglyph Order 5</t>
+  </si>
+  <si>
+    <t>Gem Reward Amount 1</t>
+  </si>
+  <si>
+    <t>Gem Reward Amount 2</t>
+  </si>
+  <si>
+    <t>Gem Reward Amount 3</t>
+  </si>
+  <si>
+    <t>Gem Reward Amount 4</t>
+  </si>
+  <si>
+    <t>Gem Reward Amount 5</t>
+  </si>
+  <si>
+    <t>Gem Reward Amount 6</t>
+  </si>
+  <si>
+    <t>Gem Reward Amount 7</t>
   </si>
 </sst>
 </file>
@@ -1454,7 +1475,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="52">
+  <borders count="53">
     <border>
       <left/>
       <right/>
@@ -2077,9 +2098,20 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left/>
+      <right style="thin">
         <color auto="1"/>
-      </left>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color theme="0" tint="-0.24994659260841701"/>
       </right>
@@ -2096,7 +2128,7 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="168">
+  <cellXfs count="173">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -2466,43 +2498,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="33" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="50" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="32" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="31" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="34" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="32" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="33" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="39" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="27" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="28" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="25" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="3" applyBorder="1" applyAlignment="1">
@@ -2511,13 +2534,13 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="28" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="42" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="41" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
@@ -2535,16 +2558,28 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="27" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="41" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="25" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="32" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2565,34 +2600,46 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="28" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="34" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="42" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="32" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="39" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="33" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="24" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="33" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="50" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="51" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="31" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="30" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="52" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2905,8 +2952,8 @@
   <dimension ref="A1:O513"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A73" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I85" sqref="I85"/>
+      <pane ySplit="1" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D93" sqref="D93:K93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -2979,16 +3026,16 @@
         <f>8*A2&amp;"-"&amp;(8*A2+7)</f>
         <v>0-7</v>
       </c>
-      <c r="D2" s="142" t="s">
+      <c r="D2" s="134" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="138"/>
-      <c r="F2" s="138"/>
-      <c r="G2" s="138"/>
-      <c r="H2" s="138"/>
-      <c r="I2" s="138"/>
-      <c r="J2" s="138"/>
-      <c r="K2" s="139"/>
+      <c r="E2" s="135"/>
+      <c r="F2" s="135"/>
+      <c r="G2" s="135"/>
+      <c r="H2" s="135"/>
+      <c r="I2" s="135"/>
+      <c r="J2" s="135"/>
+      <c r="K2" s="136"/>
       <c r="L2" s="119" t="s">
         <v>7</v>
       </c>
@@ -3006,14 +3053,14 @@
         <f t="shared" ref="C3:C33" si="1">8*A3&amp;"-"&amp;(8*A3+7)</f>
         <v>8-15</v>
       </c>
-      <c r="D3" s="143"/>
-      <c r="E3" s="144"/>
-      <c r="F3" s="144"/>
-      <c r="G3" s="144"/>
-      <c r="H3" s="144"/>
-      <c r="I3" s="144"/>
-      <c r="J3" s="144"/>
-      <c r="K3" s="145"/>
+      <c r="D3" s="140"/>
+      <c r="E3" s="141"/>
+      <c r="F3" s="141"/>
+      <c r="G3" s="141"/>
+      <c r="H3" s="141"/>
+      <c r="I3" s="141"/>
+      <c r="J3" s="141"/>
+      <c r="K3" s="142"/>
       <c r="L3" s="119" t="s">
         <v>8</v>
       </c>
@@ -5538,38 +5585,16 @@
         <v>A49</v>
       </c>
       <c r="C75" s="13"/>
-      <c r="D75" s="61" t="str">
-        <f t="shared" si="6"/>
-        <v>(Unused) Chest 79</v>
-      </c>
-      <c r="E75" s="61" t="str">
-        <f t="shared" si="6"/>
-        <v>(Unused) Chest 78</v>
-      </c>
-      <c r="F75" s="61" t="str">
-        <f t="shared" si="6"/>
-        <v>(Unused) Chest 77</v>
-      </c>
-      <c r="G75" s="61" t="str">
-        <f t="shared" si="6"/>
-        <v>(Unused) Chest 76</v>
-      </c>
-      <c r="H75" s="62" t="str">
-        <f t="shared" si="6"/>
-        <v>(Unused) Chest 75</v>
-      </c>
-      <c r="I75" s="61" t="str">
-        <f t="shared" si="6"/>
-        <v>(Unused) Chest 74</v>
-      </c>
-      <c r="J75" s="61" t="str">
-        <f t="shared" si="6"/>
-        <v>(Unused) Chest 73</v>
-      </c>
-      <c r="K75" s="61" t="str">
-        <f t="shared" si="6"/>
-        <v>(Unused) Chest 72</v>
-      </c>
+      <c r="D75" s="131" t="s">
+        <v>437</v>
+      </c>
+      <c r="E75" s="132"/>
+      <c r="F75" s="132"/>
+      <c r="G75" s="132"/>
+      <c r="H75" s="132"/>
+      <c r="I75" s="132"/>
+      <c r="J75" s="132"/>
+      <c r="K75" s="133"/>
     </row>
     <row r="76" spans="1:14">
       <c r="A76" s="12">
@@ -5581,38 +5606,16 @@
         <v>A4A</v>
       </c>
       <c r="C76" s="13"/>
-      <c r="D76" s="61" t="str">
-        <f t="shared" si="6"/>
-        <v>(Unused) Chest 87</v>
-      </c>
-      <c r="E76" s="61" t="str">
-        <f t="shared" si="6"/>
-        <v>(Unused) Chest 86</v>
-      </c>
-      <c r="F76" s="61" t="str">
-        <f t="shared" si="6"/>
-        <v>(Unused) Chest 85</v>
-      </c>
-      <c r="G76" s="61" t="str">
-        <f t="shared" si="6"/>
-        <v>(Unused) Chest 84</v>
-      </c>
-      <c r="H76" s="62" t="str">
-        <f t="shared" si="6"/>
-        <v>(Unused) Chest 83</v>
-      </c>
-      <c r="I76" s="61" t="str">
-        <f t="shared" si="6"/>
-        <v>(Unused) Chest 82</v>
-      </c>
-      <c r="J76" s="61" t="str">
-        <f t="shared" si="6"/>
-        <v>(Unused) Chest 81</v>
-      </c>
-      <c r="K76" s="61" t="str">
-        <f t="shared" si="6"/>
-        <v>(Unused) Chest 80</v>
-      </c>
+      <c r="D76" s="131" t="s">
+        <v>438</v>
+      </c>
+      <c r="E76" s="132"/>
+      <c r="F76" s="132"/>
+      <c r="G76" s="132"/>
+      <c r="H76" s="132"/>
+      <c r="I76" s="132"/>
+      <c r="J76" s="132"/>
+      <c r="K76" s="133"/>
     </row>
     <row r="77" spans="1:14">
       <c r="A77" s="12">
@@ -5624,38 +5627,16 @@
         <v>A4B</v>
       </c>
       <c r="C77" s="13"/>
-      <c r="D77" s="61" t="str">
-        <f t="shared" si="6"/>
-        <v>(Unused) Chest 95</v>
-      </c>
-      <c r="E77" s="61" t="str">
-        <f t="shared" si="6"/>
-        <v>(Unused) Chest 94</v>
-      </c>
-      <c r="F77" s="61" t="str">
-        <f t="shared" si="6"/>
-        <v>(Unused) Chest 93</v>
-      </c>
-      <c r="G77" s="61" t="str">
-        <f t="shared" si="6"/>
-        <v>(Unused) Chest 92</v>
-      </c>
-      <c r="H77" s="62" t="str">
-        <f t="shared" si="6"/>
-        <v>(Unused) Chest 91</v>
-      </c>
-      <c r="I77" s="61" t="str">
-        <f t="shared" si="6"/>
-        <v>(Unused) Chest 90</v>
-      </c>
-      <c r="J77" s="61" t="str">
-        <f t="shared" si="6"/>
-        <v>(Unused) Chest 89</v>
-      </c>
-      <c r="K77" s="61" t="str">
-        <f t="shared" si="6"/>
-        <v>(Unused) Chest 88</v>
-      </c>
+      <c r="D77" s="131" t="s">
+        <v>439</v>
+      </c>
+      <c r="E77" s="132"/>
+      <c r="F77" s="132"/>
+      <c r="G77" s="132"/>
+      <c r="H77" s="132"/>
+      <c r="I77" s="132"/>
+      <c r="J77" s="132"/>
+      <c r="K77" s="133"/>
     </row>
     <row r="78" spans="1:14">
       <c r="A78" s="12">
@@ -5667,38 +5648,16 @@
         <v>A4C</v>
       </c>
       <c r="C78" s="13"/>
-      <c r="D78" s="61" t="str">
-        <f t="shared" si="6"/>
-        <v>(Unused) Chest 103</v>
-      </c>
-      <c r="E78" s="61" t="str">
-        <f t="shared" si="6"/>
-        <v>(Unused) Chest 102</v>
-      </c>
-      <c r="F78" s="61" t="str">
-        <f t="shared" si="6"/>
-        <v>(Unused) Chest 101</v>
-      </c>
-      <c r="G78" s="61" t="str">
-        <f t="shared" si="6"/>
-        <v>(Unused) Chest 100</v>
-      </c>
-      <c r="H78" s="62" t="str">
-        <f t="shared" si="6"/>
-        <v>(Unused) Chest 99</v>
-      </c>
-      <c r="I78" s="61" t="str">
-        <f t="shared" si="6"/>
-        <v>(Unused) Chest 98</v>
-      </c>
-      <c r="J78" s="61" t="str">
-        <f t="shared" si="6"/>
-        <v>(Unused) Chest 97</v>
-      </c>
-      <c r="K78" s="61" t="str">
-        <f t="shared" si="6"/>
-        <v>(Unused) Chest 96</v>
-      </c>
+      <c r="D78" s="131" t="s">
+        <v>440</v>
+      </c>
+      <c r="E78" s="132"/>
+      <c r="F78" s="132"/>
+      <c r="G78" s="132"/>
+      <c r="H78" s="132"/>
+      <c r="I78" s="132"/>
+      <c r="J78" s="132"/>
+      <c r="K78" s="133"/>
     </row>
     <row r="79" spans="1:14">
       <c r="A79" s="12">
@@ -5710,38 +5669,16 @@
         <v>A4D</v>
       </c>
       <c r="C79" s="13"/>
-      <c r="D79" s="61" t="str">
-        <f t="shared" si="6"/>
-        <v>(Unused) Chest 111</v>
-      </c>
-      <c r="E79" s="61" t="str">
-        <f t="shared" si="6"/>
-        <v>(Unused) Chest 110</v>
-      </c>
-      <c r="F79" s="61" t="str">
-        <f t="shared" si="6"/>
-        <v>(Unused) Chest 109</v>
-      </c>
-      <c r="G79" s="61" t="str">
-        <f t="shared" si="6"/>
-        <v>(Unused) Chest 108</v>
-      </c>
-      <c r="H79" s="62" t="str">
-        <f t="shared" si="6"/>
-        <v>(Unused) Chest 107</v>
-      </c>
-      <c r="I79" s="61" t="str">
-        <f t="shared" si="6"/>
-        <v>(Unused) Chest 106</v>
-      </c>
-      <c r="J79" s="61" t="str">
-        <f t="shared" si="6"/>
-        <v>(Unused) Chest 105</v>
-      </c>
-      <c r="K79" s="61" t="str">
-        <f t="shared" si="6"/>
-        <v>(Unused) Chest 104</v>
-      </c>
+      <c r="D79" s="131" t="s">
+        <v>441</v>
+      </c>
+      <c r="E79" s="132"/>
+      <c r="F79" s="132"/>
+      <c r="G79" s="132"/>
+      <c r="H79" s="132"/>
+      <c r="I79" s="132"/>
+      <c r="J79" s="132"/>
+      <c r="K79" s="133"/>
     </row>
     <row r="80" spans="1:14">
       <c r="A80" s="12">
@@ -5753,38 +5690,16 @@
         <v>A4E</v>
       </c>
       <c r="C80" s="13"/>
-      <c r="D80" s="61" t="str">
-        <f t="shared" si="6"/>
-        <v>(Unused) Chest 119</v>
-      </c>
-      <c r="E80" s="61" t="str">
-        <f t="shared" si="6"/>
-        <v>(Unused) Chest 118</v>
-      </c>
-      <c r="F80" s="61" t="str">
-        <f t="shared" si="6"/>
-        <v>(Unused) Chest 117</v>
-      </c>
-      <c r="G80" s="61" t="str">
-        <f t="shared" si="6"/>
-        <v>(Unused) Chest 116</v>
-      </c>
-      <c r="H80" s="62" t="str">
-        <f t="shared" si="6"/>
-        <v>(Unused) Chest 115</v>
-      </c>
-      <c r="I80" s="61" t="str">
-        <f t="shared" si="6"/>
-        <v>(Unused) Chest 114</v>
-      </c>
-      <c r="J80" s="61" t="str">
-        <f t="shared" si="6"/>
-        <v>(Unused) Chest 113</v>
-      </c>
-      <c r="K80" s="61" t="str">
-        <f t="shared" si="6"/>
-        <v>(Unused) Chest 112</v>
-      </c>
+      <c r="D80" s="131" t="s">
+        <v>442</v>
+      </c>
+      <c r="E80" s="132"/>
+      <c r="F80" s="132"/>
+      <c r="G80" s="132"/>
+      <c r="H80" s="132"/>
+      <c r="I80" s="132"/>
+      <c r="J80" s="132"/>
+      <c r="K80" s="133"/>
     </row>
     <row r="81" spans="1:14" s="1" customFormat="1">
       <c r="A81" s="32">
@@ -5796,38 +5711,16 @@
         <v>A4F</v>
       </c>
       <c r="C81" s="33"/>
-      <c r="D81" s="63" t="str">
-        <f t="shared" si="6"/>
-        <v>(Unused) Chest 127</v>
-      </c>
-      <c r="E81" s="63" t="str">
-        <f t="shared" si="6"/>
-        <v>(Unused) Chest 126</v>
-      </c>
-      <c r="F81" s="63" t="str">
-        <f t="shared" si="6"/>
-        <v>(Unused) Chest 125</v>
-      </c>
-      <c r="G81" s="63" t="str">
-        <f t="shared" si="6"/>
-        <v>(Unused) Chest 124</v>
-      </c>
-      <c r="H81" s="64" t="str">
-        <f t="shared" si="6"/>
-        <v>(Unused) Chest 123</v>
-      </c>
-      <c r="I81" s="63" t="str">
-        <f t="shared" si="6"/>
-        <v>(Unused) Chest 122</v>
-      </c>
-      <c r="J81" s="63" t="str">
-        <f t="shared" si="6"/>
-        <v>(Unused) Chest 121</v>
-      </c>
-      <c r="K81" s="63" t="str">
-        <f t="shared" si="6"/>
-        <v>(Unused) Chest 120</v>
-      </c>
+      <c r="D81" s="167" t="s">
+        <v>443</v>
+      </c>
+      <c r="E81" s="168"/>
+      <c r="F81" s="168"/>
+      <c r="G81" s="168"/>
+      <c r="H81" s="168"/>
+      <c r="I81" s="168"/>
+      <c r="J81" s="168"/>
+      <c r="K81" s="169"/>
       <c r="L81" s="57"/>
       <c r="M81" s="58"/>
       <c r="N81" s="58"/>
@@ -6022,16 +5915,16 @@
         <v>A58</v>
       </c>
       <c r="C90" s="13"/>
-      <c r="D90" s="158" t="s">
+      <c r="D90" s="131" t="s">
         <v>432</v>
       </c>
-      <c r="E90" s="159"/>
-      <c r="F90" s="159"/>
-      <c r="G90" s="159"/>
-      <c r="H90" s="159"/>
-      <c r="I90" s="159"/>
-      <c r="J90" s="159"/>
-      <c r="K90" s="160"/>
+      <c r="E90" s="132"/>
+      <c r="F90" s="132"/>
+      <c r="G90" s="132"/>
+      <c r="H90" s="132"/>
+      <c r="I90" s="132"/>
+      <c r="J90" s="132"/>
+      <c r="K90" s="133"/>
     </row>
     <row r="91" spans="1:14">
       <c r="A91" s="12">
@@ -6043,16 +5936,16 @@
         <v>A59</v>
       </c>
       <c r="C91" s="13"/>
-      <c r="D91" s="158" t="s">
+      <c r="D91" s="131" t="s">
         <v>433</v>
       </c>
-      <c r="E91" s="159"/>
-      <c r="F91" s="159"/>
-      <c r="G91" s="159"/>
-      <c r="H91" s="159"/>
-      <c r="I91" s="159"/>
-      <c r="J91" s="159"/>
-      <c r="K91" s="160"/>
+      <c r="E91" s="132"/>
+      <c r="F91" s="132"/>
+      <c r="G91" s="132"/>
+      <c r="H91" s="132"/>
+      <c r="I91" s="132"/>
+      <c r="J91" s="132"/>
+      <c r="K91" s="133"/>
     </row>
     <row r="92" spans="1:14">
       <c r="A92" s="12">
@@ -6064,16 +5957,16 @@
         <v>A5A</v>
       </c>
       <c r="C92" s="13"/>
-      <c r="D92" s="158" t="s">
+      <c r="D92" s="131" t="s">
         <v>434</v>
       </c>
-      <c r="E92" s="159"/>
-      <c r="F92" s="159"/>
-      <c r="G92" s="159"/>
-      <c r="H92" s="159"/>
-      <c r="I92" s="159"/>
-      <c r="J92" s="159"/>
-      <c r="K92" s="160"/>
+      <c r="E92" s="132"/>
+      <c r="F92" s="132"/>
+      <c r="G92" s="132"/>
+      <c r="H92" s="132"/>
+      <c r="I92" s="132"/>
+      <c r="J92" s="132"/>
+      <c r="K92" s="133"/>
     </row>
     <row r="93" spans="1:14">
       <c r="A93" s="12">
@@ -6085,16 +5978,16 @@
         <v>A5B</v>
       </c>
       <c r="C93" s="13"/>
-      <c r="D93" s="161" t="s">
+      <c r="D93" s="128" t="s">
         <v>435</v>
       </c>
-      <c r="E93" s="162"/>
-      <c r="F93" s="162"/>
-      <c r="G93" s="162"/>
-      <c r="H93" s="162"/>
-      <c r="I93" s="162"/>
-      <c r="J93" s="162"/>
-      <c r="K93" s="163"/>
+      <c r="E93" s="129"/>
+      <c r="F93" s="129"/>
+      <c r="G93" s="129"/>
+      <c r="H93" s="129"/>
+      <c r="I93" s="129"/>
+      <c r="J93" s="129"/>
+      <c r="K93" s="130"/>
     </row>
     <row r="94" spans="1:14">
       <c r="A94" s="12">
@@ -6106,16 +5999,16 @@
         <v>A5C</v>
       </c>
       <c r="C94" s="13"/>
-      <c r="D94" s="161" t="s">
+      <c r="D94" s="128" t="s">
         <v>436</v>
       </c>
-      <c r="E94" s="162"/>
-      <c r="F94" s="162"/>
-      <c r="G94" s="162"/>
-      <c r="H94" s="162"/>
-      <c r="I94" s="162"/>
-      <c r="J94" s="162"/>
-      <c r="K94" s="163"/>
+      <c r="E94" s="129"/>
+      <c r="F94" s="129"/>
+      <c r="G94" s="129"/>
+      <c r="H94" s="129"/>
+      <c r="I94" s="129"/>
+      <c r="J94" s="129"/>
+      <c r="K94" s="130"/>
     </row>
     <row r="95" spans="1:14">
       <c r="A95" s="12">
@@ -6127,16 +6020,16 @@
         <v>A5D</v>
       </c>
       <c r="C95" s="13"/>
-      <c r="D95" s="161" t="s">
+      <c r="D95" s="128" t="s">
         <v>431</v>
       </c>
-      <c r="E95" s="162"/>
-      <c r="F95" s="162"/>
-      <c r="G95" s="162"/>
-      <c r="H95" s="162"/>
-      <c r="I95" s="162"/>
-      <c r="J95" s="162"/>
-      <c r="K95" s="163"/>
+      <c r="E95" s="129"/>
+      <c r="F95" s="129"/>
+      <c r="G95" s="129"/>
+      <c r="H95" s="129"/>
+      <c r="I95" s="129"/>
+      <c r="J95" s="129"/>
+      <c r="K95" s="130"/>
     </row>
     <row r="96" spans="1:14">
       <c r="A96" s="12">
@@ -6148,16 +6041,16 @@
         <v>A5E</v>
       </c>
       <c r="C96" s="13"/>
-      <c r="D96" s="158" t="s">
+      <c r="D96" s="131" t="s">
         <v>430</v>
       </c>
-      <c r="E96" s="159"/>
-      <c r="F96" s="159"/>
-      <c r="G96" s="159"/>
-      <c r="H96" s="159"/>
-      <c r="I96" s="159"/>
-      <c r="J96" s="159"/>
-      <c r="K96" s="160"/>
+      <c r="E96" s="132"/>
+      <c r="F96" s="132"/>
+      <c r="G96" s="132"/>
+      <c r="H96" s="132"/>
+      <c r="I96" s="132"/>
+      <c r="J96" s="132"/>
+      <c r="K96" s="133"/>
     </row>
     <row r="97" spans="1:14" s="1" customFormat="1">
       <c r="A97" s="32">
@@ -6170,23 +6063,23 @@
       </c>
       <c r="C97" s="33"/>
       <c r="D97" s="45"/>
-      <c r="E97" s="164"/>
-      <c r="F97" s="165" t="s">
+      <c r="E97" s="125"/>
+      <c r="F97" s="170" t="s">
         <v>429</v>
       </c>
-      <c r="G97" s="165" t="s">
+      <c r="G97" s="172" t="s">
         <v>428</v>
       </c>
-      <c r="H97" s="166" t="s">
+      <c r="H97" s="172" t="s">
         <v>427</v>
       </c>
-      <c r="I97" s="165" t="s">
+      <c r="I97" s="171" t="s">
         <v>426</v>
       </c>
-      <c r="J97" s="165" t="s">
+      <c r="J97" s="126" t="s">
         <v>425</v>
       </c>
-      <c r="K97" s="167" t="s">
+      <c r="K97" s="127" t="s">
         <v>424</v>
       </c>
       <c r="L97" s="57"/>
@@ -9096,16 +8989,16 @@
         <v>AA6</v>
       </c>
       <c r="C168" s="13"/>
-      <c r="D168" s="125" t="s">
+      <c r="D168" s="166" t="s">
         <v>348</v>
       </c>
-      <c r="E168" s="125"/>
-      <c r="F168" s="125"/>
-      <c r="G168" s="125"/>
-      <c r="H168" s="125"/>
-      <c r="I168" s="125"/>
-      <c r="J168" s="125"/>
-      <c r="K168" s="125"/>
+      <c r="E168" s="166"/>
+      <c r="F168" s="166"/>
+      <c r="G168" s="166"/>
+      <c r="H168" s="166"/>
+      <c r="I168" s="166"/>
+      <c r="J168" s="166"/>
+      <c r="K168" s="166"/>
     </row>
     <row r="169" spans="1:14">
       <c r="A169" s="12">
@@ -9212,16 +9105,16 @@
         <v>AAC</v>
       </c>
       <c r="C174" s="13"/>
-      <c r="D174" s="125" t="s">
+      <c r="D174" s="166" t="s">
         <v>349</v>
       </c>
-      <c r="E174" s="125"/>
-      <c r="F174" s="125"/>
-      <c r="G174" s="125"/>
-      <c r="H174" s="125"/>
-      <c r="I174" s="125"/>
-      <c r="J174" s="125"/>
-      <c r="K174" s="125"/>
+      <c r="E174" s="166"/>
+      <c r="F174" s="166"/>
+      <c r="G174" s="166"/>
+      <c r="H174" s="166"/>
+      <c r="I174" s="166"/>
+      <c r="J174" s="166"/>
+      <c r="K174" s="166"/>
     </row>
     <row r="175" spans="1:14">
       <c r="A175" s="12">
@@ -9233,16 +9126,16 @@
         <v>AAD</v>
       </c>
       <c r="C175" s="13"/>
-      <c r="D175" s="125" t="s">
+      <c r="D175" s="166" t="s">
         <v>349</v>
       </c>
-      <c r="E175" s="125"/>
-      <c r="F175" s="125"/>
-      <c r="G175" s="125"/>
-      <c r="H175" s="125"/>
-      <c r="I175" s="125"/>
-      <c r="J175" s="125"/>
-      <c r="K175" s="125"/>
+      <c r="E175" s="166"/>
+      <c r="F175" s="166"/>
+      <c r="G175" s="166"/>
+      <c r="H175" s="166"/>
+      <c r="I175" s="166"/>
+      <c r="J175" s="166"/>
+      <c r="K175" s="166"/>
     </row>
     <row r="176" spans="1:14">
       <c r="A176" s="12">
@@ -9295,16 +9188,16 @@
         <v>AB0</v>
       </c>
       <c r="C178" s="39"/>
-      <c r="D178" s="125" t="s">
+      <c r="D178" s="166" t="s">
         <v>350</v>
       </c>
-      <c r="E178" s="125"/>
-      <c r="F178" s="125"/>
-      <c r="G178" s="125"/>
-      <c r="H178" s="125"/>
-      <c r="I178" s="125"/>
-      <c r="J178" s="125"/>
-      <c r="K178" s="125"/>
+      <c r="E178" s="166"/>
+      <c r="F178" s="166"/>
+      <c r="G178" s="166"/>
+      <c r="H178" s="166"/>
+      <c r="I178" s="166"/>
+      <c r="J178" s="166"/>
+      <c r="K178" s="166"/>
     </row>
     <row r="179" spans="1:14">
       <c r="A179" s="12">
@@ -9373,16 +9266,16 @@
         <v>AB4</v>
       </c>
       <c r="C182" s="13"/>
-      <c r="D182" s="126" t="s">
+      <c r="D182" s="150" t="s">
         <v>351</v>
       </c>
-      <c r="E182" s="127"/>
-      <c r="F182" s="127"/>
-      <c r="G182" s="127"/>
-      <c r="H182" s="127"/>
-      <c r="I182" s="127"/>
-      <c r="J182" s="127"/>
-      <c r="K182" s="128"/>
+      <c r="E182" s="151"/>
+      <c r="F182" s="151"/>
+      <c r="G182" s="151"/>
+      <c r="H182" s="151"/>
+      <c r="I182" s="151"/>
+      <c r="J182" s="151"/>
+      <c r="K182" s="152"/>
     </row>
     <row r="183" spans="1:14">
       <c r="A183" s="12">
@@ -9394,16 +9287,16 @@
         <v>AB5</v>
       </c>
       <c r="C183" s="13"/>
-      <c r="D183" s="126" t="s">
+      <c r="D183" s="150" t="s">
         <v>352</v>
       </c>
-      <c r="E183" s="127"/>
-      <c r="F183" s="127"/>
-      <c r="G183" s="127"/>
-      <c r="H183" s="127"/>
-      <c r="I183" s="127"/>
-      <c r="J183" s="127"/>
-      <c r="K183" s="128"/>
+      <c r="E183" s="151"/>
+      <c r="F183" s="151"/>
+      <c r="G183" s="151"/>
+      <c r="H183" s="151"/>
+      <c r="I183" s="151"/>
+      <c r="J183" s="151"/>
+      <c r="K183" s="152"/>
     </row>
     <row r="184" spans="1:14">
       <c r="A184" s="12">
@@ -9415,16 +9308,16 @@
         <v>AB6</v>
       </c>
       <c r="C184" s="13"/>
-      <c r="D184" s="126" t="s">
+      <c r="D184" s="150" t="s">
         <v>353</v>
       </c>
-      <c r="E184" s="127"/>
-      <c r="F184" s="127"/>
-      <c r="G184" s="127"/>
-      <c r="H184" s="127"/>
-      <c r="I184" s="127"/>
-      <c r="J184" s="127"/>
-      <c r="K184" s="128"/>
+      <c r="E184" s="151"/>
+      <c r="F184" s="151"/>
+      <c r="G184" s="151"/>
+      <c r="H184" s="151"/>
+      <c r="I184" s="151"/>
+      <c r="J184" s="151"/>
+      <c r="K184" s="152"/>
     </row>
     <row r="185" spans="1:14">
       <c r="A185" s="12">
@@ -9436,16 +9329,16 @@
         <v>AB7</v>
       </c>
       <c r="C185" s="13"/>
-      <c r="D185" s="126" t="s">
+      <c r="D185" s="150" t="s">
         <v>354</v>
       </c>
-      <c r="E185" s="127"/>
-      <c r="F185" s="127"/>
-      <c r="G185" s="127"/>
-      <c r="H185" s="127"/>
-      <c r="I185" s="127"/>
-      <c r="J185" s="127"/>
-      <c r="K185" s="128"/>
+      <c r="E185" s="151"/>
+      <c r="F185" s="151"/>
+      <c r="G185" s="151"/>
+      <c r="H185" s="151"/>
+      <c r="I185" s="151"/>
+      <c r="J185" s="151"/>
+      <c r="K185" s="152"/>
     </row>
     <row r="186" spans="1:14">
       <c r="A186" s="12">
@@ -9457,16 +9350,16 @@
         <v>AB8</v>
       </c>
       <c r="C186" s="13"/>
-      <c r="D186" s="126" t="s">
+      <c r="D186" s="150" t="s">
         <v>355</v>
       </c>
-      <c r="E186" s="127"/>
-      <c r="F186" s="127"/>
-      <c r="G186" s="127"/>
-      <c r="H186" s="127"/>
-      <c r="I186" s="127"/>
-      <c r="J186" s="127"/>
-      <c r="K186" s="128"/>
+      <c r="E186" s="151"/>
+      <c r="F186" s="151"/>
+      <c r="G186" s="151"/>
+      <c r="H186" s="151"/>
+      <c r="I186" s="151"/>
+      <c r="J186" s="151"/>
+      <c r="K186" s="152"/>
     </row>
     <row r="187" spans="1:14">
       <c r="A187" s="12">
@@ -9478,16 +9371,16 @@
         <v>AB9</v>
       </c>
       <c r="C187" s="13"/>
-      <c r="D187" s="126" t="s">
+      <c r="D187" s="150" t="s">
         <v>356</v>
       </c>
-      <c r="E187" s="127"/>
-      <c r="F187" s="127"/>
-      <c r="G187" s="127"/>
-      <c r="H187" s="127"/>
-      <c r="I187" s="127"/>
-      <c r="J187" s="127"/>
-      <c r="K187" s="128"/>
+      <c r="E187" s="151"/>
+      <c r="F187" s="151"/>
+      <c r="G187" s="151"/>
+      <c r="H187" s="151"/>
+      <c r="I187" s="151"/>
+      <c r="J187" s="151"/>
+      <c r="K187" s="152"/>
     </row>
     <row r="188" spans="1:14">
       <c r="A188" s="12">
@@ -9499,16 +9392,16 @@
         <v>ABA</v>
       </c>
       <c r="C188" s="13"/>
-      <c r="D188" s="126" t="s">
+      <c r="D188" s="150" t="s">
         <v>357</v>
       </c>
-      <c r="E188" s="127"/>
-      <c r="F188" s="127"/>
-      <c r="G188" s="127"/>
-      <c r="H188" s="127"/>
-      <c r="I188" s="127"/>
-      <c r="J188" s="127"/>
-      <c r="K188" s="128"/>
+      <c r="E188" s="151"/>
+      <c r="F188" s="151"/>
+      <c r="G188" s="151"/>
+      <c r="H188" s="151"/>
+      <c r="I188" s="151"/>
+      <c r="J188" s="151"/>
+      <c r="K188" s="152"/>
     </row>
     <row r="189" spans="1:14">
       <c r="A189" s="12">
@@ -9520,16 +9413,16 @@
         <v>ABB</v>
       </c>
       <c r="C189" s="13"/>
-      <c r="D189" s="126" t="s">
+      <c r="D189" s="150" t="s">
         <v>358</v>
       </c>
-      <c r="E189" s="127"/>
-      <c r="F189" s="127"/>
-      <c r="G189" s="127"/>
-      <c r="H189" s="127"/>
-      <c r="I189" s="127"/>
-      <c r="J189" s="127"/>
-      <c r="K189" s="128"/>
+      <c r="E189" s="151"/>
+      <c r="F189" s="151"/>
+      <c r="G189" s="151"/>
+      <c r="H189" s="151"/>
+      <c r="I189" s="151"/>
+      <c r="J189" s="151"/>
+      <c r="K189" s="152"/>
     </row>
     <row r="190" spans="1:14">
       <c r="A190" s="12">
@@ -9541,16 +9434,16 @@
         <v>ABC</v>
       </c>
       <c r="C190" s="13"/>
-      <c r="D190" s="126" t="s">
+      <c r="D190" s="150" t="s">
         <v>359</v>
       </c>
-      <c r="E190" s="127"/>
-      <c r="F190" s="127"/>
-      <c r="G190" s="127"/>
-      <c r="H190" s="127"/>
-      <c r="I190" s="127"/>
-      <c r="J190" s="127"/>
-      <c r="K190" s="128"/>
+      <c r="E190" s="151"/>
+      <c r="F190" s="151"/>
+      <c r="G190" s="151"/>
+      <c r="H190" s="151"/>
+      <c r="I190" s="151"/>
+      <c r="J190" s="151"/>
+      <c r="K190" s="152"/>
     </row>
     <row r="191" spans="1:14">
       <c r="A191" s="12">
@@ -9562,16 +9455,16 @@
         <v>ABD</v>
       </c>
       <c r="C191" s="13"/>
-      <c r="D191" s="126" t="s">
+      <c r="D191" s="150" t="s">
         <v>360</v>
       </c>
-      <c r="E191" s="127"/>
-      <c r="F191" s="127"/>
-      <c r="G191" s="127"/>
-      <c r="H191" s="127"/>
-      <c r="I191" s="127"/>
-      <c r="J191" s="127"/>
-      <c r="K191" s="128"/>
+      <c r="E191" s="151"/>
+      <c r="F191" s="151"/>
+      <c r="G191" s="151"/>
+      <c r="H191" s="151"/>
+      <c r="I191" s="151"/>
+      <c r="J191" s="151"/>
+      <c r="K191" s="152"/>
     </row>
     <row r="192" spans="1:14">
       <c r="A192" s="12">
@@ -9583,16 +9476,16 @@
         <v>ABE</v>
       </c>
       <c r="C192" s="13"/>
-      <c r="D192" s="126" t="s">
+      <c r="D192" s="150" t="s">
         <v>361</v>
       </c>
-      <c r="E192" s="127"/>
-      <c r="F192" s="127"/>
-      <c r="G192" s="127"/>
-      <c r="H192" s="127"/>
-      <c r="I192" s="127"/>
-      <c r="J192" s="127"/>
-      <c r="K192" s="128"/>
+      <c r="E192" s="151"/>
+      <c r="F192" s="151"/>
+      <c r="G192" s="151"/>
+      <c r="H192" s="151"/>
+      <c r="I192" s="151"/>
+      <c r="J192" s="151"/>
+      <c r="K192" s="152"/>
     </row>
     <row r="193" spans="1:14" s="1" customFormat="1">
       <c r="A193" s="32">
@@ -9604,16 +9497,16 @@
         <v>ABF</v>
       </c>
       <c r="C193" s="33"/>
-      <c r="D193" s="129" t="s">
+      <c r="D193" s="163" t="s">
         <v>362</v>
       </c>
-      <c r="E193" s="130"/>
-      <c r="F193" s="130"/>
-      <c r="G193" s="130"/>
-      <c r="H193" s="130"/>
-      <c r="I193" s="130"/>
-      <c r="J193" s="130"/>
-      <c r="K193" s="131"/>
+      <c r="E193" s="164"/>
+      <c r="F193" s="164"/>
+      <c r="G193" s="164"/>
+      <c r="H193" s="164"/>
+      <c r="I193" s="164"/>
+      <c r="J193" s="164"/>
+      <c r="K193" s="165"/>
       <c r="L193" s="57"/>
       <c r="M193" s="58"/>
       <c r="N193" s="58"/>
@@ -9628,16 +9521,16 @@
         <v>AC0</v>
       </c>
       <c r="C194" s="39"/>
-      <c r="D194" s="132" t="s">
+      <c r="D194" s="145" t="s">
         <v>363</v>
       </c>
-      <c r="E194" s="133"/>
-      <c r="F194" s="133"/>
-      <c r="G194" s="133"/>
-      <c r="H194" s="133"/>
-      <c r="I194" s="133"/>
-      <c r="J194" s="133"/>
-      <c r="K194" s="134"/>
+      <c r="E194" s="138"/>
+      <c r="F194" s="138"/>
+      <c r="G194" s="138"/>
+      <c r="H194" s="138"/>
+      <c r="I194" s="138"/>
+      <c r="J194" s="138"/>
+      <c r="K194" s="146"/>
     </row>
     <row r="195" spans="1:14">
       <c r="A195" s="12">
@@ -9649,16 +9542,16 @@
         <v>AC1</v>
       </c>
       <c r="C195" s="13"/>
-      <c r="D195" s="126" t="s">
+      <c r="D195" s="150" t="s">
         <v>364</v>
       </c>
-      <c r="E195" s="127"/>
-      <c r="F195" s="127"/>
-      <c r="G195" s="127"/>
-      <c r="H195" s="127"/>
-      <c r="I195" s="127"/>
-      <c r="J195" s="127"/>
-      <c r="K195" s="128"/>
+      <c r="E195" s="151"/>
+      <c r="F195" s="151"/>
+      <c r="G195" s="151"/>
+      <c r="H195" s="151"/>
+      <c r="I195" s="151"/>
+      <c r="J195" s="151"/>
+      <c r="K195" s="152"/>
     </row>
     <row r="196" spans="1:14">
       <c r="A196" s="12">
@@ -9670,16 +9563,16 @@
         <v>AC2</v>
       </c>
       <c r="C196" s="13"/>
-      <c r="D196" s="126" t="s">
+      <c r="D196" s="150" t="s">
         <v>365</v>
       </c>
-      <c r="E196" s="127"/>
-      <c r="F196" s="127"/>
-      <c r="G196" s="127"/>
-      <c r="H196" s="127"/>
-      <c r="I196" s="127"/>
-      <c r="J196" s="127"/>
-      <c r="K196" s="128"/>
+      <c r="E196" s="151"/>
+      <c r="F196" s="151"/>
+      <c r="G196" s="151"/>
+      <c r="H196" s="151"/>
+      <c r="I196" s="151"/>
+      <c r="J196" s="151"/>
+      <c r="K196" s="152"/>
     </row>
     <row r="197" spans="1:14">
       <c r="A197" s="12">
@@ -9691,16 +9584,16 @@
         <v>AC3</v>
       </c>
       <c r="C197" s="13"/>
-      <c r="D197" s="126" t="s">
+      <c r="D197" s="150" t="s">
         <v>366</v>
       </c>
-      <c r="E197" s="127"/>
-      <c r="F197" s="127"/>
-      <c r="G197" s="127"/>
-      <c r="H197" s="127"/>
-      <c r="I197" s="127"/>
-      <c r="J197" s="127"/>
-      <c r="K197" s="128"/>
+      <c r="E197" s="151"/>
+      <c r="F197" s="151"/>
+      <c r="G197" s="151"/>
+      <c r="H197" s="151"/>
+      <c r="I197" s="151"/>
+      <c r="J197" s="151"/>
+      <c r="K197" s="152"/>
     </row>
     <row r="198" spans="1:14">
       <c r="A198" s="12">
@@ -9712,16 +9605,16 @@
         <v>AC4</v>
       </c>
       <c r="C198" s="13"/>
-      <c r="D198" s="126" t="s">
+      <c r="D198" s="150" t="s">
         <v>367</v>
       </c>
-      <c r="E198" s="127"/>
-      <c r="F198" s="127"/>
-      <c r="G198" s="127"/>
-      <c r="H198" s="127"/>
-      <c r="I198" s="127"/>
-      <c r="J198" s="127"/>
-      <c r="K198" s="128"/>
+      <c r="E198" s="151"/>
+      <c r="F198" s="151"/>
+      <c r="G198" s="151"/>
+      <c r="H198" s="151"/>
+      <c r="I198" s="151"/>
+      <c r="J198" s="151"/>
+      <c r="K198" s="152"/>
     </row>
     <row r="199" spans="1:14">
       <c r="A199" s="12">
@@ -9752,16 +9645,16 @@
         <v>AC6</v>
       </c>
       <c r="C200" s="13"/>
-      <c r="D200" s="126" t="s">
+      <c r="D200" s="150" t="s">
         <v>368</v>
       </c>
-      <c r="E200" s="127"/>
-      <c r="F200" s="127"/>
-      <c r="G200" s="127"/>
-      <c r="H200" s="127"/>
-      <c r="I200" s="127"/>
-      <c r="J200" s="127"/>
-      <c r="K200" s="128"/>
+      <c r="E200" s="151"/>
+      <c r="F200" s="151"/>
+      <c r="G200" s="151"/>
+      <c r="H200" s="151"/>
+      <c r="I200" s="151"/>
+      <c r="J200" s="151"/>
+      <c r="K200" s="152"/>
     </row>
     <row r="201" spans="1:14">
       <c r="A201" s="12">
@@ -9792,16 +9685,16 @@
         <v>AC8</v>
       </c>
       <c r="C202" s="13"/>
-      <c r="D202" s="155" t="s">
+      <c r="D202" s="156" t="s">
         <v>369</v>
       </c>
-      <c r="E202" s="156"/>
-      <c r="F202" s="156"/>
-      <c r="G202" s="156"/>
-      <c r="H202" s="156"/>
-      <c r="I202" s="156"/>
-      <c r="J202" s="156"/>
-      <c r="K202" s="157"/>
+      <c r="E202" s="157"/>
+      <c r="F202" s="157"/>
+      <c r="G202" s="157"/>
+      <c r="H202" s="157"/>
+      <c r="I202" s="157"/>
+      <c r="J202" s="157"/>
+      <c r="K202" s="158"/>
     </row>
     <row r="203" spans="1:14">
       <c r="A203" s="12">
@@ -9832,16 +9725,16 @@
         <v>ACA</v>
       </c>
       <c r="C204" s="13"/>
-      <c r="D204" s="126" t="s">
+      <c r="D204" s="150" t="s">
         <v>370</v>
       </c>
-      <c r="E204" s="127"/>
-      <c r="F204" s="127"/>
-      <c r="G204" s="127"/>
-      <c r="H204" s="127"/>
-      <c r="I204" s="127"/>
-      <c r="J204" s="127"/>
-      <c r="K204" s="128"/>
+      <c r="E204" s="151"/>
+      <c r="F204" s="151"/>
+      <c r="G204" s="151"/>
+      <c r="H204" s="151"/>
+      <c r="I204" s="151"/>
+      <c r="J204" s="151"/>
+      <c r="K204" s="152"/>
     </row>
     <row r="205" spans="1:14">
       <c r="A205" s="12">
@@ -9872,16 +9765,16 @@
         <v>ACC</v>
       </c>
       <c r="C206" s="13"/>
-      <c r="D206" s="126" t="s">
+      <c r="D206" s="150" t="s">
         <v>370</v>
       </c>
-      <c r="E206" s="127"/>
-      <c r="F206" s="127"/>
-      <c r="G206" s="127"/>
-      <c r="H206" s="127"/>
-      <c r="I206" s="127"/>
-      <c r="J206" s="127"/>
-      <c r="K206" s="128"/>
+      <c r="E206" s="151"/>
+      <c r="F206" s="151"/>
+      <c r="G206" s="151"/>
+      <c r="H206" s="151"/>
+      <c r="I206" s="151"/>
+      <c r="J206" s="151"/>
+      <c r="K206" s="152"/>
     </row>
     <row r="207" spans="1:14">
       <c r="A207" s="12">
@@ -9912,16 +9805,16 @@
         <v>ACE</v>
       </c>
       <c r="C208" s="13"/>
-      <c r="D208" s="126" t="s">
+      <c r="D208" s="150" t="s">
         <v>371</v>
       </c>
-      <c r="E208" s="127"/>
-      <c r="F208" s="127"/>
-      <c r="G208" s="127"/>
-      <c r="H208" s="127"/>
-      <c r="I208" s="127"/>
-      <c r="J208" s="127"/>
-      <c r="K208" s="128"/>
+      <c r="E208" s="151"/>
+      <c r="F208" s="151"/>
+      <c r="G208" s="151"/>
+      <c r="H208" s="151"/>
+      <c r="I208" s="151"/>
+      <c r="J208" s="151"/>
+      <c r="K208" s="152"/>
     </row>
     <row r="209" spans="1:14" s="1" customFormat="1">
       <c r="A209" s="32">
@@ -9955,16 +9848,16 @@
         <v>AD0</v>
       </c>
       <c r="C210" s="39"/>
-      <c r="D210" s="132" t="s">
+      <c r="D210" s="145" t="s">
         <v>371</v>
       </c>
-      <c r="E210" s="133"/>
-      <c r="F210" s="133"/>
-      <c r="G210" s="133"/>
-      <c r="H210" s="133"/>
-      <c r="I210" s="133"/>
-      <c r="J210" s="133"/>
-      <c r="K210" s="134"/>
+      <c r="E210" s="138"/>
+      <c r="F210" s="138"/>
+      <c r="G210" s="138"/>
+      <c r="H210" s="138"/>
+      <c r="I210" s="138"/>
+      <c r="J210" s="138"/>
+      <c r="K210" s="146"/>
     </row>
     <row r="211" spans="1:14">
       <c r="A211" s="12">
@@ -10033,16 +9926,16 @@
         <v>AD4</v>
       </c>
       <c r="C214" s="13"/>
-      <c r="D214" s="126" t="s">
+      <c r="D214" s="150" t="s">
         <v>372</v>
       </c>
-      <c r="E214" s="127"/>
-      <c r="F214" s="127"/>
-      <c r="G214" s="127"/>
-      <c r="H214" s="127"/>
-      <c r="I214" s="127"/>
-      <c r="J214" s="127"/>
-      <c r="K214" s="128"/>
+      <c r="E214" s="151"/>
+      <c r="F214" s="151"/>
+      <c r="G214" s="151"/>
+      <c r="H214" s="151"/>
+      <c r="I214" s="151"/>
+      <c r="J214" s="151"/>
+      <c r="K214" s="152"/>
     </row>
     <row r="215" spans="1:14">
       <c r="A215" s="12">
@@ -10073,16 +9966,16 @@
         <v>AD6</v>
       </c>
       <c r="C216" s="13"/>
-      <c r="D216" s="146" t="s">
+      <c r="D216" s="143" t="s">
         <v>373</v>
       </c>
-      <c r="E216" s="138"/>
-      <c r="F216" s="138"/>
-      <c r="G216" s="138"/>
-      <c r="H216" s="138"/>
-      <c r="I216" s="138"/>
-      <c r="J216" s="138"/>
-      <c r="K216" s="147"/>
+      <c r="E216" s="135"/>
+      <c r="F216" s="135"/>
+      <c r="G216" s="135"/>
+      <c r="H216" s="135"/>
+      <c r="I216" s="135"/>
+      <c r="J216" s="135"/>
+      <c r="K216" s="144"/>
     </row>
     <row r="217" spans="1:14">
       <c r="A217" s="12">
@@ -10094,14 +9987,14 @@
         <v>AD7</v>
       </c>
       <c r="C217" s="13"/>
-      <c r="D217" s="132"/>
-      <c r="E217" s="133"/>
-      <c r="F217" s="133"/>
-      <c r="G217" s="133"/>
-      <c r="H217" s="133"/>
-      <c r="I217" s="133"/>
-      <c r="J217" s="133"/>
-      <c r="K217" s="134"/>
+      <c r="D217" s="145"/>
+      <c r="E217" s="138"/>
+      <c r="F217" s="138"/>
+      <c r="G217" s="138"/>
+      <c r="H217" s="138"/>
+      <c r="I217" s="138"/>
+      <c r="J217" s="138"/>
+      <c r="K217" s="146"/>
     </row>
     <row r="218" spans="1:14">
       <c r="A218" s="12">
@@ -10113,16 +10006,16 @@
         <v>AD8</v>
       </c>
       <c r="C218" s="13"/>
-      <c r="D218" s="146" t="s">
+      <c r="D218" s="143" t="s">
         <v>374</v>
       </c>
-      <c r="E218" s="138"/>
-      <c r="F218" s="138"/>
-      <c r="G218" s="138"/>
-      <c r="H218" s="138"/>
-      <c r="I218" s="138"/>
-      <c r="J218" s="138"/>
-      <c r="K218" s="147"/>
+      <c r="E218" s="135"/>
+      <c r="F218" s="135"/>
+      <c r="G218" s="135"/>
+      <c r="H218" s="135"/>
+      <c r="I218" s="135"/>
+      <c r="J218" s="135"/>
+      <c r="K218" s="144"/>
     </row>
     <row r="219" spans="1:14">
       <c r="A219" s="12">
@@ -10134,14 +10027,14 @@
         <v>AD9</v>
       </c>
       <c r="C219" s="13"/>
-      <c r="D219" s="132"/>
-      <c r="E219" s="133"/>
-      <c r="F219" s="133"/>
-      <c r="G219" s="133"/>
-      <c r="H219" s="133"/>
-      <c r="I219" s="133"/>
-      <c r="J219" s="133"/>
-      <c r="K219" s="134"/>
+      <c r="D219" s="145"/>
+      <c r="E219" s="138"/>
+      <c r="F219" s="138"/>
+      <c r="G219" s="138"/>
+      <c r="H219" s="138"/>
+      <c r="I219" s="138"/>
+      <c r="J219" s="138"/>
+      <c r="K219" s="146"/>
     </row>
     <row r="220" spans="1:14">
       <c r="A220" s="12">
@@ -10153,16 +10046,16 @@
         <v>ADA</v>
       </c>
       <c r="C220" s="13"/>
-      <c r="D220" s="146" t="s">
+      <c r="D220" s="143" t="s">
         <v>375</v>
       </c>
-      <c r="E220" s="138"/>
-      <c r="F220" s="138"/>
-      <c r="G220" s="138"/>
-      <c r="H220" s="138"/>
-      <c r="I220" s="138"/>
-      <c r="J220" s="138"/>
-      <c r="K220" s="147"/>
+      <c r="E220" s="135"/>
+      <c r="F220" s="135"/>
+      <c r="G220" s="135"/>
+      <c r="H220" s="135"/>
+      <c r="I220" s="135"/>
+      <c r="J220" s="135"/>
+      <c r="K220" s="144"/>
     </row>
     <row r="221" spans="1:14">
       <c r="A221" s="12">
@@ -10174,14 +10067,14 @@
         <v>ADB</v>
       </c>
       <c r="C221" s="13"/>
-      <c r="D221" s="132"/>
-      <c r="E221" s="133"/>
-      <c r="F221" s="133"/>
-      <c r="G221" s="133"/>
-      <c r="H221" s="133"/>
-      <c r="I221" s="133"/>
-      <c r="J221" s="133"/>
-      <c r="K221" s="134"/>
+      <c r="D221" s="145"/>
+      <c r="E221" s="138"/>
+      <c r="F221" s="138"/>
+      <c r="G221" s="138"/>
+      <c r="H221" s="138"/>
+      <c r="I221" s="138"/>
+      <c r="J221" s="138"/>
+      <c r="K221" s="146"/>
     </row>
     <row r="222" spans="1:14">
       <c r="A222" s="12">
@@ -10193,16 +10086,16 @@
         <v>ADC</v>
       </c>
       <c r="C222" s="13"/>
-      <c r="D222" s="126" t="s">
+      <c r="D222" s="150" t="s">
         <v>376</v>
       </c>
-      <c r="E222" s="127"/>
-      <c r="F222" s="127"/>
-      <c r="G222" s="127"/>
-      <c r="H222" s="127"/>
-      <c r="I222" s="127"/>
-      <c r="J222" s="127"/>
-      <c r="K222" s="128"/>
+      <c r="E222" s="151"/>
+      <c r="F222" s="151"/>
+      <c r="G222" s="151"/>
+      <c r="H222" s="151"/>
+      <c r="I222" s="151"/>
+      <c r="J222" s="151"/>
+      <c r="K222" s="152"/>
     </row>
     <row r="223" spans="1:14">
       <c r="A223" s="12">
@@ -10233,16 +10126,16 @@
         <v>ADE</v>
       </c>
       <c r="C224" s="13"/>
-      <c r="D224" s="126" t="s">
+      <c r="D224" s="150" t="s">
         <v>377</v>
       </c>
-      <c r="E224" s="127"/>
-      <c r="F224" s="127"/>
-      <c r="G224" s="127"/>
-      <c r="H224" s="127"/>
-      <c r="I224" s="127"/>
-      <c r="J224" s="127"/>
-      <c r="K224" s="128"/>
+      <c r="E224" s="151"/>
+      <c r="F224" s="151"/>
+      <c r="G224" s="151"/>
+      <c r="H224" s="151"/>
+      <c r="I224" s="151"/>
+      <c r="J224" s="151"/>
+      <c r="K224" s="152"/>
     </row>
     <row r="225" spans="1:14" s="1" customFormat="1">
       <c r="A225" s="32">
@@ -10276,16 +10169,16 @@
         <v>AE0</v>
       </c>
       <c r="C226" s="39"/>
-      <c r="D226" s="152" t="s">
+      <c r="D226" s="153" t="s">
         <v>378</v>
       </c>
-      <c r="E226" s="153"/>
-      <c r="F226" s="153"/>
-      <c r="G226" s="153"/>
-      <c r="H226" s="153"/>
-      <c r="I226" s="153"/>
-      <c r="J226" s="153"/>
-      <c r="K226" s="154"/>
+      <c r="E226" s="154"/>
+      <c r="F226" s="154"/>
+      <c r="G226" s="154"/>
+      <c r="H226" s="154"/>
+      <c r="I226" s="154"/>
+      <c r="J226" s="154"/>
+      <c r="K226" s="155"/>
     </row>
     <row r="227" spans="1:14">
       <c r="A227" s="12">
@@ -10430,16 +10323,16 @@
         <v>AE8</v>
       </c>
       <c r="C234" s="13"/>
-      <c r="D234" s="150" t="s">
+      <c r="D234" s="147" t="s">
         <v>379</v>
       </c>
-      <c r="E234" s="136"/>
-      <c r="F234" s="136"/>
-      <c r="G234" s="136"/>
-      <c r="H234" s="136"/>
-      <c r="I234" s="136"/>
-      <c r="J234" s="136"/>
-      <c r="K234" s="151"/>
+      <c r="E234" s="148"/>
+      <c r="F234" s="148"/>
+      <c r="G234" s="148"/>
+      <c r="H234" s="148"/>
+      <c r="I234" s="148"/>
+      <c r="J234" s="148"/>
+      <c r="K234" s="149"/>
     </row>
     <row r="235" spans="1:14">
       <c r="A235" s="12">
@@ -10508,16 +10401,16 @@
         <v>AEC</v>
       </c>
       <c r="C238" s="13"/>
-      <c r="D238" s="142" t="s">
+      <c r="D238" s="134" t="s">
         <v>380</v>
       </c>
-      <c r="E238" s="138"/>
-      <c r="F238" s="138"/>
-      <c r="G238" s="138"/>
-      <c r="H238" s="138"/>
-      <c r="I238" s="138"/>
-      <c r="J238" s="138"/>
-      <c r="K238" s="139"/>
+      <c r="E238" s="135"/>
+      <c r="F238" s="135"/>
+      <c r="G238" s="135"/>
+      <c r="H238" s="135"/>
+      <c r="I238" s="135"/>
+      <c r="J238" s="135"/>
+      <c r="K238" s="136"/>
     </row>
     <row r="239" spans="1:14">
       <c r="A239" s="12">
@@ -10529,14 +10422,14 @@
         <v>AED</v>
       </c>
       <c r="C239" s="13"/>
-      <c r="D239" s="148"/>
-      <c r="E239" s="133"/>
-      <c r="F239" s="133"/>
-      <c r="G239" s="133"/>
-      <c r="H239" s="133"/>
-      <c r="I239" s="133"/>
-      <c r="J239" s="133"/>
-      <c r="K239" s="149"/>
+      <c r="D239" s="137"/>
+      <c r="E239" s="138"/>
+      <c r="F239" s="138"/>
+      <c r="G239" s="138"/>
+      <c r="H239" s="138"/>
+      <c r="I239" s="138"/>
+      <c r="J239" s="138"/>
+      <c r="K239" s="139"/>
     </row>
     <row r="240" spans="1:14">
       <c r="A240" s="12">
@@ -10548,16 +10441,16 @@
         <v>AEE</v>
       </c>
       <c r="C240" s="70"/>
-      <c r="D240" s="138" t="s">
+      <c r="D240" s="135" t="s">
         <v>381</v>
       </c>
-      <c r="E240" s="138"/>
-      <c r="F240" s="138"/>
-      <c r="G240" s="138"/>
-      <c r="H240" s="138"/>
-      <c r="I240" s="138"/>
-      <c r="J240" s="138"/>
-      <c r="K240" s="139"/>
+      <c r="E240" s="135"/>
+      <c r="F240" s="135"/>
+      <c r="G240" s="135"/>
+      <c r="H240" s="135"/>
+      <c r="I240" s="135"/>
+      <c r="J240" s="135"/>
+      <c r="K240" s="136"/>
     </row>
     <row r="241" spans="1:14" s="1" customFormat="1">
       <c r="A241" s="32">
@@ -10569,14 +10462,14 @@
         <v>AEF</v>
       </c>
       <c r="C241" s="34"/>
-      <c r="D241" s="140"/>
-      <c r="E241" s="140"/>
-      <c r="F241" s="140"/>
-      <c r="G241" s="140"/>
-      <c r="H241" s="140"/>
-      <c r="I241" s="140"/>
-      <c r="J241" s="140"/>
-      <c r="K241" s="141"/>
+      <c r="D241" s="161"/>
+      <c r="E241" s="161"/>
+      <c r="F241" s="161"/>
+      <c r="G241" s="161"/>
+      <c r="H241" s="161"/>
+      <c r="I241" s="161"/>
+      <c r="J241" s="161"/>
+      <c r="K241" s="162"/>
       <c r="L241" s="57"/>
       <c r="M241" s="58"/>
       <c r="N241" s="58"/>
@@ -10767,16 +10660,16 @@
         <v>AF8</v>
       </c>
       <c r="C250" s="13"/>
-      <c r="D250" s="135" t="s">
+      <c r="D250" s="159" t="s">
         <v>382</v>
       </c>
-      <c r="E250" s="136"/>
-      <c r="F250" s="136"/>
-      <c r="G250" s="136"/>
-      <c r="H250" s="136"/>
-      <c r="I250" s="136"/>
-      <c r="J250" s="136"/>
-      <c r="K250" s="137"/>
+      <c r="E250" s="148"/>
+      <c r="F250" s="148"/>
+      <c r="G250" s="148"/>
+      <c r="H250" s="148"/>
+      <c r="I250" s="148"/>
+      <c r="J250" s="148"/>
+      <c r="K250" s="160"/>
     </row>
     <row r="251" spans="1:14">
       <c r="A251" s="12">
@@ -11345,16 +11238,16 @@
         <v>B16</v>
       </c>
       <c r="C280" s="13"/>
-      <c r="D280" s="126" t="s">
+      <c r="D280" s="150" t="s">
         <v>383</v>
       </c>
-      <c r="E280" s="127"/>
-      <c r="F280" s="127"/>
-      <c r="G280" s="127"/>
-      <c r="H280" s="127"/>
-      <c r="I280" s="127"/>
-      <c r="J280" s="127"/>
-      <c r="K280" s="128"/>
+      <c r="E280" s="151"/>
+      <c r="F280" s="151"/>
+      <c r="G280" s="151"/>
+      <c r="H280" s="151"/>
+      <c r="I280" s="151"/>
+      <c r="J280" s="151"/>
+      <c r="K280" s="152"/>
     </row>
     <row r="281" spans="1:14">
       <c r="A281" s="12">
@@ -11461,16 +11354,16 @@
         <v>B1C</v>
       </c>
       <c r="C286" s="13"/>
-      <c r="D286" s="126" t="s">
+      <c r="D286" s="150" t="s">
         <v>384</v>
       </c>
-      <c r="E286" s="127"/>
-      <c r="F286" s="127"/>
-      <c r="G286" s="127"/>
-      <c r="H286" s="127"/>
-      <c r="I286" s="127"/>
-      <c r="J286" s="127"/>
-      <c r="K286" s="128"/>
+      <c r="E286" s="151"/>
+      <c r="F286" s="151"/>
+      <c r="G286" s="151"/>
+      <c r="H286" s="151"/>
+      <c r="I286" s="151"/>
+      <c r="J286" s="151"/>
+      <c r="K286" s="152"/>
     </row>
     <row r="287" spans="1:14">
       <c r="A287" s="12">
@@ -11658,16 +11551,16 @@
         <v>B26</v>
       </c>
       <c r="C296" s="13"/>
-      <c r="D296" s="126" t="s">
+      <c r="D296" s="150" t="s">
         <v>386</v>
       </c>
-      <c r="E296" s="127"/>
-      <c r="F296" s="127"/>
-      <c r="G296" s="127"/>
-      <c r="H296" s="127"/>
-      <c r="I296" s="127"/>
-      <c r="J296" s="127"/>
-      <c r="K296" s="128"/>
+      <c r="E296" s="151"/>
+      <c r="F296" s="151"/>
+      <c r="G296" s="151"/>
+      <c r="H296" s="151"/>
+      <c r="I296" s="151"/>
+      <c r="J296" s="151"/>
+      <c r="K296" s="152"/>
     </row>
     <row r="297" spans="1:14">
       <c r="A297" s="12">
@@ -11698,16 +11591,16 @@
         <v>B28</v>
       </c>
       <c r="C298" s="13"/>
-      <c r="D298" s="142" t="s">
+      <c r="D298" s="134" t="s">
         <v>387</v>
       </c>
-      <c r="E298" s="138"/>
-      <c r="F298" s="138"/>
-      <c r="G298" s="138"/>
-      <c r="H298" s="138"/>
-      <c r="I298" s="138"/>
-      <c r="J298" s="138"/>
-      <c r="K298" s="139"/>
+      <c r="E298" s="135"/>
+      <c r="F298" s="135"/>
+      <c r="G298" s="135"/>
+      <c r="H298" s="135"/>
+      <c r="I298" s="135"/>
+      <c r="J298" s="135"/>
+      <c r="K298" s="136"/>
     </row>
     <row r="299" spans="1:14">
       <c r="A299" s="12">
@@ -11719,14 +11612,14 @@
         <v>B29</v>
       </c>
       <c r="C299" s="13"/>
-      <c r="D299" s="148"/>
-      <c r="E299" s="133"/>
-      <c r="F299" s="133"/>
-      <c r="G299" s="133"/>
-      <c r="H299" s="133"/>
-      <c r="I299" s="133"/>
-      <c r="J299" s="133"/>
-      <c r="K299" s="149"/>
+      <c r="D299" s="137"/>
+      <c r="E299" s="138"/>
+      <c r="F299" s="138"/>
+      <c r="G299" s="138"/>
+      <c r="H299" s="138"/>
+      <c r="I299" s="138"/>
+      <c r="J299" s="138"/>
+      <c r="K299" s="139"/>
     </row>
     <row r="300" spans="1:14">
       <c r="A300" s="12">
@@ -11738,16 +11631,16 @@
         <v>B2A</v>
       </c>
       <c r="C300" s="13"/>
-      <c r="D300" s="142" t="s">
+      <c r="D300" s="134" t="s">
         <v>388</v>
       </c>
-      <c r="E300" s="138"/>
-      <c r="F300" s="138"/>
-      <c r="G300" s="138"/>
-      <c r="H300" s="138"/>
-      <c r="I300" s="138"/>
-      <c r="J300" s="138"/>
-      <c r="K300" s="139"/>
+      <c r="E300" s="135"/>
+      <c r="F300" s="135"/>
+      <c r="G300" s="135"/>
+      <c r="H300" s="135"/>
+      <c r="I300" s="135"/>
+      <c r="J300" s="135"/>
+      <c r="K300" s="136"/>
     </row>
     <row r="301" spans="1:14">
       <c r="A301" s="12">
@@ -11759,14 +11652,14 @@
         <v>B2B</v>
       </c>
       <c r="C301" s="13"/>
-      <c r="D301" s="148"/>
-      <c r="E301" s="133"/>
-      <c r="F301" s="133"/>
-      <c r="G301" s="133"/>
-      <c r="H301" s="133"/>
-      <c r="I301" s="133"/>
-      <c r="J301" s="133"/>
-      <c r="K301" s="149"/>
+      <c r="D301" s="137"/>
+      <c r="E301" s="138"/>
+      <c r="F301" s="138"/>
+      <c r="G301" s="138"/>
+      <c r="H301" s="138"/>
+      <c r="I301" s="138"/>
+      <c r="J301" s="138"/>
+      <c r="K301" s="139"/>
     </row>
     <row r="302" spans="1:14">
       <c r="A302" s="12">
@@ -11778,16 +11671,16 @@
         <v>B2C</v>
       </c>
       <c r="C302" s="13"/>
-      <c r="D302" s="142" t="s">
+      <c r="D302" s="134" t="s">
         <v>389</v>
       </c>
-      <c r="E302" s="138"/>
-      <c r="F302" s="138"/>
-      <c r="G302" s="138"/>
-      <c r="H302" s="138"/>
-      <c r="I302" s="138"/>
-      <c r="J302" s="138"/>
-      <c r="K302" s="139"/>
+      <c r="E302" s="135"/>
+      <c r="F302" s="135"/>
+      <c r="G302" s="135"/>
+      <c r="H302" s="135"/>
+      <c r="I302" s="135"/>
+      <c r="J302" s="135"/>
+      <c r="K302" s="136"/>
     </row>
     <row r="303" spans="1:14">
       <c r="A303" s="12">
@@ -11799,14 +11692,14 @@
         <v>B2D</v>
       </c>
       <c r="C303" s="13"/>
-      <c r="D303" s="148"/>
-      <c r="E303" s="133"/>
-      <c r="F303" s="133"/>
-      <c r="G303" s="133"/>
-      <c r="H303" s="133"/>
-      <c r="I303" s="133"/>
-      <c r="J303" s="133"/>
-      <c r="K303" s="149"/>
+      <c r="D303" s="137"/>
+      <c r="E303" s="138"/>
+      <c r="F303" s="138"/>
+      <c r="G303" s="138"/>
+      <c r="H303" s="138"/>
+      <c r="I303" s="138"/>
+      <c r="J303" s="138"/>
+      <c r="K303" s="139"/>
     </row>
     <row r="304" spans="1:14">
       <c r="A304" s="12">
@@ -11818,16 +11711,16 @@
         <v>B2E</v>
       </c>
       <c r="C304" s="13"/>
-      <c r="D304" s="142" t="s">
+      <c r="D304" s="134" t="s">
         <v>390</v>
       </c>
-      <c r="E304" s="138"/>
-      <c r="F304" s="138"/>
-      <c r="G304" s="138"/>
-      <c r="H304" s="138"/>
-      <c r="I304" s="138"/>
-      <c r="J304" s="138"/>
-      <c r="K304" s="139"/>
+      <c r="E304" s="135"/>
+      <c r="F304" s="135"/>
+      <c r="G304" s="135"/>
+      <c r="H304" s="135"/>
+      <c r="I304" s="135"/>
+      <c r="J304" s="135"/>
+      <c r="K304" s="136"/>
     </row>
     <row r="305" spans="1:14" s="1" customFormat="1">
       <c r="A305" s="32">
@@ -11839,14 +11732,14 @@
         <v>B2F</v>
       </c>
       <c r="C305" s="33"/>
-      <c r="D305" s="148"/>
-      <c r="E305" s="133"/>
-      <c r="F305" s="133"/>
-      <c r="G305" s="133"/>
-      <c r="H305" s="133"/>
-      <c r="I305" s="133"/>
-      <c r="J305" s="133"/>
-      <c r="K305" s="149"/>
+      <c r="D305" s="137"/>
+      <c r="E305" s="138"/>
+      <c r="F305" s="138"/>
+      <c r="G305" s="138"/>
+      <c r="H305" s="138"/>
+      <c r="I305" s="138"/>
+      <c r="J305" s="138"/>
+      <c r="K305" s="139"/>
       <c r="L305" s="57"/>
       <c r="M305" s="58"/>
       <c r="N305" s="58"/>
@@ -11861,16 +11754,16 @@
         <v>B30</v>
       </c>
       <c r="C306" s="39"/>
-      <c r="D306" s="142" t="s">
+      <c r="D306" s="134" t="s">
         <v>391</v>
       </c>
-      <c r="E306" s="138"/>
-      <c r="F306" s="138"/>
-      <c r="G306" s="138"/>
-      <c r="H306" s="138"/>
-      <c r="I306" s="138"/>
-      <c r="J306" s="138"/>
-      <c r="K306" s="139"/>
+      <c r="E306" s="135"/>
+      <c r="F306" s="135"/>
+      <c r="G306" s="135"/>
+      <c r="H306" s="135"/>
+      <c r="I306" s="135"/>
+      <c r="J306" s="135"/>
+      <c r="K306" s="136"/>
     </row>
     <row r="307" spans="1:14">
       <c r="A307" s="12">
@@ -11882,14 +11775,14 @@
         <v>B31</v>
       </c>
       <c r="C307" s="13"/>
-      <c r="D307" s="148"/>
-      <c r="E307" s="133"/>
-      <c r="F307" s="133"/>
-      <c r="G307" s="133"/>
-      <c r="H307" s="133"/>
-      <c r="I307" s="133"/>
-      <c r="J307" s="133"/>
-      <c r="K307" s="149"/>
+      <c r="D307" s="137"/>
+      <c r="E307" s="138"/>
+      <c r="F307" s="138"/>
+      <c r="G307" s="138"/>
+      <c r="H307" s="138"/>
+      <c r="I307" s="138"/>
+      <c r="J307" s="138"/>
+      <c r="K307" s="139"/>
     </row>
     <row r="308" spans="1:14">
       <c r="A308" s="12">
@@ -11901,16 +11794,16 @@
         <v>B32</v>
       </c>
       <c r="C308" s="13"/>
-      <c r="D308" s="142" t="s">
+      <c r="D308" s="134" t="s">
         <v>392</v>
       </c>
-      <c r="E308" s="138"/>
-      <c r="F308" s="138"/>
-      <c r="G308" s="138"/>
-      <c r="H308" s="138"/>
-      <c r="I308" s="138"/>
-      <c r="J308" s="138"/>
-      <c r="K308" s="139"/>
+      <c r="E308" s="135"/>
+      <c r="F308" s="135"/>
+      <c r="G308" s="135"/>
+      <c r="H308" s="135"/>
+      <c r="I308" s="135"/>
+      <c r="J308" s="135"/>
+      <c r="K308" s="136"/>
     </row>
     <row r="309" spans="1:14">
       <c r="A309" s="12">
@@ -11922,14 +11815,14 @@
         <v>B33</v>
       </c>
       <c r="C309" s="13"/>
-      <c r="D309" s="148"/>
-      <c r="E309" s="133"/>
-      <c r="F309" s="133"/>
-      <c r="G309" s="133"/>
-      <c r="H309" s="133"/>
-      <c r="I309" s="133"/>
-      <c r="J309" s="133"/>
-      <c r="K309" s="149"/>
+      <c r="D309" s="137"/>
+      <c r="E309" s="138"/>
+      <c r="F309" s="138"/>
+      <c r="G309" s="138"/>
+      <c r="H309" s="138"/>
+      <c r="I309" s="138"/>
+      <c r="J309" s="138"/>
+      <c r="K309" s="139"/>
     </row>
     <row r="310" spans="1:14">
       <c r="A310" s="12">
@@ -15808,20 +15701,32 @@
       <c r="K513" s="22"/>
     </row>
   </sheetData>
-  <mergeCells count="55">
-    <mergeCell ref="D93:K93"/>
-    <mergeCell ref="D96:K96"/>
-    <mergeCell ref="D94:K94"/>
-    <mergeCell ref="D95:K95"/>
-    <mergeCell ref="D92:K92"/>
-    <mergeCell ref="D91:K91"/>
-    <mergeCell ref="D90:K90"/>
-    <mergeCell ref="D304:K305"/>
-    <mergeCell ref="D306:K307"/>
-    <mergeCell ref="D308:K309"/>
-    <mergeCell ref="D298:K299"/>
-    <mergeCell ref="D300:K301"/>
-    <mergeCell ref="D302:K303"/>
+  <mergeCells count="62">
+    <mergeCell ref="D75:K75"/>
+    <mergeCell ref="D76:K76"/>
+    <mergeCell ref="D77:K77"/>
+    <mergeCell ref="D78:K78"/>
+    <mergeCell ref="D79:K79"/>
+    <mergeCell ref="D80:K80"/>
+    <mergeCell ref="D81:K81"/>
+    <mergeCell ref="D168:K168"/>
+    <mergeCell ref="D175:K175"/>
+    <mergeCell ref="D178:K178"/>
+    <mergeCell ref="D182:K182"/>
+    <mergeCell ref="D183:K183"/>
+    <mergeCell ref="D174:K174"/>
+    <mergeCell ref="D184:K184"/>
+    <mergeCell ref="D185:K185"/>
+    <mergeCell ref="D186:K186"/>
+    <mergeCell ref="D187:K187"/>
+    <mergeCell ref="D188:K188"/>
+    <mergeCell ref="D197:K197"/>
+    <mergeCell ref="D198:K198"/>
+    <mergeCell ref="D189:K189"/>
+    <mergeCell ref="D190:K190"/>
+    <mergeCell ref="D191:K191"/>
+    <mergeCell ref="D192:K192"/>
+    <mergeCell ref="D193:K193"/>
     <mergeCell ref="D2:K3"/>
     <mergeCell ref="D216:K217"/>
     <mergeCell ref="D218:K219"/>
@@ -15838,6 +15743,14 @@
     <mergeCell ref="D204:K204"/>
     <mergeCell ref="D206:K206"/>
     <mergeCell ref="D208:K208"/>
+    <mergeCell ref="D91:K91"/>
+    <mergeCell ref="D90:K90"/>
+    <mergeCell ref="D304:K305"/>
+    <mergeCell ref="D306:K307"/>
+    <mergeCell ref="D308:K309"/>
+    <mergeCell ref="D298:K299"/>
+    <mergeCell ref="D300:K301"/>
+    <mergeCell ref="D302:K303"/>
     <mergeCell ref="D250:K250"/>
     <mergeCell ref="D280:K280"/>
     <mergeCell ref="D286:K286"/>
@@ -15846,24 +15759,11 @@
     <mergeCell ref="D194:K194"/>
     <mergeCell ref="D195:K195"/>
     <mergeCell ref="D196:K196"/>
-    <mergeCell ref="D197:K197"/>
-    <mergeCell ref="D198:K198"/>
-    <mergeCell ref="D189:K189"/>
-    <mergeCell ref="D190:K190"/>
-    <mergeCell ref="D191:K191"/>
-    <mergeCell ref="D192:K192"/>
-    <mergeCell ref="D193:K193"/>
-    <mergeCell ref="D184:K184"/>
-    <mergeCell ref="D185:K185"/>
-    <mergeCell ref="D186:K186"/>
-    <mergeCell ref="D187:K187"/>
-    <mergeCell ref="D188:K188"/>
-    <mergeCell ref="D168:K168"/>
-    <mergeCell ref="D175:K175"/>
-    <mergeCell ref="D178:K178"/>
-    <mergeCell ref="D182:K182"/>
-    <mergeCell ref="D183:K183"/>
-    <mergeCell ref="D174:K174"/>
+    <mergeCell ref="D93:K93"/>
+    <mergeCell ref="D96:K96"/>
+    <mergeCell ref="D94:K94"/>
+    <mergeCell ref="D95:K95"/>
+    <mergeCell ref="D92:K92"/>
   </mergeCells>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="53" fitToHeight="0" orientation="landscape" r:id="rId1"/>
@@ -15949,16 +15849,16 @@
         <f>8*A2&amp;"-"&amp;(8*A2+7)</f>
         <v>0-7</v>
       </c>
-      <c r="D2" s="142" t="s">
+      <c r="D2" s="134" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="138"/>
-      <c r="F2" s="138"/>
-      <c r="G2" s="138"/>
-      <c r="H2" s="138"/>
-      <c r="I2" s="138"/>
-      <c r="J2" s="138"/>
-      <c r="K2" s="139"/>
+      <c r="E2" s="135"/>
+      <c r="F2" s="135"/>
+      <c r="G2" s="135"/>
+      <c r="H2" s="135"/>
+      <c r="I2" s="135"/>
+      <c r="J2" s="135"/>
+      <c r="K2" s="136"/>
       <c r="M2" s="3">
         <v>16</v>
       </c>
@@ -15980,14 +15880,14 @@
         <f t="shared" ref="C3:C33" si="2">8*A3&amp;"-"&amp;(8*A3+7)</f>
         <v>8-15</v>
       </c>
-      <c r="D3" s="148"/>
-      <c r="E3" s="133"/>
-      <c r="F3" s="133"/>
-      <c r="G3" s="133"/>
-      <c r="H3" s="133"/>
-      <c r="I3" s="133"/>
-      <c r="J3" s="133"/>
-      <c r="K3" s="145"/>
+      <c r="D3" s="137"/>
+      <c r="E3" s="138"/>
+      <c r="F3" s="138"/>
+      <c r="G3" s="138"/>
+      <c r="H3" s="138"/>
+      <c r="I3" s="138"/>
+      <c r="J3" s="138"/>
+      <c r="K3" s="142"/>
       <c r="M3" s="3">
         <v>17</v>
       </c>
@@ -22236,16 +22136,16 @@
         <v>AB0</v>
       </c>
       <c r="C178" s="39"/>
-      <c r="D178" s="125" t="s">
+      <c r="D178" s="166" t="s">
         <v>350</v>
       </c>
-      <c r="E178" s="125"/>
-      <c r="F178" s="125"/>
-      <c r="G178" s="125"/>
-      <c r="H178" s="125"/>
-      <c r="I178" s="125"/>
-      <c r="J178" s="125"/>
-      <c r="K178" s="125"/>
+      <c r="E178" s="166"/>
+      <c r="F178" s="166"/>
+      <c r="G178" s="166"/>
+      <c r="H178" s="166"/>
+      <c r="I178" s="166"/>
+      <c r="J178" s="166"/>
+      <c r="K178" s="166"/>
     </row>
     <row r="179" spans="1:14">
       <c r="A179" s="12">
@@ -22314,16 +22214,16 @@
         <v>AB4</v>
       </c>
       <c r="C182" s="13"/>
-      <c r="D182" s="126" t="s">
+      <c r="D182" s="150" t="s">
         <v>351</v>
       </c>
-      <c r="E182" s="127"/>
-      <c r="F182" s="127"/>
-      <c r="G182" s="127"/>
-      <c r="H182" s="127"/>
-      <c r="I182" s="127"/>
-      <c r="J182" s="127"/>
-      <c r="K182" s="128"/>
+      <c r="E182" s="151"/>
+      <c r="F182" s="151"/>
+      <c r="G182" s="151"/>
+      <c r="H182" s="151"/>
+      <c r="I182" s="151"/>
+      <c r="J182" s="151"/>
+      <c r="K182" s="152"/>
     </row>
     <row r="183" spans="1:14">
       <c r="A183" s="12">
@@ -22335,16 +22235,16 @@
         <v>AB5</v>
       </c>
       <c r="C183" s="13"/>
-      <c r="D183" s="126" t="s">
+      <c r="D183" s="150" t="s">
         <v>352</v>
       </c>
-      <c r="E183" s="127"/>
-      <c r="F183" s="127"/>
-      <c r="G183" s="127"/>
-      <c r="H183" s="127"/>
-      <c r="I183" s="127"/>
-      <c r="J183" s="127"/>
-      <c r="K183" s="128"/>
+      <c r="E183" s="151"/>
+      <c r="F183" s="151"/>
+      <c r="G183" s="151"/>
+      <c r="H183" s="151"/>
+      <c r="I183" s="151"/>
+      <c r="J183" s="151"/>
+      <c r="K183" s="152"/>
     </row>
     <row r="184" spans="1:14">
       <c r="A184" s="12">
@@ -22356,16 +22256,16 @@
         <v>AB6</v>
       </c>
       <c r="C184" s="13"/>
-      <c r="D184" s="126" t="s">
+      <c r="D184" s="150" t="s">
         <v>353</v>
       </c>
-      <c r="E184" s="127"/>
-      <c r="F184" s="127"/>
-      <c r="G184" s="127"/>
-      <c r="H184" s="127"/>
-      <c r="I184" s="127"/>
-      <c r="J184" s="127"/>
-      <c r="K184" s="128"/>
+      <c r="E184" s="151"/>
+      <c r="F184" s="151"/>
+      <c r="G184" s="151"/>
+      <c r="H184" s="151"/>
+      <c r="I184" s="151"/>
+      <c r="J184" s="151"/>
+      <c r="K184" s="152"/>
     </row>
     <row r="185" spans="1:14">
       <c r="A185" s="12">
@@ -22377,16 +22277,16 @@
         <v>AB7</v>
       </c>
       <c r="C185" s="13"/>
-      <c r="D185" s="126" t="s">
+      <c r="D185" s="150" t="s">
         <v>354</v>
       </c>
-      <c r="E185" s="127"/>
-      <c r="F185" s="127"/>
-      <c r="G185" s="127"/>
-      <c r="H185" s="127"/>
-      <c r="I185" s="127"/>
-      <c r="J185" s="127"/>
-      <c r="K185" s="128"/>
+      <c r="E185" s="151"/>
+      <c r="F185" s="151"/>
+      <c r="G185" s="151"/>
+      <c r="H185" s="151"/>
+      <c r="I185" s="151"/>
+      <c r="J185" s="151"/>
+      <c r="K185" s="152"/>
     </row>
     <row r="186" spans="1:14">
       <c r="A186" s="12">
@@ -22398,16 +22298,16 @@
         <v>AB8</v>
       </c>
       <c r="C186" s="13"/>
-      <c r="D186" s="126" t="s">
+      <c r="D186" s="150" t="s">
         <v>355</v>
       </c>
-      <c r="E186" s="127"/>
-      <c r="F186" s="127"/>
-      <c r="G186" s="127"/>
-      <c r="H186" s="127"/>
-      <c r="I186" s="127"/>
-      <c r="J186" s="127"/>
-      <c r="K186" s="128"/>
+      <c r="E186" s="151"/>
+      <c r="F186" s="151"/>
+      <c r="G186" s="151"/>
+      <c r="H186" s="151"/>
+      <c r="I186" s="151"/>
+      <c r="J186" s="151"/>
+      <c r="K186" s="152"/>
     </row>
     <row r="187" spans="1:14">
       <c r="A187" s="12">
@@ -22419,16 +22319,16 @@
         <v>AB9</v>
       </c>
       <c r="C187" s="13"/>
-      <c r="D187" s="126" t="s">
+      <c r="D187" s="150" t="s">
         <v>356</v>
       </c>
-      <c r="E187" s="127"/>
-      <c r="F187" s="127"/>
-      <c r="G187" s="127"/>
-      <c r="H187" s="127"/>
-      <c r="I187" s="127"/>
-      <c r="J187" s="127"/>
-      <c r="K187" s="128"/>
+      <c r="E187" s="151"/>
+      <c r="F187" s="151"/>
+      <c r="G187" s="151"/>
+      <c r="H187" s="151"/>
+      <c r="I187" s="151"/>
+      <c r="J187" s="151"/>
+      <c r="K187" s="152"/>
     </row>
     <row r="188" spans="1:14">
       <c r="A188" s="12">
@@ -22440,16 +22340,16 @@
         <v>ABA</v>
       </c>
       <c r="C188" s="13"/>
-      <c r="D188" s="126" t="s">
+      <c r="D188" s="150" t="s">
         <v>357</v>
       </c>
-      <c r="E188" s="127"/>
-      <c r="F188" s="127"/>
-      <c r="G188" s="127"/>
-      <c r="H188" s="127"/>
-      <c r="I188" s="127"/>
-      <c r="J188" s="127"/>
-      <c r="K188" s="128"/>
+      <c r="E188" s="151"/>
+      <c r="F188" s="151"/>
+      <c r="G188" s="151"/>
+      <c r="H188" s="151"/>
+      <c r="I188" s="151"/>
+      <c r="J188" s="151"/>
+      <c r="K188" s="152"/>
     </row>
     <row r="189" spans="1:14">
       <c r="A189" s="12">
@@ -22461,16 +22361,16 @@
         <v>ABB</v>
       </c>
       <c r="C189" s="13"/>
-      <c r="D189" s="126" t="s">
+      <c r="D189" s="150" t="s">
         <v>358</v>
       </c>
-      <c r="E189" s="127"/>
-      <c r="F189" s="127"/>
-      <c r="G189" s="127"/>
-      <c r="H189" s="127"/>
-      <c r="I189" s="127"/>
-      <c r="J189" s="127"/>
-      <c r="K189" s="128"/>
+      <c r="E189" s="151"/>
+      <c r="F189" s="151"/>
+      <c r="G189" s="151"/>
+      <c r="H189" s="151"/>
+      <c r="I189" s="151"/>
+      <c r="J189" s="151"/>
+      <c r="K189" s="152"/>
     </row>
     <row r="190" spans="1:14">
       <c r="A190" s="12">
@@ -22482,16 +22382,16 @@
         <v>ABC</v>
       </c>
       <c r="C190" s="13"/>
-      <c r="D190" s="126" t="s">
+      <c r="D190" s="150" t="s">
         <v>359</v>
       </c>
-      <c r="E190" s="127"/>
-      <c r="F190" s="127"/>
-      <c r="G190" s="127"/>
-      <c r="H190" s="127"/>
-      <c r="I190" s="127"/>
-      <c r="J190" s="127"/>
-      <c r="K190" s="128"/>
+      <c r="E190" s="151"/>
+      <c r="F190" s="151"/>
+      <c r="G190" s="151"/>
+      <c r="H190" s="151"/>
+      <c r="I190" s="151"/>
+      <c r="J190" s="151"/>
+      <c r="K190" s="152"/>
     </row>
     <row r="191" spans="1:14">
       <c r="A191" s="12">
@@ -22503,16 +22403,16 @@
         <v>ABD</v>
       </c>
       <c r="C191" s="13"/>
-      <c r="D191" s="126" t="s">
+      <c r="D191" s="150" t="s">
         <v>360</v>
       </c>
-      <c r="E191" s="127"/>
-      <c r="F191" s="127"/>
-      <c r="G191" s="127"/>
-      <c r="H191" s="127"/>
-      <c r="I191" s="127"/>
-      <c r="J191" s="127"/>
-      <c r="K191" s="128"/>
+      <c r="E191" s="151"/>
+      <c r="F191" s="151"/>
+      <c r="G191" s="151"/>
+      <c r="H191" s="151"/>
+      <c r="I191" s="151"/>
+      <c r="J191" s="151"/>
+      <c r="K191" s="152"/>
     </row>
     <row r="192" spans="1:14">
       <c r="A192" s="12">
@@ -22524,16 +22424,16 @@
         <v>ABE</v>
       </c>
       <c r="C192" s="13"/>
-      <c r="D192" s="126" t="s">
+      <c r="D192" s="150" t="s">
         <v>361</v>
       </c>
-      <c r="E192" s="127"/>
-      <c r="F192" s="127"/>
-      <c r="G192" s="127"/>
-      <c r="H192" s="127"/>
-      <c r="I192" s="127"/>
-      <c r="J192" s="127"/>
-      <c r="K192" s="128"/>
+      <c r="E192" s="151"/>
+      <c r="F192" s="151"/>
+      <c r="G192" s="151"/>
+      <c r="H192" s="151"/>
+      <c r="I192" s="151"/>
+      <c r="J192" s="151"/>
+      <c r="K192" s="152"/>
     </row>
     <row r="193" spans="1:14" s="1" customFormat="1">
       <c r="A193" s="32">
@@ -22545,16 +22445,16 @@
         <v>ABF</v>
       </c>
       <c r="C193" s="33"/>
-      <c r="D193" s="129" t="s">
+      <c r="D193" s="163" t="s">
         <v>362</v>
       </c>
-      <c r="E193" s="130"/>
-      <c r="F193" s="130"/>
-      <c r="G193" s="130"/>
-      <c r="H193" s="130"/>
-      <c r="I193" s="130"/>
-      <c r="J193" s="130"/>
-      <c r="K193" s="131"/>
+      <c r="E193" s="164"/>
+      <c r="F193" s="164"/>
+      <c r="G193" s="164"/>
+      <c r="H193" s="164"/>
+      <c r="I193" s="164"/>
+      <c r="J193" s="164"/>
+      <c r="K193" s="165"/>
       <c r="L193" s="57"/>
       <c r="M193" s="58"/>
       <c r="N193" s="58"/>
@@ -22569,16 +22469,16 @@
         <v>AC0</v>
       </c>
       <c r="C194" s="39"/>
-      <c r="D194" s="132" t="s">
+      <c r="D194" s="145" t="s">
         <v>363</v>
       </c>
-      <c r="E194" s="133"/>
-      <c r="F194" s="133"/>
-      <c r="G194" s="133"/>
-      <c r="H194" s="133"/>
-      <c r="I194" s="133"/>
-      <c r="J194" s="133"/>
-      <c r="K194" s="134"/>
+      <c r="E194" s="138"/>
+      <c r="F194" s="138"/>
+      <c r="G194" s="138"/>
+      <c r="H194" s="138"/>
+      <c r="I194" s="138"/>
+      <c r="J194" s="138"/>
+      <c r="K194" s="146"/>
     </row>
     <row r="195" spans="1:14">
       <c r="A195" s="12">
@@ -22590,16 +22490,16 @@
         <v>AC1</v>
       </c>
       <c r="C195" s="13"/>
-      <c r="D195" s="126" t="s">
+      <c r="D195" s="150" t="s">
         <v>364</v>
       </c>
-      <c r="E195" s="127"/>
-      <c r="F195" s="127"/>
-      <c r="G195" s="127"/>
-      <c r="H195" s="127"/>
-      <c r="I195" s="127"/>
-      <c r="J195" s="127"/>
-      <c r="K195" s="128"/>
+      <c r="E195" s="151"/>
+      <c r="F195" s="151"/>
+      <c r="G195" s="151"/>
+      <c r="H195" s="151"/>
+      <c r="I195" s="151"/>
+      <c r="J195" s="151"/>
+      <c r="K195" s="152"/>
     </row>
     <row r="196" spans="1:14">
       <c r="A196" s="12">
@@ -22611,16 +22511,16 @@
         <v>AC2</v>
       </c>
       <c r="C196" s="13"/>
-      <c r="D196" s="126" t="s">
+      <c r="D196" s="150" t="s">
         <v>365</v>
       </c>
-      <c r="E196" s="127"/>
-      <c r="F196" s="127"/>
-      <c r="G196" s="127"/>
-      <c r="H196" s="127"/>
-      <c r="I196" s="127"/>
-      <c r="J196" s="127"/>
-      <c r="K196" s="128"/>
+      <c r="E196" s="151"/>
+      <c r="F196" s="151"/>
+      <c r="G196" s="151"/>
+      <c r="H196" s="151"/>
+      <c r="I196" s="151"/>
+      <c r="J196" s="151"/>
+      <c r="K196" s="152"/>
     </row>
     <row r="197" spans="1:14">
       <c r="A197" s="12">
@@ -22632,16 +22532,16 @@
         <v>AC3</v>
       </c>
       <c r="C197" s="13"/>
-      <c r="D197" s="126" t="s">
+      <c r="D197" s="150" t="s">
         <v>366</v>
       </c>
-      <c r="E197" s="127"/>
-      <c r="F197" s="127"/>
-      <c r="G197" s="127"/>
-      <c r="H197" s="127"/>
-      <c r="I197" s="127"/>
-      <c r="J197" s="127"/>
-      <c r="K197" s="128"/>
+      <c r="E197" s="151"/>
+      <c r="F197" s="151"/>
+      <c r="G197" s="151"/>
+      <c r="H197" s="151"/>
+      <c r="I197" s="151"/>
+      <c r="J197" s="151"/>
+      <c r="K197" s="152"/>
     </row>
     <row r="198" spans="1:14">
       <c r="A198" s="12">
@@ -22653,16 +22553,16 @@
         <v>AC4</v>
       </c>
       <c r="C198" s="13"/>
-      <c r="D198" s="126" t="s">
+      <c r="D198" s="150" t="s">
         <v>367</v>
       </c>
-      <c r="E198" s="127"/>
-      <c r="F198" s="127"/>
-      <c r="G198" s="127"/>
-      <c r="H198" s="127"/>
-      <c r="I198" s="127"/>
-      <c r="J198" s="127"/>
-      <c r="K198" s="128"/>
+      <c r="E198" s="151"/>
+      <c r="F198" s="151"/>
+      <c r="G198" s="151"/>
+      <c r="H198" s="151"/>
+      <c r="I198" s="151"/>
+      <c r="J198" s="151"/>
+      <c r="K198" s="152"/>
     </row>
     <row r="199" spans="1:14">
       <c r="A199" s="12">
@@ -22693,16 +22593,16 @@
         <v>AC6</v>
       </c>
       <c r="C200" s="13"/>
-      <c r="D200" s="126" t="s">
+      <c r="D200" s="150" t="s">
         <v>368</v>
       </c>
-      <c r="E200" s="127"/>
-      <c r="F200" s="127"/>
-      <c r="G200" s="127"/>
-      <c r="H200" s="127"/>
-      <c r="I200" s="127"/>
-      <c r="J200" s="127"/>
-      <c r="K200" s="128"/>
+      <c r="E200" s="151"/>
+      <c r="F200" s="151"/>
+      <c r="G200" s="151"/>
+      <c r="H200" s="151"/>
+      <c r="I200" s="151"/>
+      <c r="J200" s="151"/>
+      <c r="K200" s="152"/>
     </row>
     <row r="201" spans="1:14">
       <c r="A201" s="12">
@@ -22733,16 +22633,16 @@
         <v>AC8</v>
       </c>
       <c r="C202" s="13"/>
-      <c r="D202" s="155" t="s">
+      <c r="D202" s="156" t="s">
         <v>369</v>
       </c>
-      <c r="E202" s="156"/>
-      <c r="F202" s="156"/>
-      <c r="G202" s="156"/>
-      <c r="H202" s="156"/>
-      <c r="I202" s="156"/>
-      <c r="J202" s="156"/>
-      <c r="K202" s="157"/>
+      <c r="E202" s="157"/>
+      <c r="F202" s="157"/>
+      <c r="G202" s="157"/>
+      <c r="H202" s="157"/>
+      <c r="I202" s="157"/>
+      <c r="J202" s="157"/>
+      <c r="K202" s="158"/>
     </row>
     <row r="203" spans="1:14">
       <c r="A203" s="12">
@@ -22773,16 +22673,16 @@
         <v>ACA</v>
       </c>
       <c r="C204" s="13"/>
-      <c r="D204" s="126" t="s">
+      <c r="D204" s="150" t="s">
         <v>370</v>
       </c>
-      <c r="E204" s="127"/>
-      <c r="F204" s="127"/>
-      <c r="G204" s="127"/>
-      <c r="H204" s="127"/>
-      <c r="I204" s="127"/>
-      <c r="J204" s="127"/>
-      <c r="K204" s="128"/>
+      <c r="E204" s="151"/>
+      <c r="F204" s="151"/>
+      <c r="G204" s="151"/>
+      <c r="H204" s="151"/>
+      <c r="I204" s="151"/>
+      <c r="J204" s="151"/>
+      <c r="K204" s="152"/>
     </row>
     <row r="205" spans="1:14">
       <c r="A205" s="12">
@@ -22813,16 +22713,16 @@
         <v>ACC</v>
       </c>
       <c r="C206" s="13"/>
-      <c r="D206" s="126" t="s">
+      <c r="D206" s="150" t="s">
         <v>370</v>
       </c>
-      <c r="E206" s="127"/>
-      <c r="F206" s="127"/>
-      <c r="G206" s="127"/>
-      <c r="H206" s="127"/>
-      <c r="I206" s="127"/>
-      <c r="J206" s="127"/>
-      <c r="K206" s="128"/>
+      <c r="E206" s="151"/>
+      <c r="F206" s="151"/>
+      <c r="G206" s="151"/>
+      <c r="H206" s="151"/>
+      <c r="I206" s="151"/>
+      <c r="J206" s="151"/>
+      <c r="K206" s="152"/>
     </row>
     <row r="207" spans="1:14">
       <c r="A207" s="12">
@@ -22853,16 +22753,16 @@
         <v>ACE</v>
       </c>
       <c r="C208" s="13"/>
-      <c r="D208" s="126" t="s">
+      <c r="D208" s="150" t="s">
         <v>371</v>
       </c>
-      <c r="E208" s="127"/>
-      <c r="F208" s="127"/>
-      <c r="G208" s="127"/>
-      <c r="H208" s="127"/>
-      <c r="I208" s="127"/>
-      <c r="J208" s="127"/>
-      <c r="K208" s="128"/>
+      <c r="E208" s="151"/>
+      <c r="F208" s="151"/>
+      <c r="G208" s="151"/>
+      <c r="H208" s="151"/>
+      <c r="I208" s="151"/>
+      <c r="J208" s="151"/>
+      <c r="K208" s="152"/>
     </row>
     <row r="209" spans="1:14" s="1" customFormat="1">
       <c r="A209" s="32">
@@ -22896,16 +22796,16 @@
         <v>AD0</v>
       </c>
       <c r="C210" s="39"/>
-      <c r="D210" s="132" t="s">
+      <c r="D210" s="145" t="s">
         <v>371</v>
       </c>
-      <c r="E210" s="133"/>
-      <c r="F210" s="133"/>
-      <c r="G210" s="133"/>
-      <c r="H210" s="133"/>
-      <c r="I210" s="133"/>
-      <c r="J210" s="133"/>
-      <c r="K210" s="134"/>
+      <c r="E210" s="138"/>
+      <c r="F210" s="138"/>
+      <c r="G210" s="138"/>
+      <c r="H210" s="138"/>
+      <c r="I210" s="138"/>
+      <c r="J210" s="138"/>
+      <c r="K210" s="146"/>
     </row>
     <row r="211" spans="1:14">
       <c r="A211" s="12">
@@ -22974,16 +22874,16 @@
         <v>AD4</v>
       </c>
       <c r="C214" s="13"/>
-      <c r="D214" s="126" t="s">
+      <c r="D214" s="150" t="s">
         <v>372</v>
       </c>
-      <c r="E214" s="127"/>
-      <c r="F214" s="127"/>
-      <c r="G214" s="127"/>
-      <c r="H214" s="127"/>
-      <c r="I214" s="127"/>
-      <c r="J214" s="127"/>
-      <c r="K214" s="128"/>
+      <c r="E214" s="151"/>
+      <c r="F214" s="151"/>
+      <c r="G214" s="151"/>
+      <c r="H214" s="151"/>
+      <c r="I214" s="151"/>
+      <c r="J214" s="151"/>
+      <c r="K214" s="152"/>
     </row>
     <row r="215" spans="1:14">
       <c r="A215" s="12">
@@ -23014,16 +22914,16 @@
         <v>AD6</v>
       </c>
       <c r="C216" s="13"/>
-      <c r="D216" s="146" t="s">
+      <c r="D216" s="143" t="s">
         <v>373</v>
       </c>
-      <c r="E216" s="138"/>
-      <c r="F216" s="138"/>
-      <c r="G216" s="138"/>
-      <c r="H216" s="138"/>
-      <c r="I216" s="138"/>
-      <c r="J216" s="138"/>
-      <c r="K216" s="147"/>
+      <c r="E216" s="135"/>
+      <c r="F216" s="135"/>
+      <c r="G216" s="135"/>
+      <c r="H216" s="135"/>
+      <c r="I216" s="135"/>
+      <c r="J216" s="135"/>
+      <c r="K216" s="144"/>
     </row>
     <row r="217" spans="1:14">
       <c r="A217" s="12">
@@ -23035,14 +22935,14 @@
         <v>AD7</v>
       </c>
       <c r="C217" s="13"/>
-      <c r="D217" s="132"/>
-      <c r="E217" s="133"/>
-      <c r="F217" s="133"/>
-      <c r="G217" s="133"/>
-      <c r="H217" s="133"/>
-      <c r="I217" s="133"/>
-      <c r="J217" s="133"/>
-      <c r="K217" s="134"/>
+      <c r="D217" s="145"/>
+      <c r="E217" s="138"/>
+      <c r="F217" s="138"/>
+      <c r="G217" s="138"/>
+      <c r="H217" s="138"/>
+      <c r="I217" s="138"/>
+      <c r="J217" s="138"/>
+      <c r="K217" s="146"/>
     </row>
     <row r="218" spans="1:14">
       <c r="A218" s="12">
@@ -23054,16 +22954,16 @@
         <v>AD8</v>
       </c>
       <c r="C218" s="13"/>
-      <c r="D218" s="146" t="s">
+      <c r="D218" s="143" t="s">
         <v>374</v>
       </c>
-      <c r="E218" s="138"/>
-      <c r="F218" s="138"/>
-      <c r="G218" s="138"/>
-      <c r="H218" s="138"/>
-      <c r="I218" s="138"/>
-      <c r="J218" s="138"/>
-      <c r="K218" s="147"/>
+      <c r="E218" s="135"/>
+      <c r="F218" s="135"/>
+      <c r="G218" s="135"/>
+      <c r="H218" s="135"/>
+      <c r="I218" s="135"/>
+      <c r="J218" s="135"/>
+      <c r="K218" s="144"/>
     </row>
     <row r="219" spans="1:14">
       <c r="A219" s="12">
@@ -23075,14 +22975,14 @@
         <v>AD9</v>
       </c>
       <c r="C219" s="13"/>
-      <c r="D219" s="132"/>
-      <c r="E219" s="133"/>
-      <c r="F219" s="133"/>
-      <c r="G219" s="133"/>
-      <c r="H219" s="133"/>
-      <c r="I219" s="133"/>
-      <c r="J219" s="133"/>
-      <c r="K219" s="134"/>
+      <c r="D219" s="145"/>
+      <c r="E219" s="138"/>
+      <c r="F219" s="138"/>
+      <c r="G219" s="138"/>
+      <c r="H219" s="138"/>
+      <c r="I219" s="138"/>
+      <c r="J219" s="138"/>
+      <c r="K219" s="146"/>
     </row>
     <row r="220" spans="1:14">
       <c r="A220" s="12">
@@ -23094,16 +22994,16 @@
         <v>ADA</v>
       </c>
       <c r="C220" s="13"/>
-      <c r="D220" s="146" t="s">
+      <c r="D220" s="143" t="s">
         <v>375</v>
       </c>
-      <c r="E220" s="138"/>
-      <c r="F220" s="138"/>
-      <c r="G220" s="138"/>
-      <c r="H220" s="138"/>
-      <c r="I220" s="138"/>
-      <c r="J220" s="138"/>
-      <c r="K220" s="147"/>
+      <c r="E220" s="135"/>
+      <c r="F220" s="135"/>
+      <c r="G220" s="135"/>
+      <c r="H220" s="135"/>
+      <c r="I220" s="135"/>
+      <c r="J220" s="135"/>
+      <c r="K220" s="144"/>
     </row>
     <row r="221" spans="1:14">
       <c r="A221" s="12">
@@ -23115,14 +23015,14 @@
         <v>ADB</v>
       </c>
       <c r="C221" s="13"/>
-      <c r="D221" s="132"/>
-      <c r="E221" s="133"/>
-      <c r="F221" s="133"/>
-      <c r="G221" s="133"/>
-      <c r="H221" s="133"/>
-      <c r="I221" s="133"/>
-      <c r="J221" s="133"/>
-      <c r="K221" s="134"/>
+      <c r="D221" s="145"/>
+      <c r="E221" s="138"/>
+      <c r="F221" s="138"/>
+      <c r="G221" s="138"/>
+      <c r="H221" s="138"/>
+      <c r="I221" s="138"/>
+      <c r="J221" s="138"/>
+      <c r="K221" s="146"/>
     </row>
     <row r="222" spans="1:14">
       <c r="A222" s="12">
@@ -23134,16 +23034,16 @@
         <v>ADC</v>
       </c>
       <c r="C222" s="13"/>
-      <c r="D222" s="126" t="s">
+      <c r="D222" s="150" t="s">
         <v>376</v>
       </c>
-      <c r="E222" s="127"/>
-      <c r="F222" s="127"/>
-      <c r="G222" s="127"/>
-      <c r="H222" s="127"/>
-      <c r="I222" s="127"/>
-      <c r="J222" s="127"/>
-      <c r="K222" s="128"/>
+      <c r="E222" s="151"/>
+      <c r="F222" s="151"/>
+      <c r="G222" s="151"/>
+      <c r="H222" s="151"/>
+      <c r="I222" s="151"/>
+      <c r="J222" s="151"/>
+      <c r="K222" s="152"/>
     </row>
     <row r="223" spans="1:14">
       <c r="A223" s="12">
@@ -23174,16 +23074,16 @@
         <v>ADE</v>
       </c>
       <c r="C224" s="13"/>
-      <c r="D224" s="126" t="s">
+      <c r="D224" s="150" t="s">
         <v>377</v>
       </c>
-      <c r="E224" s="127"/>
-      <c r="F224" s="127"/>
-      <c r="G224" s="127"/>
-      <c r="H224" s="127"/>
-      <c r="I224" s="127"/>
-      <c r="J224" s="127"/>
-      <c r="K224" s="128"/>
+      <c r="E224" s="151"/>
+      <c r="F224" s="151"/>
+      <c r="G224" s="151"/>
+      <c r="H224" s="151"/>
+      <c r="I224" s="151"/>
+      <c r="J224" s="151"/>
+      <c r="K224" s="152"/>
     </row>
     <row r="225" spans="1:14" s="1" customFormat="1">
       <c r="A225" s="32">
@@ -23217,16 +23117,16 @@
         <v>AE0</v>
       </c>
       <c r="C226" s="39"/>
-      <c r="D226" s="152" t="s">
+      <c r="D226" s="153" t="s">
         <v>378</v>
       </c>
-      <c r="E226" s="153"/>
-      <c r="F226" s="153"/>
-      <c r="G226" s="153"/>
-      <c r="H226" s="153"/>
-      <c r="I226" s="153"/>
-      <c r="J226" s="153"/>
-      <c r="K226" s="154"/>
+      <c r="E226" s="154"/>
+      <c r="F226" s="154"/>
+      <c r="G226" s="154"/>
+      <c r="H226" s="154"/>
+      <c r="I226" s="154"/>
+      <c r="J226" s="154"/>
+      <c r="K226" s="155"/>
     </row>
     <row r="227" spans="1:14">
       <c r="A227" s="12">
@@ -23371,16 +23271,16 @@
         <v>AE8</v>
       </c>
       <c r="C234" s="13"/>
-      <c r="D234" s="150" t="s">
+      <c r="D234" s="147" t="s">
         <v>379</v>
       </c>
-      <c r="E234" s="136"/>
-      <c r="F234" s="136"/>
-      <c r="G234" s="136"/>
-      <c r="H234" s="136"/>
-      <c r="I234" s="136"/>
-      <c r="J234" s="136"/>
-      <c r="K234" s="151"/>
+      <c r="E234" s="148"/>
+      <c r="F234" s="148"/>
+      <c r="G234" s="148"/>
+      <c r="H234" s="148"/>
+      <c r="I234" s="148"/>
+      <c r="J234" s="148"/>
+      <c r="K234" s="149"/>
     </row>
     <row r="235" spans="1:14">
       <c r="A235" s="12">
@@ -23449,16 +23349,16 @@
         <v>AEC</v>
       </c>
       <c r="C238" s="13"/>
-      <c r="D238" s="142" t="s">
+      <c r="D238" s="134" t="s">
         <v>380</v>
       </c>
-      <c r="E238" s="138"/>
-      <c r="F238" s="138"/>
-      <c r="G238" s="138"/>
-      <c r="H238" s="138"/>
-      <c r="I238" s="138"/>
-      <c r="J238" s="138"/>
-      <c r="K238" s="139"/>
+      <c r="E238" s="135"/>
+      <c r="F238" s="135"/>
+      <c r="G238" s="135"/>
+      <c r="H238" s="135"/>
+      <c r="I238" s="135"/>
+      <c r="J238" s="135"/>
+      <c r="K238" s="136"/>
     </row>
     <row r="239" spans="1:14">
       <c r="A239" s="12">
@@ -23470,14 +23370,14 @@
         <v>AED</v>
       </c>
       <c r="C239" s="13"/>
-      <c r="D239" s="148"/>
-      <c r="E239" s="133"/>
-      <c r="F239" s="133"/>
-      <c r="G239" s="133"/>
-      <c r="H239" s="133"/>
-      <c r="I239" s="133"/>
-      <c r="J239" s="133"/>
-      <c r="K239" s="149"/>
+      <c r="D239" s="137"/>
+      <c r="E239" s="138"/>
+      <c r="F239" s="138"/>
+      <c r="G239" s="138"/>
+      <c r="H239" s="138"/>
+      <c r="I239" s="138"/>
+      <c r="J239" s="138"/>
+      <c r="K239" s="139"/>
     </row>
     <row r="240" spans="1:14">
       <c r="A240" s="12">
@@ -23489,16 +23389,16 @@
         <v>AEE</v>
       </c>
       <c r="C240" s="70"/>
-      <c r="D240" s="138" t="s">
+      <c r="D240" s="135" t="s">
         <v>381</v>
       </c>
-      <c r="E240" s="138"/>
-      <c r="F240" s="138"/>
-      <c r="G240" s="138"/>
-      <c r="H240" s="138"/>
-      <c r="I240" s="138"/>
-      <c r="J240" s="138"/>
-      <c r="K240" s="139"/>
+      <c r="E240" s="135"/>
+      <c r="F240" s="135"/>
+      <c r="G240" s="135"/>
+      <c r="H240" s="135"/>
+      <c r="I240" s="135"/>
+      <c r="J240" s="135"/>
+      <c r="K240" s="136"/>
     </row>
     <row r="241" spans="1:14" s="1" customFormat="1">
       <c r="A241" s="32">
@@ -23510,14 +23410,14 @@
         <v>AEF</v>
       </c>
       <c r="C241" s="34"/>
-      <c r="D241" s="140"/>
-      <c r="E241" s="140"/>
-      <c r="F241" s="140"/>
-      <c r="G241" s="140"/>
-      <c r="H241" s="140"/>
-      <c r="I241" s="140"/>
-      <c r="J241" s="140"/>
-      <c r="K241" s="141"/>
+      <c r="D241" s="161"/>
+      <c r="E241" s="161"/>
+      <c r="F241" s="161"/>
+      <c r="G241" s="161"/>
+      <c r="H241" s="161"/>
+      <c r="I241" s="161"/>
+      <c r="J241" s="161"/>
+      <c r="K241" s="162"/>
       <c r="L241" s="57"/>
       <c r="M241" s="58"/>
       <c r="N241" s="58"/>
@@ -23708,16 +23608,16 @@
         <v>AF8</v>
       </c>
       <c r="C250" s="13"/>
-      <c r="D250" s="135" t="s">
+      <c r="D250" s="159" t="s">
         <v>382</v>
       </c>
-      <c r="E250" s="136"/>
-      <c r="F250" s="136"/>
-      <c r="G250" s="136"/>
-      <c r="H250" s="136"/>
-      <c r="I250" s="136"/>
-      <c r="J250" s="136"/>
-      <c r="K250" s="137"/>
+      <c r="E250" s="148"/>
+      <c r="F250" s="148"/>
+      <c r="G250" s="148"/>
+      <c r="H250" s="148"/>
+      <c r="I250" s="148"/>
+      <c r="J250" s="148"/>
+      <c r="K250" s="160"/>
     </row>
     <row r="251" spans="1:14">
       <c r="A251" s="12">
@@ -24286,16 +24186,16 @@
         <v>B16</v>
       </c>
       <c r="C280" s="13"/>
-      <c r="D280" s="126" t="s">
+      <c r="D280" s="150" t="s">
         <v>383</v>
       </c>
-      <c r="E280" s="127"/>
-      <c r="F280" s="127"/>
-      <c r="G280" s="127"/>
-      <c r="H280" s="127"/>
-      <c r="I280" s="127"/>
-      <c r="J280" s="127"/>
-      <c r="K280" s="128"/>
+      <c r="E280" s="151"/>
+      <c r="F280" s="151"/>
+      <c r="G280" s="151"/>
+      <c r="H280" s="151"/>
+      <c r="I280" s="151"/>
+      <c r="J280" s="151"/>
+      <c r="K280" s="152"/>
     </row>
     <row r="281" spans="1:14">
       <c r="A281" s="12">
@@ -24402,16 +24302,16 @@
         <v>B1C</v>
       </c>
       <c r="C286" s="13"/>
-      <c r="D286" s="126" t="s">
+      <c r="D286" s="150" t="s">
         <v>384</v>
       </c>
-      <c r="E286" s="127"/>
-      <c r="F286" s="127"/>
-      <c r="G286" s="127"/>
-      <c r="H286" s="127"/>
-      <c r="I286" s="127"/>
-      <c r="J286" s="127"/>
-      <c r="K286" s="128"/>
+      <c r="E286" s="151"/>
+      <c r="F286" s="151"/>
+      <c r="G286" s="151"/>
+      <c r="H286" s="151"/>
+      <c r="I286" s="151"/>
+      <c r="J286" s="151"/>
+      <c r="K286" s="152"/>
     </row>
     <row r="287" spans="1:14">
       <c r="A287" s="12">
@@ -24599,16 +24499,16 @@
         <v>B26</v>
       </c>
       <c r="C296" s="13"/>
-      <c r="D296" s="126" t="s">
+      <c r="D296" s="150" t="s">
         <v>386</v>
       </c>
-      <c r="E296" s="127"/>
-      <c r="F296" s="127"/>
-      <c r="G296" s="127"/>
-      <c r="H296" s="127"/>
-      <c r="I296" s="127"/>
-      <c r="J296" s="127"/>
-      <c r="K296" s="128"/>
+      <c r="E296" s="151"/>
+      <c r="F296" s="151"/>
+      <c r="G296" s="151"/>
+      <c r="H296" s="151"/>
+      <c r="I296" s="151"/>
+      <c r="J296" s="151"/>
+      <c r="K296" s="152"/>
     </row>
     <row r="297" spans="1:14">
       <c r="A297" s="12">
@@ -24639,16 +24539,16 @@
         <v>B28</v>
       </c>
       <c r="C298" s="13"/>
-      <c r="D298" s="142" t="s">
+      <c r="D298" s="134" t="s">
         <v>387</v>
       </c>
-      <c r="E298" s="138"/>
-      <c r="F298" s="138"/>
-      <c r="G298" s="138"/>
-      <c r="H298" s="138"/>
-      <c r="I298" s="138"/>
-      <c r="J298" s="138"/>
-      <c r="K298" s="139"/>
+      <c r="E298" s="135"/>
+      <c r="F298" s="135"/>
+      <c r="G298" s="135"/>
+      <c r="H298" s="135"/>
+      <c r="I298" s="135"/>
+      <c r="J298" s="135"/>
+      <c r="K298" s="136"/>
     </row>
     <row r="299" spans="1:14">
       <c r="A299" s="12">
@@ -24660,14 +24560,14 @@
         <v>B29</v>
       </c>
       <c r="C299" s="13"/>
-      <c r="D299" s="148"/>
-      <c r="E299" s="133"/>
-      <c r="F299" s="133"/>
-      <c r="G299" s="133"/>
-      <c r="H299" s="133"/>
-      <c r="I299" s="133"/>
-      <c r="J299" s="133"/>
-      <c r="K299" s="149"/>
+      <c r="D299" s="137"/>
+      <c r="E299" s="138"/>
+      <c r="F299" s="138"/>
+      <c r="G299" s="138"/>
+      <c r="H299" s="138"/>
+      <c r="I299" s="138"/>
+      <c r="J299" s="138"/>
+      <c r="K299" s="139"/>
     </row>
     <row r="300" spans="1:14">
       <c r="A300" s="12">
@@ -24679,16 +24579,16 @@
         <v>B2A</v>
       </c>
       <c r="C300" s="13"/>
-      <c r="D300" s="142" t="s">
+      <c r="D300" s="134" t="s">
         <v>388</v>
       </c>
-      <c r="E300" s="138"/>
-      <c r="F300" s="138"/>
-      <c r="G300" s="138"/>
-      <c r="H300" s="138"/>
-      <c r="I300" s="138"/>
-      <c r="J300" s="138"/>
-      <c r="K300" s="139"/>
+      <c r="E300" s="135"/>
+      <c r="F300" s="135"/>
+      <c r="G300" s="135"/>
+      <c r="H300" s="135"/>
+      <c r="I300" s="135"/>
+      <c r="J300" s="135"/>
+      <c r="K300" s="136"/>
     </row>
     <row r="301" spans="1:14">
       <c r="A301" s="12">
@@ -24700,14 +24600,14 @@
         <v>B2B</v>
       </c>
       <c r="C301" s="13"/>
-      <c r="D301" s="148"/>
-      <c r="E301" s="133"/>
-      <c r="F301" s="133"/>
-      <c r="G301" s="133"/>
-      <c r="H301" s="133"/>
-      <c r="I301" s="133"/>
-      <c r="J301" s="133"/>
-      <c r="K301" s="149"/>
+      <c r="D301" s="137"/>
+      <c r="E301" s="138"/>
+      <c r="F301" s="138"/>
+      <c r="G301" s="138"/>
+      <c r="H301" s="138"/>
+      <c r="I301" s="138"/>
+      <c r="J301" s="138"/>
+      <c r="K301" s="139"/>
     </row>
     <row r="302" spans="1:14">
       <c r="A302" s="12">
@@ -24719,16 +24619,16 @@
         <v>B2C</v>
       </c>
       <c r="C302" s="13"/>
-      <c r="D302" s="142" t="s">
+      <c r="D302" s="134" t="s">
         <v>389</v>
       </c>
-      <c r="E302" s="138"/>
-      <c r="F302" s="138"/>
-      <c r="G302" s="138"/>
-      <c r="H302" s="138"/>
-      <c r="I302" s="138"/>
-      <c r="J302" s="138"/>
-      <c r="K302" s="139"/>
+      <c r="E302" s="135"/>
+      <c r="F302" s="135"/>
+      <c r="G302" s="135"/>
+      <c r="H302" s="135"/>
+      <c r="I302" s="135"/>
+      <c r="J302" s="135"/>
+      <c r="K302" s="136"/>
     </row>
     <row r="303" spans="1:14">
       <c r="A303" s="12">
@@ -24740,14 +24640,14 @@
         <v>B2D</v>
       </c>
       <c r="C303" s="13"/>
-      <c r="D303" s="148"/>
-      <c r="E303" s="133"/>
-      <c r="F303" s="133"/>
-      <c r="G303" s="133"/>
-      <c r="H303" s="133"/>
-      <c r="I303" s="133"/>
-      <c r="J303" s="133"/>
-      <c r="K303" s="149"/>
+      <c r="D303" s="137"/>
+      <c r="E303" s="138"/>
+      <c r="F303" s="138"/>
+      <c r="G303" s="138"/>
+      <c r="H303" s="138"/>
+      <c r="I303" s="138"/>
+      <c r="J303" s="138"/>
+      <c r="K303" s="139"/>
     </row>
     <row r="304" spans="1:14">
       <c r="A304" s="12">
@@ -24759,16 +24659,16 @@
         <v>B2E</v>
       </c>
       <c r="C304" s="13"/>
-      <c r="D304" s="142" t="s">
+      <c r="D304" s="134" t="s">
         <v>390</v>
       </c>
-      <c r="E304" s="138"/>
-      <c r="F304" s="138"/>
-      <c r="G304" s="138"/>
-      <c r="H304" s="138"/>
-      <c r="I304" s="138"/>
-      <c r="J304" s="138"/>
-      <c r="K304" s="139"/>
+      <c r="E304" s="135"/>
+      <c r="F304" s="135"/>
+      <c r="G304" s="135"/>
+      <c r="H304" s="135"/>
+      <c r="I304" s="135"/>
+      <c r="J304" s="135"/>
+      <c r="K304" s="136"/>
     </row>
     <row r="305" spans="1:14" s="1" customFormat="1">
       <c r="A305" s="32">
@@ -24780,14 +24680,14 @@
         <v>B2F</v>
       </c>
       <c r="C305" s="33"/>
-      <c r="D305" s="148"/>
-      <c r="E305" s="133"/>
-      <c r="F305" s="133"/>
-      <c r="G305" s="133"/>
-      <c r="H305" s="133"/>
-      <c r="I305" s="133"/>
-      <c r="J305" s="133"/>
-      <c r="K305" s="149"/>
+      <c r="D305" s="137"/>
+      <c r="E305" s="138"/>
+      <c r="F305" s="138"/>
+      <c r="G305" s="138"/>
+      <c r="H305" s="138"/>
+      <c r="I305" s="138"/>
+      <c r="J305" s="138"/>
+      <c r="K305" s="139"/>
       <c r="L305" s="57"/>
       <c r="M305" s="58"/>
       <c r="N305" s="58"/>
@@ -24802,16 +24702,16 @@
         <v>B30</v>
       </c>
       <c r="C306" s="39"/>
-      <c r="D306" s="142" t="s">
+      <c r="D306" s="134" t="s">
         <v>391</v>
       </c>
-      <c r="E306" s="138"/>
-      <c r="F306" s="138"/>
-      <c r="G306" s="138"/>
-      <c r="H306" s="138"/>
-      <c r="I306" s="138"/>
-      <c r="J306" s="138"/>
-      <c r="K306" s="139"/>
+      <c r="E306" s="135"/>
+      <c r="F306" s="135"/>
+      <c r="G306" s="135"/>
+      <c r="H306" s="135"/>
+      <c r="I306" s="135"/>
+      <c r="J306" s="135"/>
+      <c r="K306" s="136"/>
     </row>
     <row r="307" spans="1:14">
       <c r="A307" s="12">
@@ -24823,14 +24723,14 @@
         <v>B31</v>
       </c>
       <c r="C307" s="13"/>
-      <c r="D307" s="148"/>
-      <c r="E307" s="133"/>
-      <c r="F307" s="133"/>
-      <c r="G307" s="133"/>
-      <c r="H307" s="133"/>
-      <c r="I307" s="133"/>
-      <c r="J307" s="133"/>
-      <c r="K307" s="149"/>
+      <c r="D307" s="137"/>
+      <c r="E307" s="138"/>
+      <c r="F307" s="138"/>
+      <c r="G307" s="138"/>
+      <c r="H307" s="138"/>
+      <c r="I307" s="138"/>
+      <c r="J307" s="138"/>
+      <c r="K307" s="139"/>
     </row>
     <row r="308" spans="1:14">
       <c r="A308" s="12">
@@ -24842,16 +24742,16 @@
         <v>B32</v>
       </c>
       <c r="C308" s="13"/>
-      <c r="D308" s="142" t="s">
+      <c r="D308" s="134" t="s">
         <v>392</v>
       </c>
-      <c r="E308" s="138"/>
-      <c r="F308" s="138"/>
-      <c r="G308" s="138"/>
-      <c r="H308" s="138"/>
-      <c r="I308" s="138"/>
-      <c r="J308" s="138"/>
-      <c r="K308" s="139"/>
+      <c r="E308" s="135"/>
+      <c r="F308" s="135"/>
+      <c r="G308" s="135"/>
+      <c r="H308" s="135"/>
+      <c r="I308" s="135"/>
+      <c r="J308" s="135"/>
+      <c r="K308" s="136"/>
     </row>
     <row r="309" spans="1:14">
       <c r="A309" s="12">
@@ -24863,14 +24763,14 @@
         <v>B33</v>
       </c>
       <c r="C309" s="13"/>
-      <c r="D309" s="148"/>
-      <c r="E309" s="133"/>
-      <c r="F309" s="133"/>
-      <c r="G309" s="133"/>
-      <c r="H309" s="133"/>
-      <c r="I309" s="133"/>
-      <c r="J309" s="133"/>
-      <c r="K309" s="149"/>
+      <c r="D309" s="137"/>
+      <c r="E309" s="138"/>
+      <c r="F309" s="138"/>
+      <c r="G309" s="138"/>
+      <c r="H309" s="138"/>
+      <c r="I309" s="138"/>
+      <c r="J309" s="138"/>
+      <c r="K309" s="139"/>
     </row>
     <row r="310" spans="1:14">
       <c r="A310" s="12">
@@ -28750,12 +28650,29 @@
     </row>
   </sheetData>
   <mergeCells count="45">
-    <mergeCell ref="D308:K309"/>
-    <mergeCell ref="D298:K299"/>
-    <mergeCell ref="D300:K301"/>
-    <mergeCell ref="D302:K303"/>
-    <mergeCell ref="D304:K305"/>
-    <mergeCell ref="D306:K307"/>
+    <mergeCell ref="D178:K178"/>
+    <mergeCell ref="D182:K182"/>
+    <mergeCell ref="D183:K183"/>
+    <mergeCell ref="D184:K184"/>
+    <mergeCell ref="D185:K185"/>
+    <mergeCell ref="D186:K186"/>
+    <mergeCell ref="D187:K187"/>
+    <mergeCell ref="D188:K188"/>
+    <mergeCell ref="D189:K189"/>
+    <mergeCell ref="D190:K190"/>
+    <mergeCell ref="D191:K191"/>
+    <mergeCell ref="D192:K192"/>
+    <mergeCell ref="D193:K193"/>
+    <mergeCell ref="D194:K194"/>
+    <mergeCell ref="D195:K195"/>
+    <mergeCell ref="D208:K208"/>
+    <mergeCell ref="D210:K210"/>
+    <mergeCell ref="D214:K214"/>
+    <mergeCell ref="D196:K196"/>
+    <mergeCell ref="D197:K197"/>
+    <mergeCell ref="D198:K198"/>
+    <mergeCell ref="D200:K200"/>
+    <mergeCell ref="D202:K202"/>
     <mergeCell ref="D280:K280"/>
     <mergeCell ref="D286:K286"/>
     <mergeCell ref="D296:K296"/>
@@ -28772,29 +28689,12 @@
     <mergeCell ref="D250:K250"/>
     <mergeCell ref="D204:K204"/>
     <mergeCell ref="D206:K206"/>
-    <mergeCell ref="D208:K208"/>
-    <mergeCell ref="D210:K210"/>
-    <mergeCell ref="D214:K214"/>
-    <mergeCell ref="D196:K196"/>
-    <mergeCell ref="D197:K197"/>
-    <mergeCell ref="D198:K198"/>
-    <mergeCell ref="D200:K200"/>
-    <mergeCell ref="D202:K202"/>
-    <mergeCell ref="D191:K191"/>
-    <mergeCell ref="D192:K192"/>
-    <mergeCell ref="D193:K193"/>
-    <mergeCell ref="D194:K194"/>
-    <mergeCell ref="D195:K195"/>
-    <mergeCell ref="D186:K186"/>
-    <mergeCell ref="D187:K187"/>
-    <mergeCell ref="D188:K188"/>
-    <mergeCell ref="D189:K189"/>
-    <mergeCell ref="D190:K190"/>
-    <mergeCell ref="D178:K178"/>
-    <mergeCell ref="D182:K182"/>
-    <mergeCell ref="D183:K183"/>
-    <mergeCell ref="D184:K184"/>
-    <mergeCell ref="D185:K185"/>
+    <mergeCell ref="D308:K309"/>
+    <mergeCell ref="D298:K299"/>
+    <mergeCell ref="D300:K301"/>
+    <mergeCell ref="D302:K303"/>
+    <mergeCell ref="D304:K305"/>
+    <mergeCell ref="D306:K307"/>
   </mergeCells>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="53" fitToHeight="0" orientation="landscape"/>

</xml_diff>

<commit_message>
Z3 mode basically works
HP and DEF jewels still bugged
</commit_message>
<xml_diff>
--- a/data/Switches.xlsx
+++ b/data/Switches.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\IoGR\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bravo Properties\Documents\Gaming\Illusion of Gaia Randomizer\IoGR\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00822147-646F-4F84-8137-16DF5A71999E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A595F55B-44D0-4CB8-BEE1-AFA994D3511F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26490" yWindow="1980" windowWidth="19140" windowHeight="12120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1635" yWindow="1305" windowWidth="24270" windowHeight="10455" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Switches_New" sheetId="4" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="816" uniqueCount="447">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="816" uniqueCount="448">
   <si>
     <t>ID</t>
   </si>
@@ -1372,6 +1372,9 @@
   </si>
   <si>
     <t>Used in credits</t>
+  </si>
+  <si>
+    <t>PIECE OF HEART</t>
   </si>
 </sst>
 </file>
@@ -2151,7 +2154,7 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="173">
+  <cellXfs count="177">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -2539,13 +2542,40 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="28" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="24" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="33" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="51" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="34" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="32" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="39" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="3" applyBorder="1" applyAlignment="1">
@@ -2557,28 +2587,31 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="28" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="33" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="42" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="27" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="25" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="41" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="28" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
@@ -2596,13 +2629,16 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="27" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="25" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="41" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2626,43 +2662,22 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="33" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="42" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="52" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="28" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="24" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="33" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="51" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="34" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="32" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="39" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3012,8 +3027,8 @@
   <dimension ref="A1:O513"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H30" sqref="H30"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -3086,16 +3101,16 @@
         <f>8*A2&amp;"-"&amp;(8*A2+7)</f>
         <v>0-7</v>
       </c>
-      <c r="D2" s="141" t="s">
+      <c r="D2" s="152" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="137"/>
-      <c r="F2" s="137"/>
-      <c r="G2" s="137"/>
-      <c r="H2" s="137"/>
-      <c r="I2" s="137"/>
-      <c r="J2" s="137"/>
-      <c r="K2" s="138"/>
+      <c r="E2" s="153"/>
+      <c r="F2" s="153"/>
+      <c r="G2" s="153"/>
+      <c r="H2" s="153"/>
+      <c r="I2" s="153"/>
+      <c r="J2" s="153"/>
+      <c r="K2" s="154"/>
       <c r="L2" s="119" t="s">
         <v>7</v>
       </c>
@@ -3113,14 +3128,14 @@
         <f t="shared" ref="C3:C33" si="1">8*A3&amp;"-"&amp;(8*A3+7)</f>
         <v>8-15</v>
       </c>
-      <c r="D3" s="145"/>
-      <c r="E3" s="146"/>
-      <c r="F3" s="146"/>
-      <c r="G3" s="146"/>
-      <c r="H3" s="146"/>
-      <c r="I3" s="146"/>
-      <c r="J3" s="146"/>
-      <c r="K3" s="147"/>
+      <c r="D3" s="155"/>
+      <c r="E3" s="156"/>
+      <c r="F3" s="156"/>
+      <c r="G3" s="156"/>
+      <c r="H3" s="156"/>
+      <c r="I3" s="156"/>
+      <c r="J3" s="156"/>
+      <c r="K3" s="157"/>
       <c r="L3" s="119" t="s">
         <v>8</v>
       </c>
@@ -4286,14 +4301,14 @@
         <f t="shared" si="0"/>
         <v>A1E</v>
       </c>
-      <c r="C32" s="13" t="str">
+      <c r="C32" s="132" t="str">
         <f t="shared" si="1"/>
         <v>240-247</v>
       </c>
-      <c r="D32" s="17" t="s">
-        <v>223</v>
-      </c>
-      <c r="E32" s="21" t="s">
+      <c r="D32" s="176" t="s">
+        <v>447</v>
+      </c>
+      <c r="E32" s="131" t="s">
         <v>224</v>
       </c>
       <c r="F32" s="90" t="s">
@@ -4331,7 +4346,7 @@
         <f t="shared" si="1"/>
         <v>248-255</v>
       </c>
-      <c r="D33" s="43"/>
+      <c r="D33" s="175"/>
       <c r="E33" s="44" t="s">
         <v>231</v>
       </c>
@@ -5645,16 +5660,16 @@
         <v>A49</v>
       </c>
       <c r="C75" s="13"/>
-      <c r="D75" s="164" t="s">
+      <c r="D75" s="133" t="s">
         <v>436</v>
       </c>
-      <c r="E75" s="165"/>
-      <c r="F75" s="165"/>
-      <c r="G75" s="165"/>
-      <c r="H75" s="165"/>
-      <c r="I75" s="165"/>
-      <c r="J75" s="165"/>
-      <c r="K75" s="166"/>
+      <c r="E75" s="134"/>
+      <c r="F75" s="134"/>
+      <c r="G75" s="134"/>
+      <c r="H75" s="134"/>
+      <c r="I75" s="134"/>
+      <c r="J75" s="134"/>
+      <c r="K75" s="135"/>
     </row>
     <row r="76" spans="1:14">
       <c r="A76" s="12">
@@ -5666,16 +5681,16 @@
         <v>A4A</v>
       </c>
       <c r="C76" s="13"/>
-      <c r="D76" s="164" t="s">
+      <c r="D76" s="133" t="s">
         <v>437</v>
       </c>
-      <c r="E76" s="165"/>
-      <c r="F76" s="165"/>
-      <c r="G76" s="165"/>
-      <c r="H76" s="165"/>
-      <c r="I76" s="165"/>
-      <c r="J76" s="165"/>
-      <c r="K76" s="166"/>
+      <c r="E76" s="134"/>
+      <c r="F76" s="134"/>
+      <c r="G76" s="134"/>
+      <c r="H76" s="134"/>
+      <c r="I76" s="134"/>
+      <c r="J76" s="134"/>
+      <c r="K76" s="135"/>
     </row>
     <row r="77" spans="1:14">
       <c r="A77" s="12">
@@ -5687,16 +5702,16 @@
         <v>A4B</v>
       </c>
       <c r="C77" s="13"/>
-      <c r="D77" s="164" t="s">
+      <c r="D77" s="133" t="s">
         <v>438</v>
       </c>
-      <c r="E77" s="165"/>
-      <c r="F77" s="165"/>
-      <c r="G77" s="165"/>
-      <c r="H77" s="165"/>
-      <c r="I77" s="165"/>
-      <c r="J77" s="165"/>
-      <c r="K77" s="166"/>
+      <c r="E77" s="134"/>
+      <c r="F77" s="134"/>
+      <c r="G77" s="134"/>
+      <c r="H77" s="134"/>
+      <c r="I77" s="134"/>
+      <c r="J77" s="134"/>
+      <c r="K77" s="135"/>
     </row>
     <row r="78" spans="1:14">
       <c r="A78" s="12">
@@ -5708,16 +5723,16 @@
         <v>A4C</v>
       </c>
       <c r="C78" s="13"/>
-      <c r="D78" s="164" t="s">
+      <c r="D78" s="133" t="s">
         <v>439</v>
       </c>
-      <c r="E78" s="165"/>
-      <c r="F78" s="165"/>
-      <c r="G78" s="165"/>
-      <c r="H78" s="165"/>
-      <c r="I78" s="165"/>
-      <c r="J78" s="165"/>
-      <c r="K78" s="166"/>
+      <c r="E78" s="134"/>
+      <c r="F78" s="134"/>
+      <c r="G78" s="134"/>
+      <c r="H78" s="134"/>
+      <c r="I78" s="134"/>
+      <c r="J78" s="134"/>
+      <c r="K78" s="135"/>
     </row>
     <row r="79" spans="1:14">
       <c r="A79" s="12">
@@ -5729,16 +5744,16 @@
         <v>A4D</v>
       </c>
       <c r="C79" s="13"/>
-      <c r="D79" s="164" t="s">
+      <c r="D79" s="133" t="s">
         <v>440</v>
       </c>
-      <c r="E79" s="165"/>
-      <c r="F79" s="165"/>
-      <c r="G79" s="165"/>
-      <c r="H79" s="165"/>
-      <c r="I79" s="165"/>
-      <c r="J79" s="165"/>
-      <c r="K79" s="166"/>
+      <c r="E79" s="134"/>
+      <c r="F79" s="134"/>
+      <c r="G79" s="134"/>
+      <c r="H79" s="134"/>
+      <c r="I79" s="134"/>
+      <c r="J79" s="134"/>
+      <c r="K79" s="135"/>
     </row>
     <row r="80" spans="1:14">
       <c r="A80" s="12">
@@ -5750,16 +5765,16 @@
         <v>A4E</v>
       </c>
       <c r="C80" s="13"/>
-      <c r="D80" s="164" t="s">
+      <c r="D80" s="133" t="s">
         <v>441</v>
       </c>
-      <c r="E80" s="165"/>
-      <c r="F80" s="165"/>
-      <c r="G80" s="165"/>
-      <c r="H80" s="165"/>
-      <c r="I80" s="165"/>
-      <c r="J80" s="165"/>
-      <c r="K80" s="166"/>
+      <c r="E80" s="134"/>
+      <c r="F80" s="134"/>
+      <c r="G80" s="134"/>
+      <c r="H80" s="134"/>
+      <c r="I80" s="134"/>
+      <c r="J80" s="134"/>
+      <c r="K80" s="135"/>
     </row>
     <row r="81" spans="1:14" s="1" customFormat="1">
       <c r="A81" s="32">
@@ -5771,16 +5786,16 @@
         <v>A4F</v>
       </c>
       <c r="C81" s="33"/>
-      <c r="D81" s="167" t="s">
+      <c r="D81" s="136" t="s">
         <v>442</v>
       </c>
-      <c r="E81" s="168"/>
-      <c r="F81" s="168"/>
-      <c r="G81" s="168"/>
-      <c r="H81" s="168"/>
-      <c r="I81" s="168"/>
-      <c r="J81" s="168"/>
-      <c r="K81" s="169"/>
+      <c r="E81" s="137"/>
+      <c r="F81" s="137"/>
+      <c r="G81" s="137"/>
+      <c r="H81" s="137"/>
+      <c r="I81" s="137"/>
+      <c r="J81" s="137"/>
+      <c r="K81" s="138"/>
       <c r="L81" s="57"/>
       <c r="M81" s="58"/>
       <c r="N81" s="58"/>
@@ -5975,16 +5990,16 @@
         <v>A58</v>
       </c>
       <c r="C90" s="13"/>
-      <c r="D90" s="164" t="s">
+      <c r="D90" s="133" t="s">
         <v>431</v>
       </c>
-      <c r="E90" s="165"/>
-      <c r="F90" s="165"/>
-      <c r="G90" s="165"/>
-      <c r="H90" s="165"/>
-      <c r="I90" s="165"/>
-      <c r="J90" s="165"/>
-      <c r="K90" s="166"/>
+      <c r="E90" s="134"/>
+      <c r="F90" s="134"/>
+      <c r="G90" s="134"/>
+      <c r="H90" s="134"/>
+      <c r="I90" s="134"/>
+      <c r="J90" s="134"/>
+      <c r="K90" s="135"/>
     </row>
     <row r="91" spans="1:14">
       <c r="A91" s="12">
@@ -5996,16 +6011,16 @@
         <v>A59</v>
       </c>
       <c r="C91" s="13"/>
-      <c r="D91" s="164" t="s">
+      <c r="D91" s="133" t="s">
         <v>432</v>
       </c>
-      <c r="E91" s="165"/>
-      <c r="F91" s="165"/>
-      <c r="G91" s="165"/>
-      <c r="H91" s="165"/>
-      <c r="I91" s="165"/>
-      <c r="J91" s="165"/>
-      <c r="K91" s="166"/>
+      <c r="E91" s="134"/>
+      <c r="F91" s="134"/>
+      <c r="G91" s="134"/>
+      <c r="H91" s="134"/>
+      <c r="I91" s="134"/>
+      <c r="J91" s="134"/>
+      <c r="K91" s="135"/>
     </row>
     <row r="92" spans="1:14">
       <c r="A92" s="12">
@@ -6017,16 +6032,16 @@
         <v>A5A</v>
       </c>
       <c r="C92" s="13"/>
-      <c r="D92" s="164" t="s">
+      <c r="D92" s="133" t="s">
         <v>433</v>
       </c>
-      <c r="E92" s="165"/>
-      <c r="F92" s="165"/>
-      <c r="G92" s="165"/>
-      <c r="H92" s="165"/>
-      <c r="I92" s="165"/>
-      <c r="J92" s="165"/>
-      <c r="K92" s="166"/>
+      <c r="E92" s="134"/>
+      <c r="F92" s="134"/>
+      <c r="G92" s="134"/>
+      <c r="H92" s="134"/>
+      <c r="I92" s="134"/>
+      <c r="J92" s="134"/>
+      <c r="K92" s="135"/>
     </row>
     <row r="93" spans="1:14">
       <c r="A93" s="12">
@@ -6038,16 +6053,16 @@
         <v>A5B</v>
       </c>
       <c r="C93" s="13"/>
-      <c r="D93" s="170" t="s">
+      <c r="D93" s="140" t="s">
         <v>434</v>
       </c>
-      <c r="E93" s="171"/>
-      <c r="F93" s="171"/>
-      <c r="G93" s="171"/>
-      <c r="H93" s="171"/>
-      <c r="I93" s="171"/>
-      <c r="J93" s="171"/>
-      <c r="K93" s="172"/>
+      <c r="E93" s="141"/>
+      <c r="F93" s="141"/>
+      <c r="G93" s="141"/>
+      <c r="H93" s="141"/>
+      <c r="I93" s="141"/>
+      <c r="J93" s="141"/>
+      <c r="K93" s="142"/>
     </row>
     <row r="94" spans="1:14">
       <c r="A94" s="12">
@@ -6059,16 +6074,16 @@
         <v>A5C</v>
       </c>
       <c r="C94" s="13"/>
-      <c r="D94" s="170" t="s">
+      <c r="D94" s="140" t="s">
         <v>435</v>
       </c>
-      <c r="E94" s="171"/>
-      <c r="F94" s="171"/>
-      <c r="G94" s="171"/>
-      <c r="H94" s="171"/>
-      <c r="I94" s="171"/>
-      <c r="J94" s="171"/>
-      <c r="K94" s="172"/>
+      <c r="E94" s="141"/>
+      <c r="F94" s="141"/>
+      <c r="G94" s="141"/>
+      <c r="H94" s="141"/>
+      <c r="I94" s="141"/>
+      <c r="J94" s="141"/>
+      <c r="K94" s="142"/>
     </row>
     <row r="95" spans="1:14">
       <c r="A95" s="12">
@@ -6080,16 +6095,16 @@
         <v>A5D</v>
       </c>
       <c r="C95" s="13"/>
-      <c r="D95" s="170" t="s">
+      <c r="D95" s="140" t="s">
         <v>430</v>
       </c>
-      <c r="E95" s="171"/>
-      <c r="F95" s="171"/>
-      <c r="G95" s="171"/>
-      <c r="H95" s="171"/>
-      <c r="I95" s="171"/>
-      <c r="J95" s="171"/>
-      <c r="K95" s="172"/>
+      <c r="E95" s="141"/>
+      <c r="F95" s="141"/>
+      <c r="G95" s="141"/>
+      <c r="H95" s="141"/>
+      <c r="I95" s="141"/>
+      <c r="J95" s="141"/>
+      <c r="K95" s="142"/>
     </row>
     <row r="96" spans="1:14">
       <c r="A96" s="12">
@@ -6101,16 +6116,16 @@
         <v>A5E</v>
       </c>
       <c r="C96" s="13"/>
-      <c r="D96" s="164" t="s">
+      <c r="D96" s="133" t="s">
         <v>429</v>
       </c>
-      <c r="E96" s="165"/>
-      <c r="F96" s="165"/>
-      <c r="G96" s="165"/>
-      <c r="H96" s="165"/>
-      <c r="I96" s="165"/>
-      <c r="J96" s="165"/>
-      <c r="K96" s="166"/>
+      <c r="E96" s="134"/>
+      <c r="F96" s="134"/>
+      <c r="G96" s="134"/>
+      <c r="H96" s="134"/>
+      <c r="I96" s="134"/>
+      <c r="J96" s="134"/>
+      <c r="K96" s="135"/>
     </row>
     <row r="97" spans="1:14" s="1" customFormat="1">
       <c r="A97" s="32">
@@ -9049,16 +9064,16 @@
         <v>AA6</v>
       </c>
       <c r="C168" s="13"/>
-      <c r="D168" s="163" t="s">
+      <c r="D168" s="139" t="s">
         <v>348</v>
       </c>
-      <c r="E168" s="163"/>
-      <c r="F168" s="163"/>
-      <c r="G168" s="163"/>
-      <c r="H168" s="163"/>
-      <c r="I168" s="163"/>
-      <c r="J168" s="163"/>
-      <c r="K168" s="163"/>
+      <c r="E168" s="139"/>
+      <c r="F168" s="139"/>
+      <c r="G168" s="139"/>
+      <c r="H168" s="139"/>
+      <c r="I168" s="139"/>
+      <c r="J168" s="139"/>
+      <c r="K168" s="139"/>
     </row>
     <row r="169" spans="1:14">
       <c r="A169" s="12">
@@ -9165,16 +9180,16 @@
         <v>AAC</v>
       </c>
       <c r="C174" s="13"/>
-      <c r="D174" s="163" t="s">
+      <c r="D174" s="139" t="s">
         <v>349</v>
       </c>
-      <c r="E174" s="163"/>
-      <c r="F174" s="163"/>
-      <c r="G174" s="163"/>
-      <c r="H174" s="163"/>
-      <c r="I174" s="163"/>
-      <c r="J174" s="163"/>
-      <c r="K174" s="163"/>
+      <c r="E174" s="139"/>
+      <c r="F174" s="139"/>
+      <c r="G174" s="139"/>
+      <c r="H174" s="139"/>
+      <c r="I174" s="139"/>
+      <c r="J174" s="139"/>
+      <c r="K174" s="139"/>
     </row>
     <row r="175" spans="1:14">
       <c r="A175" s="12">
@@ -9186,16 +9201,16 @@
         <v>AAD</v>
       </c>
       <c r="C175" s="13"/>
-      <c r="D175" s="163" t="s">
+      <c r="D175" s="139" t="s">
         <v>349</v>
       </c>
-      <c r="E175" s="163"/>
-      <c r="F175" s="163"/>
-      <c r="G175" s="163"/>
-      <c r="H175" s="163"/>
-      <c r="I175" s="163"/>
-      <c r="J175" s="163"/>
-      <c r="K175" s="163"/>
+      <c r="E175" s="139"/>
+      <c r="F175" s="139"/>
+      <c r="G175" s="139"/>
+      <c r="H175" s="139"/>
+      <c r="I175" s="139"/>
+      <c r="J175" s="139"/>
+      <c r="K175" s="139"/>
     </row>
     <row r="176" spans="1:14">
       <c r="A176" s="12">
@@ -9248,16 +9263,16 @@
         <v>AB0</v>
       </c>
       <c r="C178" s="39"/>
-      <c r="D178" s="163" t="s">
+      <c r="D178" s="139" t="s">
         <v>350</v>
       </c>
-      <c r="E178" s="163"/>
-      <c r="F178" s="163"/>
-      <c r="G178" s="163"/>
-      <c r="H178" s="163"/>
-      <c r="I178" s="163"/>
-      <c r="J178" s="163"/>
-      <c r="K178" s="163"/>
+      <c r="E178" s="139"/>
+      <c r="F178" s="139"/>
+      <c r="G178" s="139"/>
+      <c r="H178" s="139"/>
+      <c r="I178" s="139"/>
+      <c r="J178" s="139"/>
+      <c r="K178" s="139"/>
     </row>
     <row r="179" spans="1:14">
       <c r="A179" s="12">
@@ -9326,16 +9341,16 @@
         <v>AB4</v>
       </c>
       <c r="C182" s="13"/>
-      <c r="D182" s="134" t="s">
+      <c r="D182" s="143" t="s">
         <v>351</v>
       </c>
-      <c r="E182" s="135"/>
-      <c r="F182" s="135"/>
-      <c r="G182" s="135"/>
-      <c r="H182" s="135"/>
-      <c r="I182" s="135"/>
-      <c r="J182" s="135"/>
-      <c r="K182" s="136"/>
+      <c r="E182" s="144"/>
+      <c r="F182" s="144"/>
+      <c r="G182" s="144"/>
+      <c r="H182" s="144"/>
+      <c r="I182" s="144"/>
+      <c r="J182" s="144"/>
+      <c r="K182" s="145"/>
     </row>
     <row r="183" spans="1:14">
       <c r="A183" s="12">
@@ -9347,16 +9362,16 @@
         <v>AB5</v>
       </c>
       <c r="C183" s="13"/>
-      <c r="D183" s="134" t="s">
+      <c r="D183" s="143" t="s">
         <v>352</v>
       </c>
-      <c r="E183" s="135"/>
-      <c r="F183" s="135"/>
-      <c r="G183" s="135"/>
-      <c r="H183" s="135"/>
-      <c r="I183" s="135"/>
-      <c r="J183" s="135"/>
-      <c r="K183" s="136"/>
+      <c r="E183" s="144"/>
+      <c r="F183" s="144"/>
+      <c r="G183" s="144"/>
+      <c r="H183" s="144"/>
+      <c r="I183" s="144"/>
+      <c r="J183" s="144"/>
+      <c r="K183" s="145"/>
     </row>
     <row r="184" spans="1:14">
       <c r="A184" s="12">
@@ -9368,16 +9383,16 @@
         <v>AB6</v>
       </c>
       <c r="C184" s="13"/>
-      <c r="D184" s="134" t="s">
+      <c r="D184" s="143" t="s">
         <v>353</v>
       </c>
-      <c r="E184" s="135"/>
-      <c r="F184" s="135"/>
-      <c r="G184" s="135"/>
-      <c r="H184" s="135"/>
-      <c r="I184" s="135"/>
-      <c r="J184" s="135"/>
-      <c r="K184" s="136"/>
+      <c r="E184" s="144"/>
+      <c r="F184" s="144"/>
+      <c r="G184" s="144"/>
+      <c r="H184" s="144"/>
+      <c r="I184" s="144"/>
+      <c r="J184" s="144"/>
+      <c r="K184" s="145"/>
     </row>
     <row r="185" spans="1:14">
       <c r="A185" s="12">
@@ -9389,16 +9404,16 @@
         <v>AB7</v>
       </c>
       <c r="C185" s="13"/>
-      <c r="D185" s="134" t="s">
+      <c r="D185" s="143" t="s">
         <v>354</v>
       </c>
-      <c r="E185" s="135"/>
-      <c r="F185" s="135"/>
-      <c r="G185" s="135"/>
-      <c r="H185" s="135"/>
-      <c r="I185" s="135"/>
-      <c r="J185" s="135"/>
-      <c r="K185" s="136"/>
+      <c r="E185" s="144"/>
+      <c r="F185" s="144"/>
+      <c r="G185" s="144"/>
+      <c r="H185" s="144"/>
+      <c r="I185" s="144"/>
+      <c r="J185" s="144"/>
+      <c r="K185" s="145"/>
     </row>
     <row r="186" spans="1:14">
       <c r="A186" s="12">
@@ -9410,16 +9425,16 @@
         <v>AB8</v>
       </c>
       <c r="C186" s="13"/>
-      <c r="D186" s="134" t="s">
+      <c r="D186" s="143" t="s">
         <v>355</v>
       </c>
-      <c r="E186" s="135"/>
-      <c r="F186" s="135"/>
-      <c r="G186" s="135"/>
-      <c r="H186" s="135"/>
-      <c r="I186" s="135"/>
-      <c r="J186" s="135"/>
-      <c r="K186" s="136"/>
+      <c r="E186" s="144"/>
+      <c r="F186" s="144"/>
+      <c r="G186" s="144"/>
+      <c r="H186" s="144"/>
+      <c r="I186" s="144"/>
+      <c r="J186" s="144"/>
+      <c r="K186" s="145"/>
     </row>
     <row r="187" spans="1:14">
       <c r="A187" s="12">
@@ -9431,16 +9446,16 @@
         <v>AB9</v>
       </c>
       <c r="C187" s="13"/>
-      <c r="D187" s="134" t="s">
+      <c r="D187" s="143" t="s">
         <v>356</v>
       </c>
-      <c r="E187" s="135"/>
-      <c r="F187" s="135"/>
-      <c r="G187" s="135"/>
-      <c r="H187" s="135"/>
-      <c r="I187" s="135"/>
-      <c r="J187" s="135"/>
-      <c r="K187" s="136"/>
+      <c r="E187" s="144"/>
+      <c r="F187" s="144"/>
+      <c r="G187" s="144"/>
+      <c r="H187" s="144"/>
+      <c r="I187" s="144"/>
+      <c r="J187" s="144"/>
+      <c r="K187" s="145"/>
     </row>
     <row r="188" spans="1:14">
       <c r="A188" s="12">
@@ -9452,16 +9467,16 @@
         <v>ABA</v>
       </c>
       <c r="C188" s="13"/>
-      <c r="D188" s="134" t="s">
+      <c r="D188" s="143" t="s">
         <v>357</v>
       </c>
-      <c r="E188" s="135"/>
-      <c r="F188" s="135"/>
-      <c r="G188" s="135"/>
-      <c r="H188" s="135"/>
-      <c r="I188" s="135"/>
-      <c r="J188" s="135"/>
-      <c r="K188" s="136"/>
+      <c r="E188" s="144"/>
+      <c r="F188" s="144"/>
+      <c r="G188" s="144"/>
+      <c r="H188" s="144"/>
+      <c r="I188" s="144"/>
+      <c r="J188" s="144"/>
+      <c r="K188" s="145"/>
     </row>
     <row r="189" spans="1:14">
       <c r="A189" s="12">
@@ -9473,16 +9488,16 @@
         <v>ABB</v>
       </c>
       <c r="C189" s="13"/>
-      <c r="D189" s="134" t="s">
+      <c r="D189" s="143" t="s">
         <v>358</v>
       </c>
-      <c r="E189" s="135"/>
-      <c r="F189" s="135"/>
-      <c r="G189" s="135"/>
-      <c r="H189" s="135"/>
-      <c r="I189" s="135"/>
-      <c r="J189" s="135"/>
-      <c r="K189" s="136"/>
+      <c r="E189" s="144"/>
+      <c r="F189" s="144"/>
+      <c r="G189" s="144"/>
+      <c r="H189" s="144"/>
+      <c r="I189" s="144"/>
+      <c r="J189" s="144"/>
+      <c r="K189" s="145"/>
     </row>
     <row r="190" spans="1:14">
       <c r="A190" s="12">
@@ -9494,16 +9509,16 @@
         <v>ABC</v>
       </c>
       <c r="C190" s="13"/>
-      <c r="D190" s="134" t="s">
+      <c r="D190" s="143" t="s">
         <v>359</v>
       </c>
-      <c r="E190" s="135"/>
-      <c r="F190" s="135"/>
-      <c r="G190" s="135"/>
-      <c r="H190" s="135"/>
-      <c r="I190" s="135"/>
-      <c r="J190" s="135"/>
-      <c r="K190" s="136"/>
+      <c r="E190" s="144"/>
+      <c r="F190" s="144"/>
+      <c r="G190" s="144"/>
+      <c r="H190" s="144"/>
+      <c r="I190" s="144"/>
+      <c r="J190" s="144"/>
+      <c r="K190" s="145"/>
     </row>
     <row r="191" spans="1:14">
       <c r="A191" s="12">
@@ -9515,16 +9530,16 @@
         <v>ABD</v>
       </c>
       <c r="C191" s="13"/>
-      <c r="D191" s="134" t="s">
+      <c r="D191" s="143" t="s">
         <v>360</v>
       </c>
-      <c r="E191" s="135"/>
-      <c r="F191" s="135"/>
-      <c r="G191" s="135"/>
-      <c r="H191" s="135"/>
-      <c r="I191" s="135"/>
-      <c r="J191" s="135"/>
-      <c r="K191" s="136"/>
+      <c r="E191" s="144"/>
+      <c r="F191" s="144"/>
+      <c r="G191" s="144"/>
+      <c r="H191" s="144"/>
+      <c r="I191" s="144"/>
+      <c r="J191" s="144"/>
+      <c r="K191" s="145"/>
     </row>
     <row r="192" spans="1:14">
       <c r="A192" s="12">
@@ -9536,16 +9551,16 @@
         <v>ABE</v>
       </c>
       <c r="C192" s="13"/>
-      <c r="D192" s="134" t="s">
+      <c r="D192" s="143" t="s">
         <v>361</v>
       </c>
-      <c r="E192" s="135"/>
-      <c r="F192" s="135"/>
-      <c r="G192" s="135"/>
-      <c r="H192" s="135"/>
-      <c r="I192" s="135"/>
-      <c r="J192" s="135"/>
-      <c r="K192" s="136"/>
+      <c r="E192" s="144"/>
+      <c r="F192" s="144"/>
+      <c r="G192" s="144"/>
+      <c r="H192" s="144"/>
+      <c r="I192" s="144"/>
+      <c r="J192" s="144"/>
+      <c r="K192" s="145"/>
     </row>
     <row r="193" spans="1:14" s="1" customFormat="1">
       <c r="A193" s="32">
@@ -9557,16 +9572,16 @@
         <v>ABF</v>
       </c>
       <c r="C193" s="33"/>
-      <c r="D193" s="160" t="s">
+      <c r="D193" s="146" t="s">
         <v>362</v>
       </c>
-      <c r="E193" s="161"/>
-      <c r="F193" s="161"/>
-      <c r="G193" s="161"/>
-      <c r="H193" s="161"/>
-      <c r="I193" s="161"/>
-      <c r="J193" s="161"/>
-      <c r="K193" s="162"/>
+      <c r="E193" s="147"/>
+      <c r="F193" s="147"/>
+      <c r="G193" s="147"/>
+      <c r="H193" s="147"/>
+      <c r="I193" s="147"/>
+      <c r="J193" s="147"/>
+      <c r="K193" s="148"/>
       <c r="L193" s="57"/>
       <c r="M193" s="58"/>
       <c r="N193" s="58"/>
@@ -9581,15 +9596,15 @@
         <v>AC0</v>
       </c>
       <c r="C194" s="39"/>
-      <c r="D194" s="150" t="s">
+      <c r="D194" s="149" t="s">
         <v>363</v>
       </c>
-      <c r="E194" s="143"/>
-      <c r="F194" s="143"/>
-      <c r="G194" s="143"/>
-      <c r="H194" s="143"/>
-      <c r="I194" s="143"/>
-      <c r="J194" s="143"/>
+      <c r="E194" s="150"/>
+      <c r="F194" s="150"/>
+      <c r="G194" s="150"/>
+      <c r="H194" s="150"/>
+      <c r="I194" s="150"/>
+      <c r="J194" s="150"/>
       <c r="K194" s="151"/>
     </row>
     <row r="195" spans="1:14">
@@ -9602,16 +9617,16 @@
         <v>AC1</v>
       </c>
       <c r="C195" s="13"/>
-      <c r="D195" s="134" t="s">
+      <c r="D195" s="143" t="s">
         <v>364</v>
       </c>
-      <c r="E195" s="135"/>
-      <c r="F195" s="135"/>
-      <c r="G195" s="135"/>
-      <c r="H195" s="135"/>
-      <c r="I195" s="135"/>
-      <c r="J195" s="135"/>
-      <c r="K195" s="136"/>
+      <c r="E195" s="144"/>
+      <c r="F195" s="144"/>
+      <c r="G195" s="144"/>
+      <c r="H195" s="144"/>
+      <c r="I195" s="144"/>
+      <c r="J195" s="144"/>
+      <c r="K195" s="145"/>
     </row>
     <row r="196" spans="1:14">
       <c r="A196" s="12">
@@ -9623,16 +9638,16 @@
         <v>AC2</v>
       </c>
       <c r="C196" s="13"/>
-      <c r="D196" s="134" t="s">
+      <c r="D196" s="143" t="s">
         <v>365</v>
       </c>
-      <c r="E196" s="135"/>
-      <c r="F196" s="135"/>
-      <c r="G196" s="135"/>
-      <c r="H196" s="135"/>
-      <c r="I196" s="135"/>
-      <c r="J196" s="135"/>
-      <c r="K196" s="136"/>
+      <c r="E196" s="144"/>
+      <c r="F196" s="144"/>
+      <c r="G196" s="144"/>
+      <c r="H196" s="144"/>
+      <c r="I196" s="144"/>
+      <c r="J196" s="144"/>
+      <c r="K196" s="145"/>
     </row>
     <row r="197" spans="1:14">
       <c r="A197" s="12">
@@ -9644,16 +9659,16 @@
         <v>AC3</v>
       </c>
       <c r="C197" s="13"/>
-      <c r="D197" s="134" t="s">
+      <c r="D197" s="143" t="s">
         <v>366</v>
       </c>
-      <c r="E197" s="135"/>
-      <c r="F197" s="135"/>
-      <c r="G197" s="135"/>
-      <c r="H197" s="135"/>
-      <c r="I197" s="135"/>
-      <c r="J197" s="135"/>
-      <c r="K197" s="136"/>
+      <c r="E197" s="144"/>
+      <c r="F197" s="144"/>
+      <c r="G197" s="144"/>
+      <c r="H197" s="144"/>
+      <c r="I197" s="144"/>
+      <c r="J197" s="144"/>
+      <c r="K197" s="145"/>
     </row>
     <row r="198" spans="1:14">
       <c r="A198" s="12">
@@ -9665,16 +9680,16 @@
         <v>AC4</v>
       </c>
       <c r="C198" s="13"/>
-      <c r="D198" s="134" t="s">
+      <c r="D198" s="143" t="s">
         <v>367</v>
       </c>
-      <c r="E198" s="135"/>
-      <c r="F198" s="135"/>
-      <c r="G198" s="135"/>
-      <c r="H198" s="135"/>
-      <c r="I198" s="135"/>
-      <c r="J198" s="135"/>
-      <c r="K198" s="136"/>
+      <c r="E198" s="144"/>
+      <c r="F198" s="144"/>
+      <c r="G198" s="144"/>
+      <c r="H198" s="144"/>
+      <c r="I198" s="144"/>
+      <c r="J198" s="144"/>
+      <c r="K198" s="145"/>
     </row>
     <row r="199" spans="1:14">
       <c r="A199" s="12">
@@ -9705,16 +9720,16 @@
         <v>AC6</v>
       </c>
       <c r="C200" s="13"/>
-      <c r="D200" s="134" t="s">
+      <c r="D200" s="143" t="s">
         <v>368</v>
       </c>
-      <c r="E200" s="135"/>
-      <c r="F200" s="135"/>
-      <c r="G200" s="135"/>
-      <c r="H200" s="135"/>
-      <c r="I200" s="135"/>
-      <c r="J200" s="135"/>
-      <c r="K200" s="136"/>
+      <c r="E200" s="144"/>
+      <c r="F200" s="144"/>
+      <c r="G200" s="144"/>
+      <c r="H200" s="144"/>
+      <c r="I200" s="144"/>
+      <c r="J200" s="144"/>
+      <c r="K200" s="145"/>
     </row>
     <row r="201" spans="1:14">
       <c r="A201" s="12">
@@ -9745,16 +9760,16 @@
         <v>AC8</v>
       </c>
       <c r="C202" s="13"/>
-      <c r="D202" s="157" t="s">
+      <c r="D202" s="168" t="s">
         <v>369</v>
       </c>
-      <c r="E202" s="158"/>
-      <c r="F202" s="158"/>
-      <c r="G202" s="158"/>
-      <c r="H202" s="158"/>
-      <c r="I202" s="158"/>
-      <c r="J202" s="158"/>
-      <c r="K202" s="159"/>
+      <c r="E202" s="169"/>
+      <c r="F202" s="169"/>
+      <c r="G202" s="169"/>
+      <c r="H202" s="169"/>
+      <c r="I202" s="169"/>
+      <c r="J202" s="169"/>
+      <c r="K202" s="170"/>
     </row>
     <row r="203" spans="1:14">
       <c r="A203" s="12">
@@ -9785,16 +9800,16 @@
         <v>ACA</v>
       </c>
       <c r="C204" s="13"/>
-      <c r="D204" s="134" t="s">
+      <c r="D204" s="143" t="s">
         <v>370</v>
       </c>
-      <c r="E204" s="135"/>
-      <c r="F204" s="135"/>
-      <c r="G204" s="135"/>
-      <c r="H204" s="135"/>
-      <c r="I204" s="135"/>
-      <c r="J204" s="135"/>
-      <c r="K204" s="136"/>
+      <c r="E204" s="144"/>
+      <c r="F204" s="144"/>
+      <c r="G204" s="144"/>
+      <c r="H204" s="144"/>
+      <c r="I204" s="144"/>
+      <c r="J204" s="144"/>
+      <c r="K204" s="145"/>
     </row>
     <row r="205" spans="1:14">
       <c r="A205" s="12">
@@ -9825,16 +9840,16 @@
         <v>ACC</v>
       </c>
       <c r="C206" s="13"/>
-      <c r="D206" s="134" t="s">
+      <c r="D206" s="143" t="s">
         <v>370</v>
       </c>
-      <c r="E206" s="135"/>
-      <c r="F206" s="135"/>
-      <c r="G206" s="135"/>
-      <c r="H206" s="135"/>
-      <c r="I206" s="135"/>
-      <c r="J206" s="135"/>
-      <c r="K206" s="136"/>
+      <c r="E206" s="144"/>
+      <c r="F206" s="144"/>
+      <c r="G206" s="144"/>
+      <c r="H206" s="144"/>
+      <c r="I206" s="144"/>
+      <c r="J206" s="144"/>
+      <c r="K206" s="145"/>
     </row>
     <row r="207" spans="1:14">
       <c r="A207" s="12">
@@ -9865,16 +9880,16 @@
         <v>ACE</v>
       </c>
       <c r="C208" s="13"/>
-      <c r="D208" s="134" t="s">
+      <c r="D208" s="143" t="s">
         <v>371</v>
       </c>
-      <c r="E208" s="135"/>
-      <c r="F208" s="135"/>
-      <c r="G208" s="135"/>
-      <c r="H208" s="135"/>
-      <c r="I208" s="135"/>
-      <c r="J208" s="135"/>
-      <c r="K208" s="136"/>
+      <c r="E208" s="144"/>
+      <c r="F208" s="144"/>
+      <c r="G208" s="144"/>
+      <c r="H208" s="144"/>
+      <c r="I208" s="144"/>
+      <c r="J208" s="144"/>
+      <c r="K208" s="145"/>
     </row>
     <row r="209" spans="1:14" s="1" customFormat="1">
       <c r="A209" s="32">
@@ -9908,15 +9923,15 @@
         <v>AD0</v>
       </c>
       <c r="C210" s="39"/>
-      <c r="D210" s="150" t="s">
+      <c r="D210" s="149" t="s">
         <v>371</v>
       </c>
-      <c r="E210" s="143"/>
-      <c r="F210" s="143"/>
-      <c r="G210" s="143"/>
-      <c r="H210" s="143"/>
-      <c r="I210" s="143"/>
-      <c r="J210" s="143"/>
+      <c r="E210" s="150"/>
+      <c r="F210" s="150"/>
+      <c r="G210" s="150"/>
+      <c r="H210" s="150"/>
+      <c r="I210" s="150"/>
+      <c r="J210" s="150"/>
       <c r="K210" s="151"/>
     </row>
     <row r="211" spans="1:14">
@@ -9986,16 +10001,16 @@
         <v>AD4</v>
       </c>
       <c r="C214" s="13"/>
-      <c r="D214" s="134" t="s">
+      <c r="D214" s="143" t="s">
         <v>372</v>
       </c>
-      <c r="E214" s="135"/>
-      <c r="F214" s="135"/>
-      <c r="G214" s="135"/>
-      <c r="H214" s="135"/>
-      <c r="I214" s="135"/>
-      <c r="J214" s="135"/>
-      <c r="K214" s="136"/>
+      <c r="E214" s="144"/>
+      <c r="F214" s="144"/>
+      <c r="G214" s="144"/>
+      <c r="H214" s="144"/>
+      <c r="I214" s="144"/>
+      <c r="J214" s="144"/>
+      <c r="K214" s="145"/>
     </row>
     <row r="215" spans="1:14">
       <c r="A215" s="12">
@@ -10026,16 +10041,16 @@
         <v>AD6</v>
       </c>
       <c r="C216" s="13"/>
-      <c r="D216" s="148" t="s">
+      <c r="D216" s="158" t="s">
         <v>373</v>
       </c>
-      <c r="E216" s="137"/>
-      <c r="F216" s="137"/>
-      <c r="G216" s="137"/>
-      <c r="H216" s="137"/>
-      <c r="I216" s="137"/>
-      <c r="J216" s="137"/>
-      <c r="K216" s="149"/>
+      <c r="E216" s="153"/>
+      <c r="F216" s="153"/>
+      <c r="G216" s="153"/>
+      <c r="H216" s="153"/>
+      <c r="I216" s="153"/>
+      <c r="J216" s="153"/>
+      <c r="K216" s="159"/>
     </row>
     <row r="217" spans="1:14">
       <c r="A217" s="12">
@@ -10047,13 +10062,13 @@
         <v>AD7</v>
       </c>
       <c r="C217" s="13"/>
-      <c r="D217" s="150"/>
-      <c r="E217" s="143"/>
-      <c r="F217" s="143"/>
-      <c r="G217" s="143"/>
-      <c r="H217" s="143"/>
-      <c r="I217" s="143"/>
-      <c r="J217" s="143"/>
+      <c r="D217" s="149"/>
+      <c r="E217" s="150"/>
+      <c r="F217" s="150"/>
+      <c r="G217" s="150"/>
+      <c r="H217" s="150"/>
+      <c r="I217" s="150"/>
+      <c r="J217" s="150"/>
       <c r="K217" s="151"/>
     </row>
     <row r="218" spans="1:14">
@@ -10066,16 +10081,16 @@
         <v>AD8</v>
       </c>
       <c r="C218" s="13"/>
-      <c r="D218" s="148" t="s">
+      <c r="D218" s="158" t="s">
         <v>374</v>
       </c>
-      <c r="E218" s="137"/>
-      <c r="F218" s="137"/>
-      <c r="G218" s="137"/>
-      <c r="H218" s="137"/>
-      <c r="I218" s="137"/>
-      <c r="J218" s="137"/>
-      <c r="K218" s="149"/>
+      <c r="E218" s="153"/>
+      <c r="F218" s="153"/>
+      <c r="G218" s="153"/>
+      <c r="H218" s="153"/>
+      <c r="I218" s="153"/>
+      <c r="J218" s="153"/>
+      <c r="K218" s="159"/>
     </row>
     <row r="219" spans="1:14">
       <c r="A219" s="12">
@@ -10087,13 +10102,13 @@
         <v>AD9</v>
       </c>
       <c r="C219" s="13"/>
-      <c r="D219" s="150"/>
-      <c r="E219" s="143"/>
-      <c r="F219" s="143"/>
-      <c r="G219" s="143"/>
-      <c r="H219" s="143"/>
-      <c r="I219" s="143"/>
-      <c r="J219" s="143"/>
+      <c r="D219" s="149"/>
+      <c r="E219" s="150"/>
+      <c r="F219" s="150"/>
+      <c r="G219" s="150"/>
+      <c r="H219" s="150"/>
+      <c r="I219" s="150"/>
+      <c r="J219" s="150"/>
       <c r="K219" s="151"/>
     </row>
     <row r="220" spans="1:14">
@@ -10106,16 +10121,16 @@
         <v>ADA</v>
       </c>
       <c r="C220" s="13"/>
-      <c r="D220" s="148" t="s">
+      <c r="D220" s="158" t="s">
         <v>375</v>
       </c>
-      <c r="E220" s="137"/>
-      <c r="F220" s="137"/>
-      <c r="G220" s="137"/>
-      <c r="H220" s="137"/>
-      <c r="I220" s="137"/>
-      <c r="J220" s="137"/>
-      <c r="K220" s="149"/>
+      <c r="E220" s="153"/>
+      <c r="F220" s="153"/>
+      <c r="G220" s="153"/>
+      <c r="H220" s="153"/>
+      <c r="I220" s="153"/>
+      <c r="J220" s="153"/>
+      <c r="K220" s="159"/>
     </row>
     <row r="221" spans="1:14">
       <c r="A221" s="12">
@@ -10127,13 +10142,13 @@
         <v>ADB</v>
       </c>
       <c r="C221" s="13"/>
-      <c r="D221" s="150"/>
-      <c r="E221" s="143"/>
-      <c r="F221" s="143"/>
-      <c r="G221" s="143"/>
-      <c r="H221" s="143"/>
-      <c r="I221" s="143"/>
-      <c r="J221" s="143"/>
+      <c r="D221" s="149"/>
+      <c r="E221" s="150"/>
+      <c r="F221" s="150"/>
+      <c r="G221" s="150"/>
+      <c r="H221" s="150"/>
+      <c r="I221" s="150"/>
+      <c r="J221" s="150"/>
       <c r="K221" s="151"/>
     </row>
     <row r="222" spans="1:14">
@@ -10146,16 +10161,16 @@
         <v>ADC</v>
       </c>
       <c r="C222" s="13"/>
-      <c r="D222" s="134" t="s">
+      <c r="D222" s="143" t="s">
         <v>376</v>
       </c>
-      <c r="E222" s="135"/>
-      <c r="F222" s="135"/>
-      <c r="G222" s="135"/>
-      <c r="H222" s="135"/>
-      <c r="I222" s="135"/>
-      <c r="J222" s="135"/>
-      <c r="K222" s="136"/>
+      <c r="E222" s="144"/>
+      <c r="F222" s="144"/>
+      <c r="G222" s="144"/>
+      <c r="H222" s="144"/>
+      <c r="I222" s="144"/>
+      <c r="J222" s="144"/>
+      <c r="K222" s="145"/>
     </row>
     <row r="223" spans="1:14">
       <c r="A223" s="12">
@@ -10186,16 +10201,16 @@
         <v>ADE</v>
       </c>
       <c r="C224" s="13"/>
-      <c r="D224" s="134" t="s">
+      <c r="D224" s="143" t="s">
         <v>377</v>
       </c>
-      <c r="E224" s="135"/>
-      <c r="F224" s="135"/>
-      <c r="G224" s="135"/>
-      <c r="H224" s="135"/>
-      <c r="I224" s="135"/>
-      <c r="J224" s="135"/>
-      <c r="K224" s="136"/>
+      <c r="E224" s="144"/>
+      <c r="F224" s="144"/>
+      <c r="G224" s="144"/>
+      <c r="H224" s="144"/>
+      <c r="I224" s="144"/>
+      <c r="J224" s="144"/>
+      <c r="K224" s="145"/>
     </row>
     <row r="225" spans="1:14" s="1" customFormat="1">
       <c r="A225" s="32">
@@ -10229,16 +10244,16 @@
         <v>AE0</v>
       </c>
       <c r="C226" s="39"/>
-      <c r="D226" s="154" t="s">
+      <c r="D226" s="165" t="s">
         <v>378</v>
       </c>
-      <c r="E226" s="155"/>
-      <c r="F226" s="155"/>
-      <c r="G226" s="155"/>
-      <c r="H226" s="155"/>
-      <c r="I226" s="155"/>
-      <c r="J226" s="155"/>
-      <c r="K226" s="156"/>
+      <c r="E226" s="166"/>
+      <c r="F226" s="166"/>
+      <c r="G226" s="166"/>
+      <c r="H226" s="166"/>
+      <c r="I226" s="166"/>
+      <c r="J226" s="166"/>
+      <c r="K226" s="167"/>
     </row>
     <row r="227" spans="1:14">
       <c r="A227" s="12">
@@ -10383,16 +10398,16 @@
         <v>AE8</v>
       </c>
       <c r="C234" s="13"/>
-      <c r="D234" s="152" t="s">
+      <c r="D234" s="162" t="s">
         <v>379</v>
       </c>
-      <c r="E234" s="132"/>
-      <c r="F234" s="132"/>
-      <c r="G234" s="132"/>
-      <c r="H234" s="132"/>
-      <c r="I234" s="132"/>
-      <c r="J234" s="132"/>
-      <c r="K234" s="153"/>
+      <c r="E234" s="163"/>
+      <c r="F234" s="163"/>
+      <c r="G234" s="163"/>
+      <c r="H234" s="163"/>
+      <c r="I234" s="163"/>
+      <c r="J234" s="163"/>
+      <c r="K234" s="164"/>
     </row>
     <row r="235" spans="1:14">
       <c r="A235" s="12">
@@ -10461,16 +10476,16 @@
         <v>AEC</v>
       </c>
       <c r="C238" s="13"/>
-      <c r="D238" s="141" t="s">
+      <c r="D238" s="152" t="s">
         <v>380</v>
       </c>
-      <c r="E238" s="137"/>
-      <c r="F238" s="137"/>
-      <c r="G238" s="137"/>
-      <c r="H238" s="137"/>
-      <c r="I238" s="137"/>
-      <c r="J238" s="137"/>
-      <c r="K238" s="138"/>
+      <c r="E238" s="153"/>
+      <c r="F238" s="153"/>
+      <c r="G238" s="153"/>
+      <c r="H238" s="153"/>
+      <c r="I238" s="153"/>
+      <c r="J238" s="153"/>
+      <c r="K238" s="154"/>
     </row>
     <row r="239" spans="1:14">
       <c r="A239" s="12">
@@ -10482,14 +10497,14 @@
         <v>AED</v>
       </c>
       <c r="C239" s="13"/>
-      <c r="D239" s="142"/>
-      <c r="E239" s="143"/>
-      <c r="F239" s="143"/>
-      <c r="G239" s="143"/>
-      <c r="H239" s="143"/>
-      <c r="I239" s="143"/>
-      <c r="J239" s="143"/>
-      <c r="K239" s="144"/>
+      <c r="D239" s="160"/>
+      <c r="E239" s="150"/>
+      <c r="F239" s="150"/>
+      <c r="G239" s="150"/>
+      <c r="H239" s="150"/>
+      <c r="I239" s="150"/>
+      <c r="J239" s="150"/>
+      <c r="K239" s="161"/>
     </row>
     <row r="240" spans="1:14">
       <c r="A240" s="12">
@@ -10501,16 +10516,16 @@
         <v>AEE</v>
       </c>
       <c r="C240" s="70"/>
-      <c r="D240" s="137" t="s">
+      <c r="D240" s="153" t="s">
         <v>381</v>
       </c>
-      <c r="E240" s="137"/>
-      <c r="F240" s="137"/>
-      <c r="G240" s="137"/>
-      <c r="H240" s="137"/>
-      <c r="I240" s="137"/>
-      <c r="J240" s="137"/>
-      <c r="K240" s="138"/>
+      <c r="E240" s="153"/>
+      <c r="F240" s="153"/>
+      <c r="G240" s="153"/>
+      <c r="H240" s="153"/>
+      <c r="I240" s="153"/>
+      <c r="J240" s="153"/>
+      <c r="K240" s="154"/>
     </row>
     <row r="241" spans="1:14" s="1" customFormat="1">
       <c r="A241" s="32">
@@ -10522,14 +10537,14 @@
         <v>AEF</v>
       </c>
       <c r="C241" s="34"/>
-      <c r="D241" s="139"/>
-      <c r="E241" s="139"/>
-      <c r="F241" s="139"/>
-      <c r="G241" s="139"/>
-      <c r="H241" s="139"/>
-      <c r="I241" s="139"/>
-      <c r="J241" s="139"/>
-      <c r="K241" s="140"/>
+      <c r="D241" s="173"/>
+      <c r="E241" s="173"/>
+      <c r="F241" s="173"/>
+      <c r="G241" s="173"/>
+      <c r="H241" s="173"/>
+      <c r="I241" s="173"/>
+      <c r="J241" s="173"/>
+      <c r="K241" s="174"/>
       <c r="L241" s="57"/>
       <c r="M241" s="58"/>
       <c r="N241" s="58"/>
@@ -10720,16 +10735,16 @@
         <v>AF8</v>
       </c>
       <c r="C250" s="13"/>
-      <c r="D250" s="131" t="s">
+      <c r="D250" s="171" t="s">
         <v>382</v>
       </c>
-      <c r="E250" s="132"/>
-      <c r="F250" s="132"/>
-      <c r="G250" s="132"/>
-      <c r="H250" s="132"/>
-      <c r="I250" s="132"/>
-      <c r="J250" s="132"/>
-      <c r="K250" s="133"/>
+      <c r="E250" s="163"/>
+      <c r="F250" s="163"/>
+      <c r="G250" s="163"/>
+      <c r="H250" s="163"/>
+      <c r="I250" s="163"/>
+      <c r="J250" s="163"/>
+      <c r="K250" s="172"/>
     </row>
     <row r="251" spans="1:14">
       <c r="A251" s="12">
@@ -11298,16 +11313,16 @@
         <v>B16</v>
       </c>
       <c r="C280" s="13"/>
-      <c r="D280" s="134" t="s">
+      <c r="D280" s="143" t="s">
         <v>383</v>
       </c>
-      <c r="E280" s="135"/>
-      <c r="F280" s="135"/>
-      <c r="G280" s="135"/>
-      <c r="H280" s="135"/>
-      <c r="I280" s="135"/>
-      <c r="J280" s="135"/>
-      <c r="K280" s="136"/>
+      <c r="E280" s="144"/>
+      <c r="F280" s="144"/>
+      <c r="G280" s="144"/>
+      <c r="H280" s="144"/>
+      <c r="I280" s="144"/>
+      <c r="J280" s="144"/>
+      <c r="K280" s="145"/>
     </row>
     <row r="281" spans="1:14">
       <c r="A281" s="12">
@@ -11414,16 +11429,16 @@
         <v>B1C</v>
       </c>
       <c r="C286" s="13"/>
-      <c r="D286" s="134" t="s">
+      <c r="D286" s="143" t="s">
         <v>384</v>
       </c>
-      <c r="E286" s="135"/>
-      <c r="F286" s="135"/>
-      <c r="G286" s="135"/>
-      <c r="H286" s="135"/>
-      <c r="I286" s="135"/>
-      <c r="J286" s="135"/>
-      <c r="K286" s="136"/>
+      <c r="E286" s="144"/>
+      <c r="F286" s="144"/>
+      <c r="G286" s="144"/>
+      <c r="H286" s="144"/>
+      <c r="I286" s="144"/>
+      <c r="J286" s="144"/>
+      <c r="K286" s="145"/>
     </row>
     <row r="287" spans="1:14">
       <c r="A287" s="12">
@@ -11573,16 +11588,16 @@
         <v>B24</v>
       </c>
       <c r="C294" s="13"/>
-      <c r="D294" s="134" t="s">
+      <c r="D294" s="143" t="s">
         <v>445</v>
       </c>
-      <c r="E294" s="135"/>
-      <c r="F294" s="135"/>
-      <c r="G294" s="135"/>
-      <c r="H294" s="135"/>
-      <c r="I294" s="135"/>
-      <c r="J294" s="135"/>
-      <c r="K294" s="136"/>
+      <c r="E294" s="144"/>
+      <c r="F294" s="144"/>
+      <c r="G294" s="144"/>
+      <c r="H294" s="144"/>
+      <c r="I294" s="144"/>
+      <c r="J294" s="144"/>
+      <c r="K294" s="145"/>
     </row>
     <row r="295" spans="1:14">
       <c r="A295" s="12">
@@ -11613,16 +11628,16 @@
         <v>B26</v>
       </c>
       <c r="C296" s="13"/>
-      <c r="D296" s="134" t="s">
+      <c r="D296" s="143" t="s">
         <v>444</v>
       </c>
-      <c r="E296" s="135"/>
-      <c r="F296" s="135"/>
-      <c r="G296" s="135"/>
-      <c r="H296" s="135"/>
-      <c r="I296" s="135"/>
-      <c r="J296" s="135"/>
-      <c r="K296" s="136"/>
+      <c r="E296" s="144"/>
+      <c r="F296" s="144"/>
+      <c r="G296" s="144"/>
+      <c r="H296" s="144"/>
+      <c r="I296" s="144"/>
+      <c r="J296" s="144"/>
+      <c r="K296" s="145"/>
     </row>
     <row r="297" spans="1:14">
       <c r="A297" s="12">
@@ -11653,16 +11668,16 @@
         <v>B28</v>
       </c>
       <c r="C298" s="13"/>
-      <c r="D298" s="141" t="s">
+      <c r="D298" s="152" t="s">
         <v>386</v>
       </c>
-      <c r="E298" s="137"/>
-      <c r="F298" s="137"/>
-      <c r="G298" s="137"/>
-      <c r="H298" s="137"/>
-      <c r="I298" s="137"/>
-      <c r="J298" s="137"/>
-      <c r="K298" s="138"/>
+      <c r="E298" s="153"/>
+      <c r="F298" s="153"/>
+      <c r="G298" s="153"/>
+      <c r="H298" s="153"/>
+      <c r="I298" s="153"/>
+      <c r="J298" s="153"/>
+      <c r="K298" s="154"/>
     </row>
     <row r="299" spans="1:14">
       <c r="A299" s="12">
@@ -11674,14 +11689,14 @@
         <v>B29</v>
       </c>
       <c r="C299" s="13"/>
-      <c r="D299" s="142"/>
-      <c r="E299" s="143"/>
-      <c r="F299" s="143"/>
-      <c r="G299" s="143"/>
-      <c r="H299" s="143"/>
-      <c r="I299" s="143"/>
-      <c r="J299" s="143"/>
-      <c r="K299" s="144"/>
+      <c r="D299" s="160"/>
+      <c r="E299" s="150"/>
+      <c r="F299" s="150"/>
+      <c r="G299" s="150"/>
+      <c r="H299" s="150"/>
+      <c r="I299" s="150"/>
+      <c r="J299" s="150"/>
+      <c r="K299" s="161"/>
     </row>
     <row r="300" spans="1:14">
       <c r="A300" s="12">
@@ -11693,16 +11708,16 @@
         <v>B2A</v>
       </c>
       <c r="C300" s="13"/>
-      <c r="D300" s="141" t="s">
+      <c r="D300" s="152" t="s">
         <v>387</v>
       </c>
-      <c r="E300" s="137"/>
-      <c r="F300" s="137"/>
-      <c r="G300" s="137"/>
-      <c r="H300" s="137"/>
-      <c r="I300" s="137"/>
-      <c r="J300" s="137"/>
-      <c r="K300" s="138"/>
+      <c r="E300" s="153"/>
+      <c r="F300" s="153"/>
+      <c r="G300" s="153"/>
+      <c r="H300" s="153"/>
+      <c r="I300" s="153"/>
+      <c r="J300" s="153"/>
+      <c r="K300" s="154"/>
     </row>
     <row r="301" spans="1:14">
       <c r="A301" s="12">
@@ -11714,14 +11729,14 @@
         <v>B2B</v>
       </c>
       <c r="C301" s="13"/>
-      <c r="D301" s="142"/>
-      <c r="E301" s="143"/>
-      <c r="F301" s="143"/>
-      <c r="G301" s="143"/>
-      <c r="H301" s="143"/>
-      <c r="I301" s="143"/>
-      <c r="J301" s="143"/>
-      <c r="K301" s="144"/>
+      <c r="D301" s="160"/>
+      <c r="E301" s="150"/>
+      <c r="F301" s="150"/>
+      <c r="G301" s="150"/>
+      <c r="H301" s="150"/>
+      <c r="I301" s="150"/>
+      <c r="J301" s="150"/>
+      <c r="K301" s="161"/>
     </row>
     <row r="302" spans="1:14">
       <c r="A302" s="12">
@@ -11733,16 +11748,16 @@
         <v>B2C</v>
       </c>
       <c r="C302" s="13"/>
-      <c r="D302" s="141" t="s">
+      <c r="D302" s="152" t="s">
         <v>388</v>
       </c>
-      <c r="E302" s="137"/>
-      <c r="F302" s="137"/>
-      <c r="G302" s="137"/>
-      <c r="H302" s="137"/>
-      <c r="I302" s="137"/>
-      <c r="J302" s="137"/>
-      <c r="K302" s="138"/>
+      <c r="E302" s="153"/>
+      <c r="F302" s="153"/>
+      <c r="G302" s="153"/>
+      <c r="H302" s="153"/>
+      <c r="I302" s="153"/>
+      <c r="J302" s="153"/>
+      <c r="K302" s="154"/>
     </row>
     <row r="303" spans="1:14">
       <c r="A303" s="12">
@@ -11754,14 +11769,14 @@
         <v>B2D</v>
       </c>
       <c r="C303" s="13"/>
-      <c r="D303" s="142"/>
-      <c r="E303" s="143"/>
-      <c r="F303" s="143"/>
-      <c r="G303" s="143"/>
-      <c r="H303" s="143"/>
-      <c r="I303" s="143"/>
-      <c r="J303" s="143"/>
-      <c r="K303" s="144"/>
+      <c r="D303" s="160"/>
+      <c r="E303" s="150"/>
+      <c r="F303" s="150"/>
+      <c r="G303" s="150"/>
+      <c r="H303" s="150"/>
+      <c r="I303" s="150"/>
+      <c r="J303" s="150"/>
+      <c r="K303" s="161"/>
     </row>
     <row r="304" spans="1:14">
       <c r="A304" s="12">
@@ -11773,16 +11788,16 @@
         <v>B2E</v>
       </c>
       <c r="C304" s="13"/>
-      <c r="D304" s="141" t="s">
+      <c r="D304" s="152" t="s">
         <v>389</v>
       </c>
-      <c r="E304" s="137"/>
-      <c r="F304" s="137"/>
-      <c r="G304" s="137"/>
-      <c r="H304" s="137"/>
-      <c r="I304" s="137"/>
-      <c r="J304" s="137"/>
-      <c r="K304" s="138"/>
+      <c r="E304" s="153"/>
+      <c r="F304" s="153"/>
+      <c r="G304" s="153"/>
+      <c r="H304" s="153"/>
+      <c r="I304" s="153"/>
+      <c r="J304" s="153"/>
+      <c r="K304" s="154"/>
     </row>
     <row r="305" spans="1:14" s="1" customFormat="1">
       <c r="A305" s="32">
@@ -11794,14 +11809,14 @@
         <v>B2F</v>
       </c>
       <c r="C305" s="33"/>
-      <c r="D305" s="142"/>
-      <c r="E305" s="143"/>
-      <c r="F305" s="143"/>
-      <c r="G305" s="143"/>
-      <c r="H305" s="143"/>
-      <c r="I305" s="143"/>
-      <c r="J305" s="143"/>
-      <c r="K305" s="144"/>
+      <c r="D305" s="160"/>
+      <c r="E305" s="150"/>
+      <c r="F305" s="150"/>
+      <c r="G305" s="150"/>
+      <c r="H305" s="150"/>
+      <c r="I305" s="150"/>
+      <c r="J305" s="150"/>
+      <c r="K305" s="161"/>
       <c r="L305" s="57"/>
       <c r="M305" s="58"/>
       <c r="N305" s="58"/>
@@ -11816,16 +11831,16 @@
         <v>B30</v>
       </c>
       <c r="C306" s="39"/>
-      <c r="D306" s="141" t="s">
+      <c r="D306" s="152" t="s">
         <v>390</v>
       </c>
-      <c r="E306" s="137"/>
-      <c r="F306" s="137"/>
-      <c r="G306" s="137"/>
-      <c r="H306" s="137"/>
-      <c r="I306" s="137"/>
-      <c r="J306" s="137"/>
-      <c r="K306" s="138"/>
+      <c r="E306" s="153"/>
+      <c r="F306" s="153"/>
+      <c r="G306" s="153"/>
+      <c r="H306" s="153"/>
+      <c r="I306" s="153"/>
+      <c r="J306" s="153"/>
+      <c r="K306" s="154"/>
     </row>
     <row r="307" spans="1:14">
       <c r="A307" s="12">
@@ -11837,14 +11852,14 @@
         <v>B31</v>
       </c>
       <c r="C307" s="13"/>
-      <c r="D307" s="142"/>
-      <c r="E307" s="143"/>
-      <c r="F307" s="143"/>
-      <c r="G307" s="143"/>
-      <c r="H307" s="143"/>
-      <c r="I307" s="143"/>
-      <c r="J307" s="143"/>
-      <c r="K307" s="144"/>
+      <c r="D307" s="160"/>
+      <c r="E307" s="150"/>
+      <c r="F307" s="150"/>
+      <c r="G307" s="150"/>
+      <c r="H307" s="150"/>
+      <c r="I307" s="150"/>
+      <c r="J307" s="150"/>
+      <c r="K307" s="161"/>
     </row>
     <row r="308" spans="1:14">
       <c r="A308" s="12">
@@ -11856,16 +11871,16 @@
         <v>B32</v>
       </c>
       <c r="C308" s="13"/>
-      <c r="D308" s="141" t="s">
+      <c r="D308" s="152" t="s">
         <v>391</v>
       </c>
-      <c r="E308" s="137"/>
-      <c r="F308" s="137"/>
-      <c r="G308" s="137"/>
-      <c r="H308" s="137"/>
-      <c r="I308" s="137"/>
-      <c r="J308" s="137"/>
-      <c r="K308" s="138"/>
+      <c r="E308" s="153"/>
+      <c r="F308" s="153"/>
+      <c r="G308" s="153"/>
+      <c r="H308" s="153"/>
+      <c r="I308" s="153"/>
+      <c r="J308" s="153"/>
+      <c r="K308" s="154"/>
     </row>
     <row r="309" spans="1:14">
       <c r="A309" s="12">
@@ -11877,14 +11892,14 @@
         <v>B33</v>
       </c>
       <c r="C309" s="13"/>
-      <c r="D309" s="142"/>
-      <c r="E309" s="143"/>
-      <c r="F309" s="143"/>
-      <c r="G309" s="143"/>
-      <c r="H309" s="143"/>
-      <c r="I309" s="143"/>
-      <c r="J309" s="143"/>
-      <c r="K309" s="144"/>
+      <c r="D309" s="160"/>
+      <c r="E309" s="150"/>
+      <c r="F309" s="150"/>
+      <c r="G309" s="150"/>
+      <c r="H309" s="150"/>
+      <c r="I309" s="150"/>
+      <c r="J309" s="150"/>
+      <c r="K309" s="161"/>
     </row>
     <row r="310" spans="1:14">
       <c r="A310" s="12">
@@ -15764,41 +15779,18 @@
     </row>
   </sheetData>
   <mergeCells count="63">
-    <mergeCell ref="D75:K75"/>
-    <mergeCell ref="D76:K76"/>
-    <mergeCell ref="D77:K77"/>
-    <mergeCell ref="D78:K78"/>
-    <mergeCell ref="D79:K79"/>
-    <mergeCell ref="D80:K80"/>
-    <mergeCell ref="D81:K81"/>
-    <mergeCell ref="D168:K168"/>
-    <mergeCell ref="D175:K175"/>
-    <mergeCell ref="D178:K178"/>
-    <mergeCell ref="D91:K91"/>
-    <mergeCell ref="D90:K90"/>
-    <mergeCell ref="D93:K93"/>
-    <mergeCell ref="D96:K96"/>
-    <mergeCell ref="D94:K94"/>
-    <mergeCell ref="D95:K95"/>
-    <mergeCell ref="D92:K92"/>
-    <mergeCell ref="D182:K182"/>
-    <mergeCell ref="D183:K183"/>
-    <mergeCell ref="D174:K174"/>
-    <mergeCell ref="D184:K184"/>
-    <mergeCell ref="D185:K185"/>
-    <mergeCell ref="D186:K186"/>
-    <mergeCell ref="D187:K187"/>
-    <mergeCell ref="D188:K188"/>
-    <mergeCell ref="D197:K197"/>
-    <mergeCell ref="D198:K198"/>
-    <mergeCell ref="D189:K189"/>
-    <mergeCell ref="D190:K190"/>
-    <mergeCell ref="D191:K191"/>
-    <mergeCell ref="D192:K192"/>
-    <mergeCell ref="D193:K193"/>
-    <mergeCell ref="D194:K194"/>
-    <mergeCell ref="D195:K195"/>
-    <mergeCell ref="D196:K196"/>
+    <mergeCell ref="D250:K250"/>
+    <mergeCell ref="D280:K280"/>
+    <mergeCell ref="D286:K286"/>
+    <mergeCell ref="D296:K296"/>
+    <mergeCell ref="D240:K241"/>
+    <mergeCell ref="D294:K294"/>
+    <mergeCell ref="D304:K305"/>
+    <mergeCell ref="D306:K307"/>
+    <mergeCell ref="D308:K309"/>
+    <mergeCell ref="D298:K299"/>
+    <mergeCell ref="D300:K301"/>
+    <mergeCell ref="D302:K303"/>
     <mergeCell ref="D2:K3"/>
     <mergeCell ref="D216:K217"/>
     <mergeCell ref="D218:K219"/>
@@ -15815,18 +15807,41 @@
     <mergeCell ref="D204:K204"/>
     <mergeCell ref="D206:K206"/>
     <mergeCell ref="D208:K208"/>
-    <mergeCell ref="D304:K305"/>
-    <mergeCell ref="D306:K307"/>
-    <mergeCell ref="D308:K309"/>
-    <mergeCell ref="D298:K299"/>
-    <mergeCell ref="D300:K301"/>
-    <mergeCell ref="D302:K303"/>
-    <mergeCell ref="D250:K250"/>
-    <mergeCell ref="D280:K280"/>
-    <mergeCell ref="D286:K286"/>
-    <mergeCell ref="D296:K296"/>
-    <mergeCell ref="D240:K241"/>
-    <mergeCell ref="D294:K294"/>
+    <mergeCell ref="D186:K186"/>
+    <mergeCell ref="D187:K187"/>
+    <mergeCell ref="D188:K188"/>
+    <mergeCell ref="D197:K197"/>
+    <mergeCell ref="D198:K198"/>
+    <mergeCell ref="D189:K189"/>
+    <mergeCell ref="D190:K190"/>
+    <mergeCell ref="D191:K191"/>
+    <mergeCell ref="D192:K192"/>
+    <mergeCell ref="D193:K193"/>
+    <mergeCell ref="D194:K194"/>
+    <mergeCell ref="D195:K195"/>
+    <mergeCell ref="D196:K196"/>
+    <mergeCell ref="D182:K182"/>
+    <mergeCell ref="D183:K183"/>
+    <mergeCell ref="D174:K174"/>
+    <mergeCell ref="D184:K184"/>
+    <mergeCell ref="D185:K185"/>
+    <mergeCell ref="D80:K80"/>
+    <mergeCell ref="D81:K81"/>
+    <mergeCell ref="D168:K168"/>
+    <mergeCell ref="D175:K175"/>
+    <mergeCell ref="D178:K178"/>
+    <mergeCell ref="D91:K91"/>
+    <mergeCell ref="D90:K90"/>
+    <mergeCell ref="D93:K93"/>
+    <mergeCell ref="D96:K96"/>
+    <mergeCell ref="D94:K94"/>
+    <mergeCell ref="D95:K95"/>
+    <mergeCell ref="D92:K92"/>
+    <mergeCell ref="D75:K75"/>
+    <mergeCell ref="D76:K76"/>
+    <mergeCell ref="D77:K77"/>
+    <mergeCell ref="D78:K78"/>
+    <mergeCell ref="D79:K79"/>
   </mergeCells>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="53" fitToHeight="0" orientation="landscape" r:id="rId1"/>
@@ -15912,16 +15927,16 @@
         <f>8*A2&amp;"-"&amp;(8*A2+7)</f>
         <v>0-7</v>
       </c>
-      <c r="D2" s="141" t="s">
+      <c r="D2" s="152" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="137"/>
-      <c r="F2" s="137"/>
-      <c r="G2" s="137"/>
-      <c r="H2" s="137"/>
-      <c r="I2" s="137"/>
-      <c r="J2" s="137"/>
-      <c r="K2" s="138"/>
+      <c r="E2" s="153"/>
+      <c r="F2" s="153"/>
+      <c r="G2" s="153"/>
+      <c r="H2" s="153"/>
+      <c r="I2" s="153"/>
+      <c r="J2" s="153"/>
+      <c r="K2" s="154"/>
       <c r="M2" s="3">
         <v>16</v>
       </c>
@@ -15943,14 +15958,14 @@
         <f t="shared" ref="C3:C33" si="2">8*A3&amp;"-"&amp;(8*A3+7)</f>
         <v>8-15</v>
       </c>
-      <c r="D3" s="142"/>
-      <c r="E3" s="143"/>
-      <c r="F3" s="143"/>
-      <c r="G3" s="143"/>
-      <c r="H3" s="143"/>
-      <c r="I3" s="143"/>
-      <c r="J3" s="143"/>
-      <c r="K3" s="147"/>
+      <c r="D3" s="160"/>
+      <c r="E3" s="150"/>
+      <c r="F3" s="150"/>
+      <c r="G3" s="150"/>
+      <c r="H3" s="150"/>
+      <c r="I3" s="150"/>
+      <c r="J3" s="150"/>
+      <c r="K3" s="157"/>
       <c r="M3" s="3">
         <v>17</v>
       </c>
@@ -22199,16 +22214,16 @@
         <v>AB0</v>
       </c>
       <c r="C178" s="39"/>
-      <c r="D178" s="163" t="s">
+      <c r="D178" s="139" t="s">
         <v>350</v>
       </c>
-      <c r="E178" s="163"/>
-      <c r="F178" s="163"/>
-      <c r="G178" s="163"/>
-      <c r="H178" s="163"/>
-      <c r="I178" s="163"/>
-      <c r="J178" s="163"/>
-      <c r="K178" s="163"/>
+      <c r="E178" s="139"/>
+      <c r="F178" s="139"/>
+      <c r="G178" s="139"/>
+      <c r="H178" s="139"/>
+      <c r="I178" s="139"/>
+      <c r="J178" s="139"/>
+      <c r="K178" s="139"/>
     </row>
     <row r="179" spans="1:14">
       <c r="A179" s="12">
@@ -22277,16 +22292,16 @@
         <v>AB4</v>
       </c>
       <c r="C182" s="13"/>
-      <c r="D182" s="134" t="s">
+      <c r="D182" s="143" t="s">
         <v>351</v>
       </c>
-      <c r="E182" s="135"/>
-      <c r="F182" s="135"/>
-      <c r="G182" s="135"/>
-      <c r="H182" s="135"/>
-      <c r="I182" s="135"/>
-      <c r="J182" s="135"/>
-      <c r="K182" s="136"/>
+      <c r="E182" s="144"/>
+      <c r="F182" s="144"/>
+      <c r="G182" s="144"/>
+      <c r="H182" s="144"/>
+      <c r="I182" s="144"/>
+      <c r="J182" s="144"/>
+      <c r="K182" s="145"/>
     </row>
     <row r="183" spans="1:14">
       <c r="A183" s="12">
@@ -22298,16 +22313,16 @@
         <v>AB5</v>
       </c>
       <c r="C183" s="13"/>
-      <c r="D183" s="134" t="s">
+      <c r="D183" s="143" t="s">
         <v>352</v>
       </c>
-      <c r="E183" s="135"/>
-      <c r="F183" s="135"/>
-      <c r="G183" s="135"/>
-      <c r="H183" s="135"/>
-      <c r="I183" s="135"/>
-      <c r="J183" s="135"/>
-      <c r="K183" s="136"/>
+      <c r="E183" s="144"/>
+      <c r="F183" s="144"/>
+      <c r="G183" s="144"/>
+      <c r="H183" s="144"/>
+      <c r="I183" s="144"/>
+      <c r="J183" s="144"/>
+      <c r="K183" s="145"/>
     </row>
     <row r="184" spans="1:14">
       <c r="A184" s="12">
@@ -22319,16 +22334,16 @@
         <v>AB6</v>
       </c>
       <c r="C184" s="13"/>
-      <c r="D184" s="134" t="s">
+      <c r="D184" s="143" t="s">
         <v>353</v>
       </c>
-      <c r="E184" s="135"/>
-      <c r="F184" s="135"/>
-      <c r="G184" s="135"/>
-      <c r="H184" s="135"/>
-      <c r="I184" s="135"/>
-      <c r="J184" s="135"/>
-      <c r="K184" s="136"/>
+      <c r="E184" s="144"/>
+      <c r="F184" s="144"/>
+      <c r="G184" s="144"/>
+      <c r="H184" s="144"/>
+      <c r="I184" s="144"/>
+      <c r="J184" s="144"/>
+      <c r="K184" s="145"/>
     </row>
     <row r="185" spans="1:14">
       <c r="A185" s="12">
@@ -22340,16 +22355,16 @@
         <v>AB7</v>
       </c>
       <c r="C185" s="13"/>
-      <c r="D185" s="134" t="s">
+      <c r="D185" s="143" t="s">
         <v>354</v>
       </c>
-      <c r="E185" s="135"/>
-      <c r="F185" s="135"/>
-      <c r="G185" s="135"/>
-      <c r="H185" s="135"/>
-      <c r="I185" s="135"/>
-      <c r="J185" s="135"/>
-      <c r="K185" s="136"/>
+      <c r="E185" s="144"/>
+      <c r="F185" s="144"/>
+      <c r="G185" s="144"/>
+      <c r="H185" s="144"/>
+      <c r="I185" s="144"/>
+      <c r="J185" s="144"/>
+      <c r="K185" s="145"/>
     </row>
     <row r="186" spans="1:14">
       <c r="A186" s="12">
@@ -22361,16 +22376,16 @@
         <v>AB8</v>
       </c>
       <c r="C186" s="13"/>
-      <c r="D186" s="134" t="s">
+      <c r="D186" s="143" t="s">
         <v>355</v>
       </c>
-      <c r="E186" s="135"/>
-      <c r="F186" s="135"/>
-      <c r="G186" s="135"/>
-      <c r="H186" s="135"/>
-      <c r="I186" s="135"/>
-      <c r="J186" s="135"/>
-      <c r="K186" s="136"/>
+      <c r="E186" s="144"/>
+      <c r="F186" s="144"/>
+      <c r="G186" s="144"/>
+      <c r="H186" s="144"/>
+      <c r="I186" s="144"/>
+      <c r="J186" s="144"/>
+      <c r="K186" s="145"/>
     </row>
     <row r="187" spans="1:14">
       <c r="A187" s="12">
@@ -22382,16 +22397,16 @@
         <v>AB9</v>
       </c>
       <c r="C187" s="13"/>
-      <c r="D187" s="134" t="s">
+      <c r="D187" s="143" t="s">
         <v>356</v>
       </c>
-      <c r="E187" s="135"/>
-      <c r="F187" s="135"/>
-      <c r="G187" s="135"/>
-      <c r="H187" s="135"/>
-      <c r="I187" s="135"/>
-      <c r="J187" s="135"/>
-      <c r="K187" s="136"/>
+      <c r="E187" s="144"/>
+      <c r="F187" s="144"/>
+      <c r="G187" s="144"/>
+      <c r="H187" s="144"/>
+      <c r="I187" s="144"/>
+      <c r="J187" s="144"/>
+      <c r="K187" s="145"/>
     </row>
     <row r="188" spans="1:14">
       <c r="A188" s="12">
@@ -22403,16 +22418,16 @@
         <v>ABA</v>
       </c>
       <c r="C188" s="13"/>
-      <c r="D188" s="134" t="s">
+      <c r="D188" s="143" t="s">
         <v>357</v>
       </c>
-      <c r="E188" s="135"/>
-      <c r="F188" s="135"/>
-      <c r="G188" s="135"/>
-      <c r="H188" s="135"/>
-      <c r="I188" s="135"/>
-      <c r="J188" s="135"/>
-      <c r="K188" s="136"/>
+      <c r="E188" s="144"/>
+      <c r="F188" s="144"/>
+      <c r="G188" s="144"/>
+      <c r="H188" s="144"/>
+      <c r="I188" s="144"/>
+      <c r="J188" s="144"/>
+      <c r="K188" s="145"/>
     </row>
     <row r="189" spans="1:14">
       <c r="A189" s="12">
@@ -22424,16 +22439,16 @@
         <v>ABB</v>
       </c>
       <c r="C189" s="13"/>
-      <c r="D189" s="134" t="s">
+      <c r="D189" s="143" t="s">
         <v>358</v>
       </c>
-      <c r="E189" s="135"/>
-      <c r="F189" s="135"/>
-      <c r="G189" s="135"/>
-      <c r="H189" s="135"/>
-      <c r="I189" s="135"/>
-      <c r="J189" s="135"/>
-      <c r="K189" s="136"/>
+      <c r="E189" s="144"/>
+      <c r="F189" s="144"/>
+      <c r="G189" s="144"/>
+      <c r="H189" s="144"/>
+      <c r="I189" s="144"/>
+      <c r="J189" s="144"/>
+      <c r="K189" s="145"/>
     </row>
     <row r="190" spans="1:14">
       <c r="A190" s="12">
@@ -22445,16 +22460,16 @@
         <v>ABC</v>
       </c>
       <c r="C190" s="13"/>
-      <c r="D190" s="134" t="s">
+      <c r="D190" s="143" t="s">
         <v>359</v>
       </c>
-      <c r="E190" s="135"/>
-      <c r="F190" s="135"/>
-      <c r="G190" s="135"/>
-      <c r="H190" s="135"/>
-      <c r="I190" s="135"/>
-      <c r="J190" s="135"/>
-      <c r="K190" s="136"/>
+      <c r="E190" s="144"/>
+      <c r="F190" s="144"/>
+      <c r="G190" s="144"/>
+      <c r="H190" s="144"/>
+      <c r="I190" s="144"/>
+      <c r="J190" s="144"/>
+      <c r="K190" s="145"/>
     </row>
     <row r="191" spans="1:14">
       <c r="A191" s="12">
@@ -22466,16 +22481,16 @@
         <v>ABD</v>
       </c>
       <c r="C191" s="13"/>
-      <c r="D191" s="134" t="s">
+      <c r="D191" s="143" t="s">
         <v>360</v>
       </c>
-      <c r="E191" s="135"/>
-      <c r="F191" s="135"/>
-      <c r="G191" s="135"/>
-      <c r="H191" s="135"/>
-      <c r="I191" s="135"/>
-      <c r="J191" s="135"/>
-      <c r="K191" s="136"/>
+      <c r="E191" s="144"/>
+      <c r="F191" s="144"/>
+      <c r="G191" s="144"/>
+      <c r="H191" s="144"/>
+      <c r="I191" s="144"/>
+      <c r="J191" s="144"/>
+      <c r="K191" s="145"/>
     </row>
     <row r="192" spans="1:14">
       <c r="A192" s="12">
@@ -22487,16 +22502,16 @@
         <v>ABE</v>
       </c>
       <c r="C192" s="13"/>
-      <c r="D192" s="134" t="s">
+      <c r="D192" s="143" t="s">
         <v>361</v>
       </c>
-      <c r="E192" s="135"/>
-      <c r="F192" s="135"/>
-      <c r="G192" s="135"/>
-      <c r="H192" s="135"/>
-      <c r="I192" s="135"/>
-      <c r="J192" s="135"/>
-      <c r="K192" s="136"/>
+      <c r="E192" s="144"/>
+      <c r="F192" s="144"/>
+      <c r="G192" s="144"/>
+      <c r="H192" s="144"/>
+      <c r="I192" s="144"/>
+      <c r="J192" s="144"/>
+      <c r="K192" s="145"/>
     </row>
     <row r="193" spans="1:14" s="1" customFormat="1">
       <c r="A193" s="32">
@@ -22508,16 +22523,16 @@
         <v>ABF</v>
       </c>
       <c r="C193" s="33"/>
-      <c r="D193" s="160" t="s">
+      <c r="D193" s="146" t="s">
         <v>362</v>
       </c>
-      <c r="E193" s="161"/>
-      <c r="F193" s="161"/>
-      <c r="G193" s="161"/>
-      <c r="H193" s="161"/>
-      <c r="I193" s="161"/>
-      <c r="J193" s="161"/>
-      <c r="K193" s="162"/>
+      <c r="E193" s="147"/>
+      <c r="F193" s="147"/>
+      <c r="G193" s="147"/>
+      <c r="H193" s="147"/>
+      <c r="I193" s="147"/>
+      <c r="J193" s="147"/>
+      <c r="K193" s="148"/>
       <c r="L193" s="57"/>
       <c r="M193" s="58"/>
       <c r="N193" s="58"/>
@@ -22532,15 +22547,15 @@
         <v>AC0</v>
       </c>
       <c r="C194" s="39"/>
-      <c r="D194" s="150" t="s">
+      <c r="D194" s="149" t="s">
         <v>363</v>
       </c>
-      <c r="E194" s="143"/>
-      <c r="F194" s="143"/>
-      <c r="G194" s="143"/>
-      <c r="H194" s="143"/>
-      <c r="I194" s="143"/>
-      <c r="J194" s="143"/>
+      <c r="E194" s="150"/>
+      <c r="F194" s="150"/>
+      <c r="G194" s="150"/>
+      <c r="H194" s="150"/>
+      <c r="I194" s="150"/>
+      <c r="J194" s="150"/>
       <c r="K194" s="151"/>
     </row>
     <row r="195" spans="1:14">
@@ -22553,16 +22568,16 @@
         <v>AC1</v>
       </c>
       <c r="C195" s="13"/>
-      <c r="D195" s="134" t="s">
+      <c r="D195" s="143" t="s">
         <v>364</v>
       </c>
-      <c r="E195" s="135"/>
-      <c r="F195" s="135"/>
-      <c r="G195" s="135"/>
-      <c r="H195" s="135"/>
-      <c r="I195" s="135"/>
-      <c r="J195" s="135"/>
-      <c r="K195" s="136"/>
+      <c r="E195" s="144"/>
+      <c r="F195" s="144"/>
+      <c r="G195" s="144"/>
+      <c r="H195" s="144"/>
+      <c r="I195" s="144"/>
+      <c r="J195" s="144"/>
+      <c r="K195" s="145"/>
     </row>
     <row r="196" spans="1:14">
       <c r="A196" s="12">
@@ -22574,16 +22589,16 @@
         <v>AC2</v>
       </c>
       <c r="C196" s="13"/>
-      <c r="D196" s="134" t="s">
+      <c r="D196" s="143" t="s">
         <v>365</v>
       </c>
-      <c r="E196" s="135"/>
-      <c r="F196" s="135"/>
-      <c r="G196" s="135"/>
-      <c r="H196" s="135"/>
-      <c r="I196" s="135"/>
-      <c r="J196" s="135"/>
-      <c r="K196" s="136"/>
+      <c r="E196" s="144"/>
+      <c r="F196" s="144"/>
+      <c r="G196" s="144"/>
+      <c r="H196" s="144"/>
+      <c r="I196" s="144"/>
+      <c r="J196" s="144"/>
+      <c r="K196" s="145"/>
     </row>
     <row r="197" spans="1:14">
       <c r="A197" s="12">
@@ -22595,16 +22610,16 @@
         <v>AC3</v>
       </c>
       <c r="C197" s="13"/>
-      <c r="D197" s="134" t="s">
+      <c r="D197" s="143" t="s">
         <v>366</v>
       </c>
-      <c r="E197" s="135"/>
-      <c r="F197" s="135"/>
-      <c r="G197" s="135"/>
-      <c r="H197" s="135"/>
-      <c r="I197" s="135"/>
-      <c r="J197" s="135"/>
-      <c r="K197" s="136"/>
+      <c r="E197" s="144"/>
+      <c r="F197" s="144"/>
+      <c r="G197" s="144"/>
+      <c r="H197" s="144"/>
+      <c r="I197" s="144"/>
+      <c r="J197" s="144"/>
+      <c r="K197" s="145"/>
     </row>
     <row r="198" spans="1:14">
       <c r="A198" s="12">
@@ -22616,16 +22631,16 @@
         <v>AC4</v>
       </c>
       <c r="C198" s="13"/>
-      <c r="D198" s="134" t="s">
+      <c r="D198" s="143" t="s">
         <v>367</v>
       </c>
-      <c r="E198" s="135"/>
-      <c r="F198" s="135"/>
-      <c r="G198" s="135"/>
-      <c r="H198" s="135"/>
-      <c r="I198" s="135"/>
-      <c r="J198" s="135"/>
-      <c r="K198" s="136"/>
+      <c r="E198" s="144"/>
+      <c r="F198" s="144"/>
+      <c r="G198" s="144"/>
+      <c r="H198" s="144"/>
+      <c r="I198" s="144"/>
+      <c r="J198" s="144"/>
+      <c r="K198" s="145"/>
     </row>
     <row r="199" spans="1:14">
       <c r="A199" s="12">
@@ -22656,16 +22671,16 @@
         <v>AC6</v>
       </c>
       <c r="C200" s="13"/>
-      <c r="D200" s="134" t="s">
+      <c r="D200" s="143" t="s">
         <v>368</v>
       </c>
-      <c r="E200" s="135"/>
-      <c r="F200" s="135"/>
-      <c r="G200" s="135"/>
-      <c r="H200" s="135"/>
-      <c r="I200" s="135"/>
-      <c r="J200" s="135"/>
-      <c r="K200" s="136"/>
+      <c r="E200" s="144"/>
+      <c r="F200" s="144"/>
+      <c r="G200" s="144"/>
+      <c r="H200" s="144"/>
+      <c r="I200" s="144"/>
+      <c r="J200" s="144"/>
+      <c r="K200" s="145"/>
     </row>
     <row r="201" spans="1:14">
       <c r="A201" s="12">
@@ -22696,16 +22711,16 @@
         <v>AC8</v>
       </c>
       <c r="C202" s="13"/>
-      <c r="D202" s="157" t="s">
+      <c r="D202" s="168" t="s">
         <v>369</v>
       </c>
-      <c r="E202" s="158"/>
-      <c r="F202" s="158"/>
-      <c r="G202" s="158"/>
-      <c r="H202" s="158"/>
-      <c r="I202" s="158"/>
-      <c r="J202" s="158"/>
-      <c r="K202" s="159"/>
+      <c r="E202" s="169"/>
+      <c r="F202" s="169"/>
+      <c r="G202" s="169"/>
+      <c r="H202" s="169"/>
+      <c r="I202" s="169"/>
+      <c r="J202" s="169"/>
+      <c r="K202" s="170"/>
     </row>
     <row r="203" spans="1:14">
       <c r="A203" s="12">
@@ -22736,16 +22751,16 @@
         <v>ACA</v>
       </c>
       <c r="C204" s="13"/>
-      <c r="D204" s="134" t="s">
+      <c r="D204" s="143" t="s">
         <v>370</v>
       </c>
-      <c r="E204" s="135"/>
-      <c r="F204" s="135"/>
-      <c r="G204" s="135"/>
-      <c r="H204" s="135"/>
-      <c r="I204" s="135"/>
-      <c r="J204" s="135"/>
-      <c r="K204" s="136"/>
+      <c r="E204" s="144"/>
+      <c r="F204" s="144"/>
+      <c r="G204" s="144"/>
+      <c r="H204" s="144"/>
+      <c r="I204" s="144"/>
+      <c r="J204" s="144"/>
+      <c r="K204" s="145"/>
     </row>
     <row r="205" spans="1:14">
       <c r="A205" s="12">
@@ -22776,16 +22791,16 @@
         <v>ACC</v>
       </c>
       <c r="C206" s="13"/>
-      <c r="D206" s="134" t="s">
+      <c r="D206" s="143" t="s">
         <v>370</v>
       </c>
-      <c r="E206" s="135"/>
-      <c r="F206" s="135"/>
-      <c r="G206" s="135"/>
-      <c r="H206" s="135"/>
-      <c r="I206" s="135"/>
-      <c r="J206" s="135"/>
-      <c r="K206" s="136"/>
+      <c r="E206" s="144"/>
+      <c r="F206" s="144"/>
+      <c r="G206" s="144"/>
+      <c r="H206" s="144"/>
+      <c r="I206" s="144"/>
+      <c r="J206" s="144"/>
+      <c r="K206" s="145"/>
     </row>
     <row r="207" spans="1:14">
       <c r="A207" s="12">
@@ -22816,16 +22831,16 @@
         <v>ACE</v>
       </c>
       <c r="C208" s="13"/>
-      <c r="D208" s="134" t="s">
+      <c r="D208" s="143" t="s">
         <v>371</v>
       </c>
-      <c r="E208" s="135"/>
-      <c r="F208" s="135"/>
-      <c r="G208" s="135"/>
-      <c r="H208" s="135"/>
-      <c r="I208" s="135"/>
-      <c r="J208" s="135"/>
-      <c r="K208" s="136"/>
+      <c r="E208" s="144"/>
+      <c r="F208" s="144"/>
+      <c r="G208" s="144"/>
+      <c r="H208" s="144"/>
+      <c r="I208" s="144"/>
+      <c r="J208" s="144"/>
+      <c r="K208" s="145"/>
     </row>
     <row r="209" spans="1:14" s="1" customFormat="1">
       <c r="A209" s="32">
@@ -22859,15 +22874,15 @@
         <v>AD0</v>
       </c>
       <c r="C210" s="39"/>
-      <c r="D210" s="150" t="s">
+      <c r="D210" s="149" t="s">
         <v>371</v>
       </c>
-      <c r="E210" s="143"/>
-      <c r="F210" s="143"/>
-      <c r="G210" s="143"/>
-      <c r="H210" s="143"/>
-      <c r="I210" s="143"/>
-      <c r="J210" s="143"/>
+      <c r="E210" s="150"/>
+      <c r="F210" s="150"/>
+      <c r="G210" s="150"/>
+      <c r="H210" s="150"/>
+      <c r="I210" s="150"/>
+      <c r="J210" s="150"/>
       <c r="K210" s="151"/>
     </row>
     <row r="211" spans="1:14">
@@ -22937,16 +22952,16 @@
         <v>AD4</v>
       </c>
       <c r="C214" s="13"/>
-      <c r="D214" s="134" t="s">
+      <c r="D214" s="143" t="s">
         <v>372</v>
       </c>
-      <c r="E214" s="135"/>
-      <c r="F214" s="135"/>
-      <c r="G214" s="135"/>
-      <c r="H214" s="135"/>
-      <c r="I214" s="135"/>
-      <c r="J214" s="135"/>
-      <c r="K214" s="136"/>
+      <c r="E214" s="144"/>
+      <c r="F214" s="144"/>
+      <c r="G214" s="144"/>
+      <c r="H214" s="144"/>
+      <c r="I214" s="144"/>
+      <c r="J214" s="144"/>
+      <c r="K214" s="145"/>
     </row>
     <row r="215" spans="1:14">
       <c r="A215" s="12">
@@ -22977,16 +22992,16 @@
         <v>AD6</v>
       </c>
       <c r="C216" s="13"/>
-      <c r="D216" s="148" t="s">
+      <c r="D216" s="158" t="s">
         <v>373</v>
       </c>
-      <c r="E216" s="137"/>
-      <c r="F216" s="137"/>
-      <c r="G216" s="137"/>
-      <c r="H216" s="137"/>
-      <c r="I216" s="137"/>
-      <c r="J216" s="137"/>
-      <c r="K216" s="149"/>
+      <c r="E216" s="153"/>
+      <c r="F216" s="153"/>
+      <c r="G216" s="153"/>
+      <c r="H216" s="153"/>
+      <c r="I216" s="153"/>
+      <c r="J216" s="153"/>
+      <c r="K216" s="159"/>
     </row>
     <row r="217" spans="1:14">
       <c r="A217" s="12">
@@ -22998,13 +23013,13 @@
         <v>AD7</v>
       </c>
       <c r="C217" s="13"/>
-      <c r="D217" s="150"/>
-      <c r="E217" s="143"/>
-      <c r="F217" s="143"/>
-      <c r="G217" s="143"/>
-      <c r="H217" s="143"/>
-      <c r="I217" s="143"/>
-      <c r="J217" s="143"/>
+      <c r="D217" s="149"/>
+      <c r="E217" s="150"/>
+      <c r="F217" s="150"/>
+      <c r="G217" s="150"/>
+      <c r="H217" s="150"/>
+      <c r="I217" s="150"/>
+      <c r="J217" s="150"/>
       <c r="K217" s="151"/>
     </row>
     <row r="218" spans="1:14">
@@ -23017,16 +23032,16 @@
         <v>AD8</v>
       </c>
       <c r="C218" s="13"/>
-      <c r="D218" s="148" t="s">
+      <c r="D218" s="158" t="s">
         <v>374</v>
       </c>
-      <c r="E218" s="137"/>
-      <c r="F218" s="137"/>
-      <c r="G218" s="137"/>
-      <c r="H218" s="137"/>
-      <c r="I218" s="137"/>
-      <c r="J218" s="137"/>
-      <c r="K218" s="149"/>
+      <c r="E218" s="153"/>
+      <c r="F218" s="153"/>
+      <c r="G218" s="153"/>
+      <c r="H218" s="153"/>
+      <c r="I218" s="153"/>
+      <c r="J218" s="153"/>
+      <c r="K218" s="159"/>
     </row>
     <row r="219" spans="1:14">
       <c r="A219" s="12">
@@ -23038,13 +23053,13 @@
         <v>AD9</v>
       </c>
       <c r="C219" s="13"/>
-      <c r="D219" s="150"/>
-      <c r="E219" s="143"/>
-      <c r="F219" s="143"/>
-      <c r="G219" s="143"/>
-      <c r="H219" s="143"/>
-      <c r="I219" s="143"/>
-      <c r="J219" s="143"/>
+      <c r="D219" s="149"/>
+      <c r="E219" s="150"/>
+      <c r="F219" s="150"/>
+      <c r="G219" s="150"/>
+      <c r="H219" s="150"/>
+      <c r="I219" s="150"/>
+      <c r="J219" s="150"/>
       <c r="K219" s="151"/>
     </row>
     <row r="220" spans="1:14">
@@ -23057,16 +23072,16 @@
         <v>ADA</v>
       </c>
       <c r="C220" s="13"/>
-      <c r="D220" s="148" t="s">
+      <c r="D220" s="158" t="s">
         <v>375</v>
       </c>
-      <c r="E220" s="137"/>
-      <c r="F220" s="137"/>
-      <c r="G220" s="137"/>
-      <c r="H220" s="137"/>
-      <c r="I220" s="137"/>
-      <c r="J220" s="137"/>
-      <c r="K220" s="149"/>
+      <c r="E220" s="153"/>
+      <c r="F220" s="153"/>
+      <c r="G220" s="153"/>
+      <c r="H220" s="153"/>
+      <c r="I220" s="153"/>
+      <c r="J220" s="153"/>
+      <c r="K220" s="159"/>
     </row>
     <row r="221" spans="1:14">
       <c r="A221" s="12">
@@ -23078,13 +23093,13 @@
         <v>ADB</v>
       </c>
       <c r="C221" s="13"/>
-      <c r="D221" s="150"/>
-      <c r="E221" s="143"/>
-      <c r="F221" s="143"/>
-      <c r="G221" s="143"/>
-      <c r="H221" s="143"/>
-      <c r="I221" s="143"/>
-      <c r="J221" s="143"/>
+      <c r="D221" s="149"/>
+      <c r="E221" s="150"/>
+      <c r="F221" s="150"/>
+      <c r="G221" s="150"/>
+      <c r="H221" s="150"/>
+      <c r="I221" s="150"/>
+      <c r="J221" s="150"/>
       <c r="K221" s="151"/>
     </row>
     <row r="222" spans="1:14">
@@ -23097,16 +23112,16 @@
         <v>ADC</v>
       </c>
       <c r="C222" s="13"/>
-      <c r="D222" s="134" t="s">
+      <c r="D222" s="143" t="s">
         <v>376</v>
       </c>
-      <c r="E222" s="135"/>
-      <c r="F222" s="135"/>
-      <c r="G222" s="135"/>
-      <c r="H222" s="135"/>
-      <c r="I222" s="135"/>
-      <c r="J222" s="135"/>
-      <c r="K222" s="136"/>
+      <c r="E222" s="144"/>
+      <c r="F222" s="144"/>
+      <c r="G222" s="144"/>
+      <c r="H222" s="144"/>
+      <c r="I222" s="144"/>
+      <c r="J222" s="144"/>
+      <c r="K222" s="145"/>
     </row>
     <row r="223" spans="1:14">
       <c r="A223" s="12">
@@ -23137,16 +23152,16 @@
         <v>ADE</v>
       </c>
       <c r="C224" s="13"/>
-      <c r="D224" s="134" t="s">
+      <c r="D224" s="143" t="s">
         <v>377</v>
       </c>
-      <c r="E224" s="135"/>
-      <c r="F224" s="135"/>
-      <c r="G224" s="135"/>
-      <c r="H224" s="135"/>
-      <c r="I224" s="135"/>
-      <c r="J224" s="135"/>
-      <c r="K224" s="136"/>
+      <c r="E224" s="144"/>
+      <c r="F224" s="144"/>
+      <c r="G224" s="144"/>
+      <c r="H224" s="144"/>
+      <c r="I224" s="144"/>
+      <c r="J224" s="144"/>
+      <c r="K224" s="145"/>
     </row>
     <row r="225" spans="1:14" s="1" customFormat="1">
       <c r="A225" s="32">
@@ -23180,16 +23195,16 @@
         <v>AE0</v>
       </c>
       <c r="C226" s="39"/>
-      <c r="D226" s="154" t="s">
+      <c r="D226" s="165" t="s">
         <v>378</v>
       </c>
-      <c r="E226" s="155"/>
-      <c r="F226" s="155"/>
-      <c r="G226" s="155"/>
-      <c r="H226" s="155"/>
-      <c r="I226" s="155"/>
-      <c r="J226" s="155"/>
-      <c r="K226" s="156"/>
+      <c r="E226" s="166"/>
+      <c r="F226" s="166"/>
+      <c r="G226" s="166"/>
+      <c r="H226" s="166"/>
+      <c r="I226" s="166"/>
+      <c r="J226" s="166"/>
+      <c r="K226" s="167"/>
     </row>
     <row r="227" spans="1:14">
       <c r="A227" s="12">
@@ -23334,16 +23349,16 @@
         <v>AE8</v>
       </c>
       <c r="C234" s="13"/>
-      <c r="D234" s="152" t="s">
+      <c r="D234" s="162" t="s">
         <v>379</v>
       </c>
-      <c r="E234" s="132"/>
-      <c r="F234" s="132"/>
-      <c r="G234" s="132"/>
-      <c r="H234" s="132"/>
-      <c r="I234" s="132"/>
-      <c r="J234" s="132"/>
-      <c r="K234" s="153"/>
+      <c r="E234" s="163"/>
+      <c r="F234" s="163"/>
+      <c r="G234" s="163"/>
+      <c r="H234" s="163"/>
+      <c r="I234" s="163"/>
+      <c r="J234" s="163"/>
+      <c r="K234" s="164"/>
     </row>
     <row r="235" spans="1:14">
       <c r="A235" s="12">
@@ -23412,16 +23427,16 @@
         <v>AEC</v>
       </c>
       <c r="C238" s="13"/>
-      <c r="D238" s="141" t="s">
+      <c r="D238" s="152" t="s">
         <v>380</v>
       </c>
-      <c r="E238" s="137"/>
-      <c r="F238" s="137"/>
-      <c r="G238" s="137"/>
-      <c r="H238" s="137"/>
-      <c r="I238" s="137"/>
-      <c r="J238" s="137"/>
-      <c r="K238" s="138"/>
+      <c r="E238" s="153"/>
+      <c r="F238" s="153"/>
+      <c r="G238" s="153"/>
+      <c r="H238" s="153"/>
+      <c r="I238" s="153"/>
+      <c r="J238" s="153"/>
+      <c r="K238" s="154"/>
     </row>
     <row r="239" spans="1:14">
       <c r="A239" s="12">
@@ -23433,14 +23448,14 @@
         <v>AED</v>
       </c>
       <c r="C239" s="13"/>
-      <c r="D239" s="142"/>
-      <c r="E239" s="143"/>
-      <c r="F239" s="143"/>
-      <c r="G239" s="143"/>
-      <c r="H239" s="143"/>
-      <c r="I239" s="143"/>
-      <c r="J239" s="143"/>
-      <c r="K239" s="144"/>
+      <c r="D239" s="160"/>
+      <c r="E239" s="150"/>
+      <c r="F239" s="150"/>
+      <c r="G239" s="150"/>
+      <c r="H239" s="150"/>
+      <c r="I239" s="150"/>
+      <c r="J239" s="150"/>
+      <c r="K239" s="161"/>
     </row>
     <row r="240" spans="1:14">
       <c r="A240" s="12">
@@ -23452,16 +23467,16 @@
         <v>AEE</v>
       </c>
       <c r="C240" s="70"/>
-      <c r="D240" s="137" t="s">
+      <c r="D240" s="153" t="s">
         <v>381</v>
       </c>
-      <c r="E240" s="137"/>
-      <c r="F240" s="137"/>
-      <c r="G240" s="137"/>
-      <c r="H240" s="137"/>
-      <c r="I240" s="137"/>
-      <c r="J240" s="137"/>
-      <c r="K240" s="138"/>
+      <c r="E240" s="153"/>
+      <c r="F240" s="153"/>
+      <c r="G240" s="153"/>
+      <c r="H240" s="153"/>
+      <c r="I240" s="153"/>
+      <c r="J240" s="153"/>
+      <c r="K240" s="154"/>
     </row>
     <row r="241" spans="1:14" s="1" customFormat="1">
       <c r="A241" s="32">
@@ -23473,14 +23488,14 @@
         <v>AEF</v>
       </c>
       <c r="C241" s="34"/>
-      <c r="D241" s="139"/>
-      <c r="E241" s="139"/>
-      <c r="F241" s="139"/>
-      <c r="G241" s="139"/>
-      <c r="H241" s="139"/>
-      <c r="I241" s="139"/>
-      <c r="J241" s="139"/>
-      <c r="K241" s="140"/>
+      <c r="D241" s="173"/>
+      <c r="E241" s="173"/>
+      <c r="F241" s="173"/>
+      <c r="G241" s="173"/>
+      <c r="H241" s="173"/>
+      <c r="I241" s="173"/>
+      <c r="J241" s="173"/>
+      <c r="K241" s="174"/>
       <c r="L241" s="57"/>
       <c r="M241" s="58"/>
       <c r="N241" s="58"/>
@@ -23671,16 +23686,16 @@
         <v>AF8</v>
       </c>
       <c r="C250" s="13"/>
-      <c r="D250" s="131" t="s">
+      <c r="D250" s="171" t="s">
         <v>382</v>
       </c>
-      <c r="E250" s="132"/>
-      <c r="F250" s="132"/>
-      <c r="G250" s="132"/>
-      <c r="H250" s="132"/>
-      <c r="I250" s="132"/>
-      <c r="J250" s="132"/>
-      <c r="K250" s="133"/>
+      <c r="E250" s="163"/>
+      <c r="F250" s="163"/>
+      <c r="G250" s="163"/>
+      <c r="H250" s="163"/>
+      <c r="I250" s="163"/>
+      <c r="J250" s="163"/>
+      <c r="K250" s="172"/>
     </row>
     <row r="251" spans="1:14">
       <c r="A251" s="12">
@@ -24249,16 +24264,16 @@
         <v>B16</v>
       </c>
       <c r="C280" s="13"/>
-      <c r="D280" s="134" t="s">
+      <c r="D280" s="143" t="s">
         <v>383</v>
       </c>
-      <c r="E280" s="135"/>
-      <c r="F280" s="135"/>
-      <c r="G280" s="135"/>
-      <c r="H280" s="135"/>
-      <c r="I280" s="135"/>
-      <c r="J280" s="135"/>
-      <c r="K280" s="136"/>
+      <c r="E280" s="144"/>
+      <c r="F280" s="144"/>
+      <c r="G280" s="144"/>
+      <c r="H280" s="144"/>
+      <c r="I280" s="144"/>
+      <c r="J280" s="144"/>
+      <c r="K280" s="145"/>
     </row>
     <row r="281" spans="1:14">
       <c r="A281" s="12">
@@ -24365,16 +24380,16 @@
         <v>B1C</v>
       </c>
       <c r="C286" s="13"/>
-      <c r="D286" s="134" t="s">
+      <c r="D286" s="143" t="s">
         <v>384</v>
       </c>
-      <c r="E286" s="135"/>
-      <c r="F286" s="135"/>
-      <c r="G286" s="135"/>
-      <c r="H286" s="135"/>
-      <c r="I286" s="135"/>
-      <c r="J286" s="135"/>
-      <c r="K286" s="136"/>
+      <c r="E286" s="144"/>
+      <c r="F286" s="144"/>
+      <c r="G286" s="144"/>
+      <c r="H286" s="144"/>
+      <c r="I286" s="144"/>
+      <c r="J286" s="144"/>
+      <c r="K286" s="145"/>
     </row>
     <row r="287" spans="1:14">
       <c r="A287" s="12">
@@ -24524,16 +24539,16 @@
         <v>B24</v>
       </c>
       <c r="C294" s="13"/>
-      <c r="D294" s="134" t="s">
+      <c r="D294" s="143" t="s">
         <v>443</v>
       </c>
-      <c r="E294" s="135"/>
-      <c r="F294" s="135"/>
-      <c r="G294" s="135"/>
-      <c r="H294" s="135"/>
-      <c r="I294" s="135"/>
-      <c r="J294" s="135"/>
-      <c r="K294" s="136"/>
+      <c r="E294" s="144"/>
+      <c r="F294" s="144"/>
+      <c r="G294" s="144"/>
+      <c r="H294" s="144"/>
+      <c r="I294" s="144"/>
+      <c r="J294" s="144"/>
+      <c r="K294" s="145"/>
     </row>
     <row r="295" spans="1:14">
       <c r="A295" s="12">
@@ -24564,16 +24579,16 @@
         <v>B26</v>
       </c>
       <c r="C296" s="13"/>
-      <c r="D296" s="134" t="s">
+      <c r="D296" s="143" t="s">
         <v>444</v>
       </c>
-      <c r="E296" s="135"/>
-      <c r="F296" s="135"/>
-      <c r="G296" s="135"/>
-      <c r="H296" s="135"/>
-      <c r="I296" s="135"/>
-      <c r="J296" s="135"/>
-      <c r="K296" s="136"/>
+      <c r="E296" s="144"/>
+      <c r="F296" s="144"/>
+      <c r="G296" s="144"/>
+      <c r="H296" s="144"/>
+      <c r="I296" s="144"/>
+      <c r="J296" s="144"/>
+      <c r="K296" s="145"/>
     </row>
     <row r="297" spans="1:14">
       <c r="A297" s="12">
@@ -24604,16 +24619,16 @@
         <v>B28</v>
       </c>
       <c r="C298" s="13"/>
-      <c r="D298" s="141" t="s">
+      <c r="D298" s="152" t="s">
         <v>386</v>
       </c>
-      <c r="E298" s="137"/>
-      <c r="F298" s="137"/>
-      <c r="G298" s="137"/>
-      <c r="H298" s="137"/>
-      <c r="I298" s="137"/>
-      <c r="J298" s="137"/>
-      <c r="K298" s="138"/>
+      <c r="E298" s="153"/>
+      <c r="F298" s="153"/>
+      <c r="G298" s="153"/>
+      <c r="H298" s="153"/>
+      <c r="I298" s="153"/>
+      <c r="J298" s="153"/>
+      <c r="K298" s="154"/>
     </row>
     <row r="299" spans="1:14">
       <c r="A299" s="12">
@@ -24625,14 +24640,14 @@
         <v>B29</v>
       </c>
       <c r="C299" s="13"/>
-      <c r="D299" s="142"/>
-      <c r="E299" s="143"/>
-      <c r="F299" s="143"/>
-      <c r="G299" s="143"/>
-      <c r="H299" s="143"/>
-      <c r="I299" s="143"/>
-      <c r="J299" s="143"/>
-      <c r="K299" s="144"/>
+      <c r="D299" s="160"/>
+      <c r="E299" s="150"/>
+      <c r="F299" s="150"/>
+      <c r="G299" s="150"/>
+      <c r="H299" s="150"/>
+      <c r="I299" s="150"/>
+      <c r="J299" s="150"/>
+      <c r="K299" s="161"/>
     </row>
     <row r="300" spans="1:14">
       <c r="A300" s="12">
@@ -24644,16 +24659,16 @@
         <v>B2A</v>
       </c>
       <c r="C300" s="13"/>
-      <c r="D300" s="141" t="s">
+      <c r="D300" s="152" t="s">
         <v>387</v>
       </c>
-      <c r="E300" s="137"/>
-      <c r="F300" s="137"/>
-      <c r="G300" s="137"/>
-      <c r="H300" s="137"/>
-      <c r="I300" s="137"/>
-      <c r="J300" s="137"/>
-      <c r="K300" s="138"/>
+      <c r="E300" s="153"/>
+      <c r="F300" s="153"/>
+      <c r="G300" s="153"/>
+      <c r="H300" s="153"/>
+      <c r="I300" s="153"/>
+      <c r="J300" s="153"/>
+      <c r="K300" s="154"/>
     </row>
     <row r="301" spans="1:14">
       <c r="A301" s="12">
@@ -24665,14 +24680,14 @@
         <v>B2B</v>
       </c>
       <c r="C301" s="13"/>
-      <c r="D301" s="142"/>
-      <c r="E301" s="143"/>
-      <c r="F301" s="143"/>
-      <c r="G301" s="143"/>
-      <c r="H301" s="143"/>
-      <c r="I301" s="143"/>
-      <c r="J301" s="143"/>
-      <c r="K301" s="144"/>
+      <c r="D301" s="160"/>
+      <c r="E301" s="150"/>
+      <c r="F301" s="150"/>
+      <c r="G301" s="150"/>
+      <c r="H301" s="150"/>
+      <c r="I301" s="150"/>
+      <c r="J301" s="150"/>
+      <c r="K301" s="161"/>
     </row>
     <row r="302" spans="1:14">
       <c r="A302" s="12">
@@ -24684,16 +24699,16 @@
         <v>B2C</v>
       </c>
       <c r="C302" s="13"/>
-      <c r="D302" s="141" t="s">
+      <c r="D302" s="152" t="s">
         <v>388</v>
       </c>
-      <c r="E302" s="137"/>
-      <c r="F302" s="137"/>
-      <c r="G302" s="137"/>
-      <c r="H302" s="137"/>
-      <c r="I302" s="137"/>
-      <c r="J302" s="137"/>
-      <c r="K302" s="138"/>
+      <c r="E302" s="153"/>
+      <c r="F302" s="153"/>
+      <c r="G302" s="153"/>
+      <c r="H302" s="153"/>
+      <c r="I302" s="153"/>
+      <c r="J302" s="153"/>
+      <c r="K302" s="154"/>
     </row>
     <row r="303" spans="1:14">
       <c r="A303" s="12">
@@ -24705,14 +24720,14 @@
         <v>B2D</v>
       </c>
       <c r="C303" s="13"/>
-      <c r="D303" s="142"/>
-      <c r="E303" s="143"/>
-      <c r="F303" s="143"/>
-      <c r="G303" s="143"/>
-      <c r="H303" s="143"/>
-      <c r="I303" s="143"/>
-      <c r="J303" s="143"/>
-      <c r="K303" s="144"/>
+      <c r="D303" s="160"/>
+      <c r="E303" s="150"/>
+      <c r="F303" s="150"/>
+      <c r="G303" s="150"/>
+      <c r="H303" s="150"/>
+      <c r="I303" s="150"/>
+      <c r="J303" s="150"/>
+      <c r="K303" s="161"/>
     </row>
     <row r="304" spans="1:14">
       <c r="A304" s="12">
@@ -24724,16 +24739,16 @@
         <v>B2E</v>
       </c>
       <c r="C304" s="13"/>
-      <c r="D304" s="141" t="s">
+      <c r="D304" s="152" t="s">
         <v>389</v>
       </c>
-      <c r="E304" s="137"/>
-      <c r="F304" s="137"/>
-      <c r="G304" s="137"/>
-      <c r="H304" s="137"/>
-      <c r="I304" s="137"/>
-      <c r="J304" s="137"/>
-      <c r="K304" s="138"/>
+      <c r="E304" s="153"/>
+      <c r="F304" s="153"/>
+      <c r="G304" s="153"/>
+      <c r="H304" s="153"/>
+      <c r="I304" s="153"/>
+      <c r="J304" s="153"/>
+      <c r="K304" s="154"/>
     </row>
     <row r="305" spans="1:14" s="1" customFormat="1">
       <c r="A305" s="32">
@@ -24745,14 +24760,14 @@
         <v>B2F</v>
       </c>
       <c r="C305" s="33"/>
-      <c r="D305" s="142"/>
-      <c r="E305" s="143"/>
-      <c r="F305" s="143"/>
-      <c r="G305" s="143"/>
-      <c r="H305" s="143"/>
-      <c r="I305" s="143"/>
-      <c r="J305" s="143"/>
-      <c r="K305" s="144"/>
+      <c r="D305" s="160"/>
+      <c r="E305" s="150"/>
+      <c r="F305" s="150"/>
+      <c r="G305" s="150"/>
+      <c r="H305" s="150"/>
+      <c r="I305" s="150"/>
+      <c r="J305" s="150"/>
+      <c r="K305" s="161"/>
       <c r="L305" s="57"/>
       <c r="M305" s="58"/>
       <c r="N305" s="58"/>
@@ -24767,16 +24782,16 @@
         <v>B30</v>
       </c>
       <c r="C306" s="39"/>
-      <c r="D306" s="141" t="s">
+      <c r="D306" s="152" t="s">
         <v>390</v>
       </c>
-      <c r="E306" s="137"/>
-      <c r="F306" s="137"/>
-      <c r="G306" s="137"/>
-      <c r="H306" s="137"/>
-      <c r="I306" s="137"/>
-      <c r="J306" s="137"/>
-      <c r="K306" s="138"/>
+      <c r="E306" s="153"/>
+      <c r="F306" s="153"/>
+      <c r="G306" s="153"/>
+      <c r="H306" s="153"/>
+      <c r="I306" s="153"/>
+      <c r="J306" s="153"/>
+      <c r="K306" s="154"/>
     </row>
     <row r="307" spans="1:14">
       <c r="A307" s="12">
@@ -24788,14 +24803,14 @@
         <v>B31</v>
       </c>
       <c r="C307" s="13"/>
-      <c r="D307" s="142"/>
-      <c r="E307" s="143"/>
-      <c r="F307" s="143"/>
-      <c r="G307" s="143"/>
-      <c r="H307" s="143"/>
-      <c r="I307" s="143"/>
-      <c r="J307" s="143"/>
-      <c r="K307" s="144"/>
+      <c r="D307" s="160"/>
+      <c r="E307" s="150"/>
+      <c r="F307" s="150"/>
+      <c r="G307" s="150"/>
+      <c r="H307" s="150"/>
+      <c r="I307" s="150"/>
+      <c r="J307" s="150"/>
+      <c r="K307" s="161"/>
     </row>
     <row r="308" spans="1:14">
       <c r="A308" s="12">
@@ -24807,16 +24822,16 @@
         <v>B32</v>
       </c>
       <c r="C308" s="13"/>
-      <c r="D308" s="141" t="s">
+      <c r="D308" s="152" t="s">
         <v>391</v>
       </c>
-      <c r="E308" s="137"/>
-      <c r="F308" s="137"/>
-      <c r="G308" s="137"/>
-      <c r="H308" s="137"/>
-      <c r="I308" s="137"/>
-      <c r="J308" s="137"/>
-      <c r="K308" s="138"/>
+      <c r="E308" s="153"/>
+      <c r="F308" s="153"/>
+      <c r="G308" s="153"/>
+      <c r="H308" s="153"/>
+      <c r="I308" s="153"/>
+      <c r="J308" s="153"/>
+      <c r="K308" s="154"/>
     </row>
     <row r="309" spans="1:14">
       <c r="A309" s="12">
@@ -24828,14 +24843,14 @@
         <v>B33</v>
       </c>
       <c r="C309" s="13"/>
-      <c r="D309" s="142"/>
-      <c r="E309" s="143"/>
-      <c r="F309" s="143"/>
-      <c r="G309" s="143"/>
-      <c r="H309" s="143"/>
-      <c r="I309" s="143"/>
-      <c r="J309" s="143"/>
-      <c r="K309" s="144"/>
+      <c r="D309" s="160"/>
+      <c r="E309" s="150"/>
+      <c r="F309" s="150"/>
+      <c r="G309" s="150"/>
+      <c r="H309" s="150"/>
+      <c r="I309" s="150"/>
+      <c r="J309" s="150"/>
+      <c r="K309" s="161"/>
     </row>
     <row r="310" spans="1:14">
       <c r="A310" s="12">
@@ -28715,29 +28730,13 @@
     </row>
   </sheetData>
   <mergeCells count="46">
-    <mergeCell ref="D178:K178"/>
-    <mergeCell ref="D182:K182"/>
-    <mergeCell ref="D183:K183"/>
-    <mergeCell ref="D184:K184"/>
-    <mergeCell ref="D185:K185"/>
-    <mergeCell ref="D186:K186"/>
-    <mergeCell ref="D187:K187"/>
-    <mergeCell ref="D188:K188"/>
-    <mergeCell ref="D189:K189"/>
-    <mergeCell ref="D190:K190"/>
-    <mergeCell ref="D191:K191"/>
-    <mergeCell ref="D192:K192"/>
-    <mergeCell ref="D193:K193"/>
-    <mergeCell ref="D194:K194"/>
-    <mergeCell ref="D195:K195"/>
-    <mergeCell ref="D208:K208"/>
-    <mergeCell ref="D210:K210"/>
-    <mergeCell ref="D214:K214"/>
-    <mergeCell ref="D196:K196"/>
-    <mergeCell ref="D197:K197"/>
-    <mergeCell ref="D198:K198"/>
-    <mergeCell ref="D200:K200"/>
-    <mergeCell ref="D202:K202"/>
+    <mergeCell ref="D294:K294"/>
+    <mergeCell ref="D308:K309"/>
+    <mergeCell ref="D298:K299"/>
+    <mergeCell ref="D300:K301"/>
+    <mergeCell ref="D302:K303"/>
+    <mergeCell ref="D304:K305"/>
+    <mergeCell ref="D306:K307"/>
     <mergeCell ref="D280:K280"/>
     <mergeCell ref="D286:K286"/>
     <mergeCell ref="D296:K296"/>
@@ -28754,13 +28753,29 @@
     <mergeCell ref="D250:K250"/>
     <mergeCell ref="D204:K204"/>
     <mergeCell ref="D206:K206"/>
-    <mergeCell ref="D294:K294"/>
-    <mergeCell ref="D308:K309"/>
-    <mergeCell ref="D298:K299"/>
-    <mergeCell ref="D300:K301"/>
-    <mergeCell ref="D302:K303"/>
-    <mergeCell ref="D304:K305"/>
-    <mergeCell ref="D306:K307"/>
+    <mergeCell ref="D208:K208"/>
+    <mergeCell ref="D210:K210"/>
+    <mergeCell ref="D214:K214"/>
+    <mergeCell ref="D196:K196"/>
+    <mergeCell ref="D197:K197"/>
+    <mergeCell ref="D198:K198"/>
+    <mergeCell ref="D200:K200"/>
+    <mergeCell ref="D202:K202"/>
+    <mergeCell ref="D191:K191"/>
+    <mergeCell ref="D192:K192"/>
+    <mergeCell ref="D193:K193"/>
+    <mergeCell ref="D194:K194"/>
+    <mergeCell ref="D195:K195"/>
+    <mergeCell ref="D186:K186"/>
+    <mergeCell ref="D187:K187"/>
+    <mergeCell ref="D188:K188"/>
+    <mergeCell ref="D189:K189"/>
+    <mergeCell ref="D190:K190"/>
+    <mergeCell ref="D178:K178"/>
+    <mergeCell ref="D182:K182"/>
+    <mergeCell ref="D183:K183"/>
+    <mergeCell ref="D184:K184"/>
+    <mergeCell ref="D185:K185"/>
   </mergeCells>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="53" fitToHeight="0" orientation="landscape"/>

</xml_diff>